<commit_message>
Update ARM instructions table
</commit_message>
<xml_diff>
--- a/docs/ARM instructions.xlsx
+++ b/docs/ARM instructions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Drive\Etudes\Supérieur\SI3\Architecture et réseaux\Architecture\PARM\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCDB9F7F-83F1-4EE1-82A0-DB6566979194}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89574475-12C0-4079-93F0-FAB937BBD4C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1E4904EC-9B68-40DD-B685-7BD66B9DE8BA}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="135">
   <si>
     <t>Description</t>
   </si>
@@ -1707,6 +1707,97 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
+      <t>C</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>o</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>mp</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>are</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Add </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>8-bit immediate</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Sub</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>stract 8-bit immediate</t>
+    </r>
+  </si>
+  <si>
+    <t>AL</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>imm11</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
       <t>Al</t>
     </r>
     <r>
@@ -1716,110 +1807,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>ways (unconditional)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">none or </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>AL</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>C</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>o</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>mp</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>are</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Add </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>8-bit immediate</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Sub</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>stract 8-bit immediate</t>
+      <t>ways</t>
     </r>
   </si>
 </sst>
@@ -1998,7 +1986,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="50">
+  <borders count="51">
     <border>
       <left/>
       <right/>
@@ -2476,19 +2464,6 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -2635,16 +2610,38 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="140">
+  <cellXfs count="151">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2680,10 +2677,10 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2737,7 +2734,7 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="15" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2767,10 +2764,10 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2818,7 +2815,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2851,7 +2848,7 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2866,31 +2863,28 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2899,7 +2893,7 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2920,143 +2914,179 @@
     <xf numFmtId="0" fontId="5" fillId="10" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3465,15 +3495,15 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Y65"/>
+  <dimension ref="A1:Z66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="145" zoomScalePageLayoutView="145" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.42578125" style="95" customWidth="1"/>
+    <col min="1" max="1" width="28.7109375" style="93" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" style="77" customWidth="1"/>
     <col min="3" max="5" width="11.42578125" style="77"/>
     <col min="6" max="25" width="3.7109375" style="77" customWidth="1"/>
@@ -3481,50 +3511,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="98" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="102" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="100"/>
-      <c r="D1" s="100"/>
-      <c r="E1" s="101"/>
-      <c r="F1" s="100" t="s">
+      <c r="A1" s="134" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="136" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="127"/>
+      <c r="D1" s="127"/>
+      <c r="E1" s="128"/>
+      <c r="F1" s="127" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="100"/>
-      <c r="H1" s="100"/>
-      <c r="I1" s="100"/>
-      <c r="J1" s="100"/>
-      <c r="K1" s="100"/>
-      <c r="L1" s="100"/>
-      <c r="M1" s="100"/>
-      <c r="N1" s="100"/>
-      <c r="O1" s="100"/>
-      <c r="P1" s="100"/>
-      <c r="Q1" s="100"/>
-      <c r="R1" s="100"/>
-      <c r="S1" s="100"/>
-      <c r="T1" s="100"/>
-      <c r="U1" s="101"/>
-      <c r="V1" s="104" t="s">
+      <c r="G1" s="127"/>
+      <c r="H1" s="127"/>
+      <c r="I1" s="127"/>
+      <c r="J1" s="127"/>
+      <c r="K1" s="127"/>
+      <c r="L1" s="127"/>
+      <c r="M1" s="127"/>
+      <c r="N1" s="127"/>
+      <c r="O1" s="127"/>
+      <c r="P1" s="127"/>
+      <c r="Q1" s="127"/>
+      <c r="R1" s="127"/>
+      <c r="S1" s="127"/>
+      <c r="T1" s="127"/>
+      <c r="U1" s="128"/>
+      <c r="V1" s="126" t="s">
         <v>3</v>
       </c>
-      <c r="W1" s="100"/>
-      <c r="X1" s="100"/>
-      <c r="Y1" s="101"/>
+      <c r="W1" s="127"/>
+      <c r="X1" s="127"/>
+      <c r="Y1" s="128"/>
     </row>
     <row r="2" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="99"/>
+      <c r="A2" s="135"/>
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="100" t="s">
+      <c r="C2" s="127" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="100"/>
-      <c r="E2" s="101"/>
+      <c r="D2" s="127"/>
+      <c r="E2" s="128"/>
       <c r="F2" s="2">
         <v>15</v>
       </c>
@@ -3587,7 +3617,7 @@
       </c>
     </row>
     <row r="3" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="82" t="s">
+      <c r="A3" s="148" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="78"/>
@@ -3600,13 +3630,13 @@
       <c r="G3" s="10">
         <v>0</v>
       </c>
-      <c r="H3" s="103" t="s">
+      <c r="H3" s="111" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="103"/>
-      <c r="J3" s="103"/>
-      <c r="K3" s="103"/>
-      <c r="L3" s="103"/>
+      <c r="I3" s="111"/>
+      <c r="J3" s="111"/>
+      <c r="K3" s="111"/>
+      <c r="L3" s="111"/>
       <c r="M3" s="11"/>
       <c r="N3" s="11"/>
       <c r="O3" s="11"/>
@@ -3622,7 +3652,7 @@
       <c r="Y3" s="12"/>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A4" s="84" t="s">
+      <c r="A4" s="83" t="s">
         <v>77</v>
       </c>
       <c r="B4" s="14" t="s">
@@ -3652,23 +3682,23 @@
       <c r="J4" s="20">
         <v>0</v>
       </c>
-      <c r="K4" s="96" t="s">
+      <c r="K4" s="104" t="s">
         <v>15</v>
       </c>
-      <c r="L4" s="96"/>
-      <c r="M4" s="96"/>
-      <c r="N4" s="96"/>
-      <c r="O4" s="96"/>
-      <c r="P4" s="110" t="s">
+      <c r="L4" s="104"/>
+      <c r="M4" s="104"/>
+      <c r="N4" s="104"/>
+      <c r="O4" s="104"/>
+      <c r="P4" s="133" t="s">
         <v>16</v>
       </c>
-      <c r="Q4" s="110"/>
-      <c r="R4" s="110"/>
-      <c r="S4" s="96" t="s">
+      <c r="Q4" s="133"/>
+      <c r="R4" s="133"/>
+      <c r="S4" s="104" t="s">
         <v>17</v>
       </c>
-      <c r="T4" s="96"/>
-      <c r="U4" s="97"/>
+      <c r="T4" s="104"/>
+      <c r="U4" s="105"/>
       <c r="V4" s="22" t="s">
         <v>18</v>
       </c>
@@ -3681,7 +3711,7 @@
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A5" s="85" t="s">
+      <c r="A5" s="84" t="s">
         <v>79</v>
       </c>
       <c r="B5" s="14" t="s">
@@ -3711,23 +3741,23 @@
       <c r="J5" s="26">
         <v>1</v>
       </c>
-      <c r="K5" s="96" t="s">
+      <c r="K5" s="104" t="s">
         <v>15</v>
       </c>
-      <c r="L5" s="96"/>
-      <c r="M5" s="96"/>
-      <c r="N5" s="96"/>
-      <c r="O5" s="96"/>
-      <c r="P5" s="96" t="s">
+      <c r="L5" s="104"/>
+      <c r="M5" s="104"/>
+      <c r="N5" s="104"/>
+      <c r="O5" s="104"/>
+      <c r="P5" s="104" t="s">
         <v>16</v>
       </c>
-      <c r="Q5" s="96"/>
-      <c r="R5" s="96"/>
-      <c r="S5" s="96" t="s">
+      <c r="Q5" s="104"/>
+      <c r="R5" s="104"/>
+      <c r="S5" s="104" t="s">
         <v>17</v>
       </c>
-      <c r="T5" s="96"/>
-      <c r="U5" s="97"/>
+      <c r="T5" s="104"/>
+      <c r="U5" s="105"/>
       <c r="V5" s="22"/>
       <c r="W5" s="19"/>
       <c r="X5" s="19" t="s">
@@ -3738,7 +3768,7 @@
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A6" s="86" t="s">
+      <c r="A6" s="85" t="s">
         <v>81</v>
       </c>
       <c r="B6" s="14" t="s">
@@ -3768,23 +3798,23 @@
       <c r="J6" s="20">
         <v>0</v>
       </c>
-      <c r="K6" s="96" t="s">
+      <c r="K6" s="104" t="s">
         <v>15</v>
       </c>
-      <c r="L6" s="96"/>
-      <c r="M6" s="96"/>
-      <c r="N6" s="96"/>
-      <c r="O6" s="96"/>
-      <c r="P6" s="96" t="s">
+      <c r="L6" s="104"/>
+      <c r="M6" s="104"/>
+      <c r="N6" s="104"/>
+      <c r="O6" s="104"/>
+      <c r="P6" s="104" t="s">
         <v>16</v>
       </c>
-      <c r="Q6" s="96"/>
-      <c r="R6" s="96"/>
-      <c r="S6" s="96" t="s">
+      <c r="Q6" s="104"/>
+      <c r="R6" s="104"/>
+      <c r="S6" s="104" t="s">
         <v>17</v>
       </c>
-      <c r="T6" s="96"/>
-      <c r="U6" s="97"/>
+      <c r="T6" s="104"/>
+      <c r="U6" s="105"/>
       <c r="V6" s="22" t="s">
         <v>18</v>
       </c>
@@ -3797,7 +3827,7 @@
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A7" s="87" t="s">
+      <c r="A7" s="86" t="s">
         <v>83</v>
       </c>
       <c r="B7" s="14" t="s">
@@ -3833,21 +3863,21 @@
       <c r="L7" s="31">
         <v>0</v>
       </c>
-      <c r="M7" s="96" t="s">
+      <c r="M7" s="104" t="s">
         <v>16</v>
       </c>
-      <c r="N7" s="96"/>
-      <c r="O7" s="96"/>
-      <c r="P7" s="96" t="s">
+      <c r="N7" s="104"/>
+      <c r="O7" s="104"/>
+      <c r="P7" s="104" t="s">
         <v>20</v>
       </c>
-      <c r="Q7" s="96"/>
-      <c r="R7" s="96"/>
-      <c r="S7" s="96" t="s">
+      <c r="Q7" s="104"/>
+      <c r="R7" s="104"/>
+      <c r="S7" s="104" t="s">
         <v>17</v>
       </c>
-      <c r="T7" s="96"/>
-      <c r="U7" s="97"/>
+      <c r="T7" s="104"/>
+      <c r="U7" s="105"/>
       <c r="V7" s="22" t="s">
         <v>18</v>
       </c>
@@ -3862,7 +3892,7 @@
       </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A8" s="85" t="s">
+      <c r="A8" s="84" t="s">
         <v>85</v>
       </c>
       <c r="B8" s="14" t="s">
@@ -3898,21 +3928,21 @@
       <c r="L8" s="32">
         <v>1</v>
       </c>
-      <c r="M8" s="96" t="s">
+      <c r="M8" s="104" t="s">
         <v>16</v>
       </c>
-      <c r="N8" s="96"/>
-      <c r="O8" s="96"/>
-      <c r="P8" s="96" t="s">
+      <c r="N8" s="104"/>
+      <c r="O8" s="104"/>
+      <c r="P8" s="104" t="s">
         <v>20</v>
       </c>
-      <c r="Q8" s="96"/>
-      <c r="R8" s="96"/>
-      <c r="S8" s="96" t="s">
+      <c r="Q8" s="104"/>
+      <c r="R8" s="104"/>
+      <c r="S8" s="104" t="s">
         <v>17</v>
       </c>
-      <c r="T8" s="96"/>
-      <c r="U8" s="97"/>
+      <c r="T8" s="104"/>
+      <c r="U8" s="105"/>
       <c r="V8" s="22" t="s">
         <v>18</v>
       </c>
@@ -3927,7 +3957,7 @@
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A9" s="85" t="s">
+      <c r="A9" s="84" t="s">
         <v>87</v>
       </c>
       <c r="B9" s="14" t="s">
@@ -3963,21 +3993,21 @@
       <c r="L9" s="31">
         <v>0</v>
       </c>
-      <c r="M9" s="96" t="s">
+      <c r="M9" s="104" t="s">
         <v>22</v>
       </c>
-      <c r="N9" s="96"/>
-      <c r="O9" s="96"/>
-      <c r="P9" s="96" t="s">
+      <c r="N9" s="104"/>
+      <c r="O9" s="104"/>
+      <c r="P9" s="104" t="s">
         <v>20</v>
       </c>
-      <c r="Q9" s="96"/>
-      <c r="R9" s="96"/>
-      <c r="S9" s="96" t="s">
+      <c r="Q9" s="104"/>
+      <c r="R9" s="104"/>
+      <c r="S9" s="104" t="s">
         <v>17</v>
       </c>
-      <c r="T9" s="96"/>
-      <c r="U9" s="97"/>
+      <c r="T9" s="104"/>
+      <c r="U9" s="105"/>
       <c r="V9" s="22" t="s">
         <v>18</v>
       </c>
@@ -3992,19 +4022,19 @@
       </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A10" s="86" t="s">
+      <c r="A10" s="85" t="s">
         <v>88</v>
       </c>
-      <c r="B10" s="131" t="s">
+      <c r="B10" s="95" t="s">
         <v>86</v>
       </c>
-      <c r="C10" s="132" t="s">
+      <c r="C10" s="96" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="133" t="s">
+      <c r="D10" s="97" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="134" t="s">
+      <c r="E10" s="98" t="s">
         <v>21</v>
       </c>
       <c r="F10" s="29">
@@ -4028,21 +4058,21 @@
       <c r="L10" s="32">
         <v>1</v>
       </c>
-      <c r="M10" s="96" t="s">
+      <c r="M10" s="104" t="s">
         <v>22</v>
       </c>
-      <c r="N10" s="96"/>
-      <c r="O10" s="96"/>
-      <c r="P10" s="96" t="s">
+      <c r="N10" s="104"/>
+      <c r="O10" s="104"/>
+      <c r="P10" s="104" t="s">
         <v>20</v>
       </c>
-      <c r="Q10" s="96"/>
-      <c r="R10" s="96"/>
-      <c r="S10" s="96" t="s">
+      <c r="Q10" s="104"/>
+      <c r="R10" s="104"/>
+      <c r="S10" s="104" t="s">
         <v>17</v>
       </c>
-      <c r="T10" s="96"/>
-      <c r="U10" s="97"/>
+      <c r="T10" s="104"/>
+      <c r="U10" s="105"/>
       <c r="V10" s="22" t="s">
         <v>18</v>
       </c>
@@ -4057,20 +4087,20 @@
       </c>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A11" s="136" t="s">
+      <c r="A11" s="84" t="s">
         <v>89</v>
       </c>
-      <c r="B11" s="137" t="s">
+      <c r="B11" s="100" t="s">
         <v>90</v>
       </c>
-      <c r="C11" s="138" t="s">
+      <c r="C11" s="101" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="135" t="s">
+      <c r="D11" s="99" t="s">
         <v>23</v>
       </c>
       <c r="E11" s="47"/>
-      <c r="F11" s="139">
+      <c r="F11" s="102">
         <v>0</v>
       </c>
       <c r="G11" s="30">
@@ -4085,21 +4115,21 @@
       <c r="J11" s="31">
         <v>0</v>
       </c>
-      <c r="K11" s="121" t="s">
+      <c r="K11" s="103" t="s">
         <v>17</v>
       </c>
-      <c r="L11" s="121"/>
-      <c r="M11" s="121"/>
-      <c r="N11" s="96" t="s">
+      <c r="L11" s="103"/>
+      <c r="M11" s="103"/>
+      <c r="N11" s="104" t="s">
         <v>24</v>
       </c>
-      <c r="O11" s="96"/>
-      <c r="P11" s="96"/>
-      <c r="Q11" s="96"/>
-      <c r="R11" s="96"/>
-      <c r="S11" s="96"/>
-      <c r="T11" s="96"/>
-      <c r="U11" s="97"/>
+      <c r="O11" s="104"/>
+      <c r="P11" s="104"/>
+      <c r="Q11" s="104"/>
+      <c r="R11" s="104"/>
+      <c r="S11" s="104"/>
+      <c r="T11" s="104"/>
+      <c r="U11" s="105"/>
       <c r="V11" s="22"/>
       <c r="W11" s="19"/>
       <c r="X11" s="19" t="s">
@@ -4110,8 +4140,8 @@
       </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A12" s="136" t="s">
-        <v>130</v>
+      <c r="A12" s="84" t="s">
+        <v>128</v>
       </c>
       <c r="B12" s="14" t="s">
         <v>32</v>
@@ -4119,11 +4149,11 @@
       <c r="C12" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="135" t="s">
+      <c r="D12" s="99" t="s">
         <v>23</v>
       </c>
       <c r="E12" s="47"/>
-      <c r="F12" s="139">
+      <c r="F12" s="102">
         <v>0</v>
       </c>
       <c r="G12" s="30">
@@ -4138,21 +4168,21 @@
       <c r="J12" s="32">
         <v>1</v>
       </c>
-      <c r="K12" s="121" t="s">
+      <c r="K12" s="103" t="s">
         <v>17</v>
       </c>
-      <c r="L12" s="121"/>
-      <c r="M12" s="121"/>
-      <c r="N12" s="96" t="s">
+      <c r="L12" s="103"/>
+      <c r="M12" s="103"/>
+      <c r="N12" s="104" t="s">
         <v>24</v>
       </c>
-      <c r="O12" s="96"/>
-      <c r="P12" s="96"/>
-      <c r="Q12" s="96"/>
-      <c r="R12" s="96"/>
-      <c r="S12" s="96"/>
-      <c r="T12" s="96"/>
-      <c r="U12" s="97"/>
+      <c r="O12" s="104"/>
+      <c r="P12" s="104"/>
+      <c r="Q12" s="104"/>
+      <c r="R12" s="104"/>
+      <c r="S12" s="104"/>
+      <c r="T12" s="104"/>
+      <c r="U12" s="105"/>
       <c r="V12" s="19" t="s">
         <v>18</v>
       </c>
@@ -4167,8 +4197,8 @@
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A13" s="136" t="s">
-        <v>131</v>
+      <c r="A13" s="84" t="s">
+        <v>129</v>
       </c>
       <c r="B13" s="14" t="s">
         <v>84</v>
@@ -4176,7 +4206,7 @@
       <c r="C13" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="135" t="s">
+      <c r="D13" s="99" t="s">
         <v>23</v>
       </c>
       <c r="E13" s="21"/>
@@ -4195,21 +4225,21 @@
       <c r="J13" s="31">
         <v>0</v>
       </c>
-      <c r="K13" s="121" t="s">
+      <c r="K13" s="103" t="s">
         <v>17</v>
       </c>
-      <c r="L13" s="121"/>
-      <c r="M13" s="121"/>
-      <c r="N13" s="96" t="s">
+      <c r="L13" s="103"/>
+      <c r="M13" s="103"/>
+      <c r="N13" s="104" t="s">
         <v>24</v>
       </c>
-      <c r="O13" s="96"/>
-      <c r="P13" s="96"/>
-      <c r="Q13" s="96"/>
-      <c r="R13" s="96"/>
-      <c r="S13" s="96"/>
-      <c r="T13" s="96"/>
-      <c r="U13" s="97"/>
+      <c r="O13" s="104"/>
+      <c r="P13" s="104"/>
+      <c r="Q13" s="104"/>
+      <c r="R13" s="104"/>
+      <c r="S13" s="104"/>
+      <c r="T13" s="104"/>
+      <c r="U13" s="105"/>
       <c r="V13" s="19" t="s">
         <v>18</v>
       </c>
@@ -4224,8 +4254,8 @@
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A14" s="86" t="s">
-        <v>132</v>
+      <c r="A14" s="85" t="s">
+        <v>130</v>
       </c>
       <c r="B14" s="14" t="s">
         <v>86</v>
@@ -4233,7 +4263,7 @@
       <c r="C14" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="135" t="s">
+      <c r="D14" s="99" t="s">
         <v>23</v>
       </c>
       <c r="E14" s="21"/>
@@ -4252,21 +4282,21 @@
       <c r="J14" s="31">
         <v>0</v>
       </c>
-      <c r="K14" s="121" t="s">
+      <c r="K14" s="103" t="s">
         <v>17</v>
       </c>
-      <c r="L14" s="121"/>
-      <c r="M14" s="121"/>
-      <c r="N14" s="96" t="s">
+      <c r="L14" s="103"/>
+      <c r="M14" s="103"/>
+      <c r="N14" s="104" t="s">
         <v>24</v>
       </c>
-      <c r="O14" s="96"/>
-      <c r="P14" s="96"/>
-      <c r="Q14" s="96"/>
-      <c r="R14" s="96"/>
-      <c r="S14" s="96"/>
-      <c r="T14" s="96"/>
-      <c r="U14" s="97"/>
+      <c r="O14" s="104"/>
+      <c r="P14" s="104"/>
+      <c r="Q14" s="104"/>
+      <c r="R14" s="104"/>
+      <c r="S14" s="104"/>
+      <c r="T14" s="104"/>
+      <c r="U14" s="105"/>
       <c r="V14" s="19" t="s">
         <v>18</v>
       </c>
@@ -4281,7 +4311,7 @@
       </c>
     </row>
     <row r="15" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="83" t="s">
+      <c r="A15" s="82" t="s">
         <v>25</v>
       </c>
       <c r="B15" s="36"/>
@@ -4306,12 +4336,12 @@
       <c r="K15" s="39">
         <v>0</v>
       </c>
-      <c r="L15" s="103" t="s">
+      <c r="L15" s="111" t="s">
         <v>11</v>
       </c>
-      <c r="M15" s="103"/>
-      <c r="N15" s="103"/>
-      <c r="O15" s="103"/>
+      <c r="M15" s="111"/>
+      <c r="N15" s="111"/>
+      <c r="O15" s="111"/>
       <c r="P15" s="36"/>
       <c r="Q15" s="36"/>
       <c r="R15" s="40"/>
@@ -4332,7 +4362,7 @@
       </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A16" s="88" t="s">
+      <c r="A16" s="87" t="s">
         <v>91</v>
       </c>
       <c r="B16" s="43" t="s">
@@ -4375,16 +4405,16 @@
       <c r="O16" s="20">
         <v>0</v>
       </c>
-      <c r="P16" s="105" t="s">
+      <c r="P16" s="129" t="s">
         <v>16</v>
       </c>
-      <c r="Q16" s="106"/>
-      <c r="R16" s="106"/>
-      <c r="S16" s="107" t="s">
+      <c r="Q16" s="130"/>
+      <c r="R16" s="130"/>
+      <c r="S16" s="131" t="s">
         <v>27</v>
       </c>
-      <c r="T16" s="107"/>
-      <c r="U16" s="108"/>
+      <c r="T16" s="131"/>
+      <c r="U16" s="132"/>
       <c r="V16" s="22"/>
       <c r="W16" s="19"/>
       <c r="X16" s="19" t="s">
@@ -4395,7 +4425,7 @@
       </c>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A17" s="88" t="s">
+      <c r="A17" s="87" t="s">
         <v>93</v>
       </c>
       <c r="B17" s="14" t="s">
@@ -4438,16 +4468,16 @@
       <c r="O17" s="26">
         <v>1</v>
       </c>
-      <c r="P17" s="109" t="s">
+      <c r="P17" s="114" t="s">
         <v>16</v>
       </c>
-      <c r="Q17" s="96"/>
-      <c r="R17" s="96"/>
-      <c r="S17" s="96" t="s">
+      <c r="Q17" s="104"/>
+      <c r="R17" s="104"/>
+      <c r="S17" s="104" t="s">
         <v>27</v>
       </c>
-      <c r="T17" s="96"/>
-      <c r="U17" s="97"/>
+      <c r="T17" s="104"/>
+      <c r="U17" s="105"/>
       <c r="V17" s="22"/>
       <c r="W17" s="19"/>
       <c r="X17" s="19" t="s">
@@ -4458,7 +4488,7 @@
       </c>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A18" s="88" t="s">
+      <c r="A18" s="87" t="s">
         <v>77</v>
       </c>
       <c r="B18" s="14" t="s">
@@ -4501,16 +4531,16 @@
       <c r="O18" s="20">
         <v>0</v>
       </c>
-      <c r="P18" s="109" t="s">
+      <c r="P18" s="114" t="s">
         <v>16</v>
       </c>
-      <c r="Q18" s="96"/>
-      <c r="R18" s="96"/>
-      <c r="S18" s="96" t="s">
+      <c r="Q18" s="104"/>
+      <c r="R18" s="104"/>
+      <c r="S18" s="104" t="s">
         <v>27</v>
       </c>
-      <c r="T18" s="96"/>
-      <c r="U18" s="97"/>
+      <c r="T18" s="104"/>
+      <c r="U18" s="105"/>
       <c r="V18" s="22" t="s">
         <v>18</v>
       </c>
@@ -4523,7 +4553,7 @@
       </c>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A19" s="88" t="s">
+      <c r="A19" s="87" t="s">
         <v>79</v>
       </c>
       <c r="B19" s="14" t="s">
@@ -4566,16 +4596,16 @@
       <c r="O19" s="26">
         <v>1</v>
       </c>
-      <c r="P19" s="109" t="s">
+      <c r="P19" s="114" t="s">
         <v>16</v>
       </c>
-      <c r="Q19" s="96"/>
-      <c r="R19" s="96"/>
-      <c r="S19" s="96" t="s">
+      <c r="Q19" s="104"/>
+      <c r="R19" s="104"/>
+      <c r="S19" s="104" t="s">
         <v>27</v>
       </c>
-      <c r="T19" s="96"/>
-      <c r="U19" s="97"/>
+      <c r="T19" s="104"/>
+      <c r="U19" s="105"/>
       <c r="V19" s="22" t="s">
         <v>18</v>
       </c>
@@ -4588,7 +4618,7 @@
       </c>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A20" s="88" t="s">
+      <c r="A20" s="87" t="s">
         <v>81</v>
       </c>
       <c r="B20" s="14" t="s">
@@ -4631,16 +4661,16 @@
       <c r="O20" s="20">
         <v>0</v>
       </c>
-      <c r="P20" s="109" t="s">
+      <c r="P20" s="114" t="s">
         <v>16</v>
       </c>
-      <c r="Q20" s="96"/>
-      <c r="R20" s="96"/>
-      <c r="S20" s="96" t="s">
+      <c r="Q20" s="104"/>
+      <c r="R20" s="104"/>
+      <c r="S20" s="104" t="s">
         <v>27</v>
       </c>
-      <c r="T20" s="96"/>
-      <c r="U20" s="97"/>
+      <c r="T20" s="104"/>
+      <c r="U20" s="105"/>
       <c r="V20" s="22" t="s">
         <v>18</v>
       </c>
@@ -4653,7 +4683,7 @@
       </c>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A21" s="88" t="s">
+      <c r="A21" s="87" t="s">
         <v>95</v>
       </c>
       <c r="B21" s="14" t="s">
@@ -4696,16 +4726,16 @@
       <c r="O21" s="26">
         <v>1</v>
       </c>
-      <c r="P21" s="109" t="s">
+      <c r="P21" s="114" t="s">
         <v>16</v>
       </c>
-      <c r="Q21" s="96"/>
-      <c r="R21" s="96"/>
-      <c r="S21" s="96" t="s">
+      <c r="Q21" s="104"/>
+      <c r="R21" s="104"/>
+      <c r="S21" s="104" t="s">
         <v>27</v>
       </c>
-      <c r="T21" s="96"/>
-      <c r="U21" s="97"/>
+      <c r="T21" s="104"/>
+      <c r="U21" s="105"/>
       <c r="V21" s="22" t="s">
         <v>18</v>
       </c>
@@ -4720,7 +4750,7 @@
       </c>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A22" s="88" t="s">
+      <c r="A22" s="87" t="s">
         <v>97</v>
       </c>
       <c r="B22" s="14" t="s">
@@ -4763,16 +4793,16 @@
       <c r="O22" s="20">
         <v>0</v>
       </c>
-      <c r="P22" s="109" t="s">
+      <c r="P22" s="114" t="s">
         <v>16</v>
       </c>
-      <c r="Q22" s="96"/>
-      <c r="R22" s="96"/>
-      <c r="S22" s="96" t="s">
+      <c r="Q22" s="104"/>
+      <c r="R22" s="104"/>
+      <c r="S22" s="104" t="s">
         <v>27</v>
       </c>
-      <c r="T22" s="96"/>
-      <c r="U22" s="97"/>
+      <c r="T22" s="104"/>
+      <c r="U22" s="105"/>
       <c r="V22" s="22" t="s">
         <v>18</v>
       </c>
@@ -4787,7 +4817,7 @@
       </c>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A23" s="88" t="s">
+      <c r="A23" s="87" t="s">
         <v>99</v>
       </c>
       <c r="B23" s="14" t="s">
@@ -4830,16 +4860,16 @@
       <c r="O23" s="26">
         <v>1</v>
       </c>
-      <c r="P23" s="109" t="s">
+      <c r="P23" s="114" t="s">
         <v>16</v>
       </c>
-      <c r="Q23" s="96"/>
-      <c r="R23" s="96"/>
-      <c r="S23" s="96" t="s">
+      <c r="Q23" s="104"/>
+      <c r="R23" s="104"/>
+      <c r="S23" s="104" t="s">
         <v>27</v>
       </c>
-      <c r="T23" s="96"/>
-      <c r="U23" s="97"/>
+      <c r="T23" s="104"/>
+      <c r="U23" s="105"/>
       <c r="V23" s="22" t="s">
         <v>18</v>
       </c>
@@ -4852,7 +4882,7 @@
       </c>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A24" s="88" t="s">
+      <c r="A24" s="87" t="s">
         <v>28</v>
       </c>
       <c r="B24" s="14" t="s">
@@ -4895,16 +4925,16 @@
       <c r="O24" s="20">
         <v>0</v>
       </c>
-      <c r="P24" s="109" t="s">
+      <c r="P24" s="114" t="s">
         <v>16</v>
       </c>
-      <c r="Q24" s="96"/>
-      <c r="R24" s="96"/>
-      <c r="S24" s="96" t="s">
+      <c r="Q24" s="104"/>
+      <c r="R24" s="104"/>
+      <c r="S24" s="104" t="s">
         <v>20</v>
       </c>
-      <c r="T24" s="96"/>
-      <c r="U24" s="97"/>
+      <c r="T24" s="104"/>
+      <c r="U24" s="105"/>
       <c r="V24" s="22"/>
       <c r="W24" s="19"/>
       <c r="X24" s="19" t="s">
@@ -4915,7 +4945,7 @@
       </c>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A25" s="88" t="s">
+      <c r="A25" s="87" t="s">
         <v>101</v>
       </c>
       <c r="B25" s="14" t="s">
@@ -4960,16 +4990,16 @@
       <c r="O25" s="26">
         <v>1</v>
       </c>
-      <c r="P25" s="109" t="s">
+      <c r="P25" s="114" t="s">
         <v>20</v>
       </c>
-      <c r="Q25" s="96"/>
-      <c r="R25" s="96"/>
-      <c r="S25" s="96" t="s">
+      <c r="Q25" s="104"/>
+      <c r="R25" s="104"/>
+      <c r="S25" s="104" t="s">
         <v>17</v>
       </c>
-      <c r="T25" s="96"/>
-      <c r="U25" s="97"/>
+      <c r="T25" s="104"/>
+      <c r="U25" s="105"/>
       <c r="V25" s="22"/>
       <c r="W25" s="19"/>
       <c r="X25" s="19" t="s">
@@ -4980,7 +5010,7 @@
       </c>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A26" s="88" t="s">
+      <c r="A26" s="87" t="s">
         <v>31</v>
       </c>
       <c r="B26" s="14" t="s">
@@ -5023,16 +5053,16 @@
       <c r="O26" s="20">
         <v>0</v>
       </c>
-      <c r="P26" s="109" t="s">
+      <c r="P26" s="114" t="s">
         <v>16</v>
       </c>
-      <c r="Q26" s="96"/>
-      <c r="R26" s="96"/>
-      <c r="S26" s="96" t="s">
+      <c r="Q26" s="104"/>
+      <c r="R26" s="104"/>
+      <c r="S26" s="104" t="s">
         <v>20</v>
       </c>
-      <c r="T26" s="96"/>
-      <c r="U26" s="97"/>
+      <c r="T26" s="104"/>
+      <c r="U26" s="105"/>
       <c r="V26" s="22" t="s">
         <v>18</v>
       </c>
@@ -5047,7 +5077,7 @@
       </c>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A27" s="88" t="s">
+      <c r="A27" s="87" t="s">
         <v>33</v>
       </c>
       <c r="B27" s="14" t="s">
@@ -5090,16 +5120,16 @@
       <c r="O27" s="26">
         <v>1</v>
       </c>
-      <c r="P27" s="109" t="s">
+      <c r="P27" s="114" t="s">
         <v>16</v>
       </c>
-      <c r="Q27" s="96"/>
-      <c r="R27" s="96"/>
-      <c r="S27" s="96" t="s">
+      <c r="Q27" s="104"/>
+      <c r="R27" s="104"/>
+      <c r="S27" s="104" t="s">
         <v>20</v>
       </c>
-      <c r="T27" s="96"/>
-      <c r="U27" s="97"/>
+      <c r="T27" s="104"/>
+      <c r="U27" s="105"/>
       <c r="V27" s="22" t="s">
         <v>18</v>
       </c>
@@ -5114,7 +5144,7 @@
       </c>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A28" s="88" t="s">
+      <c r="A28" s="87" t="s">
         <v>103</v>
       </c>
       <c r="B28" s="14" t="s">
@@ -5157,16 +5187,16 @@
       <c r="O28" s="20">
         <v>0</v>
       </c>
-      <c r="P28" s="109" t="s">
+      <c r="P28" s="114" t="s">
         <v>16</v>
       </c>
-      <c r="Q28" s="96"/>
-      <c r="R28" s="96"/>
-      <c r="S28" s="96" t="s">
+      <c r="Q28" s="104"/>
+      <c r="R28" s="104"/>
+      <c r="S28" s="104" t="s">
         <v>27</v>
       </c>
-      <c r="T28" s="96"/>
-      <c r="U28" s="97"/>
+      <c r="T28" s="104"/>
+      <c r="U28" s="105"/>
       <c r="V28" s="22"/>
       <c r="W28" s="19"/>
       <c r="X28" s="19" t="s">
@@ -5177,7 +5207,7 @@
       </c>
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A29" s="88" t="s">
+      <c r="A29" s="87" t="s">
         <v>105</v>
       </c>
       <c r="B29" s="14" t="s">
@@ -5222,16 +5252,16 @@
       <c r="O29" s="26">
         <v>1</v>
       </c>
-      <c r="P29" s="109" t="s">
+      <c r="P29" s="114" t="s">
         <v>20</v>
       </c>
-      <c r="Q29" s="96"/>
-      <c r="R29" s="96"/>
-      <c r="S29" s="123" t="s">
+      <c r="Q29" s="104"/>
+      <c r="R29" s="104"/>
+      <c r="S29" s="115" t="s">
         <v>36</v>
       </c>
-      <c r="T29" s="123"/>
-      <c r="U29" s="124"/>
+      <c r="T29" s="115"/>
+      <c r="U29" s="116"/>
       <c r="V29" s="22"/>
       <c r="W29" s="19"/>
       <c r="X29" s="19" t="s">
@@ -5242,7 +5272,7 @@
       </c>
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A30" s="88" t="s">
+      <c r="A30" s="87" t="s">
         <v>107</v>
       </c>
       <c r="B30" s="14" t="s">
@@ -5285,16 +5315,16 @@
       <c r="O30" s="20">
         <v>0</v>
       </c>
-      <c r="P30" s="109" t="s">
+      <c r="P30" s="114" t="s">
         <v>16</v>
       </c>
-      <c r="Q30" s="96"/>
-      <c r="R30" s="96"/>
-      <c r="S30" s="96" t="s">
+      <c r="Q30" s="104"/>
+      <c r="R30" s="104"/>
+      <c r="S30" s="104" t="s">
         <v>27</v>
       </c>
-      <c r="T30" s="96"/>
-      <c r="U30" s="97"/>
+      <c r="T30" s="104"/>
+      <c r="U30" s="105"/>
       <c r="V30" s="22"/>
       <c r="W30" s="19"/>
       <c r="X30" s="19" t="s">
@@ -5305,7 +5335,7 @@
       </c>
     </row>
     <row r="31" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="89" t="s">
+      <c r="A31" s="88" t="s">
         <v>37</v>
       </c>
       <c r="B31" s="33" t="s">
@@ -5348,16 +5378,16 @@
       <c r="O31" s="58">
         <v>1</v>
       </c>
-      <c r="P31" s="127" t="s">
+      <c r="P31" s="119" t="s">
         <v>16</v>
       </c>
-      <c r="Q31" s="125"/>
-      <c r="R31" s="125"/>
-      <c r="S31" s="125" t="s">
+      <c r="Q31" s="117"/>
+      <c r="R31" s="117"/>
+      <c r="S31" s="117" t="s">
         <v>17</v>
       </c>
-      <c r="T31" s="125"/>
-      <c r="U31" s="126"/>
+      <c r="T31" s="117"/>
+      <c r="U31" s="118"/>
       <c r="V31" s="54"/>
       <c r="W31" s="56"/>
       <c r="X31" s="56" t="s">
@@ -5367,8 +5397,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="83" t="s">
+    <row r="32" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="82" t="s">
         <v>38</v>
       </c>
       <c r="B32" s="36"/>
@@ -5413,7 +5443,7 @@
       </c>
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A33" s="90" t="s">
+      <c r="A33" s="89" t="s">
         <v>110</v>
       </c>
       <c r="B33" s="43" t="s">
@@ -5422,10 +5452,10 @@
       <c r="C33" s="60" t="s">
         <v>40</v>
       </c>
-      <c r="D33" s="111" t="s">
+      <c r="D33" s="120" t="s">
         <v>41</v>
       </c>
-      <c r="E33" s="112"/>
+      <c r="E33" s="121"/>
       <c r="F33" s="61">
         <v>1</v>
       </c>
@@ -5441,28 +5471,28 @@
       <c r="J33" s="64">
         <v>0</v>
       </c>
-      <c r="K33" s="115" t="s">
+      <c r="K33" s="124" t="s">
         <v>42</v>
       </c>
-      <c r="L33" s="115"/>
-      <c r="M33" s="115"/>
-      <c r="N33" s="116" t="s">
+      <c r="L33" s="124"/>
+      <c r="M33" s="124"/>
+      <c r="N33" s="112" t="s">
         <v>24</v>
       </c>
-      <c r="O33" s="116"/>
-      <c r="P33" s="116"/>
-      <c r="Q33" s="116"/>
-      <c r="R33" s="116"/>
-      <c r="S33" s="116"/>
-      <c r="T33" s="116"/>
-      <c r="U33" s="117"/>
+      <c r="O33" s="112"/>
+      <c r="P33" s="112"/>
+      <c r="Q33" s="112"/>
+      <c r="R33" s="112"/>
+      <c r="S33" s="112"/>
+      <c r="T33" s="112"/>
+      <c r="U33" s="113"/>
       <c r="V33" s="22"/>
       <c r="W33" s="19"/>
       <c r="X33" s="19"/>
       <c r="Y33" s="21"/>
     </row>
     <row r="34" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="90" t="s">
+      <c r="A34" s="89" t="s">
         <v>111</v>
       </c>
       <c r="B34" s="33" t="s">
@@ -5471,10 +5501,10 @@
       <c r="C34" s="65" t="s">
         <v>40</v>
       </c>
-      <c r="D34" s="113" t="s">
+      <c r="D34" s="122" t="s">
         <v>44</v>
       </c>
-      <c r="E34" s="114"/>
+      <c r="E34" s="123"/>
       <c r="F34" s="67">
         <v>1</v>
       </c>
@@ -5490,28 +5520,28 @@
       <c r="J34" s="70">
         <v>1</v>
       </c>
-      <c r="K34" s="118" t="s">
+      <c r="K34" s="125" t="s">
         <v>42</v>
       </c>
-      <c r="L34" s="118"/>
-      <c r="M34" s="118"/>
-      <c r="N34" s="119" t="s">
+      <c r="L34" s="125"/>
+      <c r="M34" s="125"/>
+      <c r="N34" s="107" t="s">
         <v>24</v>
       </c>
-      <c r="O34" s="119"/>
-      <c r="P34" s="119"/>
-      <c r="Q34" s="119"/>
-      <c r="R34" s="119"/>
-      <c r="S34" s="119"/>
-      <c r="T34" s="119"/>
-      <c r="U34" s="120"/>
+      <c r="O34" s="107"/>
+      <c r="P34" s="107"/>
+      <c r="Q34" s="107"/>
+      <c r="R34" s="107"/>
+      <c r="S34" s="107"/>
+      <c r="T34" s="107"/>
+      <c r="U34" s="108"/>
       <c r="V34" s="22"/>
       <c r="W34" s="19"/>
       <c r="X34" s="19"/>
       <c r="Y34" s="21"/>
     </row>
     <row r="35" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="83" t="s">
+      <c r="A35" s="82" t="s">
         <v>45</v>
       </c>
       <c r="B35" s="36"/>
@@ -5530,15 +5560,15 @@
       <c r="I35" s="36">
         <v>1</v>
       </c>
-      <c r="J35" s="122" t="s">
+      <c r="J35" s="109" t="s">
         <v>11</v>
       </c>
-      <c r="K35" s="122"/>
-      <c r="L35" s="122"/>
-      <c r="M35" s="122"/>
-      <c r="N35" s="122"/>
-      <c r="O35" s="122"/>
-      <c r="P35" s="122"/>
+      <c r="K35" s="109"/>
+      <c r="L35" s="109"/>
+      <c r="M35" s="109"/>
+      <c r="N35" s="109"/>
+      <c r="O35" s="109"/>
+      <c r="P35" s="109"/>
       <c r="Q35" s="36"/>
       <c r="R35" s="36"/>
       <c r="S35" s="36"/>
@@ -5558,7 +5588,7 @@
       </c>
     </row>
     <row r="36" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A36" s="91" t="s">
+      <c r="A36" s="90" t="s">
         <v>112</v>
       </c>
       <c r="B36" s="43" t="s">
@@ -5600,22 +5630,22 @@
       <c r="N36" s="64">
         <v>0</v>
       </c>
-      <c r="O36" s="116" t="s">
+      <c r="O36" s="112" t="s">
         <v>50</v>
       </c>
-      <c r="P36" s="116"/>
-      <c r="Q36" s="116"/>
-      <c r="R36" s="116"/>
-      <c r="S36" s="116"/>
-      <c r="T36" s="116"/>
-      <c r="U36" s="117"/>
+      <c r="P36" s="112"/>
+      <c r="Q36" s="112"/>
+      <c r="R36" s="112"/>
+      <c r="S36" s="112"/>
+      <c r="T36" s="112"/>
+      <c r="U36" s="113"/>
       <c r="V36" s="22"/>
       <c r="W36" s="19"/>
       <c r="X36" s="19"/>
       <c r="Y36" s="21"/>
     </row>
     <row r="37" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="91" t="s">
+      <c r="A37" s="90" t="s">
         <v>113</v>
       </c>
       <c r="B37" s="33" t="s">
@@ -5657,22 +5687,22 @@
       <c r="N37" s="75">
         <v>1</v>
       </c>
-      <c r="O37" s="119" t="s">
+      <c r="O37" s="107" t="s">
         <v>50</v>
       </c>
-      <c r="P37" s="119"/>
-      <c r="Q37" s="119"/>
-      <c r="R37" s="119"/>
-      <c r="S37" s="119"/>
-      <c r="T37" s="119"/>
-      <c r="U37" s="120"/>
+      <c r="P37" s="107"/>
+      <c r="Q37" s="107"/>
+      <c r="R37" s="107"/>
+      <c r="S37" s="107"/>
+      <c r="T37" s="107"/>
+      <c r="U37" s="108"/>
       <c r="V37" s="22"/>
       <c r="W37" s="19"/>
       <c r="X37" s="19"/>
       <c r="Y37" s="21"/>
     </row>
     <row r="38" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A38" s="83" t="s">
+      <c r="A38" s="82" t="s">
         <v>52</v>
       </c>
       <c r="B38" s="36" t="s">
@@ -5695,27 +5725,27 @@
       <c r="I38" s="36">
         <v>1</v>
       </c>
-      <c r="J38" s="122" t="s">
+      <c r="J38" s="109" t="s">
         <v>11</v>
       </c>
-      <c r="K38" s="122"/>
-      <c r="L38" s="122"/>
-      <c r="M38" s="122"/>
-      <c r="N38" s="122"/>
-      <c r="O38" s="122"/>
-      <c r="P38" s="122"/>
-      <c r="Q38" s="122"/>
-      <c r="R38" s="122"/>
-      <c r="S38" s="122"/>
-      <c r="T38" s="122"/>
-      <c r="U38" s="128"/>
+      <c r="K38" s="109"/>
+      <c r="L38" s="109"/>
+      <c r="M38" s="109"/>
+      <c r="N38" s="109"/>
+      <c r="O38" s="109"/>
+      <c r="P38" s="109"/>
+      <c r="Q38" s="109"/>
+      <c r="R38" s="109"/>
+      <c r="S38" s="109"/>
+      <c r="T38" s="109"/>
+      <c r="U38" s="110"/>
       <c r="V38" s="42"/>
       <c r="W38" s="36"/>
       <c r="X38" s="36"/>
       <c r="Y38" s="37"/>
     </row>
     <row r="39" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="83"/>
+      <c r="A39" s="82"/>
       <c r="B39" s="36" t="s">
         <v>55</v>
       </c>
@@ -5726,22 +5756,22 @@
       <c r="G39" s="36"/>
       <c r="H39" s="36"/>
       <c r="I39" s="36"/>
-      <c r="J39" s="122" t="s">
+      <c r="J39" s="109" t="s">
         <v>56</v>
       </c>
-      <c r="K39" s="122"/>
-      <c r="L39" s="122"/>
-      <c r="M39" s="122"/>
-      <c r="N39" s="122" t="s">
+      <c r="K39" s="109"/>
+      <c r="L39" s="109"/>
+      <c r="M39" s="109"/>
+      <c r="N39" s="109" t="s">
         <v>24</v>
       </c>
-      <c r="O39" s="122"/>
-      <c r="P39" s="122"/>
-      <c r="Q39" s="122"/>
-      <c r="R39" s="122"/>
-      <c r="S39" s="122"/>
-      <c r="T39" s="122"/>
-      <c r="U39" s="128"/>
+      <c r="O39" s="109"/>
+      <c r="P39" s="109"/>
+      <c r="Q39" s="109"/>
+      <c r="R39" s="109"/>
+      <c r="S39" s="109"/>
+      <c r="T39" s="109"/>
+      <c r="U39" s="110"/>
       <c r="V39" s="42" t="s">
         <v>6</v>
       </c>
@@ -5756,7 +5786,7 @@
       </c>
     </row>
     <row r="40" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A40" s="92" t="s">
+      <c r="A40" s="91" t="s">
         <v>114</v>
       </c>
       <c r="B40" s="76" t="s">
@@ -5791,16 +5821,16 @@
       <c r="M40" s="20">
         <v>0</v>
       </c>
-      <c r="N40" s="96" t="s">
+      <c r="N40" s="104" t="s">
         <v>24</v>
       </c>
-      <c r="O40" s="96"/>
-      <c r="P40" s="96"/>
-      <c r="Q40" s="96"/>
-      <c r="R40" s="96"/>
-      <c r="S40" s="96"/>
-      <c r="T40" s="96"/>
-      <c r="U40" s="97"/>
+      <c r="O40" s="104"/>
+      <c r="P40" s="104"/>
+      <c r="Q40" s="104"/>
+      <c r="R40" s="104"/>
+      <c r="S40" s="104"/>
+      <c r="T40" s="104"/>
+      <c r="U40" s="105"/>
       <c r="V40" s="22"/>
       <c r="W40" s="19"/>
       <c r="X40" s="19"/>
@@ -5809,7 +5839,7 @@
       </c>
     </row>
     <row r="41" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A41" s="92" t="s">
+      <c r="A41" s="91" t="s">
         <v>115</v>
       </c>
       <c r="B41" s="14" t="s">
@@ -5844,16 +5874,16 @@
       <c r="M41" s="20">
         <v>1</v>
       </c>
-      <c r="N41" s="96" t="s">
+      <c r="N41" s="104" t="s">
         <v>24</v>
       </c>
-      <c r="O41" s="96"/>
-      <c r="P41" s="96"/>
-      <c r="Q41" s="96"/>
-      <c r="R41" s="96"/>
-      <c r="S41" s="96"/>
-      <c r="T41" s="96"/>
-      <c r="U41" s="97"/>
+      <c r="O41" s="104"/>
+      <c r="P41" s="104"/>
+      <c r="Q41" s="104"/>
+      <c r="R41" s="104"/>
+      <c r="S41" s="104"/>
+      <c r="T41" s="104"/>
+      <c r="U41" s="105"/>
       <c r="V41" s="22"/>
       <c r="W41" s="19"/>
       <c r="X41" s="19"/>
@@ -5862,7 +5892,7 @@
       </c>
     </row>
     <row r="42" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A42" s="92" t="s">
+      <c r="A42" s="91" t="s">
         <v>116</v>
       </c>
       <c r="B42" s="14" t="s">
@@ -5897,16 +5927,16 @@
       <c r="M42" s="20">
         <v>0</v>
       </c>
-      <c r="N42" s="96" t="s">
+      <c r="N42" s="104" t="s">
         <v>24</v>
       </c>
-      <c r="O42" s="96"/>
-      <c r="P42" s="96"/>
-      <c r="Q42" s="96"/>
-      <c r="R42" s="96"/>
-      <c r="S42" s="96"/>
-      <c r="T42" s="96"/>
-      <c r="U42" s="97"/>
+      <c r="O42" s="104"/>
+      <c r="P42" s="104"/>
+      <c r="Q42" s="104"/>
+      <c r="R42" s="104"/>
+      <c r="S42" s="104"/>
+      <c r="T42" s="104"/>
+      <c r="U42" s="105"/>
       <c r="V42" s="22">
         <v>1</v>
       </c>
@@ -5915,7 +5945,7 @@
       <c r="Y42" s="21"/>
     </row>
     <row r="43" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A43" s="93" t="s">
+      <c r="A43" s="92" t="s">
         <v>117</v>
       </c>
       <c r="B43" s="14" t="s">
@@ -5950,16 +5980,16 @@
       <c r="M43" s="20">
         <v>1</v>
       </c>
-      <c r="N43" s="96" t="s">
+      <c r="N43" s="104" t="s">
         <v>24</v>
       </c>
-      <c r="O43" s="96"/>
-      <c r="P43" s="96"/>
-      <c r="Q43" s="96"/>
-      <c r="R43" s="96"/>
-      <c r="S43" s="96"/>
-      <c r="T43" s="96"/>
-      <c r="U43" s="97"/>
+      <c r="O43" s="104"/>
+      <c r="P43" s="104"/>
+      <c r="Q43" s="104"/>
+      <c r="R43" s="104"/>
+      <c r="S43" s="104"/>
+      <c r="T43" s="104"/>
+      <c r="U43" s="105"/>
       <c r="V43" s="22">
         <v>0</v>
       </c>
@@ -5968,7 +5998,7 @@
       <c r="Y43" s="21"/>
     </row>
     <row r="44" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A44" s="93" t="s">
+      <c r="A44" s="92" t="s">
         <v>118</v>
       </c>
       <c r="B44" s="14" t="s">
@@ -6003,16 +6033,16 @@
       <c r="M44" s="20">
         <v>0</v>
       </c>
-      <c r="N44" s="96" t="s">
+      <c r="N44" s="104" t="s">
         <v>24</v>
       </c>
-      <c r="O44" s="96"/>
-      <c r="P44" s="96"/>
-      <c r="Q44" s="96"/>
-      <c r="R44" s="96"/>
-      <c r="S44" s="96"/>
-      <c r="T44" s="96"/>
-      <c r="U44" s="97"/>
+      <c r="O44" s="104"/>
+      <c r="P44" s="104"/>
+      <c r="Q44" s="104"/>
+      <c r="R44" s="104"/>
+      <c r="S44" s="104"/>
+      <c r="T44" s="104"/>
+      <c r="U44" s="105"/>
       <c r="V44" s="22"/>
       <c r="W44" s="19"/>
       <c r="X44" s="19">
@@ -6021,7 +6051,7 @@
       <c r="Y44" s="21"/>
     </row>
     <row r="45" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A45" s="93" t="s">
+      <c r="A45" s="92" t="s">
         <v>119</v>
       </c>
       <c r="B45" s="14" t="s">
@@ -6056,16 +6086,16 @@
       <c r="M45" s="20">
         <v>1</v>
       </c>
-      <c r="N45" s="96" t="s">
+      <c r="N45" s="104" t="s">
         <v>24</v>
       </c>
-      <c r="O45" s="96"/>
-      <c r="P45" s="96"/>
-      <c r="Q45" s="96"/>
-      <c r="R45" s="96"/>
-      <c r="S45" s="96"/>
-      <c r="T45" s="96"/>
-      <c r="U45" s="97"/>
+      <c r="O45" s="104"/>
+      <c r="P45" s="104"/>
+      <c r="Q45" s="104"/>
+      <c r="R45" s="104"/>
+      <c r="S45" s="104"/>
+      <c r="T45" s="104"/>
+      <c r="U45" s="105"/>
       <c r="V45" s="22"/>
       <c r="W45" s="19"/>
       <c r="X45" s="19">
@@ -6074,7 +6104,7 @@
       <c r="Y45" s="21"/>
     </row>
     <row r="46" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A46" s="92" t="s">
+      <c r="A46" s="91" t="s">
         <v>120</v>
       </c>
       <c r="B46" s="14" t="s">
@@ -6109,16 +6139,16 @@
       <c r="M46" s="20">
         <v>0</v>
       </c>
-      <c r="N46" s="96" t="s">
+      <c r="N46" s="104" t="s">
         <v>24</v>
       </c>
-      <c r="O46" s="96"/>
-      <c r="P46" s="96"/>
-      <c r="Q46" s="96"/>
-      <c r="R46" s="96"/>
-      <c r="S46" s="96"/>
-      <c r="T46" s="96"/>
-      <c r="U46" s="97"/>
+      <c r="O46" s="104"/>
+      <c r="P46" s="104"/>
+      <c r="Q46" s="104"/>
+      <c r="R46" s="104"/>
+      <c r="S46" s="104"/>
+      <c r="T46" s="104"/>
+      <c r="U46" s="105"/>
       <c r="V46" s="22"/>
       <c r="W46" s="19">
         <v>1</v>
@@ -6127,7 +6157,7 @@
       <c r="Y46" s="21"/>
     </row>
     <row r="47" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A47" s="92" t="s">
+      <c r="A47" s="91" t="s">
         <v>121</v>
       </c>
       <c r="B47" s="14" t="s">
@@ -6162,16 +6192,16 @@
       <c r="M47" s="20">
         <v>1</v>
       </c>
-      <c r="N47" s="96" t="s">
+      <c r="N47" s="104" t="s">
         <v>24</v>
       </c>
-      <c r="O47" s="96"/>
-      <c r="P47" s="96"/>
-      <c r="Q47" s="96"/>
-      <c r="R47" s="96"/>
-      <c r="S47" s="96"/>
-      <c r="T47" s="96"/>
-      <c r="U47" s="97"/>
+      <c r="O47" s="104"/>
+      <c r="P47" s="104"/>
+      <c r="Q47" s="104"/>
+      <c r="R47" s="104"/>
+      <c r="S47" s="104"/>
+      <c r="T47" s="104"/>
+      <c r="U47" s="105"/>
       <c r="V47" s="22"/>
       <c r="W47" s="19">
         <v>0</v>
@@ -6180,7 +6210,7 @@
       <c r="Y47" s="21"/>
     </row>
     <row r="48" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A48" s="92" t="s">
+      <c r="A48" s="147" t="s">
         <v>122</v>
       </c>
       <c r="B48" s="14" t="s">
@@ -6215,25 +6245,25 @@
       <c r="M48" s="20">
         <v>0</v>
       </c>
-      <c r="N48" s="96" t="s">
+      <c r="N48" s="104" t="s">
         <v>24</v>
       </c>
-      <c r="O48" s="96"/>
-      <c r="P48" s="96"/>
-      <c r="Q48" s="96"/>
-      <c r="R48" s="96"/>
-      <c r="S48" s="96"/>
-      <c r="T48" s="96"/>
-      <c r="U48" s="97"/>
-      <c r="V48" s="129" t="s">
+      <c r="O48" s="104"/>
+      <c r="P48" s="104"/>
+      <c r="Q48" s="104"/>
+      <c r="R48" s="104"/>
+      <c r="S48" s="104"/>
+      <c r="T48" s="104"/>
+      <c r="U48" s="105"/>
+      <c r="V48" s="106" t="s">
         <v>66</v>
       </c>
-      <c r="W48" s="96"/>
-      <c r="X48" s="96"/>
-      <c r="Y48" s="97"/>
+      <c r="W48" s="104"/>
+      <c r="X48" s="104"/>
+      <c r="Y48" s="105"/>
     </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A49" s="92" t="s">
+    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A49" s="147" t="s">
         <v>123</v>
       </c>
       <c r="B49" s="14" t="s">
@@ -6268,25 +6298,25 @@
       <c r="M49" s="20">
         <v>1</v>
       </c>
-      <c r="N49" s="96" t="s">
+      <c r="N49" s="104" t="s">
         <v>24</v>
       </c>
-      <c r="O49" s="96"/>
-      <c r="P49" s="96"/>
-      <c r="Q49" s="96"/>
-      <c r="R49" s="96"/>
-      <c r="S49" s="96"/>
-      <c r="T49" s="96"/>
-      <c r="U49" s="97"/>
-      <c r="V49" s="129" t="s">
+      <c r="O49" s="104"/>
+      <c r="P49" s="104"/>
+      <c r="Q49" s="104"/>
+      <c r="R49" s="104"/>
+      <c r="S49" s="104"/>
+      <c r="T49" s="104"/>
+      <c r="U49" s="105"/>
+      <c r="V49" s="106" t="s">
         <v>68</v>
       </c>
-      <c r="W49" s="96"/>
-      <c r="X49" s="96"/>
-      <c r="Y49" s="97"/>
+      <c r="W49" s="104"/>
+      <c r="X49" s="104"/>
+      <c r="Y49" s="105"/>
     </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A50" s="92" t="s">
+    <row r="50" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A50" s="147" t="s">
         <v>124</v>
       </c>
       <c r="B50" s="14" t="s">
@@ -6321,25 +6351,25 @@
       <c r="M50" s="20">
         <v>0</v>
       </c>
-      <c r="N50" s="96" t="s">
+      <c r="N50" s="104" t="s">
         <v>24</v>
       </c>
-      <c r="O50" s="96"/>
-      <c r="P50" s="96"/>
-      <c r="Q50" s="96"/>
-      <c r="R50" s="96"/>
-      <c r="S50" s="96"/>
-      <c r="T50" s="96"/>
-      <c r="U50" s="97"/>
-      <c r="V50" s="129" t="s">
+      <c r="O50" s="104"/>
+      <c r="P50" s="104"/>
+      <c r="Q50" s="104"/>
+      <c r="R50" s="104"/>
+      <c r="S50" s="104"/>
+      <c r="T50" s="104"/>
+      <c r="U50" s="105"/>
+      <c r="V50" s="106" t="s">
         <v>70</v>
       </c>
-      <c r="W50" s="96"/>
-      <c r="X50" s="96"/>
-      <c r="Y50" s="97"/>
+      <c r="W50" s="104"/>
+      <c r="X50" s="104"/>
+      <c r="Y50" s="105"/>
     </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A51" s="92" t="s">
+    <row r="51" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A51" s="147" t="s">
         <v>125</v>
       </c>
       <c r="B51" s="14" t="s">
@@ -6374,25 +6404,25 @@
       <c r="M51" s="20">
         <v>1</v>
       </c>
-      <c r="N51" s="96" t="s">
+      <c r="N51" s="104" t="s">
         <v>24</v>
       </c>
-      <c r="O51" s="96"/>
-      <c r="P51" s="96"/>
-      <c r="Q51" s="96"/>
-      <c r="R51" s="96"/>
-      <c r="S51" s="96"/>
-      <c r="T51" s="96"/>
-      <c r="U51" s="97"/>
-      <c r="V51" s="129" t="s">
+      <c r="O51" s="104"/>
+      <c r="P51" s="104"/>
+      <c r="Q51" s="104"/>
+      <c r="R51" s="104"/>
+      <c r="S51" s="104"/>
+      <c r="T51" s="104"/>
+      <c r="U51" s="105"/>
+      <c r="V51" s="106" t="s">
         <v>72</v>
       </c>
-      <c r="W51" s="96"/>
-      <c r="X51" s="96"/>
-      <c r="Y51" s="97"/>
+      <c r="W51" s="104"/>
+      <c r="X51" s="104"/>
+      <c r="Y51" s="105"/>
     </row>
-    <row r="52" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A52" s="92" t="s">
+    <row r="52" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A52" s="147" t="s">
         <v>126</v>
       </c>
       <c r="B52" s="14" t="s">
@@ -6427,162 +6457,311 @@
       <c r="M52" s="20">
         <v>0</v>
       </c>
-      <c r="N52" s="96" t="s">
+      <c r="N52" s="104" t="s">
         <v>24</v>
       </c>
-      <c r="O52" s="96"/>
-      <c r="P52" s="96"/>
-      <c r="Q52" s="96"/>
-      <c r="R52" s="96"/>
-      <c r="S52" s="96"/>
-      <c r="T52" s="96"/>
-      <c r="U52" s="97"/>
-      <c r="V52" s="129" t="s">
+      <c r="O52" s="104"/>
+      <c r="P52" s="104"/>
+      <c r="Q52" s="104"/>
+      <c r="R52" s="104"/>
+      <c r="S52" s="104"/>
+      <c r="T52" s="104"/>
+      <c r="U52" s="105"/>
+      <c r="V52" s="106" t="s">
         <v>74</v>
       </c>
-      <c r="W52" s="96"/>
-      <c r="X52" s="96"/>
-      <c r="Y52" s="97"/>
+      <c r="W52" s="104"/>
+      <c r="X52" s="104"/>
+      <c r="Y52" s="105"/>
     </row>
-    <row r="53" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A53" s="92" t="s">
+    <row r="53" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A53" s="146" t="s">
         <v>127</v>
       </c>
-      <c r="B53" s="14" t="s">
+      <c r="B53" s="95" t="s">
         <v>75</v>
       </c>
-      <c r="C53" s="18" t="s">
+      <c r="C53" s="94" t="s">
         <v>54</v>
       </c>
-      <c r="D53" s="19"/>
-      <c r="E53" s="21"/>
-      <c r="F53" s="18">
-        <v>1</v>
-      </c>
-      <c r="G53" s="19">
-        <v>1</v>
-      </c>
-      <c r="H53" s="19">
-        <v>0</v>
-      </c>
-      <c r="I53" s="19">
-        <v>1</v>
-      </c>
-      <c r="J53" s="20">
-        <v>1</v>
-      </c>
-      <c r="K53" s="20">
-        <v>1</v>
-      </c>
-      <c r="L53" s="20">
-        <v>0</v>
-      </c>
-      <c r="M53" s="20">
-        <v>1</v>
-      </c>
-      <c r="N53" s="96" t="s">
+      <c r="D53" s="56"/>
+      <c r="E53" s="59"/>
+      <c r="F53" s="94">
+        <v>1</v>
+      </c>
+      <c r="G53" s="56">
+        <v>1</v>
+      </c>
+      <c r="H53" s="56">
+        <v>0</v>
+      </c>
+      <c r="I53" s="56">
+        <v>1</v>
+      </c>
+      <c r="J53" s="137">
+        <v>1</v>
+      </c>
+      <c r="K53" s="137">
+        <v>1</v>
+      </c>
+      <c r="L53" s="137">
+        <v>0</v>
+      </c>
+      <c r="M53" s="137">
+        <v>1</v>
+      </c>
+      <c r="N53" s="117" t="s">
         <v>24</v>
       </c>
-      <c r="O53" s="96"/>
-      <c r="P53" s="96"/>
-      <c r="Q53" s="96"/>
-      <c r="R53" s="96"/>
-      <c r="S53" s="96"/>
-      <c r="T53" s="96"/>
-      <c r="U53" s="97"/>
-      <c r="V53" s="129" t="s">
+      <c r="O53" s="117"/>
+      <c r="P53" s="117"/>
+      <c r="Q53" s="117"/>
+      <c r="R53" s="117"/>
+      <c r="S53" s="117"/>
+      <c r="T53" s="117"/>
+      <c r="U53" s="118"/>
+      <c r="V53" s="138" t="s">
         <v>76</v>
       </c>
-      <c r="W53" s="96"/>
-      <c r="X53" s="96"/>
-      <c r="Y53" s="97"/>
+      <c r="W53" s="117"/>
+      <c r="X53" s="117"/>
+      <c r="Y53" s="118"/>
     </row>
-    <row r="54" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="94" t="s">
-        <v>128</v>
-      </c>
-      <c r="B54" s="33" t="s">
-        <v>129</v>
-      </c>
-      <c r="C54" s="73" t="s">
+    <row r="54" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A54" s="149" t="s">
+        <v>134</v>
+      </c>
+      <c r="B54" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="C54" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="D54" s="68"/>
-      <c r="E54" s="35"/>
-      <c r="F54" s="73">
-        <v>1</v>
-      </c>
-      <c r="G54" s="68">
-        <v>1</v>
-      </c>
-      <c r="H54" s="68">
-        <v>0</v>
-      </c>
-      <c r="I54" s="68">
-        <v>1</v>
-      </c>
-      <c r="J54" s="75">
-        <v>1</v>
-      </c>
-      <c r="K54" s="75">
-        <v>1</v>
-      </c>
-      <c r="L54" s="75">
-        <v>1</v>
-      </c>
-      <c r="M54" s="75">
-        <v>0</v>
-      </c>
-      <c r="N54" s="119" t="s">
+      <c r="D54" s="19"/>
+      <c r="E54" s="47"/>
+      <c r="F54" s="22">
+        <v>1</v>
+      </c>
+      <c r="G54" s="19">
+        <v>1</v>
+      </c>
+      <c r="H54" s="19">
+        <v>0</v>
+      </c>
+      <c r="I54" s="19">
+        <v>1</v>
+      </c>
+      <c r="J54" s="20">
+        <v>1</v>
+      </c>
+      <c r="K54" s="20">
+        <v>1</v>
+      </c>
+      <c r="L54" s="20">
+        <v>1</v>
+      </c>
+      <c r="M54" s="20">
+        <v>0</v>
+      </c>
+      <c r="N54" s="104" t="s">
         <v>24</v>
       </c>
-      <c r="O54" s="119"/>
-      <c r="P54" s="119"/>
-      <c r="Q54" s="119"/>
-      <c r="R54" s="119"/>
-      <c r="S54" s="119"/>
-      <c r="T54" s="119"/>
-      <c r="U54" s="120"/>
-      <c r="V54" s="130"/>
-      <c r="W54" s="119"/>
-      <c r="X54" s="119"/>
-      <c r="Y54" s="120"/>
+      <c r="O54" s="104"/>
+      <c r="P54" s="104"/>
+      <c r="Q54" s="104"/>
+      <c r="R54" s="104"/>
+      <c r="S54" s="104"/>
+      <c r="T54" s="104"/>
+      <c r="U54" s="139"/>
+      <c r="V54" s="106"/>
+      <c r="W54" s="104"/>
+      <c r="X54" s="104"/>
+      <c r="Y54" s="139"/>
+      <c r="Z54" s="140"/>
     </row>
-    <row r="55" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B55" s="81"/>
+    <row r="55" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="150"/>
+      <c r="B55" s="143" t="s">
+        <v>132</v>
+      </c>
+      <c r="C55" s="54" t="s">
+        <v>54</v>
+      </c>
+      <c r="D55" s="56"/>
+      <c r="E55" s="57"/>
+      <c r="F55" s="54">
+        <v>1</v>
+      </c>
+      <c r="G55" s="56">
+        <v>1</v>
+      </c>
+      <c r="H55" s="56">
+        <v>0</v>
+      </c>
+      <c r="I55" s="56">
+        <v>1</v>
+      </c>
+      <c r="J55" s="117" t="s">
+        <v>133</v>
+      </c>
+      <c r="K55" s="117"/>
+      <c r="L55" s="117"/>
+      <c r="M55" s="117"/>
+      <c r="N55" s="117"/>
+      <c r="O55" s="117"/>
+      <c r="P55" s="117"/>
+      <c r="Q55" s="117"/>
+      <c r="R55" s="117"/>
+      <c r="S55" s="117"/>
+      <c r="T55" s="117"/>
+      <c r="U55" s="141"/>
+      <c r="V55" s="138"/>
+      <c r="W55" s="117"/>
+      <c r="X55" s="117"/>
+      <c r="Y55" s="141"/>
+      <c r="Z55" s="140"/>
     </row>
-    <row r="56" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B56" s="81"/>
+    <row r="56" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A56" s="144"/>
+      <c r="B56" s="145"/>
+      <c r="C56" s="142"/>
+      <c r="D56" s="142"/>
+      <c r="E56" s="142"/>
+      <c r="F56" s="142"/>
+      <c r="G56" s="142"/>
+      <c r="H56" s="142"/>
+      <c r="I56" s="142"/>
+      <c r="J56" s="142"/>
+      <c r="K56" s="142"/>
+      <c r="L56" s="142"/>
+      <c r="M56" s="142"/>
+      <c r="N56" s="142"/>
+      <c r="O56" s="142"/>
+      <c r="P56" s="142"/>
+      <c r="Q56" s="142"/>
+      <c r="R56" s="142"/>
+      <c r="S56" s="142"/>
+      <c r="T56" s="142"/>
+      <c r="U56" s="142"/>
+      <c r="V56" s="142"/>
+      <c r="W56" s="142"/>
+      <c r="X56" s="142"/>
+      <c r="Y56" s="142"/>
     </row>
-    <row r="57" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B57" s="81"/>
     </row>
-    <row r="58" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B58" s="81"/>
     </row>
-    <row r="59" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B59" s="81"/>
     </row>
-    <row r="60" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B60" s="81"/>
     </row>
-    <row r="61" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B61" s="81"/>
     </row>
-    <row r="62" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B62" s="81"/>
     </row>
-    <row r="63" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B63" s="81"/>
     </row>
-    <row r="64" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B64" s="81"/>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B65" s="81"/>
     </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B66" s="81"/>
+    </row>
   </sheetData>
-  <mergeCells count="103">
+  <mergeCells count="106">
+    <mergeCell ref="V55:Y55"/>
+    <mergeCell ref="J55:U55"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:U1"/>
+    <mergeCell ref="K4:O4"/>
+    <mergeCell ref="H3:L3"/>
+    <mergeCell ref="S10:U10"/>
+    <mergeCell ref="K5:O5"/>
+    <mergeCell ref="K6:O6"/>
+    <mergeCell ref="S7:U7"/>
+    <mergeCell ref="P8:R8"/>
+    <mergeCell ref="S8:U8"/>
+    <mergeCell ref="M7:O7"/>
+    <mergeCell ref="M8:O8"/>
+    <mergeCell ref="M9:O9"/>
+    <mergeCell ref="M10:O10"/>
+    <mergeCell ref="S27:U27"/>
+    <mergeCell ref="P25:R25"/>
+    <mergeCell ref="P26:R26"/>
+    <mergeCell ref="P27:R27"/>
+    <mergeCell ref="P24:R24"/>
+    <mergeCell ref="V1:Y1"/>
+    <mergeCell ref="P16:R16"/>
+    <mergeCell ref="S16:U16"/>
+    <mergeCell ref="P17:R17"/>
+    <mergeCell ref="P18:R18"/>
+    <mergeCell ref="S17:U17"/>
+    <mergeCell ref="S18:U18"/>
+    <mergeCell ref="P4:R4"/>
+    <mergeCell ref="S4:U4"/>
+    <mergeCell ref="P5:R5"/>
+    <mergeCell ref="S5:U5"/>
+    <mergeCell ref="P6:R6"/>
+    <mergeCell ref="S6:U6"/>
+    <mergeCell ref="P7:R7"/>
+    <mergeCell ref="N11:U11"/>
+    <mergeCell ref="S9:U9"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="K33:M33"/>
+    <mergeCell ref="N33:U33"/>
+    <mergeCell ref="K34:M34"/>
+    <mergeCell ref="N34:U34"/>
+    <mergeCell ref="P28:R28"/>
+    <mergeCell ref="P29:R29"/>
+    <mergeCell ref="P30:R30"/>
+    <mergeCell ref="L15:O15"/>
+    <mergeCell ref="P9:R9"/>
+    <mergeCell ref="K11:M11"/>
+    <mergeCell ref="P10:R10"/>
+    <mergeCell ref="O36:U36"/>
+    <mergeCell ref="J35:P35"/>
+    <mergeCell ref="P19:R19"/>
+    <mergeCell ref="P20:R20"/>
+    <mergeCell ref="P21:R21"/>
+    <mergeCell ref="P22:R22"/>
+    <mergeCell ref="P23:R23"/>
+    <mergeCell ref="S28:U28"/>
+    <mergeCell ref="S29:U29"/>
+    <mergeCell ref="S30:U30"/>
+    <mergeCell ref="S31:U31"/>
+    <mergeCell ref="P31:R31"/>
+    <mergeCell ref="S19:U19"/>
+    <mergeCell ref="S20:U20"/>
+    <mergeCell ref="S21:U21"/>
+    <mergeCell ref="S22:U22"/>
+    <mergeCell ref="S23:U23"/>
+    <mergeCell ref="S24:U24"/>
+    <mergeCell ref="S25:U25"/>
+    <mergeCell ref="S26:U26"/>
+    <mergeCell ref="N41:U41"/>
+    <mergeCell ref="N42:U42"/>
+    <mergeCell ref="N43:U43"/>
+    <mergeCell ref="N44:U44"/>
+    <mergeCell ref="O37:U37"/>
+    <mergeCell ref="J38:M38"/>
+    <mergeCell ref="N38:U38"/>
+    <mergeCell ref="J39:M39"/>
+    <mergeCell ref="N39:U39"/>
     <mergeCell ref="K13:M13"/>
     <mergeCell ref="N13:U13"/>
     <mergeCell ref="K12:M12"/>
@@ -6607,93 +6786,14 @@
     <mergeCell ref="N53:U53"/>
     <mergeCell ref="N54:U54"/>
     <mergeCell ref="N40:U40"/>
-    <mergeCell ref="N41:U41"/>
-    <mergeCell ref="N42:U42"/>
-    <mergeCell ref="N43:U43"/>
-    <mergeCell ref="N44:U44"/>
-    <mergeCell ref="O37:U37"/>
-    <mergeCell ref="J38:M38"/>
-    <mergeCell ref="N38:U38"/>
-    <mergeCell ref="J39:M39"/>
-    <mergeCell ref="N39:U39"/>
-    <mergeCell ref="L15:O15"/>
-    <mergeCell ref="P9:R9"/>
-    <mergeCell ref="K11:M11"/>
-    <mergeCell ref="P10:R10"/>
-    <mergeCell ref="O36:U36"/>
-    <mergeCell ref="J35:P35"/>
-    <mergeCell ref="P19:R19"/>
-    <mergeCell ref="P20:R20"/>
-    <mergeCell ref="P21:R21"/>
-    <mergeCell ref="P22:R22"/>
-    <mergeCell ref="P23:R23"/>
-    <mergeCell ref="S28:U28"/>
-    <mergeCell ref="S29:U29"/>
-    <mergeCell ref="S30:U30"/>
-    <mergeCell ref="S31:U31"/>
-    <mergeCell ref="P31:R31"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="K33:M33"/>
-    <mergeCell ref="N33:U33"/>
-    <mergeCell ref="K34:M34"/>
-    <mergeCell ref="N34:U34"/>
-    <mergeCell ref="P28:R28"/>
-    <mergeCell ref="P29:R29"/>
-    <mergeCell ref="P30:R30"/>
-    <mergeCell ref="S19:U19"/>
-    <mergeCell ref="S20:U20"/>
-    <mergeCell ref="S21:U21"/>
-    <mergeCell ref="S22:U22"/>
-    <mergeCell ref="S23:U23"/>
-    <mergeCell ref="S24:U24"/>
-    <mergeCell ref="S25:U25"/>
-    <mergeCell ref="S26:U26"/>
-    <mergeCell ref="S27:U27"/>
-    <mergeCell ref="P25:R25"/>
-    <mergeCell ref="P26:R26"/>
-    <mergeCell ref="P27:R27"/>
-    <mergeCell ref="P24:R24"/>
-    <mergeCell ref="V1:Y1"/>
-    <mergeCell ref="P16:R16"/>
-    <mergeCell ref="S16:U16"/>
-    <mergeCell ref="P17:R17"/>
-    <mergeCell ref="P18:R18"/>
-    <mergeCell ref="S17:U17"/>
-    <mergeCell ref="S18:U18"/>
-    <mergeCell ref="P4:R4"/>
-    <mergeCell ref="S4:U4"/>
-    <mergeCell ref="P5:R5"/>
-    <mergeCell ref="S5:U5"/>
-    <mergeCell ref="P6:R6"/>
-    <mergeCell ref="S6:U6"/>
-    <mergeCell ref="P7:R7"/>
-    <mergeCell ref="N11:U11"/>
-    <mergeCell ref="S9:U9"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:U1"/>
-    <mergeCell ref="K4:O4"/>
-    <mergeCell ref="H3:L3"/>
-    <mergeCell ref="S10:U10"/>
-    <mergeCell ref="K5:O5"/>
-    <mergeCell ref="K6:O6"/>
-    <mergeCell ref="S7:U7"/>
-    <mergeCell ref="P8:R8"/>
-    <mergeCell ref="S8:U8"/>
-    <mergeCell ref="M7:O7"/>
-    <mergeCell ref="M8:O8"/>
-    <mergeCell ref="M9:O9"/>
-    <mergeCell ref="M10:O10"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="F4:U54">
+  <conditionalFormatting sqref="F4:U54 F55:J55">
     <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F39:M39 V39:Y39 F40:Y54 F1:Y38">
+  <conditionalFormatting sqref="F1:Y38 F39:M39 V39:Y39 F40:Y54 F55:J55 V55:Y55">
     <cfRule type="containsText" dxfId="8" priority="2" operator="containsText" text="imm">
       <formula>NOT(ISERROR(SEARCH("imm",F1)))</formula>
     </cfRule>
@@ -6727,11 +6827,20 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="64" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="59" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010096649AD79A527B47A67D905693C83B0C" ma:contentTypeVersion="7" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="44d09355696640e2dc56270e449341cd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="98b34aae-4bd1-40d2-80e1-46205a35d283" xmlns:ns4="4c17d7eb-fa2b-4fbc-8175-1cef2629d4d8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="73bda8d09c620ff6c543bf34844bea48" ns3:_="" ns4:_="">
     <xsd:import namespace="98b34aae-4bd1-40d2-80e1-46205a35d283"/>
@@ -6916,15 +7025,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -6932,6 +7032,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AAD58D5F-4A46-4F63-A2BD-BBB590555A8D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90060F17-AE26-48CA-A0B9-2F516B758ECF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6946,14 +7054,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AAD58D5F-4A46-4F63-A2BD-BBB590555A8D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Generate test vectors for DataProcessing and ShiftAddSubMove
</commit_message>
<xml_diff>
--- a/docs/ARM instructions.xlsx
+++ b/docs/ARM instructions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Drive\Etudes\Supérieur\SI3\Architecture et réseaux\Architecture\PARM\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CB64F18-45D6-4909-B507-CC4FB70C33C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13B2E786-DC77-47EF-8E79-01A9970655F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1E4904EC-9B68-40DD-B685-7BD66B9DE8BA}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1E4904EC-9B68-40DD-B685-7BD66B9DE8BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="138">
   <si>
     <t>Description</t>
   </si>
@@ -2998,13 +2998,112 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3019,106 +3118,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3126,6 +3126,19 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="15">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -3158,19 +3171,6 @@
       <fill>
         <patternFill>
           <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3565,8 +3565,8 @@
   </sheetPr>
   <dimension ref="A1:Z70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="145" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="145" zoomScalePageLayoutView="145" workbookViewId="0">
+      <selection activeCell="AB9" sqref="AB9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3579,50 +3579,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="117" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="121" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="119"/>
-      <c r="D1" s="119"/>
-      <c r="E1" s="120"/>
-      <c r="F1" s="119" t="s">
+      <c r="A1" s="150" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="152" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="141"/>
+      <c r="D1" s="141"/>
+      <c r="E1" s="142"/>
+      <c r="F1" s="141" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="119"/>
-      <c r="H1" s="119"/>
-      <c r="I1" s="119"/>
-      <c r="J1" s="119"/>
-      <c r="K1" s="119"/>
-      <c r="L1" s="119"/>
-      <c r="M1" s="119"/>
-      <c r="N1" s="119"/>
-      <c r="O1" s="119"/>
-      <c r="P1" s="119"/>
-      <c r="Q1" s="119"/>
-      <c r="R1" s="119"/>
-      <c r="S1" s="119"/>
-      <c r="T1" s="119"/>
-      <c r="U1" s="120"/>
-      <c r="V1" s="126" t="s">
+      <c r="G1" s="141"/>
+      <c r="H1" s="141"/>
+      <c r="I1" s="141"/>
+      <c r="J1" s="141"/>
+      <c r="K1" s="141"/>
+      <c r="L1" s="141"/>
+      <c r="M1" s="141"/>
+      <c r="N1" s="141"/>
+      <c r="O1" s="141"/>
+      <c r="P1" s="141"/>
+      <c r="Q1" s="141"/>
+      <c r="R1" s="141"/>
+      <c r="S1" s="141"/>
+      <c r="T1" s="141"/>
+      <c r="U1" s="142"/>
+      <c r="V1" s="140" t="s">
         <v>3</v>
       </c>
-      <c r="W1" s="119"/>
-      <c r="X1" s="119"/>
-      <c r="Y1" s="120"/>
+      <c r="W1" s="141"/>
+      <c r="X1" s="141"/>
+      <c r="Y1" s="142"/>
     </row>
     <row r="2" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="118"/>
+      <c r="A2" s="151"/>
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="119" t="s">
+      <c r="C2" s="141" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="119"/>
-      <c r="E2" s="120"/>
+      <c r="D2" s="141"/>
+      <c r="E2" s="142"/>
       <c r="F2" s="2">
         <v>15</v>
       </c>
@@ -3698,13 +3698,13 @@
       <c r="G3" s="10">
         <v>0</v>
       </c>
-      <c r="H3" s="123" t="s">
+      <c r="H3" s="147" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="123"/>
-      <c r="J3" s="123"/>
-      <c r="K3" s="123"/>
-      <c r="L3" s="123"/>
+      <c r="I3" s="147"/>
+      <c r="J3" s="147"/>
+      <c r="K3" s="147"/>
+      <c r="L3" s="147"/>
       <c r="M3" s="11"/>
       <c r="N3" s="11"/>
       <c r="O3" s="11"/>
@@ -3750,23 +3750,23 @@
       <c r="J4" s="20">
         <v>0</v>
       </c>
-      <c r="K4" s="122" t="s">
+      <c r="K4" s="114" t="s">
         <v>15</v>
       </c>
-      <c r="L4" s="122"/>
-      <c r="M4" s="122"/>
-      <c r="N4" s="122"/>
-      <c r="O4" s="122"/>
-      <c r="P4" s="131" t="s">
+      <c r="L4" s="114"/>
+      <c r="M4" s="114"/>
+      <c r="N4" s="114"/>
+      <c r="O4" s="114"/>
+      <c r="P4" s="120" t="s">
         <v>16</v>
       </c>
-      <c r="Q4" s="131"/>
-      <c r="R4" s="131"/>
-      <c r="S4" s="122" t="s">
+      <c r="Q4" s="120"/>
+      <c r="R4" s="120"/>
+      <c r="S4" s="114" t="s">
         <v>17</v>
       </c>
-      <c r="T4" s="122"/>
-      <c r="U4" s="124"/>
+      <c r="T4" s="114"/>
+      <c r="U4" s="115"/>
       <c r="V4" s="22" t="s">
         <v>18</v>
       </c>
@@ -3809,24 +3809,26 @@
       <c r="J5" s="26">
         <v>1</v>
       </c>
-      <c r="K5" s="122" t="s">
+      <c r="K5" s="114" t="s">
         <v>15</v>
       </c>
-      <c r="L5" s="122"/>
-      <c r="M5" s="122"/>
-      <c r="N5" s="122"/>
-      <c r="O5" s="122"/>
-      <c r="P5" s="122" t="s">
+      <c r="L5" s="114"/>
+      <c r="M5" s="114"/>
+      <c r="N5" s="114"/>
+      <c r="O5" s="114"/>
+      <c r="P5" s="114" t="s">
         <v>16</v>
       </c>
-      <c r="Q5" s="122"/>
-      <c r="R5" s="122"/>
-      <c r="S5" s="122" t="s">
+      <c r="Q5" s="114"/>
+      <c r="R5" s="114"/>
+      <c r="S5" s="114" t="s">
         <v>17</v>
       </c>
-      <c r="T5" s="122"/>
-      <c r="U5" s="124"/>
-      <c r="V5" s="22"/>
+      <c r="T5" s="114"/>
+      <c r="U5" s="115"/>
+      <c r="V5" s="22" t="s">
+        <v>18</v>
+      </c>
       <c r="W5" s="19"/>
       <c r="X5" s="19" t="s">
         <v>18</v>
@@ -3866,23 +3868,23 @@
       <c r="J6" s="20">
         <v>0</v>
       </c>
-      <c r="K6" s="122" t="s">
+      <c r="K6" s="114" t="s">
         <v>15</v>
       </c>
-      <c r="L6" s="122"/>
-      <c r="M6" s="122"/>
-      <c r="N6" s="122"/>
-      <c r="O6" s="122"/>
-      <c r="P6" s="122" t="s">
+      <c r="L6" s="114"/>
+      <c r="M6" s="114"/>
+      <c r="N6" s="114"/>
+      <c r="O6" s="114"/>
+      <c r="P6" s="114" t="s">
         <v>16</v>
       </c>
-      <c r="Q6" s="122"/>
-      <c r="R6" s="122"/>
-      <c r="S6" s="122" t="s">
+      <c r="Q6" s="114"/>
+      <c r="R6" s="114"/>
+      <c r="S6" s="114" t="s">
         <v>17</v>
       </c>
-      <c r="T6" s="122"/>
-      <c r="U6" s="124"/>
+      <c r="T6" s="114"/>
+      <c r="U6" s="115"/>
       <c r="V6" s="22" t="s">
         <v>18</v>
       </c>
@@ -3931,21 +3933,21 @@
       <c r="L7" s="31">
         <v>0</v>
       </c>
-      <c r="M7" s="122" t="s">
+      <c r="M7" s="114" t="s">
         <v>16</v>
       </c>
-      <c r="N7" s="122"/>
-      <c r="O7" s="122"/>
-      <c r="P7" s="122" t="s">
+      <c r="N7" s="114"/>
+      <c r="O7" s="114"/>
+      <c r="P7" s="114" t="s">
         <v>20</v>
       </c>
-      <c r="Q7" s="122"/>
-      <c r="R7" s="122"/>
-      <c r="S7" s="122" t="s">
+      <c r="Q7" s="114"/>
+      <c r="R7" s="114"/>
+      <c r="S7" s="114" t="s">
         <v>17</v>
       </c>
-      <c r="T7" s="122"/>
-      <c r="U7" s="124"/>
+      <c r="T7" s="114"/>
+      <c r="U7" s="115"/>
       <c r="V7" s="22" t="s">
         <v>18</v>
       </c>
@@ -3996,21 +3998,21 @@
       <c r="L8" s="32">
         <v>1</v>
       </c>
-      <c r="M8" s="122" t="s">
+      <c r="M8" s="114" t="s">
         <v>16</v>
       </c>
-      <c r="N8" s="122"/>
-      <c r="O8" s="122"/>
-      <c r="P8" s="122" t="s">
+      <c r="N8" s="114"/>
+      <c r="O8" s="114"/>
+      <c r="P8" s="114" t="s">
         <v>20</v>
       </c>
-      <c r="Q8" s="122"/>
-      <c r="R8" s="122"/>
-      <c r="S8" s="122" t="s">
+      <c r="Q8" s="114"/>
+      <c r="R8" s="114"/>
+      <c r="S8" s="114" t="s">
         <v>17</v>
       </c>
-      <c r="T8" s="122"/>
-      <c r="U8" s="124"/>
+      <c r="T8" s="114"/>
+      <c r="U8" s="115"/>
       <c r="V8" s="22" t="s">
         <v>18</v>
       </c>
@@ -4061,21 +4063,21 @@
       <c r="L9" s="31">
         <v>0</v>
       </c>
-      <c r="M9" s="122" t="s">
+      <c r="M9" s="114" t="s">
         <v>22</v>
       </c>
-      <c r="N9" s="122"/>
-      <c r="O9" s="122"/>
-      <c r="P9" s="122" t="s">
+      <c r="N9" s="114"/>
+      <c r="O9" s="114"/>
+      <c r="P9" s="114" t="s">
         <v>20</v>
       </c>
-      <c r="Q9" s="122"/>
-      <c r="R9" s="122"/>
-      <c r="S9" s="122" t="s">
+      <c r="Q9" s="114"/>
+      <c r="R9" s="114"/>
+      <c r="S9" s="114" t="s">
         <v>17</v>
       </c>
-      <c r="T9" s="122"/>
-      <c r="U9" s="124"/>
+      <c r="T9" s="114"/>
+      <c r="U9" s="115"/>
       <c r="V9" s="22" t="s">
         <v>18</v>
       </c>
@@ -4126,21 +4128,21 @@
       <c r="L10" s="32">
         <v>1</v>
       </c>
-      <c r="M10" s="122" t="s">
+      <c r="M10" s="114" t="s">
         <v>22</v>
       </c>
-      <c r="N10" s="122"/>
-      <c r="O10" s="122"/>
-      <c r="P10" s="122" t="s">
+      <c r="N10" s="114"/>
+      <c r="O10" s="114"/>
+      <c r="P10" s="114" t="s">
         <v>20</v>
       </c>
-      <c r="Q10" s="122"/>
-      <c r="R10" s="122"/>
-      <c r="S10" s="122" t="s">
+      <c r="Q10" s="114"/>
+      <c r="R10" s="114"/>
+      <c r="S10" s="114" t="s">
         <v>17</v>
       </c>
-      <c r="T10" s="122"/>
-      <c r="U10" s="124"/>
+      <c r="T10" s="114"/>
+      <c r="U10" s="115"/>
       <c r="V10" s="22" t="s">
         <v>18</v>
       </c>
@@ -4183,21 +4185,21 @@
       <c r="J11" s="31">
         <v>0</v>
       </c>
-      <c r="K11" s="132" t="s">
+      <c r="K11" s="121" t="s">
         <v>17</v>
       </c>
-      <c r="L11" s="132"/>
-      <c r="M11" s="132"/>
-      <c r="N11" s="122" t="s">
+      <c r="L11" s="121"/>
+      <c r="M11" s="121"/>
+      <c r="N11" s="114" t="s">
         <v>24</v>
       </c>
-      <c r="O11" s="122"/>
-      <c r="P11" s="122"/>
-      <c r="Q11" s="122"/>
-      <c r="R11" s="122"/>
-      <c r="S11" s="122"/>
-      <c r="T11" s="122"/>
-      <c r="U11" s="124"/>
+      <c r="O11" s="114"/>
+      <c r="P11" s="114"/>
+      <c r="Q11" s="114"/>
+      <c r="R11" s="114"/>
+      <c r="S11" s="114"/>
+      <c r="T11" s="114"/>
+      <c r="U11" s="115"/>
       <c r="V11" s="22"/>
       <c r="W11" s="19"/>
       <c r="X11" s="19" t="s">
@@ -4236,21 +4238,21 @@
       <c r="J12" s="32">
         <v>1</v>
       </c>
-      <c r="K12" s="132" t="s">
+      <c r="K12" s="121" t="s">
         <v>17</v>
       </c>
-      <c r="L12" s="132"/>
-      <c r="M12" s="132"/>
-      <c r="N12" s="122" t="s">
+      <c r="L12" s="121"/>
+      <c r="M12" s="121"/>
+      <c r="N12" s="114" t="s">
         <v>24</v>
       </c>
-      <c r="O12" s="122"/>
-      <c r="P12" s="122"/>
-      <c r="Q12" s="122"/>
-      <c r="R12" s="122"/>
-      <c r="S12" s="122"/>
-      <c r="T12" s="122"/>
-      <c r="U12" s="124"/>
+      <c r="O12" s="114"/>
+      <c r="P12" s="114"/>
+      <c r="Q12" s="114"/>
+      <c r="R12" s="114"/>
+      <c r="S12" s="114"/>
+      <c r="T12" s="114"/>
+      <c r="U12" s="115"/>
       <c r="V12" s="19" t="s">
         <v>18</v>
       </c>
@@ -4293,21 +4295,21 @@
       <c r="J13" s="31">
         <v>0</v>
       </c>
-      <c r="K13" s="132" t="s">
+      <c r="K13" s="121" t="s">
         <v>17</v>
       </c>
-      <c r="L13" s="132"/>
-      <c r="M13" s="132"/>
-      <c r="N13" s="122" t="s">
+      <c r="L13" s="121"/>
+      <c r="M13" s="121"/>
+      <c r="N13" s="114" t="s">
         <v>24</v>
       </c>
-      <c r="O13" s="122"/>
-      <c r="P13" s="122"/>
-      <c r="Q13" s="122"/>
-      <c r="R13" s="122"/>
-      <c r="S13" s="122"/>
-      <c r="T13" s="122"/>
-      <c r="U13" s="124"/>
+      <c r="O13" s="114"/>
+      <c r="P13" s="114"/>
+      <c r="Q13" s="114"/>
+      <c r="R13" s="114"/>
+      <c r="S13" s="114"/>
+      <c r="T13" s="114"/>
+      <c r="U13" s="115"/>
       <c r="V13" s="19" t="s">
         <v>18</v>
       </c>
@@ -4348,23 +4350,23 @@
         <v>1</v>
       </c>
       <c r="J14" s="31">
-        <v>0</v>
-      </c>
-      <c r="K14" s="132" t="s">
+        <v>1</v>
+      </c>
+      <c r="K14" s="121" t="s">
         <v>17</v>
       </c>
-      <c r="L14" s="132"/>
-      <c r="M14" s="132"/>
-      <c r="N14" s="122" t="s">
+      <c r="L14" s="121"/>
+      <c r="M14" s="121"/>
+      <c r="N14" s="114" t="s">
         <v>24</v>
       </c>
-      <c r="O14" s="122"/>
-      <c r="P14" s="122"/>
-      <c r="Q14" s="122"/>
-      <c r="R14" s="122"/>
-      <c r="S14" s="122"/>
-      <c r="T14" s="122"/>
-      <c r="U14" s="124"/>
+      <c r="O14" s="114"/>
+      <c r="P14" s="114"/>
+      <c r="Q14" s="114"/>
+      <c r="R14" s="114"/>
+      <c r="S14" s="114"/>
+      <c r="T14" s="114"/>
+      <c r="U14" s="115"/>
       <c r="V14" s="19" t="s">
         <v>18</v>
       </c>
@@ -4404,12 +4406,12 @@
       <c r="K15" s="39">
         <v>0</v>
       </c>
-      <c r="L15" s="123" t="s">
+      <c r="L15" s="147" t="s">
         <v>11</v>
       </c>
-      <c r="M15" s="123"/>
-      <c r="N15" s="123"/>
-      <c r="O15" s="123"/>
+      <c r="M15" s="147"/>
+      <c r="N15" s="147"/>
+      <c r="O15" s="147"/>
       <c r="P15" s="36"/>
       <c r="Q15" s="36"/>
       <c r="R15" s="40"/>
@@ -4473,17 +4475,19 @@
       <c r="O16" s="20">
         <v>0</v>
       </c>
-      <c r="P16" s="127" t="s">
+      <c r="P16" s="143" t="s">
         <v>16</v>
       </c>
-      <c r="Q16" s="128"/>
-      <c r="R16" s="128"/>
-      <c r="S16" s="129" t="s">
+      <c r="Q16" s="144"/>
+      <c r="R16" s="144"/>
+      <c r="S16" s="145" t="s">
         <v>27</v>
       </c>
-      <c r="T16" s="129"/>
-      <c r="U16" s="130"/>
-      <c r="V16" s="22"/>
+      <c r="T16" s="145"/>
+      <c r="U16" s="146"/>
+      <c r="V16" s="22" t="s">
+        <v>18</v>
+      </c>
       <c r="W16" s="19"/>
       <c r="X16" s="19" t="s">
         <v>18</v>
@@ -4536,17 +4540,19 @@
       <c r="O17" s="26">
         <v>1</v>
       </c>
-      <c r="P17" s="125" t="s">
+      <c r="P17" s="132" t="s">
         <v>16</v>
       </c>
-      <c r="Q17" s="122"/>
-      <c r="R17" s="122"/>
-      <c r="S17" s="122" t="s">
+      <c r="Q17" s="114"/>
+      <c r="R17" s="114"/>
+      <c r="S17" s="114" t="s">
         <v>27</v>
       </c>
-      <c r="T17" s="122"/>
-      <c r="U17" s="124"/>
-      <c r="V17" s="22"/>
+      <c r="T17" s="114"/>
+      <c r="U17" s="115"/>
+      <c r="V17" s="22" t="s">
+        <v>18</v>
+      </c>
       <c r="W17" s="19"/>
       <c r="X17" s="19" t="s">
         <v>18</v>
@@ -4599,16 +4605,16 @@
       <c r="O18" s="20">
         <v>0</v>
       </c>
-      <c r="P18" s="125" t="s">
+      <c r="P18" s="132" t="s">
         <v>16</v>
       </c>
-      <c r="Q18" s="122"/>
-      <c r="R18" s="122"/>
-      <c r="S18" s="122" t="s">
+      <c r="Q18" s="114"/>
+      <c r="R18" s="114"/>
+      <c r="S18" s="114" t="s">
         <v>27</v>
       </c>
-      <c r="T18" s="122"/>
-      <c r="U18" s="124"/>
+      <c r="T18" s="114"/>
+      <c r="U18" s="115"/>
       <c r="V18" s="22" t="s">
         <v>18</v>
       </c>
@@ -4664,16 +4670,16 @@
       <c r="O19" s="26">
         <v>1</v>
       </c>
-      <c r="P19" s="125" t="s">
+      <c r="P19" s="132" t="s">
         <v>16</v>
       </c>
-      <c r="Q19" s="122"/>
-      <c r="R19" s="122"/>
-      <c r="S19" s="122" t="s">
+      <c r="Q19" s="114"/>
+      <c r="R19" s="114"/>
+      <c r="S19" s="114" t="s">
         <v>27</v>
       </c>
-      <c r="T19" s="122"/>
-      <c r="U19" s="124"/>
+      <c r="T19" s="114"/>
+      <c r="U19" s="115"/>
       <c r="V19" s="22" t="s">
         <v>18</v>
       </c>
@@ -4729,16 +4735,16 @@
       <c r="O20" s="20">
         <v>0</v>
       </c>
-      <c r="P20" s="125" t="s">
+      <c r="P20" s="132" t="s">
         <v>16</v>
       </c>
-      <c r="Q20" s="122"/>
-      <c r="R20" s="122"/>
-      <c r="S20" s="122" t="s">
+      <c r="Q20" s="114"/>
+      <c r="R20" s="114"/>
+      <c r="S20" s="114" t="s">
         <v>27</v>
       </c>
-      <c r="T20" s="122"/>
-      <c r="U20" s="124"/>
+      <c r="T20" s="114"/>
+      <c r="U20" s="115"/>
       <c r="V20" s="22" t="s">
         <v>18</v>
       </c>
@@ -4794,16 +4800,16 @@
       <c r="O21" s="26">
         <v>1</v>
       </c>
-      <c r="P21" s="125" t="s">
+      <c r="P21" s="132" t="s">
         <v>16</v>
       </c>
-      <c r="Q21" s="122"/>
-      <c r="R21" s="122"/>
-      <c r="S21" s="122" t="s">
+      <c r="Q21" s="114"/>
+      <c r="R21" s="114"/>
+      <c r="S21" s="114" t="s">
         <v>27</v>
       </c>
-      <c r="T21" s="122"/>
-      <c r="U21" s="124"/>
+      <c r="T21" s="114"/>
+      <c r="U21" s="115"/>
       <c r="V21" s="22" t="s">
         <v>18</v>
       </c>
@@ -4861,16 +4867,16 @@
       <c r="O22" s="20">
         <v>0</v>
       </c>
-      <c r="P22" s="125" t="s">
+      <c r="P22" s="132" t="s">
         <v>16</v>
       </c>
-      <c r="Q22" s="122"/>
-      <c r="R22" s="122"/>
-      <c r="S22" s="122" t="s">
+      <c r="Q22" s="114"/>
+      <c r="R22" s="114"/>
+      <c r="S22" s="114" t="s">
         <v>27</v>
       </c>
-      <c r="T22" s="122"/>
-      <c r="U22" s="124"/>
+      <c r="T22" s="114"/>
+      <c r="U22" s="115"/>
       <c r="V22" s="22" t="s">
         <v>18</v>
       </c>
@@ -4928,16 +4934,16 @@
       <c r="O23" s="26">
         <v>1</v>
       </c>
-      <c r="P23" s="125" t="s">
+      <c r="P23" s="132" t="s">
         <v>16</v>
       </c>
-      <c r="Q23" s="122"/>
-      <c r="R23" s="122"/>
-      <c r="S23" s="122" t="s">
+      <c r="Q23" s="114"/>
+      <c r="R23" s="114"/>
+      <c r="S23" s="114" t="s">
         <v>27</v>
       </c>
-      <c r="T23" s="122"/>
-      <c r="U23" s="124"/>
+      <c r="T23" s="114"/>
+      <c r="U23" s="115"/>
       <c r="V23" s="22" t="s">
         <v>18</v>
       </c>
@@ -4993,17 +4999,19 @@
       <c r="O24" s="20">
         <v>0</v>
       </c>
-      <c r="P24" s="125" t="s">
+      <c r="P24" s="132" t="s">
         <v>16</v>
       </c>
-      <c r="Q24" s="122"/>
-      <c r="R24" s="122"/>
-      <c r="S24" s="122" t="s">
+      <c r="Q24" s="114"/>
+      <c r="R24" s="114"/>
+      <c r="S24" s="114" t="s">
         <v>20</v>
       </c>
-      <c r="T24" s="122"/>
-      <c r="U24" s="124"/>
-      <c r="V24" s="22"/>
+      <c r="T24" s="114"/>
+      <c r="U24" s="115"/>
+      <c r="V24" s="22" t="s">
+        <v>18</v>
+      </c>
       <c r="W24" s="19"/>
       <c r="X24" s="19" t="s">
         <v>18</v>
@@ -5058,18 +5066,22 @@
       <c r="O25" s="26">
         <v>1</v>
       </c>
-      <c r="P25" s="125" t="s">
+      <c r="P25" s="132" t="s">
         <v>20</v>
       </c>
-      <c r="Q25" s="122"/>
-      <c r="R25" s="122"/>
-      <c r="S25" s="122" t="s">
+      <c r="Q25" s="114"/>
+      <c r="R25" s="114"/>
+      <c r="S25" s="114" t="s">
         <v>17</v>
       </c>
-      <c r="T25" s="122"/>
-      <c r="U25" s="124"/>
-      <c r="V25" s="22"/>
-      <c r="W25" s="19"/>
+      <c r="T25" s="114"/>
+      <c r="U25" s="115"/>
+      <c r="V25" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="W25" s="22" t="s">
+        <v>18</v>
+      </c>
       <c r="X25" s="19" t="s">
         <v>18</v>
       </c>
@@ -5121,16 +5133,16 @@
       <c r="O26" s="20">
         <v>0</v>
       </c>
-      <c r="P26" s="125" t="s">
+      <c r="P26" s="132" t="s">
         <v>16</v>
       </c>
-      <c r="Q26" s="122"/>
-      <c r="R26" s="122"/>
-      <c r="S26" s="122" t="s">
+      <c r="Q26" s="114"/>
+      <c r="R26" s="114"/>
+      <c r="S26" s="114" t="s">
         <v>20</v>
       </c>
-      <c r="T26" s="122"/>
-      <c r="U26" s="124"/>
+      <c r="T26" s="114"/>
+      <c r="U26" s="115"/>
       <c r="V26" s="22" t="s">
         <v>18</v>
       </c>
@@ -5188,16 +5200,16 @@
       <c r="O27" s="26">
         <v>1</v>
       </c>
-      <c r="P27" s="125" t="s">
+      <c r="P27" s="132" t="s">
         <v>16</v>
       </c>
-      <c r="Q27" s="122"/>
-      <c r="R27" s="122"/>
-      <c r="S27" s="122" t="s">
+      <c r="Q27" s="114"/>
+      <c r="R27" s="114"/>
+      <c r="S27" s="114" t="s">
         <v>20</v>
       </c>
-      <c r="T27" s="122"/>
-      <c r="U27" s="124"/>
+      <c r="T27" s="114"/>
+      <c r="U27" s="115"/>
       <c r="V27" s="22" t="s">
         <v>18</v>
       </c>
@@ -5255,17 +5267,19 @@
       <c r="O28" s="20">
         <v>0</v>
       </c>
-      <c r="P28" s="125" t="s">
+      <c r="P28" s="132" t="s">
         <v>16</v>
       </c>
-      <c r="Q28" s="122"/>
-      <c r="R28" s="122"/>
-      <c r="S28" s="122" t="s">
+      <c r="Q28" s="114"/>
+      <c r="R28" s="114"/>
+      <c r="S28" s="114" t="s">
         <v>27</v>
       </c>
-      <c r="T28" s="122"/>
-      <c r="U28" s="124"/>
-      <c r="V28" s="22"/>
+      <c r="T28" s="114"/>
+      <c r="U28" s="115"/>
+      <c r="V28" s="22" t="s">
+        <v>18</v>
+      </c>
       <c r="W28" s="19"/>
       <c r="X28" s="19" t="s">
         <v>18</v>
@@ -5320,16 +5334,16 @@
       <c r="O29" s="26">
         <v>1</v>
       </c>
-      <c r="P29" s="125" t="s">
+      <c r="P29" s="132" t="s">
         <v>20</v>
       </c>
-      <c r="Q29" s="122"/>
-      <c r="R29" s="122"/>
-      <c r="S29" s="143" t="s">
+      <c r="Q29" s="114"/>
+      <c r="R29" s="114"/>
+      <c r="S29" s="133" t="s">
         <v>36</v>
       </c>
-      <c r="T29" s="143"/>
-      <c r="U29" s="144"/>
+      <c r="T29" s="133"/>
+      <c r="U29" s="134"/>
       <c r="V29" s="22"/>
       <c r="W29" s="19"/>
       <c r="X29" s="19" t="s">
@@ -5383,17 +5397,19 @@
       <c r="O30" s="20">
         <v>0</v>
       </c>
-      <c r="P30" s="125" t="s">
+      <c r="P30" s="132" t="s">
         <v>16</v>
       </c>
-      <c r="Q30" s="122"/>
-      <c r="R30" s="122"/>
-      <c r="S30" s="122" t="s">
+      <c r="Q30" s="114"/>
+      <c r="R30" s="114"/>
+      <c r="S30" s="114" t="s">
         <v>27</v>
       </c>
-      <c r="T30" s="122"/>
-      <c r="U30" s="124"/>
-      <c r="V30" s="22"/>
+      <c r="T30" s="114"/>
+      <c r="U30" s="115"/>
+      <c r="V30" s="22" t="s">
+        <v>18</v>
+      </c>
       <c r="W30" s="19"/>
       <c r="X30" s="19" t="s">
         <v>18</v>
@@ -5446,17 +5462,19 @@
       <c r="O31" s="58">
         <v>1</v>
       </c>
-      <c r="P31" s="146" t="s">
+      <c r="P31" s="135" t="s">
         <v>16</v>
       </c>
-      <c r="Q31" s="113"/>
-      <c r="R31" s="113"/>
-      <c r="S31" s="113" t="s">
+      <c r="Q31" s="112"/>
+      <c r="R31" s="112"/>
+      <c r="S31" s="112" t="s">
         <v>17</v>
       </c>
-      <c r="T31" s="113"/>
-      <c r="U31" s="145"/>
-      <c r="V31" s="54"/>
+      <c r="T31" s="112"/>
+      <c r="U31" s="123"/>
+      <c r="V31" s="22" t="s">
+        <v>18</v>
+      </c>
       <c r="W31" s="56"/>
       <c r="X31" s="56" t="s">
         <v>18</v>
@@ -5554,16 +5572,16 @@
       <c r="O33" s="99">
         <v>0</v>
       </c>
-      <c r="P33" s="131" t="s">
+      <c r="P33" s="120" t="s">
         <v>16</v>
       </c>
-      <c r="Q33" s="131"/>
-      <c r="R33" s="131"/>
-      <c r="S33" s="122" t="s">
+      <c r="Q33" s="120"/>
+      <c r="R33" s="120"/>
+      <c r="S33" s="114" t="s">
         <v>17</v>
       </c>
-      <c r="T33" s="122"/>
-      <c r="U33" s="124"/>
+      <c r="T33" s="114"/>
+      <c r="U33" s="115"/>
       <c r="V33" s="22" t="s">
         <v>18</v>
       </c>
@@ -5630,10 +5648,10 @@
       <c r="C35" s="60" t="s">
         <v>40</v>
       </c>
-      <c r="D35" s="133" t="s">
+      <c r="D35" s="136" t="s">
         <v>43</v>
       </c>
-      <c r="E35" s="134"/>
+      <c r="E35" s="137"/>
       <c r="F35" s="61">
         <v>1</v>
       </c>
@@ -5649,21 +5667,21 @@
       <c r="J35" s="64">
         <v>0</v>
       </c>
-      <c r="K35" s="135" t="s">
+      <c r="K35" s="138" t="s">
         <v>41</v>
       </c>
-      <c r="L35" s="135"/>
-      <c r="M35" s="135"/>
-      <c r="N35" s="136" t="s">
+      <c r="L35" s="138"/>
+      <c r="M35" s="138"/>
+      <c r="N35" s="130" t="s">
         <v>24</v>
       </c>
-      <c r="O35" s="136"/>
-      <c r="P35" s="136"/>
-      <c r="Q35" s="136"/>
-      <c r="R35" s="136"/>
-      <c r="S35" s="136"/>
-      <c r="T35" s="136"/>
-      <c r="U35" s="137"/>
+      <c r="O35" s="130"/>
+      <c r="P35" s="130"/>
+      <c r="Q35" s="130"/>
+      <c r="R35" s="130"/>
+      <c r="S35" s="130"/>
+      <c r="T35" s="130"/>
+      <c r="U35" s="131"/>
       <c r="V35" s="22"/>
       <c r="W35" s="19"/>
       <c r="X35" s="19"/>
@@ -5679,10 +5697,10 @@
       <c r="C36" s="65" t="s">
         <v>40</v>
       </c>
-      <c r="D36" s="133" t="s">
+      <c r="D36" s="136" t="s">
         <v>43</v>
       </c>
-      <c r="E36" s="134"/>
+      <c r="E36" s="137"/>
       <c r="F36" s="67">
         <v>1</v>
       </c>
@@ -5698,21 +5716,21 @@
       <c r="J36" s="70">
         <v>1</v>
       </c>
-      <c r="K36" s="138" t="s">
+      <c r="K36" s="139" t="s">
         <v>41</v>
       </c>
-      <c r="L36" s="138"/>
-      <c r="M36" s="138"/>
-      <c r="N36" s="139" t="s">
+      <c r="L36" s="139"/>
+      <c r="M36" s="139"/>
+      <c r="N36" s="126" t="s">
         <v>24</v>
       </c>
-      <c r="O36" s="139"/>
-      <c r="P36" s="139"/>
-      <c r="Q36" s="139"/>
-      <c r="R36" s="139"/>
-      <c r="S36" s="139"/>
-      <c r="T36" s="139"/>
-      <c r="U36" s="140"/>
+      <c r="O36" s="126"/>
+      <c r="P36" s="126"/>
+      <c r="Q36" s="126"/>
+      <c r="R36" s="126"/>
+      <c r="S36" s="126"/>
+      <c r="T36" s="126"/>
+      <c r="U36" s="127"/>
       <c r="V36" s="22"/>
       <c r="W36" s="19"/>
       <c r="X36" s="19"/>
@@ -5738,15 +5756,15 @@
       <c r="I37" s="36">
         <v>1</v>
       </c>
-      <c r="J37" s="141" t="s">
+      <c r="J37" s="128" t="s">
         <v>11</v>
       </c>
-      <c r="K37" s="141"/>
-      <c r="L37" s="141"/>
-      <c r="M37" s="141"/>
-      <c r="N37" s="141"/>
-      <c r="O37" s="141"/>
-      <c r="P37" s="141"/>
+      <c r="K37" s="128"/>
+      <c r="L37" s="128"/>
+      <c r="M37" s="128"/>
+      <c r="N37" s="128"/>
+      <c r="O37" s="128"/>
+      <c r="P37" s="128"/>
       <c r="Q37" s="36"/>
       <c r="R37" s="36"/>
       <c r="S37" s="36"/>
@@ -5808,15 +5826,15 @@
       <c r="N38" s="64">
         <v>0</v>
       </c>
-      <c r="O38" s="136" t="s">
+      <c r="O38" s="130" t="s">
         <v>48</v>
       </c>
-      <c r="P38" s="136"/>
-      <c r="Q38" s="136"/>
-      <c r="R38" s="136"/>
-      <c r="S38" s="136"/>
-      <c r="T38" s="136"/>
-      <c r="U38" s="137"/>
+      <c r="P38" s="130"/>
+      <c r="Q38" s="130"/>
+      <c r="R38" s="130"/>
+      <c r="S38" s="130"/>
+      <c r="T38" s="130"/>
+      <c r="U38" s="131"/>
       <c r="V38" s="22"/>
       <c r="W38" s="19"/>
       <c r="X38" s="19"/>
@@ -5865,15 +5883,15 @@
       <c r="N39" s="75">
         <v>1</v>
       </c>
-      <c r="O39" s="139" t="s">
+      <c r="O39" s="126" t="s">
         <v>48</v>
       </c>
-      <c r="P39" s="139"/>
-      <c r="Q39" s="139"/>
-      <c r="R39" s="139"/>
-      <c r="S39" s="139"/>
-      <c r="T39" s="139"/>
-      <c r="U39" s="140"/>
+      <c r="P39" s="126"/>
+      <c r="Q39" s="126"/>
+      <c r="R39" s="126"/>
+      <c r="S39" s="126"/>
+      <c r="T39" s="126"/>
+      <c r="U39" s="127"/>
       <c r="V39" s="22"/>
       <c r="W39" s="19"/>
       <c r="X39" s="19"/>
@@ -5903,20 +5921,20 @@
       <c r="I40" s="36">
         <v>1</v>
       </c>
-      <c r="J40" s="141" t="s">
+      <c r="J40" s="128" t="s">
         <v>11</v>
       </c>
-      <c r="K40" s="141"/>
-      <c r="L40" s="141"/>
-      <c r="M40" s="141"/>
-      <c r="N40" s="141"/>
-      <c r="O40" s="141"/>
-      <c r="P40" s="141"/>
-      <c r="Q40" s="141"/>
-      <c r="R40" s="141"/>
-      <c r="S40" s="141"/>
-      <c r="T40" s="141"/>
-      <c r="U40" s="142"/>
+      <c r="K40" s="128"/>
+      <c r="L40" s="128"/>
+      <c r="M40" s="128"/>
+      <c r="N40" s="128"/>
+      <c r="O40" s="128"/>
+      <c r="P40" s="128"/>
+      <c r="Q40" s="128"/>
+      <c r="R40" s="128"/>
+      <c r="S40" s="128"/>
+      <c r="T40" s="128"/>
+      <c r="U40" s="129"/>
       <c r="V40" s="42"/>
       <c r="W40" s="36"/>
       <c r="X40" s="36"/>
@@ -5934,22 +5952,22 @@
       <c r="G41" s="36"/>
       <c r="H41" s="36"/>
       <c r="I41" s="36"/>
-      <c r="J41" s="141" t="s">
+      <c r="J41" s="128" t="s">
         <v>54</v>
       </c>
-      <c r="K41" s="141"/>
-      <c r="L41" s="141"/>
-      <c r="M41" s="141"/>
-      <c r="N41" s="141" t="s">
+      <c r="K41" s="128"/>
+      <c r="L41" s="128"/>
+      <c r="M41" s="128"/>
+      <c r="N41" s="128" t="s">
         <v>24</v>
       </c>
-      <c r="O41" s="141"/>
-      <c r="P41" s="141"/>
-      <c r="Q41" s="141"/>
-      <c r="R41" s="141"/>
-      <c r="S41" s="141"/>
-      <c r="T41" s="141"/>
-      <c r="U41" s="142"/>
+      <c r="O41" s="128"/>
+      <c r="P41" s="128"/>
+      <c r="Q41" s="128"/>
+      <c r="R41" s="128"/>
+      <c r="S41" s="128"/>
+      <c r="T41" s="128"/>
+      <c r="U41" s="129"/>
       <c r="V41" s="42" t="s">
         <v>6</v>
       </c>
@@ -5999,16 +6017,16 @@
       <c r="M42" s="20">
         <v>0</v>
       </c>
-      <c r="N42" s="122" t="s">
+      <c r="N42" s="114" t="s">
         <v>24</v>
       </c>
-      <c r="O42" s="122"/>
-      <c r="P42" s="122"/>
-      <c r="Q42" s="122"/>
-      <c r="R42" s="122"/>
-      <c r="S42" s="122"/>
-      <c r="T42" s="122"/>
-      <c r="U42" s="124"/>
+      <c r="O42" s="114"/>
+      <c r="P42" s="114"/>
+      <c r="Q42" s="114"/>
+      <c r="R42" s="114"/>
+      <c r="S42" s="114"/>
+      <c r="T42" s="114"/>
+      <c r="U42" s="115"/>
       <c r="V42" s="22"/>
       <c r="W42" s="19"/>
       <c r="X42" s="19"/>
@@ -6052,16 +6070,16 @@
       <c r="M43" s="20">
         <v>1</v>
       </c>
-      <c r="N43" s="122" t="s">
+      <c r="N43" s="114" t="s">
         <v>24</v>
       </c>
-      <c r="O43" s="122"/>
-      <c r="P43" s="122"/>
-      <c r="Q43" s="122"/>
-      <c r="R43" s="122"/>
-      <c r="S43" s="122"/>
-      <c r="T43" s="122"/>
-      <c r="U43" s="124"/>
+      <c r="O43" s="114"/>
+      <c r="P43" s="114"/>
+      <c r="Q43" s="114"/>
+      <c r="R43" s="114"/>
+      <c r="S43" s="114"/>
+      <c r="T43" s="114"/>
+      <c r="U43" s="115"/>
       <c r="V43" s="22"/>
       <c r="W43" s="19"/>
       <c r="X43" s="19"/>
@@ -6070,7 +6088,7 @@
       </c>
     </row>
     <row r="44" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A44" s="149" t="s">
+      <c r="A44" s="116" t="s">
         <v>113</v>
       </c>
       <c r="B44" s="14" t="s">
@@ -6105,16 +6123,16 @@
       <c r="M44" s="20">
         <v>0</v>
       </c>
-      <c r="N44" s="122" t="s">
+      <c r="N44" s="114" t="s">
         <v>24</v>
       </c>
-      <c r="O44" s="122"/>
-      <c r="P44" s="122"/>
-      <c r="Q44" s="122"/>
-      <c r="R44" s="122"/>
-      <c r="S44" s="122"/>
-      <c r="T44" s="122"/>
-      <c r="U44" s="124"/>
+      <c r="O44" s="114"/>
+      <c r="P44" s="114"/>
+      <c r="Q44" s="114"/>
+      <c r="R44" s="114"/>
+      <c r="S44" s="114"/>
+      <c r="T44" s="114"/>
+      <c r="U44" s="115"/>
       <c r="V44" s="22">
         <v>1</v>
       </c>
@@ -6123,7 +6141,7 @@
       <c r="Y44" s="21"/>
     </row>
     <row r="45" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A45" s="150"/>
+      <c r="A45" s="117"/>
       <c r="B45" s="14" t="s">
         <v>132</v>
       </c>
@@ -6156,16 +6174,16 @@
       <c r="M45" s="20">
         <v>0</v>
       </c>
-      <c r="N45" s="122" t="s">
+      <c r="N45" s="114" t="s">
         <v>24</v>
       </c>
-      <c r="O45" s="122"/>
-      <c r="P45" s="122"/>
-      <c r="Q45" s="122"/>
-      <c r="R45" s="122"/>
-      <c r="S45" s="122"/>
-      <c r="T45" s="122"/>
-      <c r="U45" s="124"/>
+      <c r="O45" s="114"/>
+      <c r="P45" s="114"/>
+      <c r="Q45" s="114"/>
+      <c r="R45" s="114"/>
+      <c r="S45" s="114"/>
+      <c r="T45" s="114"/>
+      <c r="U45" s="115"/>
       <c r="V45" s="22">
         <v>1</v>
       </c>
@@ -6174,7 +6192,7 @@
       <c r="Y45" s="21"/>
     </row>
     <row r="46" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A46" s="151" t="s">
+      <c r="A46" s="118" t="s">
         <v>114</v>
       </c>
       <c r="B46" s="14" t="s">
@@ -6209,16 +6227,16 @@
       <c r="M46" s="20">
         <v>1</v>
       </c>
-      <c r="N46" s="122" t="s">
+      <c r="N46" s="114" t="s">
         <v>24</v>
       </c>
-      <c r="O46" s="122"/>
-      <c r="P46" s="122"/>
-      <c r="Q46" s="122"/>
-      <c r="R46" s="122"/>
-      <c r="S46" s="122"/>
-      <c r="T46" s="122"/>
-      <c r="U46" s="124"/>
+      <c r="O46" s="114"/>
+      <c r="P46" s="114"/>
+      <c r="Q46" s="114"/>
+      <c r="R46" s="114"/>
+      <c r="S46" s="114"/>
+      <c r="T46" s="114"/>
+      <c r="U46" s="115"/>
       <c r="V46" s="22">
         <v>0</v>
       </c>
@@ -6227,7 +6245,7 @@
       <c r="Y46" s="21"/>
     </row>
     <row r="47" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A47" s="152"/>
+      <c r="A47" s="119"/>
       <c r="B47" s="14" t="s">
         <v>133</v>
       </c>
@@ -6260,16 +6278,16 @@
       <c r="M47" s="20">
         <v>1</v>
       </c>
-      <c r="N47" s="122" t="s">
+      <c r="N47" s="114" t="s">
         <v>24</v>
       </c>
-      <c r="O47" s="122"/>
-      <c r="P47" s="122"/>
-      <c r="Q47" s="122"/>
-      <c r="R47" s="122"/>
-      <c r="S47" s="122"/>
-      <c r="T47" s="122"/>
-      <c r="U47" s="124"/>
+      <c r="O47" s="114"/>
+      <c r="P47" s="114"/>
+      <c r="Q47" s="114"/>
+      <c r="R47" s="114"/>
+      <c r="S47" s="114"/>
+      <c r="T47" s="114"/>
+      <c r="U47" s="115"/>
       <c r="V47" s="22">
         <v>0</v>
       </c>
@@ -6313,16 +6331,16 @@
       <c r="M48" s="20">
         <v>0</v>
       </c>
-      <c r="N48" s="122" t="s">
+      <c r="N48" s="114" t="s">
         <v>24</v>
       </c>
-      <c r="O48" s="122"/>
-      <c r="P48" s="122"/>
-      <c r="Q48" s="122"/>
-      <c r="R48" s="122"/>
-      <c r="S48" s="122"/>
-      <c r="T48" s="122"/>
-      <c r="U48" s="124"/>
+      <c r="O48" s="114"/>
+      <c r="P48" s="114"/>
+      <c r="Q48" s="114"/>
+      <c r="R48" s="114"/>
+      <c r="S48" s="114"/>
+      <c r="T48" s="114"/>
+      <c r="U48" s="115"/>
       <c r="V48" s="22"/>
       <c r="W48" s="19"/>
       <c r="X48" s="19">
@@ -6366,16 +6384,16 @@
       <c r="M49" s="20">
         <v>1</v>
       </c>
-      <c r="N49" s="122" t="s">
+      <c r="N49" s="114" t="s">
         <v>24</v>
       </c>
-      <c r="O49" s="122"/>
-      <c r="P49" s="122"/>
-      <c r="Q49" s="122"/>
-      <c r="R49" s="122"/>
-      <c r="S49" s="122"/>
-      <c r="T49" s="122"/>
-      <c r="U49" s="124"/>
+      <c r="O49" s="114"/>
+      <c r="P49" s="114"/>
+      <c r="Q49" s="114"/>
+      <c r="R49" s="114"/>
+      <c r="S49" s="114"/>
+      <c r="T49" s="114"/>
+      <c r="U49" s="115"/>
       <c r="V49" s="22"/>
       <c r="W49" s="19"/>
       <c r="X49" s="19">
@@ -6419,16 +6437,16 @@
       <c r="M50" s="20">
         <v>0</v>
       </c>
-      <c r="N50" s="122" t="s">
+      <c r="N50" s="114" t="s">
         <v>24</v>
       </c>
-      <c r="O50" s="122"/>
-      <c r="P50" s="122"/>
-      <c r="Q50" s="122"/>
-      <c r="R50" s="122"/>
-      <c r="S50" s="122"/>
-      <c r="T50" s="122"/>
-      <c r="U50" s="124"/>
+      <c r="O50" s="114"/>
+      <c r="P50" s="114"/>
+      <c r="Q50" s="114"/>
+      <c r="R50" s="114"/>
+      <c r="S50" s="114"/>
+      <c r="T50" s="114"/>
+      <c r="U50" s="115"/>
       <c r="V50" s="22"/>
       <c r="W50" s="19">
         <v>1</v>
@@ -6472,16 +6490,16 @@
       <c r="M51" s="20">
         <v>1</v>
       </c>
-      <c r="N51" s="122" t="s">
+      <c r="N51" s="114" t="s">
         <v>24</v>
       </c>
-      <c r="O51" s="122"/>
-      <c r="P51" s="122"/>
-      <c r="Q51" s="122"/>
-      <c r="R51" s="122"/>
-      <c r="S51" s="122"/>
-      <c r="T51" s="122"/>
-      <c r="U51" s="124"/>
+      <c r="O51" s="114"/>
+      <c r="P51" s="114"/>
+      <c r="Q51" s="114"/>
+      <c r="R51" s="114"/>
+      <c r="S51" s="114"/>
+      <c r="T51" s="114"/>
+      <c r="U51" s="115"/>
       <c r="V51" s="22"/>
       <c r="W51" s="19">
         <v>0</v>
@@ -6525,22 +6543,22 @@
       <c r="M52" s="20">
         <v>0</v>
       </c>
-      <c r="N52" s="122" t="s">
+      <c r="N52" s="114" t="s">
         <v>24</v>
       </c>
-      <c r="O52" s="122"/>
-      <c r="P52" s="122"/>
-      <c r="Q52" s="122"/>
-      <c r="R52" s="122"/>
-      <c r="S52" s="122"/>
-      <c r="T52" s="122"/>
-      <c r="U52" s="124"/>
-      <c r="V52" s="147" t="s">
+      <c r="O52" s="114"/>
+      <c r="P52" s="114"/>
+      <c r="Q52" s="114"/>
+      <c r="R52" s="114"/>
+      <c r="S52" s="114"/>
+      <c r="T52" s="114"/>
+      <c r="U52" s="115"/>
+      <c r="V52" s="124" t="s">
         <v>64</v>
       </c>
-      <c r="W52" s="122"/>
-      <c r="X52" s="122"/>
-      <c r="Y52" s="124"/>
+      <c r="W52" s="114"/>
+      <c r="X52" s="114"/>
+      <c r="Y52" s="115"/>
     </row>
     <row r="53" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A53" s="110" t="s">
@@ -6578,22 +6596,22 @@
       <c r="M53" s="20">
         <v>1</v>
       </c>
-      <c r="N53" s="122" t="s">
+      <c r="N53" s="114" t="s">
         <v>24</v>
       </c>
-      <c r="O53" s="122"/>
-      <c r="P53" s="122"/>
-      <c r="Q53" s="122"/>
-      <c r="R53" s="122"/>
-      <c r="S53" s="122"/>
-      <c r="T53" s="122"/>
-      <c r="U53" s="124"/>
-      <c r="V53" s="147" t="s">
+      <c r="O53" s="114"/>
+      <c r="P53" s="114"/>
+      <c r="Q53" s="114"/>
+      <c r="R53" s="114"/>
+      <c r="S53" s="114"/>
+      <c r="T53" s="114"/>
+      <c r="U53" s="115"/>
+      <c r="V53" s="124" t="s">
         <v>66</v>
       </c>
-      <c r="W53" s="122"/>
-      <c r="X53" s="122"/>
-      <c r="Y53" s="124"/>
+      <c r="W53" s="114"/>
+      <c r="X53" s="114"/>
+      <c r="Y53" s="115"/>
     </row>
     <row r="54" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A54" s="110" t="s">
@@ -6631,22 +6649,22 @@
       <c r="M54" s="20">
         <v>0</v>
       </c>
-      <c r="N54" s="122" t="s">
+      <c r="N54" s="114" t="s">
         <v>24</v>
       </c>
-      <c r="O54" s="122"/>
-      <c r="P54" s="122"/>
-      <c r="Q54" s="122"/>
-      <c r="R54" s="122"/>
-      <c r="S54" s="122"/>
-      <c r="T54" s="122"/>
-      <c r="U54" s="124"/>
-      <c r="V54" s="147" t="s">
+      <c r="O54" s="114"/>
+      <c r="P54" s="114"/>
+      <c r="Q54" s="114"/>
+      <c r="R54" s="114"/>
+      <c r="S54" s="114"/>
+      <c r="T54" s="114"/>
+      <c r="U54" s="115"/>
+      <c r="V54" s="124" t="s">
         <v>68</v>
       </c>
-      <c r="W54" s="122"/>
-      <c r="X54" s="122"/>
-      <c r="Y54" s="124"/>
+      <c r="W54" s="114"/>
+      <c r="X54" s="114"/>
+      <c r="Y54" s="115"/>
     </row>
     <row r="55" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A55" s="110" t="s">
@@ -6684,22 +6702,22 @@
       <c r="M55" s="20">
         <v>1</v>
       </c>
-      <c r="N55" s="122" t="s">
+      <c r="N55" s="114" t="s">
         <v>24</v>
       </c>
-      <c r="O55" s="122"/>
-      <c r="P55" s="122"/>
-      <c r="Q55" s="122"/>
-      <c r="R55" s="122"/>
-      <c r="S55" s="122"/>
-      <c r="T55" s="122"/>
-      <c r="U55" s="124"/>
-      <c r="V55" s="147" t="s">
+      <c r="O55" s="114"/>
+      <c r="P55" s="114"/>
+      <c r="Q55" s="114"/>
+      <c r="R55" s="114"/>
+      <c r="S55" s="114"/>
+      <c r="T55" s="114"/>
+      <c r="U55" s="115"/>
+      <c r="V55" s="124" t="s">
         <v>70</v>
       </c>
-      <c r="W55" s="122"/>
-      <c r="X55" s="122"/>
-      <c r="Y55" s="124"/>
+      <c r="W55" s="114"/>
+      <c r="X55" s="114"/>
+      <c r="Y55" s="115"/>
     </row>
     <row r="56" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A56" s="110" t="s">
@@ -6737,22 +6755,22 @@
       <c r="M56" s="20">
         <v>0</v>
       </c>
-      <c r="N56" s="122" t="s">
+      <c r="N56" s="114" t="s">
         <v>24</v>
       </c>
-      <c r="O56" s="122"/>
-      <c r="P56" s="122"/>
-      <c r="Q56" s="122"/>
-      <c r="R56" s="122"/>
-      <c r="S56" s="122"/>
-      <c r="T56" s="122"/>
-      <c r="U56" s="124"/>
-      <c r="V56" s="147" t="s">
+      <c r="O56" s="114"/>
+      <c r="P56" s="114"/>
+      <c r="Q56" s="114"/>
+      <c r="R56" s="114"/>
+      <c r="S56" s="114"/>
+      <c r="T56" s="114"/>
+      <c r="U56" s="115"/>
+      <c r="V56" s="124" t="s">
         <v>72</v>
       </c>
-      <c r="W56" s="122"/>
-      <c r="X56" s="122"/>
-      <c r="Y56" s="124"/>
+      <c r="W56" s="114"/>
+      <c r="X56" s="114"/>
+      <c r="Y56" s="115"/>
     </row>
     <row r="57" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A57" s="109" t="s">
@@ -6790,25 +6808,25 @@
       <c r="M57" s="103">
         <v>1</v>
       </c>
-      <c r="N57" s="113" t="s">
+      <c r="N57" s="112" t="s">
         <v>24</v>
       </c>
-      <c r="O57" s="113"/>
-      <c r="P57" s="113"/>
-      <c r="Q57" s="113"/>
-      <c r="R57" s="113"/>
-      <c r="S57" s="113"/>
-      <c r="T57" s="113"/>
-      <c r="U57" s="145"/>
-      <c r="V57" s="112" t="s">
+      <c r="O57" s="112"/>
+      <c r="P57" s="112"/>
+      <c r="Q57" s="112"/>
+      <c r="R57" s="112"/>
+      <c r="S57" s="112"/>
+      <c r="T57" s="112"/>
+      <c r="U57" s="123"/>
+      <c r="V57" s="122" t="s">
         <v>74</v>
       </c>
-      <c r="W57" s="113"/>
-      <c r="X57" s="113"/>
-      <c r="Y57" s="145"/>
+      <c r="W57" s="112"/>
+      <c r="X57" s="112"/>
+      <c r="Y57" s="123"/>
     </row>
     <row r="58" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A58" s="115" t="s">
+      <c r="A58" s="148" t="s">
         <v>130</v>
       </c>
       <c r="B58" s="14" t="s">
@@ -6831,28 +6849,28 @@
       <c r="I58" s="19">
         <v>1</v>
       </c>
-      <c r="J58" s="113" t="s">
+      <c r="J58" s="112" t="s">
         <v>129</v>
       </c>
-      <c r="K58" s="113"/>
-      <c r="L58" s="113"/>
-      <c r="M58" s="113"/>
-      <c r="N58" s="113"/>
-      <c r="O58" s="113"/>
-      <c r="P58" s="113"/>
-      <c r="Q58" s="113"/>
-      <c r="R58" s="113"/>
-      <c r="S58" s="113"/>
-      <c r="T58" s="113"/>
-      <c r="U58" s="114"/>
-      <c r="V58" s="147"/>
-      <c r="W58" s="122"/>
-      <c r="X58" s="122"/>
-      <c r="Y58" s="148"/>
+      <c r="K58" s="112"/>
+      <c r="L58" s="112"/>
+      <c r="M58" s="112"/>
+      <c r="N58" s="112"/>
+      <c r="O58" s="112"/>
+      <c r="P58" s="112"/>
+      <c r="Q58" s="112"/>
+      <c r="R58" s="112"/>
+      <c r="S58" s="112"/>
+      <c r="T58" s="112"/>
+      <c r="U58" s="113"/>
+      <c r="V58" s="124"/>
+      <c r="W58" s="114"/>
+      <c r="X58" s="114"/>
+      <c r="Y58" s="125"/>
       <c r="Z58" s="104"/>
     </row>
     <row r="59" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="116"/>
+      <c r="A59" s="149"/>
       <c r="B59" s="106" t="s">
         <v>128</v>
       </c>
@@ -6873,24 +6891,24 @@
       <c r="I59" s="56">
         <v>1</v>
       </c>
-      <c r="J59" s="113" t="s">
+      <c r="J59" s="112" t="s">
         <v>129</v>
       </c>
-      <c r="K59" s="113"/>
-      <c r="L59" s="113"/>
-      <c r="M59" s="113"/>
-      <c r="N59" s="113"/>
-      <c r="O59" s="113"/>
-      <c r="P59" s="113"/>
-      <c r="Q59" s="113"/>
-      <c r="R59" s="113"/>
-      <c r="S59" s="113"/>
-      <c r="T59" s="113"/>
-      <c r="U59" s="114"/>
-      <c r="V59" s="112"/>
-      <c r="W59" s="113"/>
-      <c r="X59" s="113"/>
-      <c r="Y59" s="114"/>
+      <c r="K59" s="112"/>
+      <c r="L59" s="112"/>
+      <c r="M59" s="112"/>
+      <c r="N59" s="112"/>
+      <c r="O59" s="112"/>
+      <c r="P59" s="112"/>
+      <c r="Q59" s="112"/>
+      <c r="R59" s="112"/>
+      <c r="S59" s="112"/>
+      <c r="T59" s="112"/>
+      <c r="U59" s="113"/>
+      <c r="V59" s="122"/>
+      <c r="W59" s="112"/>
+      <c r="X59" s="112"/>
+      <c r="Y59" s="113"/>
       <c r="Z59" s="104"/>
     </row>
     <row r="60" spans="1:26" x14ac:dyDescent="0.25">
@@ -6952,70 +6970,30 @@
     </row>
   </sheetData>
   <mergeCells count="112">
-    <mergeCell ref="J58:U58"/>
-    <mergeCell ref="N44:U44"/>
-    <mergeCell ref="N46:U46"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="P33:R33"/>
-    <mergeCell ref="S33:U33"/>
-    <mergeCell ref="K14:M14"/>
-    <mergeCell ref="N14:U14"/>
-    <mergeCell ref="V57:Y57"/>
-    <mergeCell ref="V58:Y58"/>
-    <mergeCell ref="N52:U52"/>
-    <mergeCell ref="N53:U53"/>
-    <mergeCell ref="N54:U54"/>
-    <mergeCell ref="N55:U55"/>
-    <mergeCell ref="N56:U56"/>
-    <mergeCell ref="V52:Y52"/>
-    <mergeCell ref="V53:Y53"/>
-    <mergeCell ref="V54:Y54"/>
-    <mergeCell ref="V55:Y55"/>
-    <mergeCell ref="V56:Y56"/>
-    <mergeCell ref="N49:U49"/>
-    <mergeCell ref="N50:U50"/>
-    <mergeCell ref="N51:U51"/>
-    <mergeCell ref="N57:U57"/>
-    <mergeCell ref="N42:U42"/>
-    <mergeCell ref="N43:U43"/>
-    <mergeCell ref="N45:U45"/>
-    <mergeCell ref="N47:U47"/>
-    <mergeCell ref="N48:U48"/>
-    <mergeCell ref="O39:U39"/>
-    <mergeCell ref="J40:M40"/>
-    <mergeCell ref="N40:U40"/>
-    <mergeCell ref="J41:M41"/>
-    <mergeCell ref="N41:U41"/>
-    <mergeCell ref="O38:U38"/>
-    <mergeCell ref="J37:P37"/>
-    <mergeCell ref="P19:R19"/>
-    <mergeCell ref="P20:R20"/>
-    <mergeCell ref="P21:R21"/>
-    <mergeCell ref="P22:R22"/>
-    <mergeCell ref="P23:R23"/>
-    <mergeCell ref="S28:U28"/>
-    <mergeCell ref="S29:U29"/>
-    <mergeCell ref="S30:U30"/>
-    <mergeCell ref="S31:U31"/>
-    <mergeCell ref="P31:R31"/>
-    <mergeCell ref="S19:U19"/>
-    <mergeCell ref="S20:U20"/>
-    <mergeCell ref="S21:U21"/>
-    <mergeCell ref="S22:U22"/>
-    <mergeCell ref="S23:U23"/>
-    <mergeCell ref="S24:U24"/>
-    <mergeCell ref="S25:U25"/>
-    <mergeCell ref="S26:U26"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="K35:M35"/>
-    <mergeCell ref="N35:U35"/>
-    <mergeCell ref="K36:M36"/>
-    <mergeCell ref="N36:U36"/>
-    <mergeCell ref="P28:R28"/>
-    <mergeCell ref="P29:R29"/>
-    <mergeCell ref="P30:R30"/>
+    <mergeCell ref="V59:Y59"/>
+    <mergeCell ref="J59:U59"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:U1"/>
+    <mergeCell ref="K4:O4"/>
+    <mergeCell ref="H3:L3"/>
+    <mergeCell ref="S10:U10"/>
+    <mergeCell ref="K5:O5"/>
+    <mergeCell ref="K6:O6"/>
+    <mergeCell ref="S7:U7"/>
+    <mergeCell ref="P8:R8"/>
+    <mergeCell ref="S8:U8"/>
+    <mergeCell ref="M7:O7"/>
+    <mergeCell ref="M8:O8"/>
+    <mergeCell ref="M9:O9"/>
+    <mergeCell ref="M10:O10"/>
+    <mergeCell ref="S27:U27"/>
+    <mergeCell ref="P25:R25"/>
+    <mergeCell ref="P26:R26"/>
+    <mergeCell ref="P27:R27"/>
+    <mergeCell ref="P24:R24"/>
     <mergeCell ref="V1:Y1"/>
     <mergeCell ref="P16:R16"/>
     <mergeCell ref="S16:U16"/>
@@ -7040,38 +7018,78 @@
     <mergeCell ref="N13:U13"/>
     <mergeCell ref="K12:M12"/>
     <mergeCell ref="N12:U12"/>
-    <mergeCell ref="V59:Y59"/>
-    <mergeCell ref="J59:U59"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:U1"/>
-    <mergeCell ref="K4:O4"/>
-    <mergeCell ref="H3:L3"/>
-    <mergeCell ref="S10:U10"/>
-    <mergeCell ref="K5:O5"/>
-    <mergeCell ref="K6:O6"/>
-    <mergeCell ref="S7:U7"/>
-    <mergeCell ref="P8:R8"/>
-    <mergeCell ref="S8:U8"/>
-    <mergeCell ref="M7:O7"/>
-    <mergeCell ref="M8:O8"/>
-    <mergeCell ref="M9:O9"/>
-    <mergeCell ref="M10:O10"/>
-    <mergeCell ref="S27:U27"/>
-    <mergeCell ref="P25:R25"/>
-    <mergeCell ref="P26:R26"/>
-    <mergeCell ref="P27:R27"/>
-    <mergeCell ref="P24:R24"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="K35:M35"/>
+    <mergeCell ref="N35:U35"/>
+    <mergeCell ref="K36:M36"/>
+    <mergeCell ref="N36:U36"/>
+    <mergeCell ref="P28:R28"/>
+    <mergeCell ref="P29:R29"/>
+    <mergeCell ref="P30:R30"/>
+    <mergeCell ref="P19:R19"/>
+    <mergeCell ref="P20:R20"/>
+    <mergeCell ref="P21:R21"/>
+    <mergeCell ref="P22:R22"/>
+    <mergeCell ref="P23:R23"/>
+    <mergeCell ref="S28:U28"/>
+    <mergeCell ref="S29:U29"/>
+    <mergeCell ref="S30:U30"/>
+    <mergeCell ref="S31:U31"/>
+    <mergeCell ref="P31:R31"/>
+    <mergeCell ref="S19:U19"/>
+    <mergeCell ref="S20:U20"/>
+    <mergeCell ref="S21:U21"/>
+    <mergeCell ref="S22:U22"/>
+    <mergeCell ref="S23:U23"/>
+    <mergeCell ref="S24:U24"/>
+    <mergeCell ref="S25:U25"/>
+    <mergeCell ref="S26:U26"/>
+    <mergeCell ref="V57:Y57"/>
+    <mergeCell ref="V58:Y58"/>
+    <mergeCell ref="N52:U52"/>
+    <mergeCell ref="N53:U53"/>
+    <mergeCell ref="N54:U54"/>
+    <mergeCell ref="N55:U55"/>
+    <mergeCell ref="N56:U56"/>
+    <mergeCell ref="V52:Y52"/>
+    <mergeCell ref="V53:Y53"/>
+    <mergeCell ref="V54:Y54"/>
+    <mergeCell ref="V55:Y55"/>
+    <mergeCell ref="V56:Y56"/>
+    <mergeCell ref="N57:U57"/>
+    <mergeCell ref="J58:U58"/>
+    <mergeCell ref="N44:U44"/>
+    <mergeCell ref="N46:U46"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="P33:R33"/>
+    <mergeCell ref="S33:U33"/>
+    <mergeCell ref="K14:M14"/>
+    <mergeCell ref="N14:U14"/>
+    <mergeCell ref="N49:U49"/>
+    <mergeCell ref="N50:U50"/>
+    <mergeCell ref="N51:U51"/>
+    <mergeCell ref="N42:U42"/>
+    <mergeCell ref="N43:U43"/>
+    <mergeCell ref="N45:U45"/>
+    <mergeCell ref="N47:U47"/>
+    <mergeCell ref="N48:U48"/>
+    <mergeCell ref="O39:U39"/>
+    <mergeCell ref="J40:M40"/>
+    <mergeCell ref="N40:U40"/>
+    <mergeCell ref="J41:M41"/>
+    <mergeCell ref="N41:U41"/>
+    <mergeCell ref="O38:U38"/>
+    <mergeCell ref="J37:P37"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="F58:J59 F4:U57">
+  <conditionalFormatting sqref="F4:U57 F58:J59">
     <cfRule type="cellIs" dxfId="14" priority="6" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F41:M41 V41:Y41 V58:Y59 F58:J59 F42:Y57 F1:Y40">
+  <conditionalFormatting sqref="F41:M41 V41:Y41 F42:Y57 F58:J59 V58:Y59 F1:Y40">
     <cfRule type="containsText" dxfId="13" priority="7" operator="containsText" text="imm">
       <formula>NOT(ISERROR(SEARCH("imm",F1)))</formula>
     </cfRule>
@@ -7099,25 +7117,25 @@
       <formula>"Rm"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P16:R16">
-    <cfRule type="cellIs" dxfId="5" priority="15" operator="equal">
+  <conditionalFormatting sqref="H33:U33">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+      <formula>"Rd"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+      <formula>"Rn"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+      <formula>"Rd"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+      <formula>"Rdn"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
       <formula>"Rm"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H33:U33">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
-      <formula>"Rd"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
-      <formula>"Rn"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
-      <formula>"Rd"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
-      <formula>"Rdn"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="5" operator="equal">
+  <conditionalFormatting sqref="P16:R16">
+    <cfRule type="cellIs" dxfId="0" priority="15" operator="equal">
       <formula>"Rm"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7127,6 +7145,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010096649AD79A527B47A67D905693C83B0C" ma:contentTypeVersion="7" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="44d09355696640e2dc56270e449341cd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="98b34aae-4bd1-40d2-80e1-46205a35d283" xmlns:ns4="4c17d7eb-fa2b-4fbc-8175-1cef2629d4d8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="73bda8d09c620ff6c543bf34844bea48" ns3:_="" ns4:_="">
     <xsd:import namespace="98b34aae-4bd1-40d2-80e1-46205a35d283"/>
@@ -7311,15 +7338,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -7327,6 +7345,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AAD58D5F-4A46-4F63-A2BD-BBB590555A8D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90060F17-AE26-48CA-A0B9-2F516B758ECF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7341,14 +7367,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AAD58D5F-4A46-4F63-A2BD-BBB590555A8D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Fix an error in the table with unconditional branch
</commit_message>
<xml_diff>
--- a/docs/ARM instructions.xlsx
+++ b/docs/ARM instructions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Drive\Etudes\Supérieur\SI3\Architecture et réseaux\Architecture\PARM\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13B2E786-DC77-47EF-8E79-01A9970655F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{225F16FF-0A8D-4148-9444-6C93FF188A52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1E4904EC-9B68-40DD-B685-7BD66B9DE8BA}"/>
   </bookViews>
@@ -2013,7 +2013,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="51">
+  <borders count="54">
     <border>
       <left/>
       <right/>
@@ -2659,11 +2659,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="153">
+  <cellXfs count="158">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3119,13 +3156,55 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="19">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFF9999"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC99FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9999"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -3565,8 +3644,8 @@
   </sheetPr>
   <dimension ref="A1:Z70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="145" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="AB9" sqref="AB9"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" zoomScaleSheetLayoutView="145" zoomScalePageLayoutView="145" workbookViewId="0">
+      <selection activeCell="N61" sqref="N61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6844,25 +6923,27 @@
         <v>1</v>
       </c>
       <c r="H58" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I58" s="19">
-        <v>1</v>
-      </c>
-      <c r="J58" s="112" t="s">
+        <v>0</v>
+      </c>
+      <c r="J58" s="19">
+        <v>0</v>
+      </c>
+      <c r="K58" s="125" t="s">
         <v>129</v>
       </c>
-      <c r="K58" s="112"/>
-      <c r="L58" s="112"/>
-      <c r="M58" s="112"/>
-      <c r="N58" s="112"/>
-      <c r="O58" s="112"/>
-      <c r="P58" s="112"/>
-      <c r="Q58" s="112"/>
-      <c r="R58" s="112"/>
-      <c r="S58" s="112"/>
-      <c r="T58" s="112"/>
-      <c r="U58" s="113"/>
+      <c r="L58" s="153"/>
+      <c r="M58" s="153"/>
+      <c r="N58" s="153"/>
+      <c r="O58" s="153"/>
+      <c r="P58" s="153"/>
+      <c r="Q58" s="153"/>
+      <c r="R58" s="153"/>
+      <c r="S58" s="153"/>
+      <c r="T58" s="153"/>
+      <c r="U58" s="154"/>
       <c r="V58" s="124"/>
       <c r="W58" s="114"/>
       <c r="X58" s="114"/>
@@ -6886,25 +6967,27 @@
         <v>1</v>
       </c>
       <c r="H59" s="56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I59" s="56">
-        <v>1</v>
-      </c>
-      <c r="J59" s="112" t="s">
+        <v>0</v>
+      </c>
+      <c r="J59" s="56">
+        <v>0</v>
+      </c>
+      <c r="K59" s="155" t="s">
         <v>129</v>
       </c>
-      <c r="K59" s="112"/>
-      <c r="L59" s="112"/>
-      <c r="M59" s="112"/>
-      <c r="N59" s="112"/>
-      <c r="O59" s="112"/>
-      <c r="P59" s="112"/>
-      <c r="Q59" s="112"/>
-      <c r="R59" s="112"/>
-      <c r="S59" s="112"/>
-      <c r="T59" s="112"/>
-      <c r="U59" s="113"/>
+      <c r="L59" s="156"/>
+      <c r="M59" s="156"/>
+      <c r="N59" s="156"/>
+      <c r="O59" s="156"/>
+      <c r="P59" s="156"/>
+      <c r="Q59" s="156"/>
+      <c r="R59" s="156"/>
+      <c r="S59" s="156"/>
+      <c r="T59" s="156"/>
+      <c r="U59" s="157"/>
       <c r="V59" s="122"/>
       <c r="W59" s="112"/>
       <c r="X59" s="112"/>
@@ -6970,8 +7053,8 @@
     </row>
   </sheetData>
   <mergeCells count="112">
+    <mergeCell ref="K59:U59"/>
     <mergeCell ref="V59:Y59"/>
-    <mergeCell ref="J59:U59"/>
     <mergeCell ref="A58:A59"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="C2:E2"/>
@@ -7058,7 +7141,7 @@
     <mergeCell ref="V55:Y55"/>
     <mergeCell ref="V56:Y56"/>
     <mergeCell ref="N57:U57"/>
-    <mergeCell ref="J58:U58"/>
+    <mergeCell ref="K58:U58"/>
     <mergeCell ref="N44:U44"/>
     <mergeCell ref="N46:U46"/>
     <mergeCell ref="A44:A45"/>
@@ -7084,59 +7167,75 @@
     <mergeCell ref="J37:P37"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="F4:U57 F58:J59">
-    <cfRule type="cellIs" dxfId="14" priority="6" operator="equal">
+  <conditionalFormatting sqref="F4:U57 K58:K59 F58:I59">
+    <cfRule type="cellIs" dxfId="18" priority="10" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F41:M41 V41:Y41 F42:Y57 F58:J59 V58:Y59 F1:Y40">
-    <cfRule type="containsText" dxfId="13" priority="7" operator="containsText" text="imm">
+  <conditionalFormatting sqref="F41:M41 V41:Y41 F42:Y57 V58:Y59 F1:Y40 K58:K59 F58:I59">
+    <cfRule type="containsText" dxfId="17" priority="11" operator="containsText" text="imm">
       <formula>NOT(ISERROR(SEARCH("imm",F1)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="12" operator="equal">
       <formula>"imm3"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="13" operator="equal">
       <formula>"imm5"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:U31">
-    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="14" operator="equal">
       <formula>"Rd"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="15" operator="equal">
       <formula>"Rn"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="16" operator="equal">
       <formula>"Rd"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="17" operator="equal">
       <formula>"Rdn"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="18" operator="equal">
       <formula>"Rm"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H33:U33">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
       <formula>"Rd"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="6" operator="equal">
       <formula>"Rn"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
       <formula>"Rd"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
       <formula>"Rdn"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="9" operator="equal">
       <formula>"Rm"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P16:R16">
-    <cfRule type="cellIs" dxfId="0" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="19" operator="equal">
       <formula>"Rm"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J58:J59">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J58:J59">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="imm">
+      <formula>NOT(ISERROR(SEARCH("imm",J58)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+      <formula>"imm3"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
+      <formula>"imm5"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update VS and VC names in the table
</commit_message>
<xml_diff>
--- a/docs/ARM instructions.xlsx
+++ b/docs/ARM instructions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Drive\Etudes\Supérieur\SI3\Architecture et réseaux\Architecture\PARM\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{225F16FF-0A8D-4148-9444-6C93FF188A52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BC655D6-233E-4AA0-BD98-B825F9F7E0DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1E4904EC-9B68-40DD-B685-7BD66B9DE8BA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1E4904EC-9B68-40DD-B685-7BD66B9DE8BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -1386,6 +1386,411 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">Unsigned </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>hi</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>ghier</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Undigned </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>l</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">ower or </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>ame</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Signed </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>g</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">reater than or </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>e</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>qual</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Signed </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>l</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">ess </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>t</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>han</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Signed </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>g</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">reater </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>t</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>han</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Signed </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>l</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">ess than or </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>e</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>qual</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Add </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>8-bit immediate</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Sub</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>stract 8-bit immediate</t>
+    </r>
+  </si>
+  <si>
+    <t>AL</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>imm11</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Al</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>ways</t>
+    </r>
+  </si>
+  <si>
+    <t>{SP}</t>
+  </si>
+  <si>
+    <t>HS</t>
+  </si>
+  <si>
+    <t>LO</t>
+  </si>
+  <si>
+    <t>Special data instructions</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Mov</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>e register</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Mov</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>e immediate</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>C</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>o</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>mp</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>are immediate</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t>O</t>
     </r>
     <r>
@@ -1405,79 +1810,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>erflow</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>No o</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>v</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>erflow</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Unsigned </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>hi</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>ghier</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Undigned </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>l</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">ower or </t>
+      <t xml:space="preserve">erflow </t>
     </r>
     <r>
       <rPr>
@@ -1496,345 +1829,47 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>ame</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Signed </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>g</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">reater than or </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>e</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>qual</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Signed </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>l</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">ess </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>t</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>han</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Signed </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>g</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">reater </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>t</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>han</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Signed </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>l</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">ess than or </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>e</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>qual</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Add </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>8-bit immediate</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Sub</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>stract 8-bit immediate</t>
-    </r>
-  </si>
-  <si>
-    <t>AL</t>
-  </si>
-  <si>
-    <t>none</t>
-  </si>
-  <si>
-    <t>imm11</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Al</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>ways</t>
-    </r>
-  </si>
-  <si>
-    <t>{SP}</t>
-  </si>
-  <si>
-    <t>HS</t>
-  </si>
-  <si>
-    <t>LO</t>
-  </si>
-  <si>
-    <t>Special data instructions</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Mov</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>e register</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Mov</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>e immediate</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>C</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>o</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>mp</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>are immediate</t>
+      <t>et</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Ov</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">erflow </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>c</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>lear</t>
     </r>
   </si>
 </sst>
@@ -2700,7 +2735,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="158">
+  <cellXfs count="157">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2972,12 +3007,6 @@
     <xf numFmtId="0" fontId="4" fillId="9" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -3026,37 +3055,67 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3065,22 +3124,52 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3089,122 +3178,20 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="19">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF9999"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCC99FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9999"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -3287,6 +3274,33 @@
           <bgColor theme="5" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFF9999"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC99FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9999"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
     </dxf>
     <dxf>
       <fill>
@@ -3644,13 +3658,13 @@
   </sheetPr>
   <dimension ref="A1:Z70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" zoomScaleSheetLayoutView="145" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="N61" sqref="N61"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" zoomScaleSheetLayoutView="145" zoomScalePageLayoutView="145" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.7109375" style="93" customWidth="1"/>
+    <col min="1" max="1" width="28.7109375" style="91" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" style="77" customWidth="1"/>
     <col min="3" max="5" width="11.42578125" style="77"/>
     <col min="6" max="25" width="3.7109375" style="77" customWidth="1"/>
@@ -3658,50 +3672,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="150" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="152" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="141"/>
-      <c r="D1" s="141"/>
-      <c r="E1" s="142"/>
-      <c r="F1" s="141" t="s">
+      <c r="A1" s="114" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="118" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="116"/>
+      <c r="D1" s="116"/>
+      <c r="E1" s="117"/>
+      <c r="F1" s="116" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="141"/>
-      <c r="H1" s="141"/>
-      <c r="I1" s="141"/>
-      <c r="J1" s="141"/>
-      <c r="K1" s="141"/>
-      <c r="L1" s="141"/>
-      <c r="M1" s="141"/>
-      <c r="N1" s="141"/>
-      <c r="O1" s="141"/>
-      <c r="P1" s="141"/>
-      <c r="Q1" s="141"/>
-      <c r="R1" s="141"/>
-      <c r="S1" s="141"/>
-      <c r="T1" s="141"/>
-      <c r="U1" s="142"/>
-      <c r="V1" s="140" t="s">
+      <c r="G1" s="116"/>
+      <c r="H1" s="116"/>
+      <c r="I1" s="116"/>
+      <c r="J1" s="116"/>
+      <c r="K1" s="116"/>
+      <c r="L1" s="116"/>
+      <c r="M1" s="116"/>
+      <c r="N1" s="116"/>
+      <c r="O1" s="116"/>
+      <c r="P1" s="116"/>
+      <c r="Q1" s="116"/>
+      <c r="R1" s="116"/>
+      <c r="S1" s="116"/>
+      <c r="T1" s="116"/>
+      <c r="U1" s="117"/>
+      <c r="V1" s="123" t="s">
         <v>3</v>
       </c>
-      <c r="W1" s="141"/>
-      <c r="X1" s="141"/>
-      <c r="Y1" s="142"/>
+      <c r="W1" s="116"/>
+      <c r="X1" s="116"/>
+      <c r="Y1" s="117"/>
     </row>
     <row r="2" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="151"/>
+      <c r="A2" s="115"/>
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="141" t="s">
+      <c r="C2" s="116" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="141"/>
-      <c r="E2" s="142"/>
+      <c r="D2" s="116"/>
+      <c r="E2" s="117"/>
       <c r="F2" s="2">
         <v>15</v>
       </c>
@@ -3764,7 +3778,7 @@
       </c>
     </row>
     <row r="3" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="111" t="s">
+      <c r="A3" s="107" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="78"/>
@@ -3777,13 +3791,13 @@
       <c r="G3" s="10">
         <v>0</v>
       </c>
-      <c r="H3" s="147" t="s">
+      <c r="H3" s="120" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="147"/>
-      <c r="J3" s="147"/>
-      <c r="K3" s="147"/>
-      <c r="L3" s="147"/>
+      <c r="I3" s="120"/>
+      <c r="J3" s="120"/>
+      <c r="K3" s="120"/>
+      <c r="L3" s="120"/>
       <c r="M3" s="11"/>
       <c r="N3" s="11"/>
       <c r="O3" s="11"/>
@@ -3829,23 +3843,23 @@
       <c r="J4" s="20">
         <v>0</v>
       </c>
-      <c r="K4" s="114" t="s">
+      <c r="K4" s="119" t="s">
         <v>15</v>
       </c>
-      <c r="L4" s="114"/>
-      <c r="M4" s="114"/>
-      <c r="N4" s="114"/>
-      <c r="O4" s="114"/>
-      <c r="P4" s="120" t="s">
+      <c r="L4" s="119"/>
+      <c r="M4" s="119"/>
+      <c r="N4" s="119"/>
+      <c r="O4" s="119"/>
+      <c r="P4" s="128" t="s">
         <v>16</v>
       </c>
-      <c r="Q4" s="120"/>
-      <c r="R4" s="120"/>
-      <c r="S4" s="114" t="s">
+      <c r="Q4" s="128"/>
+      <c r="R4" s="128"/>
+      <c r="S4" s="119" t="s">
         <v>17</v>
       </c>
-      <c r="T4" s="114"/>
-      <c r="U4" s="115"/>
+      <c r="T4" s="119"/>
+      <c r="U4" s="121"/>
       <c r="V4" s="22" t="s">
         <v>18</v>
       </c>
@@ -3888,23 +3902,23 @@
       <c r="J5" s="26">
         <v>1</v>
       </c>
-      <c r="K5" s="114" t="s">
+      <c r="K5" s="119" t="s">
         <v>15</v>
       </c>
-      <c r="L5" s="114"/>
-      <c r="M5" s="114"/>
-      <c r="N5" s="114"/>
-      <c r="O5" s="114"/>
-      <c r="P5" s="114" t="s">
+      <c r="L5" s="119"/>
+      <c r="M5" s="119"/>
+      <c r="N5" s="119"/>
+      <c r="O5" s="119"/>
+      <c r="P5" s="119" t="s">
         <v>16</v>
       </c>
-      <c r="Q5" s="114"/>
-      <c r="R5" s="114"/>
-      <c r="S5" s="114" t="s">
+      <c r="Q5" s="119"/>
+      <c r="R5" s="119"/>
+      <c r="S5" s="119" t="s">
         <v>17</v>
       </c>
-      <c r="T5" s="114"/>
-      <c r="U5" s="115"/>
+      <c r="T5" s="119"/>
+      <c r="U5" s="121"/>
       <c r="V5" s="22" t="s">
         <v>18</v>
       </c>
@@ -3947,23 +3961,23 @@
       <c r="J6" s="20">
         <v>0</v>
       </c>
-      <c r="K6" s="114" t="s">
+      <c r="K6" s="119" t="s">
         <v>15</v>
       </c>
-      <c r="L6" s="114"/>
-      <c r="M6" s="114"/>
-      <c r="N6" s="114"/>
-      <c r="O6" s="114"/>
-      <c r="P6" s="114" t="s">
+      <c r="L6" s="119"/>
+      <c r="M6" s="119"/>
+      <c r="N6" s="119"/>
+      <c r="O6" s="119"/>
+      <c r="P6" s="119" t="s">
         <v>16</v>
       </c>
-      <c r="Q6" s="114"/>
-      <c r="R6" s="114"/>
-      <c r="S6" s="114" t="s">
+      <c r="Q6" s="119"/>
+      <c r="R6" s="119"/>
+      <c r="S6" s="119" t="s">
         <v>17</v>
       </c>
-      <c r="T6" s="114"/>
-      <c r="U6" s="115"/>
+      <c r="T6" s="119"/>
+      <c r="U6" s="121"/>
       <c r="V6" s="22" t="s">
         <v>18</v>
       </c>
@@ -4012,21 +4026,21 @@
       <c r="L7" s="31">
         <v>0</v>
       </c>
-      <c r="M7" s="114" t="s">
+      <c r="M7" s="119" t="s">
         <v>16</v>
       </c>
-      <c r="N7" s="114"/>
-      <c r="O7" s="114"/>
-      <c r="P7" s="114" t="s">
+      <c r="N7" s="119"/>
+      <c r="O7" s="119"/>
+      <c r="P7" s="119" t="s">
         <v>20</v>
       </c>
-      <c r="Q7" s="114"/>
-      <c r="R7" s="114"/>
-      <c r="S7" s="114" t="s">
+      <c r="Q7" s="119"/>
+      <c r="R7" s="119"/>
+      <c r="S7" s="119" t="s">
         <v>17</v>
       </c>
-      <c r="T7" s="114"/>
-      <c r="U7" s="115"/>
+      <c r="T7" s="119"/>
+      <c r="U7" s="121"/>
       <c r="V7" s="22" t="s">
         <v>18</v>
       </c>
@@ -4077,21 +4091,21 @@
       <c r="L8" s="32">
         <v>1</v>
       </c>
-      <c r="M8" s="114" t="s">
+      <c r="M8" s="119" t="s">
         <v>16</v>
       </c>
-      <c r="N8" s="114"/>
-      <c r="O8" s="114"/>
-      <c r="P8" s="114" t="s">
+      <c r="N8" s="119"/>
+      <c r="O8" s="119"/>
+      <c r="P8" s="119" t="s">
         <v>20</v>
       </c>
-      <c r="Q8" s="114"/>
-      <c r="R8" s="114"/>
-      <c r="S8" s="114" t="s">
+      <c r="Q8" s="119"/>
+      <c r="R8" s="119"/>
+      <c r="S8" s="119" t="s">
         <v>17</v>
       </c>
-      <c r="T8" s="114"/>
-      <c r="U8" s="115"/>
+      <c r="T8" s="119"/>
+      <c r="U8" s="121"/>
       <c r="V8" s="22" t="s">
         <v>18</v>
       </c>
@@ -4142,21 +4156,21 @@
       <c r="L9" s="31">
         <v>0</v>
       </c>
-      <c r="M9" s="114" t="s">
+      <c r="M9" s="119" t="s">
         <v>22</v>
       </c>
-      <c r="N9" s="114"/>
-      <c r="O9" s="114"/>
-      <c r="P9" s="114" t="s">
+      <c r="N9" s="119"/>
+      <c r="O9" s="119"/>
+      <c r="P9" s="119" t="s">
         <v>20</v>
       </c>
-      <c r="Q9" s="114"/>
-      <c r="R9" s="114"/>
-      <c r="S9" s="114" t="s">
+      <c r="Q9" s="119"/>
+      <c r="R9" s="119"/>
+      <c r="S9" s="119" t="s">
         <v>17</v>
       </c>
-      <c r="T9" s="114"/>
-      <c r="U9" s="115"/>
+      <c r="T9" s="119"/>
+      <c r="U9" s="121"/>
       <c r="V9" s="22" t="s">
         <v>18</v>
       </c>
@@ -4174,16 +4188,16 @@
       <c r="A10" s="85" t="s">
         <v>86</v>
       </c>
-      <c r="B10" s="95" t="s">
+      <c r="B10" s="93" t="s">
         <v>84</v>
       </c>
-      <c r="C10" s="96" t="s">
+      <c r="C10" s="94" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="97" t="s">
+      <c r="D10" s="95" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="98" t="s">
+      <c r="E10" s="96" t="s">
         <v>21</v>
       </c>
       <c r="F10" s="29">
@@ -4207,21 +4221,21 @@
       <c r="L10" s="32">
         <v>1</v>
       </c>
-      <c r="M10" s="114" t="s">
+      <c r="M10" s="119" t="s">
         <v>22</v>
       </c>
-      <c r="N10" s="114"/>
-      <c r="O10" s="114"/>
-      <c r="P10" s="114" t="s">
+      <c r="N10" s="119"/>
+      <c r="O10" s="119"/>
+      <c r="P10" s="119" t="s">
         <v>20</v>
       </c>
-      <c r="Q10" s="114"/>
-      <c r="R10" s="114"/>
-      <c r="S10" s="114" t="s">
+      <c r="Q10" s="119"/>
+      <c r="R10" s="119"/>
+      <c r="S10" s="119" t="s">
         <v>17</v>
       </c>
-      <c r="T10" s="114"/>
-      <c r="U10" s="115"/>
+      <c r="T10" s="119"/>
+      <c r="U10" s="121"/>
       <c r="V10" s="22" t="s">
         <v>18</v>
       </c>
@@ -4237,19 +4251,19 @@
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" s="84" t="s">
-        <v>136</v>
-      </c>
-      <c r="B11" s="100" t="s">
+        <v>134</v>
+      </c>
+      <c r="B11" s="98" t="s">
         <v>87</v>
       </c>
-      <c r="C11" s="101" t="s">
+      <c r="C11" s="99" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="99" t="s">
+      <c r="D11" s="97" t="s">
         <v>23</v>
       </c>
       <c r="E11" s="47"/>
-      <c r="F11" s="102">
+      <c r="F11" s="100">
         <v>0</v>
       </c>
       <c r="G11" s="30">
@@ -4264,21 +4278,21 @@
       <c r="J11" s="31">
         <v>0</v>
       </c>
-      <c r="K11" s="121" t="s">
+      <c r="K11" s="129" t="s">
         <v>17</v>
       </c>
-      <c r="L11" s="121"/>
-      <c r="M11" s="121"/>
-      <c r="N11" s="114" t="s">
+      <c r="L11" s="129"/>
+      <c r="M11" s="129"/>
+      <c r="N11" s="119" t="s">
         <v>24</v>
       </c>
-      <c r="O11" s="114"/>
-      <c r="P11" s="114"/>
-      <c r="Q11" s="114"/>
-      <c r="R11" s="114"/>
-      <c r="S11" s="114"/>
-      <c r="T11" s="114"/>
-      <c r="U11" s="115"/>
+      <c r="O11" s="119"/>
+      <c r="P11" s="119"/>
+      <c r="Q11" s="119"/>
+      <c r="R11" s="119"/>
+      <c r="S11" s="119"/>
+      <c r="T11" s="119"/>
+      <c r="U11" s="121"/>
       <c r="V11" s="22"/>
       <c r="W11" s="19"/>
       <c r="X11" s="19" t="s">
@@ -4290,7 +4304,7 @@
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="84" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B12" s="14" t="s">
         <v>32</v>
@@ -4298,11 +4312,11 @@
       <c r="C12" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="99" t="s">
+      <c r="D12" s="97" t="s">
         <v>23</v>
       </c>
       <c r="E12" s="47"/>
-      <c r="F12" s="102">
+      <c r="F12" s="100">
         <v>0</v>
       </c>
       <c r="G12" s="30">
@@ -4317,21 +4331,21 @@
       <c r="J12" s="32">
         <v>1</v>
       </c>
-      <c r="K12" s="121" t="s">
+      <c r="K12" s="129" t="s">
         <v>17</v>
       </c>
-      <c r="L12" s="121"/>
-      <c r="M12" s="121"/>
-      <c r="N12" s="114" t="s">
+      <c r="L12" s="129"/>
+      <c r="M12" s="129"/>
+      <c r="N12" s="119" t="s">
         <v>24</v>
       </c>
-      <c r="O12" s="114"/>
-      <c r="P12" s="114"/>
-      <c r="Q12" s="114"/>
-      <c r="R12" s="114"/>
-      <c r="S12" s="114"/>
-      <c r="T12" s="114"/>
-      <c r="U12" s="115"/>
+      <c r="O12" s="119"/>
+      <c r="P12" s="119"/>
+      <c r="Q12" s="119"/>
+      <c r="R12" s="119"/>
+      <c r="S12" s="119"/>
+      <c r="T12" s="119"/>
+      <c r="U12" s="121"/>
       <c r="V12" s="19" t="s">
         <v>18</v>
       </c>
@@ -4347,7 +4361,7 @@
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="84" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B13" s="14" t="s">
         <v>82</v>
@@ -4355,7 +4369,7 @@
       <c r="C13" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="99" t="s">
+      <c r="D13" s="97" t="s">
         <v>23</v>
       </c>
       <c r="E13" s="21"/>
@@ -4374,21 +4388,21 @@
       <c r="J13" s="31">
         <v>0</v>
       </c>
-      <c r="K13" s="121" t="s">
+      <c r="K13" s="129" t="s">
         <v>17</v>
       </c>
-      <c r="L13" s="121"/>
-      <c r="M13" s="121"/>
-      <c r="N13" s="114" t="s">
+      <c r="L13" s="129"/>
+      <c r="M13" s="129"/>
+      <c r="N13" s="119" t="s">
         <v>24</v>
       </c>
-      <c r="O13" s="114"/>
-      <c r="P13" s="114"/>
-      <c r="Q13" s="114"/>
-      <c r="R13" s="114"/>
-      <c r="S13" s="114"/>
-      <c r="T13" s="114"/>
-      <c r="U13" s="115"/>
+      <c r="O13" s="119"/>
+      <c r="P13" s="119"/>
+      <c r="Q13" s="119"/>
+      <c r="R13" s="119"/>
+      <c r="S13" s="119"/>
+      <c r="T13" s="119"/>
+      <c r="U13" s="121"/>
       <c r="V13" s="19" t="s">
         <v>18</v>
       </c>
@@ -4404,7 +4418,7 @@
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" s="85" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B14" s="14" t="s">
         <v>84</v>
@@ -4412,7 +4426,7 @@
       <c r="C14" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="99" t="s">
+      <c r="D14" s="97" t="s">
         <v>23</v>
       </c>
       <c r="E14" s="21"/>
@@ -4431,21 +4445,21 @@
       <c r="J14" s="31">
         <v>1</v>
       </c>
-      <c r="K14" s="121" t="s">
+      <c r="K14" s="129" t="s">
         <v>17</v>
       </c>
-      <c r="L14" s="121"/>
-      <c r="M14" s="121"/>
-      <c r="N14" s="114" t="s">
+      <c r="L14" s="129"/>
+      <c r="M14" s="129"/>
+      <c r="N14" s="119" t="s">
         <v>24</v>
       </c>
-      <c r="O14" s="114"/>
-      <c r="P14" s="114"/>
-      <c r="Q14" s="114"/>
-      <c r="R14" s="114"/>
-      <c r="S14" s="114"/>
-      <c r="T14" s="114"/>
-      <c r="U14" s="115"/>
+      <c r="O14" s="119"/>
+      <c r="P14" s="119"/>
+      <c r="Q14" s="119"/>
+      <c r="R14" s="119"/>
+      <c r="S14" s="119"/>
+      <c r="T14" s="119"/>
+      <c r="U14" s="121"/>
       <c r="V14" s="19" t="s">
         <v>18</v>
       </c>
@@ -4485,12 +4499,12 @@
       <c r="K15" s="39">
         <v>0</v>
       </c>
-      <c r="L15" s="147" t="s">
+      <c r="L15" s="120" t="s">
         <v>11</v>
       </c>
-      <c r="M15" s="147"/>
-      <c r="N15" s="147"/>
-      <c r="O15" s="147"/>
+      <c r="M15" s="120"/>
+      <c r="N15" s="120"/>
+      <c r="O15" s="120"/>
       <c r="P15" s="36"/>
       <c r="Q15" s="36"/>
       <c r="R15" s="40"/>
@@ -4554,16 +4568,16 @@
       <c r="O16" s="20">
         <v>0</v>
       </c>
-      <c r="P16" s="143" t="s">
+      <c r="P16" s="124" t="s">
         <v>16</v>
       </c>
-      <c r="Q16" s="144"/>
-      <c r="R16" s="144"/>
-      <c r="S16" s="145" t="s">
+      <c r="Q16" s="125"/>
+      <c r="R16" s="125"/>
+      <c r="S16" s="126" t="s">
         <v>27</v>
       </c>
-      <c r="T16" s="145"/>
-      <c r="U16" s="146"/>
+      <c r="T16" s="126"/>
+      <c r="U16" s="127"/>
       <c r="V16" s="22" t="s">
         <v>18</v>
       </c>
@@ -4619,16 +4633,16 @@
       <c r="O17" s="26">
         <v>1</v>
       </c>
-      <c r="P17" s="132" t="s">
+      <c r="P17" s="122" t="s">
         <v>16</v>
       </c>
-      <c r="Q17" s="114"/>
-      <c r="R17" s="114"/>
-      <c r="S17" s="114" t="s">
+      <c r="Q17" s="119"/>
+      <c r="R17" s="119"/>
+      <c r="S17" s="119" t="s">
         <v>27</v>
       </c>
-      <c r="T17" s="114"/>
-      <c r="U17" s="115"/>
+      <c r="T17" s="119"/>
+      <c r="U17" s="121"/>
       <c r="V17" s="22" t="s">
         <v>18</v>
       </c>
@@ -4684,16 +4698,16 @@
       <c r="O18" s="20">
         <v>0</v>
       </c>
-      <c r="P18" s="132" t="s">
+      <c r="P18" s="122" t="s">
         <v>16</v>
       </c>
-      <c r="Q18" s="114"/>
-      <c r="R18" s="114"/>
-      <c r="S18" s="114" t="s">
+      <c r="Q18" s="119"/>
+      <c r="R18" s="119"/>
+      <c r="S18" s="119" t="s">
         <v>27</v>
       </c>
-      <c r="T18" s="114"/>
-      <c r="U18" s="115"/>
+      <c r="T18" s="119"/>
+      <c r="U18" s="121"/>
       <c r="V18" s="22" t="s">
         <v>18</v>
       </c>
@@ -4749,16 +4763,16 @@
       <c r="O19" s="26">
         <v>1</v>
       </c>
-      <c r="P19" s="132" t="s">
+      <c r="P19" s="122" t="s">
         <v>16</v>
       </c>
-      <c r="Q19" s="114"/>
-      <c r="R19" s="114"/>
-      <c r="S19" s="114" t="s">
+      <c r="Q19" s="119"/>
+      <c r="R19" s="119"/>
+      <c r="S19" s="119" t="s">
         <v>27</v>
       </c>
-      <c r="T19" s="114"/>
-      <c r="U19" s="115"/>
+      <c r="T19" s="119"/>
+      <c r="U19" s="121"/>
       <c r="V19" s="22" t="s">
         <v>18</v>
       </c>
@@ -4814,16 +4828,16 @@
       <c r="O20" s="20">
         <v>0</v>
       </c>
-      <c r="P20" s="132" t="s">
+      <c r="P20" s="122" t="s">
         <v>16</v>
       </c>
-      <c r="Q20" s="114"/>
-      <c r="R20" s="114"/>
-      <c r="S20" s="114" t="s">
+      <c r="Q20" s="119"/>
+      <c r="R20" s="119"/>
+      <c r="S20" s="119" t="s">
         <v>27</v>
       </c>
-      <c r="T20" s="114"/>
-      <c r="U20" s="115"/>
+      <c r="T20" s="119"/>
+      <c r="U20" s="121"/>
       <c r="V20" s="22" t="s">
         <v>18</v>
       </c>
@@ -4879,16 +4893,16 @@
       <c r="O21" s="26">
         <v>1</v>
       </c>
-      <c r="P21" s="132" t="s">
+      <c r="P21" s="122" t="s">
         <v>16</v>
       </c>
-      <c r="Q21" s="114"/>
-      <c r="R21" s="114"/>
-      <c r="S21" s="114" t="s">
+      <c r="Q21" s="119"/>
+      <c r="R21" s="119"/>
+      <c r="S21" s="119" t="s">
         <v>27</v>
       </c>
-      <c r="T21" s="114"/>
-      <c r="U21" s="115"/>
+      <c r="T21" s="119"/>
+      <c r="U21" s="121"/>
       <c r="V21" s="22" t="s">
         <v>18</v>
       </c>
@@ -4946,16 +4960,16 @@
       <c r="O22" s="20">
         <v>0</v>
       </c>
-      <c r="P22" s="132" t="s">
+      <c r="P22" s="122" t="s">
         <v>16</v>
       </c>
-      <c r="Q22" s="114"/>
-      <c r="R22" s="114"/>
-      <c r="S22" s="114" t="s">
+      <c r="Q22" s="119"/>
+      <c r="R22" s="119"/>
+      <c r="S22" s="119" t="s">
         <v>27</v>
       </c>
-      <c r="T22" s="114"/>
-      <c r="U22" s="115"/>
+      <c r="T22" s="119"/>
+      <c r="U22" s="121"/>
       <c r="V22" s="22" t="s">
         <v>18</v>
       </c>
@@ -5013,16 +5027,16 @@
       <c r="O23" s="26">
         <v>1</v>
       </c>
-      <c r="P23" s="132" t="s">
+      <c r="P23" s="122" t="s">
         <v>16</v>
       </c>
-      <c r="Q23" s="114"/>
-      <c r="R23" s="114"/>
-      <c r="S23" s="114" t="s">
+      <c r="Q23" s="119"/>
+      <c r="R23" s="119"/>
+      <c r="S23" s="119" t="s">
         <v>27</v>
       </c>
-      <c r="T23" s="114"/>
-      <c r="U23" s="115"/>
+      <c r="T23" s="119"/>
+      <c r="U23" s="121"/>
       <c r="V23" s="22" t="s">
         <v>18</v>
       </c>
@@ -5078,16 +5092,16 @@
       <c r="O24" s="20">
         <v>0</v>
       </c>
-      <c r="P24" s="132" t="s">
+      <c r="P24" s="122" t="s">
         <v>16</v>
       </c>
-      <c r="Q24" s="114"/>
-      <c r="R24" s="114"/>
-      <c r="S24" s="114" t="s">
+      <c r="Q24" s="119"/>
+      <c r="R24" s="119"/>
+      <c r="S24" s="119" t="s">
         <v>20</v>
       </c>
-      <c r="T24" s="114"/>
-      <c r="U24" s="115"/>
+      <c r="T24" s="119"/>
+      <c r="U24" s="121"/>
       <c r="V24" s="22" t="s">
         <v>18</v>
       </c>
@@ -5145,16 +5159,16 @@
       <c r="O25" s="26">
         <v>1</v>
       </c>
-      <c r="P25" s="132" t="s">
+      <c r="P25" s="122" t="s">
         <v>20</v>
       </c>
-      <c r="Q25" s="114"/>
-      <c r="R25" s="114"/>
-      <c r="S25" s="114" t="s">
+      <c r="Q25" s="119"/>
+      <c r="R25" s="119"/>
+      <c r="S25" s="119" t="s">
         <v>17</v>
       </c>
-      <c r="T25" s="114"/>
-      <c r="U25" s="115"/>
+      <c r="T25" s="119"/>
+      <c r="U25" s="121"/>
       <c r="V25" s="22" t="s">
         <v>18</v>
       </c>
@@ -5212,16 +5226,16 @@
       <c r="O26" s="20">
         <v>0</v>
       </c>
-      <c r="P26" s="132" t="s">
+      <c r="P26" s="122" t="s">
         <v>16</v>
       </c>
-      <c r="Q26" s="114"/>
-      <c r="R26" s="114"/>
-      <c r="S26" s="114" t="s">
+      <c r="Q26" s="119"/>
+      <c r="R26" s="119"/>
+      <c r="S26" s="119" t="s">
         <v>20</v>
       </c>
-      <c r="T26" s="114"/>
-      <c r="U26" s="115"/>
+      <c r="T26" s="119"/>
+      <c r="U26" s="121"/>
       <c r="V26" s="22" t="s">
         <v>18</v>
       </c>
@@ -5279,16 +5293,16 @@
       <c r="O27" s="26">
         <v>1</v>
       </c>
-      <c r="P27" s="132" t="s">
+      <c r="P27" s="122" t="s">
         <v>16</v>
       </c>
-      <c r="Q27" s="114"/>
-      <c r="R27" s="114"/>
-      <c r="S27" s="114" t="s">
+      <c r="Q27" s="119"/>
+      <c r="R27" s="119"/>
+      <c r="S27" s="119" t="s">
         <v>20</v>
       </c>
-      <c r="T27" s="114"/>
-      <c r="U27" s="115"/>
+      <c r="T27" s="119"/>
+      <c r="U27" s="121"/>
       <c r="V27" s="22" t="s">
         <v>18</v>
       </c>
@@ -5346,16 +5360,16 @@
       <c r="O28" s="20">
         <v>0</v>
       </c>
-      <c r="P28" s="132" t="s">
+      <c r="P28" s="122" t="s">
         <v>16</v>
       </c>
-      <c r="Q28" s="114"/>
-      <c r="R28" s="114"/>
-      <c r="S28" s="114" t="s">
+      <c r="Q28" s="119"/>
+      <c r="R28" s="119"/>
+      <c r="S28" s="119" t="s">
         <v>27</v>
       </c>
-      <c r="T28" s="114"/>
-      <c r="U28" s="115"/>
+      <c r="T28" s="119"/>
+      <c r="U28" s="121"/>
       <c r="V28" s="22" t="s">
         <v>18</v>
       </c>
@@ -5413,16 +5427,16 @@
       <c r="O29" s="26">
         <v>1</v>
       </c>
-      <c r="P29" s="132" t="s">
+      <c r="P29" s="122" t="s">
         <v>20</v>
       </c>
-      <c r="Q29" s="114"/>
-      <c r="R29" s="114"/>
-      <c r="S29" s="133" t="s">
+      <c r="Q29" s="119"/>
+      <c r="R29" s="119"/>
+      <c r="S29" s="138" t="s">
         <v>36</v>
       </c>
-      <c r="T29" s="133"/>
-      <c r="U29" s="134"/>
+      <c r="T29" s="138"/>
+      <c r="U29" s="139"/>
       <c r="V29" s="22"/>
       <c r="W29" s="19"/>
       <c r="X29" s="19" t="s">
@@ -5476,16 +5490,16 @@
       <c r="O30" s="20">
         <v>0</v>
       </c>
-      <c r="P30" s="132" t="s">
+      <c r="P30" s="122" t="s">
         <v>16</v>
       </c>
-      <c r="Q30" s="114"/>
-      <c r="R30" s="114"/>
-      <c r="S30" s="114" t="s">
+      <c r="Q30" s="119"/>
+      <c r="R30" s="119"/>
+      <c r="S30" s="119" t="s">
         <v>27</v>
       </c>
-      <c r="T30" s="114"/>
-      <c r="U30" s="115"/>
+      <c r="T30" s="119"/>
+      <c r="U30" s="121"/>
       <c r="V30" s="22" t="s">
         <v>18</v>
       </c>
@@ -5541,7 +5555,7 @@
       <c r="O31" s="58">
         <v>1</v>
       </c>
-      <c r="P31" s="135" t="s">
+      <c r="P31" s="141" t="s">
         <v>16</v>
       </c>
       <c r="Q31" s="112"/>
@@ -5550,7 +5564,7 @@
         <v>17</v>
       </c>
       <c r="T31" s="112"/>
-      <c r="U31" s="123"/>
+      <c r="U31" s="140"/>
       <c r="V31" s="22" t="s">
         <v>18</v>
       </c>
@@ -5564,7 +5578,7 @@
     </row>
     <row r="32" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="82" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B32" s="36"/>
       <c r="C32" s="36"/>
@@ -5609,12 +5623,12 @@
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A33" s="84" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B33" s="43" t="s">
         <v>87</v>
       </c>
-      <c r="C33" s="101" t="s">
+      <c r="C33" s="99" t="s">
         <v>12</v>
       </c>
       <c r="D33" s="24" t="s">
@@ -5636,31 +5650,31 @@
       <c r="J33" s="20">
         <v>0</v>
       </c>
-      <c r="K33" s="99">
-        <v>0</v>
-      </c>
-      <c r="L33" s="99">
-        <v>0</v>
-      </c>
-      <c r="M33" s="99">
-        <v>0</v>
-      </c>
-      <c r="N33" s="99">
-        <v>0</v>
-      </c>
-      <c r="O33" s="99">
-        <v>0</v>
-      </c>
-      <c r="P33" s="120" t="s">
+      <c r="K33" s="97">
+        <v>0</v>
+      </c>
+      <c r="L33" s="97">
+        <v>0</v>
+      </c>
+      <c r="M33" s="97">
+        <v>0</v>
+      </c>
+      <c r="N33" s="97">
+        <v>0</v>
+      </c>
+      <c r="O33" s="97">
+        <v>0</v>
+      </c>
+      <c r="P33" s="128" t="s">
         <v>16</v>
       </c>
-      <c r="Q33" s="120"/>
-      <c r="R33" s="120"/>
-      <c r="S33" s="114" t="s">
+      <c r="Q33" s="128"/>
+      <c r="R33" s="128"/>
+      <c r="S33" s="119" t="s">
         <v>17</v>
       </c>
-      <c r="T33" s="114"/>
-      <c r="U33" s="115"/>
+      <c r="T33" s="119"/>
+      <c r="U33" s="121"/>
       <c r="V33" s="22" t="s">
         <v>18</v>
       </c>
@@ -5727,10 +5741,10 @@
       <c r="C35" s="60" t="s">
         <v>40</v>
       </c>
-      <c r="D35" s="136" t="s">
+      <c r="D35" s="130" t="s">
         <v>43</v>
       </c>
-      <c r="E35" s="137"/>
+      <c r="E35" s="131"/>
       <c r="F35" s="61">
         <v>1</v>
       </c>
@@ -5746,21 +5760,21 @@
       <c r="J35" s="64">
         <v>0</v>
       </c>
-      <c r="K35" s="138" t="s">
+      <c r="K35" s="132" t="s">
         <v>41</v>
       </c>
-      <c r="L35" s="138"/>
-      <c r="M35" s="138"/>
-      <c r="N35" s="130" t="s">
+      <c r="L35" s="132"/>
+      <c r="M35" s="132"/>
+      <c r="N35" s="133" t="s">
         <v>24</v>
       </c>
-      <c r="O35" s="130"/>
-      <c r="P35" s="130"/>
-      <c r="Q35" s="130"/>
-      <c r="R35" s="130"/>
-      <c r="S35" s="130"/>
-      <c r="T35" s="130"/>
-      <c r="U35" s="131"/>
+      <c r="O35" s="133"/>
+      <c r="P35" s="133"/>
+      <c r="Q35" s="133"/>
+      <c r="R35" s="133"/>
+      <c r="S35" s="133"/>
+      <c r="T35" s="133"/>
+      <c r="U35" s="134"/>
       <c r="V35" s="22"/>
       <c r="W35" s="19"/>
       <c r="X35" s="19"/>
@@ -5776,10 +5790,10 @@
       <c r="C36" s="65" t="s">
         <v>40</v>
       </c>
-      <c r="D36" s="136" t="s">
+      <c r="D36" s="130" t="s">
         <v>43</v>
       </c>
-      <c r="E36" s="137"/>
+      <c r="E36" s="131"/>
       <c r="F36" s="67">
         <v>1</v>
       </c>
@@ -5795,21 +5809,21 @@
       <c r="J36" s="70">
         <v>1</v>
       </c>
-      <c r="K36" s="139" t="s">
+      <c r="K36" s="135" t="s">
         <v>41</v>
       </c>
-      <c r="L36" s="139"/>
-      <c r="M36" s="139"/>
-      <c r="N36" s="126" t="s">
+      <c r="L36" s="135"/>
+      <c r="M36" s="135"/>
+      <c r="N36" s="136" t="s">
         <v>24</v>
       </c>
-      <c r="O36" s="126"/>
-      <c r="P36" s="126"/>
-      <c r="Q36" s="126"/>
-      <c r="R36" s="126"/>
-      <c r="S36" s="126"/>
-      <c r="T36" s="126"/>
-      <c r="U36" s="127"/>
+      <c r="O36" s="136"/>
+      <c r="P36" s="136"/>
+      <c r="Q36" s="136"/>
+      <c r="R36" s="136"/>
+      <c r="S36" s="136"/>
+      <c r="T36" s="136"/>
+      <c r="U36" s="137"/>
       <c r="V36" s="22"/>
       <c r="W36" s="19"/>
       <c r="X36" s="19"/>
@@ -5835,15 +5849,15 @@
       <c r="I37" s="36">
         <v>1</v>
       </c>
-      <c r="J37" s="128" t="s">
+      <c r="J37" s="146" t="s">
         <v>11</v>
       </c>
-      <c r="K37" s="128"/>
-      <c r="L37" s="128"/>
-      <c r="M37" s="128"/>
-      <c r="N37" s="128"/>
-      <c r="O37" s="128"/>
-      <c r="P37" s="128"/>
+      <c r="K37" s="146"/>
+      <c r="L37" s="146"/>
+      <c r="M37" s="146"/>
+      <c r="N37" s="146"/>
+      <c r="O37" s="146"/>
+      <c r="P37" s="146"/>
       <c r="Q37" s="36"/>
       <c r="R37" s="36"/>
       <c r="S37" s="36"/>
@@ -5873,7 +5887,7 @@
         <v>46</v>
       </c>
       <c r="D38" s="62" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E38" s="17" t="s">
         <v>47</v>
@@ -5905,15 +5919,15 @@
       <c r="N38" s="64">
         <v>0</v>
       </c>
-      <c r="O38" s="130" t="s">
+      <c r="O38" s="133" t="s">
         <v>48</v>
       </c>
-      <c r="P38" s="130"/>
-      <c r="Q38" s="130"/>
-      <c r="R38" s="130"/>
-      <c r="S38" s="130"/>
-      <c r="T38" s="130"/>
-      <c r="U38" s="131"/>
+      <c r="P38" s="133"/>
+      <c r="Q38" s="133"/>
+      <c r="R38" s="133"/>
+      <c r="S38" s="133"/>
+      <c r="T38" s="133"/>
+      <c r="U38" s="134"/>
       <c r="V38" s="22"/>
       <c r="W38" s="19"/>
       <c r="X38" s="19"/>
@@ -5930,7 +5944,7 @@
         <v>46</v>
       </c>
       <c r="D39" s="68" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E39" s="66" t="s">
         <v>47</v>
@@ -5962,15 +5976,15 @@
       <c r="N39" s="75">
         <v>1</v>
       </c>
-      <c r="O39" s="126" t="s">
+      <c r="O39" s="136" t="s">
         <v>48</v>
       </c>
-      <c r="P39" s="126"/>
-      <c r="Q39" s="126"/>
-      <c r="R39" s="126"/>
-      <c r="S39" s="126"/>
-      <c r="T39" s="126"/>
-      <c r="U39" s="127"/>
+      <c r="P39" s="136"/>
+      <c r="Q39" s="136"/>
+      <c r="R39" s="136"/>
+      <c r="S39" s="136"/>
+      <c r="T39" s="136"/>
+      <c r="U39" s="137"/>
       <c r="V39" s="22"/>
       <c r="W39" s="19"/>
       <c r="X39" s="19"/>
@@ -6000,20 +6014,20 @@
       <c r="I40" s="36">
         <v>1</v>
       </c>
-      <c r="J40" s="128" t="s">
+      <c r="J40" s="146" t="s">
         <v>11</v>
       </c>
-      <c r="K40" s="128"/>
-      <c r="L40" s="128"/>
-      <c r="M40" s="128"/>
-      <c r="N40" s="128"/>
-      <c r="O40" s="128"/>
-      <c r="P40" s="128"/>
-      <c r="Q40" s="128"/>
-      <c r="R40" s="128"/>
-      <c r="S40" s="128"/>
-      <c r="T40" s="128"/>
-      <c r="U40" s="129"/>
+      <c r="K40" s="146"/>
+      <c r="L40" s="146"/>
+      <c r="M40" s="146"/>
+      <c r="N40" s="146"/>
+      <c r="O40" s="146"/>
+      <c r="P40" s="146"/>
+      <c r="Q40" s="146"/>
+      <c r="R40" s="146"/>
+      <c r="S40" s="146"/>
+      <c r="T40" s="146"/>
+      <c r="U40" s="147"/>
       <c r="V40" s="42"/>
       <c r="W40" s="36"/>
       <c r="X40" s="36"/>
@@ -6031,22 +6045,22 @@
       <c r="G41" s="36"/>
       <c r="H41" s="36"/>
       <c r="I41" s="36"/>
-      <c r="J41" s="128" t="s">
+      <c r="J41" s="146" t="s">
         <v>54</v>
       </c>
-      <c r="K41" s="128"/>
-      <c r="L41" s="128"/>
-      <c r="M41" s="128"/>
-      <c r="N41" s="128" t="s">
+      <c r="K41" s="146"/>
+      <c r="L41" s="146"/>
+      <c r="M41" s="146"/>
+      <c r="N41" s="146" t="s">
         <v>24</v>
       </c>
-      <c r="O41" s="128"/>
-      <c r="P41" s="128"/>
-      <c r="Q41" s="128"/>
-      <c r="R41" s="128"/>
-      <c r="S41" s="128"/>
-      <c r="T41" s="128"/>
-      <c r="U41" s="129"/>
+      <c r="O41" s="146"/>
+      <c r="P41" s="146"/>
+      <c r="Q41" s="146"/>
+      <c r="R41" s="146"/>
+      <c r="S41" s="146"/>
+      <c r="T41" s="146"/>
+      <c r="U41" s="147"/>
       <c r="V41" s="42" t="s">
         <v>6</v>
       </c>
@@ -6061,7 +6075,7 @@
       </c>
     </row>
     <row r="42" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A42" s="91" t="s">
+      <c r="A42" s="148" t="s">
         <v>111</v>
       </c>
       <c r="B42" s="76" t="s">
@@ -6096,16 +6110,16 @@
       <c r="M42" s="20">
         <v>0</v>
       </c>
-      <c r="N42" s="114" t="s">
+      <c r="N42" s="119" t="s">
         <v>24</v>
       </c>
-      <c r="O42" s="114"/>
-      <c r="P42" s="114"/>
-      <c r="Q42" s="114"/>
-      <c r="R42" s="114"/>
-      <c r="S42" s="114"/>
-      <c r="T42" s="114"/>
-      <c r="U42" s="115"/>
+      <c r="O42" s="119"/>
+      <c r="P42" s="119"/>
+      <c r="Q42" s="119"/>
+      <c r="R42" s="119"/>
+      <c r="S42" s="119"/>
+      <c r="T42" s="119"/>
+      <c r="U42" s="121"/>
       <c r="V42" s="22"/>
       <c r="W42" s="19"/>
       <c r="X42" s="19"/>
@@ -6114,7 +6128,7 @@
       </c>
     </row>
     <row r="43" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A43" s="91" t="s">
+      <c r="A43" s="148" t="s">
         <v>112</v>
       </c>
       <c r="B43" s="14" t="s">
@@ -6149,16 +6163,16 @@
       <c r="M43" s="20">
         <v>1</v>
       </c>
-      <c r="N43" s="114" t="s">
+      <c r="N43" s="119" t="s">
         <v>24</v>
       </c>
-      <c r="O43" s="114"/>
-      <c r="P43" s="114"/>
-      <c r="Q43" s="114"/>
-      <c r="R43" s="114"/>
-      <c r="S43" s="114"/>
-      <c r="T43" s="114"/>
-      <c r="U43" s="115"/>
+      <c r="O43" s="119"/>
+      <c r="P43" s="119"/>
+      <c r="Q43" s="119"/>
+      <c r="R43" s="119"/>
+      <c r="S43" s="119"/>
+      <c r="T43" s="119"/>
+      <c r="U43" s="121"/>
       <c r="V43" s="22"/>
       <c r="W43" s="19"/>
       <c r="X43" s="19"/>
@@ -6167,7 +6181,7 @@
       </c>
     </row>
     <row r="44" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A44" s="116" t="s">
+      <c r="A44" s="149" t="s">
         <v>113</v>
       </c>
       <c r="B44" s="14" t="s">
@@ -6202,16 +6216,16 @@
       <c r="M44" s="20">
         <v>0</v>
       </c>
-      <c r="N44" s="114" t="s">
+      <c r="N44" s="119" t="s">
         <v>24</v>
       </c>
-      <c r="O44" s="114"/>
-      <c r="P44" s="114"/>
-      <c r="Q44" s="114"/>
-      <c r="R44" s="114"/>
-      <c r="S44" s="114"/>
-      <c r="T44" s="114"/>
-      <c r="U44" s="115"/>
+      <c r="O44" s="119"/>
+      <c r="P44" s="119"/>
+      <c r="Q44" s="119"/>
+      <c r="R44" s="119"/>
+      <c r="S44" s="119"/>
+      <c r="T44" s="119"/>
+      <c r="U44" s="121"/>
       <c r="V44" s="22">
         <v>1</v>
       </c>
@@ -6220,9 +6234,9 @@
       <c r="Y44" s="21"/>
     </row>
     <row r="45" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A45" s="117"/>
+      <c r="A45" s="150"/>
       <c r="B45" s="14" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C45" s="18" t="s">
         <v>52</v>
@@ -6253,16 +6267,16 @@
       <c r="M45" s="20">
         <v>0</v>
       </c>
-      <c r="N45" s="114" t="s">
+      <c r="N45" s="119" t="s">
         <v>24</v>
       </c>
-      <c r="O45" s="114"/>
-      <c r="P45" s="114"/>
-      <c r="Q45" s="114"/>
-      <c r="R45" s="114"/>
-      <c r="S45" s="114"/>
-      <c r="T45" s="114"/>
-      <c r="U45" s="115"/>
+      <c r="O45" s="119"/>
+      <c r="P45" s="119"/>
+      <c r="Q45" s="119"/>
+      <c r="R45" s="119"/>
+      <c r="S45" s="119"/>
+      <c r="T45" s="119"/>
+      <c r="U45" s="121"/>
       <c r="V45" s="22">
         <v>1</v>
       </c>
@@ -6271,7 +6285,7 @@
       <c r="Y45" s="21"/>
     </row>
     <row r="46" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A46" s="118" t="s">
+      <c r="A46" s="151" t="s">
         <v>114</v>
       </c>
       <c r="B46" s="14" t="s">
@@ -6306,16 +6320,16 @@
       <c r="M46" s="20">
         <v>1</v>
       </c>
-      <c r="N46" s="114" t="s">
+      <c r="N46" s="119" t="s">
         <v>24</v>
       </c>
-      <c r="O46" s="114"/>
-      <c r="P46" s="114"/>
-      <c r="Q46" s="114"/>
-      <c r="R46" s="114"/>
-      <c r="S46" s="114"/>
-      <c r="T46" s="114"/>
-      <c r="U46" s="115"/>
+      <c r="O46" s="119"/>
+      <c r="P46" s="119"/>
+      <c r="Q46" s="119"/>
+      <c r="R46" s="119"/>
+      <c r="S46" s="119"/>
+      <c r="T46" s="119"/>
+      <c r="U46" s="121"/>
       <c r="V46" s="22">
         <v>0</v>
       </c>
@@ -6324,9 +6338,9 @@
       <c r="Y46" s="21"/>
     </row>
     <row r="47" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A47" s="119"/>
+      <c r="A47" s="152"/>
       <c r="B47" s="14" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C47" s="18" t="s">
         <v>52</v>
@@ -6357,16 +6371,16 @@
       <c r="M47" s="20">
         <v>1</v>
       </c>
-      <c r="N47" s="114" t="s">
+      <c r="N47" s="119" t="s">
         <v>24</v>
       </c>
-      <c r="O47" s="114"/>
-      <c r="P47" s="114"/>
-      <c r="Q47" s="114"/>
-      <c r="R47" s="114"/>
-      <c r="S47" s="114"/>
-      <c r="T47" s="114"/>
-      <c r="U47" s="115"/>
+      <c r="O47" s="119"/>
+      <c r="P47" s="119"/>
+      <c r="Q47" s="119"/>
+      <c r="R47" s="119"/>
+      <c r="S47" s="119"/>
+      <c r="T47" s="119"/>
+      <c r="U47" s="121"/>
       <c r="V47" s="22">
         <v>0</v>
       </c>
@@ -6375,7 +6389,7 @@
       <c r="Y47" s="21"/>
     </row>
     <row r="48" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A48" s="92" t="s">
+      <c r="A48" s="153" t="s">
         <v>115</v>
       </c>
       <c r="B48" s="14" t="s">
@@ -6410,16 +6424,16 @@
       <c r="M48" s="20">
         <v>0</v>
       </c>
-      <c r="N48" s="114" t="s">
+      <c r="N48" s="119" t="s">
         <v>24</v>
       </c>
-      <c r="O48" s="114"/>
-      <c r="P48" s="114"/>
-      <c r="Q48" s="114"/>
-      <c r="R48" s="114"/>
-      <c r="S48" s="114"/>
-      <c r="T48" s="114"/>
-      <c r="U48" s="115"/>
+      <c r="O48" s="119"/>
+      <c r="P48" s="119"/>
+      <c r="Q48" s="119"/>
+      <c r="R48" s="119"/>
+      <c r="S48" s="119"/>
+      <c r="T48" s="119"/>
+      <c r="U48" s="121"/>
       <c r="V48" s="22"/>
       <c r="W48" s="19"/>
       <c r="X48" s="19">
@@ -6428,7 +6442,7 @@
       <c r="Y48" s="21"/>
     </row>
     <row r="49" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A49" s="92" t="s">
+      <c r="A49" s="153" t="s">
         <v>116</v>
       </c>
       <c r="B49" s="14" t="s">
@@ -6463,16 +6477,16 @@
       <c r="M49" s="20">
         <v>1</v>
       </c>
-      <c r="N49" s="114" t="s">
+      <c r="N49" s="119" t="s">
         <v>24</v>
       </c>
-      <c r="O49" s="114"/>
-      <c r="P49" s="114"/>
-      <c r="Q49" s="114"/>
-      <c r="R49" s="114"/>
-      <c r="S49" s="114"/>
-      <c r="T49" s="114"/>
-      <c r="U49" s="115"/>
+      <c r="O49" s="119"/>
+      <c r="P49" s="119"/>
+      <c r="Q49" s="119"/>
+      <c r="R49" s="119"/>
+      <c r="S49" s="119"/>
+      <c r="T49" s="119"/>
+      <c r="U49" s="121"/>
       <c r="V49" s="22"/>
       <c r="W49" s="19"/>
       <c r="X49" s="19">
@@ -6481,8 +6495,8 @@
       <c r="Y49" s="21"/>
     </row>
     <row r="50" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A50" s="91" t="s">
-        <v>117</v>
+      <c r="A50" s="148" t="s">
+        <v>136</v>
       </c>
       <c r="B50" s="14" t="s">
         <v>61</v>
@@ -6516,16 +6530,16 @@
       <c r="M50" s="20">
         <v>0</v>
       </c>
-      <c r="N50" s="114" t="s">
+      <c r="N50" s="119" t="s">
         <v>24</v>
       </c>
-      <c r="O50" s="114"/>
-      <c r="P50" s="114"/>
-      <c r="Q50" s="114"/>
-      <c r="R50" s="114"/>
-      <c r="S50" s="114"/>
-      <c r="T50" s="114"/>
-      <c r="U50" s="115"/>
+      <c r="O50" s="119"/>
+      <c r="P50" s="119"/>
+      <c r="Q50" s="119"/>
+      <c r="R50" s="119"/>
+      <c r="S50" s="119"/>
+      <c r="T50" s="119"/>
+      <c r="U50" s="121"/>
       <c r="V50" s="22"/>
       <c r="W50" s="19">
         <v>1</v>
@@ -6534,8 +6548,8 @@
       <c r="Y50" s="21"/>
     </row>
     <row r="51" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A51" s="91" t="s">
-        <v>118</v>
+      <c r="A51" s="148" t="s">
+        <v>137</v>
       </c>
       <c r="B51" s="14" t="s">
         <v>62</v>
@@ -6569,16 +6583,16 @@
       <c r="M51" s="20">
         <v>1</v>
       </c>
-      <c r="N51" s="114" t="s">
+      <c r="N51" s="119" t="s">
         <v>24</v>
       </c>
-      <c r="O51" s="114"/>
-      <c r="P51" s="114"/>
-      <c r="Q51" s="114"/>
-      <c r="R51" s="114"/>
-      <c r="S51" s="114"/>
-      <c r="T51" s="114"/>
-      <c r="U51" s="115"/>
+      <c r="O51" s="119"/>
+      <c r="P51" s="119"/>
+      <c r="Q51" s="119"/>
+      <c r="R51" s="119"/>
+      <c r="S51" s="119"/>
+      <c r="T51" s="119"/>
+      <c r="U51" s="121"/>
       <c r="V51" s="22"/>
       <c r="W51" s="19">
         <v>0</v>
@@ -6587,8 +6601,8 @@
       <c r="Y51" s="21"/>
     </row>
     <row r="52" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A52" s="110" t="s">
-        <v>119</v>
+      <c r="A52" s="154" t="s">
+        <v>117</v>
       </c>
       <c r="B52" s="14" t="s">
         <v>63</v>
@@ -6622,26 +6636,26 @@
       <c r="M52" s="20">
         <v>0</v>
       </c>
-      <c r="N52" s="114" t="s">
+      <c r="N52" s="119" t="s">
         <v>24</v>
       </c>
-      <c r="O52" s="114"/>
-      <c r="P52" s="114"/>
-      <c r="Q52" s="114"/>
-      <c r="R52" s="114"/>
-      <c r="S52" s="114"/>
-      <c r="T52" s="114"/>
-      <c r="U52" s="115"/>
-      <c r="V52" s="124" t="s">
+      <c r="O52" s="119"/>
+      <c r="P52" s="119"/>
+      <c r="Q52" s="119"/>
+      <c r="R52" s="119"/>
+      <c r="S52" s="119"/>
+      <c r="T52" s="119"/>
+      <c r="U52" s="121"/>
+      <c r="V52" s="142" t="s">
         <v>64</v>
       </c>
-      <c r="W52" s="114"/>
-      <c r="X52" s="114"/>
-      <c r="Y52" s="115"/>
+      <c r="W52" s="119"/>
+      <c r="X52" s="119"/>
+      <c r="Y52" s="121"/>
     </row>
     <row r="53" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A53" s="110" t="s">
-        <v>120</v>
+      <c r="A53" s="154" t="s">
+        <v>118</v>
       </c>
       <c r="B53" s="14" t="s">
         <v>65</v>
@@ -6675,26 +6689,26 @@
       <c r="M53" s="20">
         <v>1</v>
       </c>
-      <c r="N53" s="114" t="s">
+      <c r="N53" s="119" t="s">
         <v>24</v>
       </c>
-      <c r="O53" s="114"/>
-      <c r="P53" s="114"/>
-      <c r="Q53" s="114"/>
-      <c r="R53" s="114"/>
-      <c r="S53" s="114"/>
-      <c r="T53" s="114"/>
-      <c r="U53" s="115"/>
-      <c r="V53" s="124" t="s">
+      <c r="O53" s="119"/>
+      <c r="P53" s="119"/>
+      <c r="Q53" s="119"/>
+      <c r="R53" s="119"/>
+      <c r="S53" s="119"/>
+      <c r="T53" s="119"/>
+      <c r="U53" s="121"/>
+      <c r="V53" s="142" t="s">
         <v>66</v>
       </c>
-      <c r="W53" s="114"/>
-      <c r="X53" s="114"/>
-      <c r="Y53" s="115"/>
+      <c r="W53" s="119"/>
+      <c r="X53" s="119"/>
+      <c r="Y53" s="121"/>
     </row>
     <row r="54" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A54" s="110" t="s">
-        <v>121</v>
+      <c r="A54" s="154" t="s">
+        <v>119</v>
       </c>
       <c r="B54" s="14" t="s">
         <v>67</v>
@@ -6728,26 +6742,26 @@
       <c r="M54" s="20">
         <v>0</v>
       </c>
-      <c r="N54" s="114" t="s">
+      <c r="N54" s="119" t="s">
         <v>24</v>
       </c>
-      <c r="O54" s="114"/>
-      <c r="P54" s="114"/>
-      <c r="Q54" s="114"/>
-      <c r="R54" s="114"/>
-      <c r="S54" s="114"/>
-      <c r="T54" s="114"/>
-      <c r="U54" s="115"/>
-      <c r="V54" s="124" t="s">
+      <c r="O54" s="119"/>
+      <c r="P54" s="119"/>
+      <c r="Q54" s="119"/>
+      <c r="R54" s="119"/>
+      <c r="S54" s="119"/>
+      <c r="T54" s="119"/>
+      <c r="U54" s="121"/>
+      <c r="V54" s="142" t="s">
         <v>68</v>
       </c>
-      <c r="W54" s="114"/>
-      <c r="X54" s="114"/>
-      <c r="Y54" s="115"/>
+      <c r="W54" s="119"/>
+      <c r="X54" s="119"/>
+      <c r="Y54" s="121"/>
     </row>
     <row r="55" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A55" s="110" t="s">
-        <v>122</v>
+      <c r="A55" s="154" t="s">
+        <v>120</v>
       </c>
       <c r="B55" s="14" t="s">
         <v>69</v>
@@ -6781,26 +6795,26 @@
       <c r="M55" s="20">
         <v>1</v>
       </c>
-      <c r="N55" s="114" t="s">
+      <c r="N55" s="119" t="s">
         <v>24</v>
       </c>
-      <c r="O55" s="114"/>
-      <c r="P55" s="114"/>
-      <c r="Q55" s="114"/>
-      <c r="R55" s="114"/>
-      <c r="S55" s="114"/>
-      <c r="T55" s="114"/>
-      <c r="U55" s="115"/>
-      <c r="V55" s="124" t="s">
+      <c r="O55" s="119"/>
+      <c r="P55" s="119"/>
+      <c r="Q55" s="119"/>
+      <c r="R55" s="119"/>
+      <c r="S55" s="119"/>
+      <c r="T55" s="119"/>
+      <c r="U55" s="121"/>
+      <c r="V55" s="142" t="s">
         <v>70</v>
       </c>
-      <c r="W55" s="114"/>
-      <c r="X55" s="114"/>
-      <c r="Y55" s="115"/>
+      <c r="W55" s="119"/>
+      <c r="X55" s="119"/>
+      <c r="Y55" s="121"/>
     </row>
     <row r="56" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A56" s="110" t="s">
-        <v>123</v>
+      <c r="A56" s="154" t="s">
+        <v>121</v>
       </c>
       <c r="B56" s="14" t="s">
         <v>71</v>
@@ -6834,36 +6848,36 @@
       <c r="M56" s="20">
         <v>0</v>
       </c>
-      <c r="N56" s="114" t="s">
+      <c r="N56" s="119" t="s">
         <v>24</v>
       </c>
-      <c r="O56" s="114"/>
-      <c r="P56" s="114"/>
-      <c r="Q56" s="114"/>
-      <c r="R56" s="114"/>
-      <c r="S56" s="114"/>
-      <c r="T56" s="114"/>
-      <c r="U56" s="115"/>
-      <c r="V56" s="124" t="s">
+      <c r="O56" s="119"/>
+      <c r="P56" s="119"/>
+      <c r="Q56" s="119"/>
+      <c r="R56" s="119"/>
+      <c r="S56" s="119"/>
+      <c r="T56" s="119"/>
+      <c r="U56" s="121"/>
+      <c r="V56" s="142" t="s">
         <v>72</v>
       </c>
-      <c r="W56" s="114"/>
-      <c r="X56" s="114"/>
-      <c r="Y56" s="115"/>
+      <c r="W56" s="119"/>
+      <c r="X56" s="119"/>
+      <c r="Y56" s="121"/>
     </row>
     <row r="57" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A57" s="109" t="s">
-        <v>124</v>
-      </c>
-      <c r="B57" s="95" t="s">
+      <c r="A57" s="155" t="s">
+        <v>122</v>
+      </c>
+      <c r="B57" s="93" t="s">
         <v>73</v>
       </c>
-      <c r="C57" s="94" t="s">
+      <c r="C57" s="92" t="s">
         <v>52</v>
       </c>
       <c r="D57" s="56"/>
       <c r="E57" s="59"/>
-      <c r="F57" s="94">
+      <c r="F57" s="92">
         <v>1</v>
       </c>
       <c r="G57" s="56">
@@ -6875,16 +6889,16 @@
       <c r="I57" s="56">
         <v>1</v>
       </c>
-      <c r="J57" s="103">
-        <v>1</v>
-      </c>
-      <c r="K57" s="103">
-        <v>1</v>
-      </c>
-      <c r="L57" s="103">
-        <v>0</v>
-      </c>
-      <c r="M57" s="103">
+      <c r="J57" s="101">
+        <v>1</v>
+      </c>
+      <c r="K57" s="101">
+        <v>1</v>
+      </c>
+      <c r="L57" s="101">
+        <v>0</v>
+      </c>
+      <c r="M57" s="101">
         <v>1</v>
       </c>
       <c r="N57" s="112" t="s">
@@ -6896,20 +6910,20 @@
       <c r="R57" s="112"/>
       <c r="S57" s="112"/>
       <c r="T57" s="112"/>
-      <c r="U57" s="123"/>
-      <c r="V57" s="122" t="s">
+      <c r="U57" s="140"/>
+      <c r="V57" s="111" t="s">
         <v>74</v>
       </c>
       <c r="W57" s="112"/>
       <c r="X57" s="112"/>
-      <c r="Y57" s="123"/>
+      <c r="Y57" s="140"/>
     </row>
     <row r="58" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A58" s="148" t="s">
-        <v>130</v>
+      <c r="A58" s="149" t="s">
+        <v>128</v>
       </c>
       <c r="B58" s="14" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C58" s="18" t="s">
         <v>52</v>
@@ -6931,29 +6945,29 @@
       <c r="J58" s="19">
         <v>0</v>
       </c>
-      <c r="K58" s="125" t="s">
-        <v>129</v>
-      </c>
-      <c r="L58" s="153"/>
-      <c r="M58" s="153"/>
-      <c r="N58" s="153"/>
-      <c r="O58" s="153"/>
-      <c r="P58" s="153"/>
-      <c r="Q58" s="153"/>
-      <c r="R58" s="153"/>
-      <c r="S58" s="153"/>
-      <c r="T58" s="153"/>
-      <c r="U58" s="154"/>
-      <c r="V58" s="124"/>
-      <c r="W58" s="114"/>
-      <c r="X58" s="114"/>
-      <c r="Y58" s="125"/>
-      <c r="Z58" s="104"/>
+      <c r="K58" s="143" t="s">
+        <v>127</v>
+      </c>
+      <c r="L58" s="144"/>
+      <c r="M58" s="144"/>
+      <c r="N58" s="144"/>
+      <c r="O58" s="144"/>
+      <c r="P58" s="144"/>
+      <c r="Q58" s="144"/>
+      <c r="R58" s="144"/>
+      <c r="S58" s="144"/>
+      <c r="T58" s="144"/>
+      <c r="U58" s="145"/>
+      <c r="V58" s="142"/>
+      <c r="W58" s="119"/>
+      <c r="X58" s="119"/>
+      <c r="Y58" s="143"/>
+      <c r="Z58" s="102"/>
     </row>
     <row r="59" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="149"/>
-      <c r="B59" s="106" t="s">
-        <v>128</v>
+      <c r="A59" s="156"/>
+      <c r="B59" s="104" t="s">
+        <v>126</v>
       </c>
       <c r="C59" s="54" t="s">
         <v>52</v>
@@ -6975,51 +6989,51 @@
       <c r="J59" s="56">
         <v>0</v>
       </c>
-      <c r="K59" s="155" t="s">
-        <v>129</v>
-      </c>
-      <c r="L59" s="156"/>
-      <c r="M59" s="156"/>
-      <c r="N59" s="156"/>
-      <c r="O59" s="156"/>
-      <c r="P59" s="156"/>
-      <c r="Q59" s="156"/>
-      <c r="R59" s="156"/>
-      <c r="S59" s="156"/>
-      <c r="T59" s="156"/>
-      <c r="U59" s="157"/>
-      <c r="V59" s="122"/>
+      <c r="K59" s="108" t="s">
+        <v>127</v>
+      </c>
+      <c r="L59" s="109"/>
+      <c r="M59" s="109"/>
+      <c r="N59" s="109"/>
+      <c r="O59" s="109"/>
+      <c r="P59" s="109"/>
+      <c r="Q59" s="109"/>
+      <c r="R59" s="109"/>
+      <c r="S59" s="109"/>
+      <c r="T59" s="109"/>
+      <c r="U59" s="110"/>
+      <c r="V59" s="111"/>
       <c r="W59" s="112"/>
       <c r="X59" s="112"/>
       <c r="Y59" s="113"/>
-      <c r="Z59" s="104"/>
+      <c r="Z59" s="102"/>
     </row>
     <row r="60" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A60" s="107"/>
-      <c r="B60" s="108"/>
-      <c r="C60" s="105"/>
-      <c r="D60" s="105"/>
-      <c r="E60" s="105"/>
-      <c r="F60" s="105"/>
-      <c r="G60" s="105"/>
-      <c r="H60" s="105"/>
-      <c r="I60" s="105"/>
-      <c r="J60" s="105"/>
-      <c r="K60" s="105"/>
-      <c r="L60" s="105"/>
-      <c r="M60" s="105"/>
-      <c r="N60" s="105"/>
-      <c r="O60" s="105"/>
-      <c r="P60" s="105"/>
-      <c r="Q60" s="105"/>
-      <c r="R60" s="105"/>
-      <c r="S60" s="105"/>
-      <c r="T60" s="105"/>
-      <c r="U60" s="105"/>
-      <c r="V60" s="105"/>
-      <c r="W60" s="105"/>
-      <c r="X60" s="105"/>
-      <c r="Y60" s="105"/>
+      <c r="A60" s="105"/>
+      <c r="B60" s="106"/>
+      <c r="C60" s="103"/>
+      <c r="D60" s="103"/>
+      <c r="E60" s="103"/>
+      <c r="F60" s="103"/>
+      <c r="G60" s="103"/>
+      <c r="H60" s="103"/>
+      <c r="I60" s="103"/>
+      <c r="J60" s="103"/>
+      <c r="K60" s="103"/>
+      <c r="L60" s="103"/>
+      <c r="M60" s="103"/>
+      <c r="N60" s="103"/>
+      <c r="O60" s="103"/>
+      <c r="P60" s="103"/>
+      <c r="Q60" s="103"/>
+      <c r="R60" s="103"/>
+      <c r="S60" s="103"/>
+      <c r="T60" s="103"/>
+      <c r="U60" s="103"/>
+      <c r="V60" s="103"/>
+      <c r="W60" s="103"/>
+      <c r="X60" s="103"/>
+      <c r="Y60" s="103"/>
     </row>
     <row r="61" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B61" s="81"/>
@@ -7053,6 +7067,94 @@
     </row>
   </sheetData>
   <mergeCells count="112">
+    <mergeCell ref="N50:U50"/>
+    <mergeCell ref="N51:U51"/>
+    <mergeCell ref="N42:U42"/>
+    <mergeCell ref="N43:U43"/>
+    <mergeCell ref="N45:U45"/>
+    <mergeCell ref="N47:U47"/>
+    <mergeCell ref="N48:U48"/>
+    <mergeCell ref="O39:U39"/>
+    <mergeCell ref="J40:M40"/>
+    <mergeCell ref="N40:U40"/>
+    <mergeCell ref="J41:M41"/>
+    <mergeCell ref="N41:U41"/>
+    <mergeCell ref="N44:U44"/>
+    <mergeCell ref="N46:U46"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="P33:R33"/>
+    <mergeCell ref="S33:U33"/>
+    <mergeCell ref="K14:M14"/>
+    <mergeCell ref="N14:U14"/>
+    <mergeCell ref="N49:U49"/>
+    <mergeCell ref="O38:U38"/>
+    <mergeCell ref="J37:P37"/>
+    <mergeCell ref="V57:Y57"/>
+    <mergeCell ref="V58:Y58"/>
+    <mergeCell ref="N52:U52"/>
+    <mergeCell ref="N53:U53"/>
+    <mergeCell ref="N54:U54"/>
+    <mergeCell ref="N55:U55"/>
+    <mergeCell ref="N56:U56"/>
+    <mergeCell ref="V52:Y52"/>
+    <mergeCell ref="V53:Y53"/>
+    <mergeCell ref="V54:Y54"/>
+    <mergeCell ref="V55:Y55"/>
+    <mergeCell ref="V56:Y56"/>
+    <mergeCell ref="N57:U57"/>
+    <mergeCell ref="K58:U58"/>
+    <mergeCell ref="P19:R19"/>
+    <mergeCell ref="P20:R20"/>
+    <mergeCell ref="P21:R21"/>
+    <mergeCell ref="P22:R22"/>
+    <mergeCell ref="P23:R23"/>
+    <mergeCell ref="S28:U28"/>
+    <mergeCell ref="S29:U29"/>
+    <mergeCell ref="S30:U30"/>
+    <mergeCell ref="S31:U31"/>
+    <mergeCell ref="P31:R31"/>
+    <mergeCell ref="S19:U19"/>
+    <mergeCell ref="S20:U20"/>
+    <mergeCell ref="S21:U21"/>
+    <mergeCell ref="S22:U22"/>
+    <mergeCell ref="S23:U23"/>
+    <mergeCell ref="S24:U24"/>
+    <mergeCell ref="S25:U25"/>
+    <mergeCell ref="S26:U26"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="K35:M35"/>
+    <mergeCell ref="N35:U35"/>
+    <mergeCell ref="K36:M36"/>
+    <mergeCell ref="N36:U36"/>
+    <mergeCell ref="P28:R28"/>
+    <mergeCell ref="P29:R29"/>
+    <mergeCell ref="P30:R30"/>
+    <mergeCell ref="V1:Y1"/>
+    <mergeCell ref="P16:R16"/>
+    <mergeCell ref="S16:U16"/>
+    <mergeCell ref="P17:R17"/>
+    <mergeCell ref="P18:R18"/>
+    <mergeCell ref="S17:U17"/>
+    <mergeCell ref="S18:U18"/>
+    <mergeCell ref="P4:R4"/>
+    <mergeCell ref="S4:U4"/>
+    <mergeCell ref="P5:R5"/>
+    <mergeCell ref="S5:U5"/>
+    <mergeCell ref="P6:R6"/>
+    <mergeCell ref="S6:U6"/>
+    <mergeCell ref="P7:R7"/>
+    <mergeCell ref="N11:U11"/>
+    <mergeCell ref="S9:U9"/>
+    <mergeCell ref="L15:O15"/>
+    <mergeCell ref="P9:R9"/>
+    <mergeCell ref="K11:M11"/>
+    <mergeCell ref="P10:R10"/>
+    <mergeCell ref="K13:M13"/>
+    <mergeCell ref="N13:U13"/>
+    <mergeCell ref="K12:M12"/>
+    <mergeCell ref="N12:U12"/>
     <mergeCell ref="K59:U59"/>
     <mergeCell ref="V59:Y59"/>
     <mergeCell ref="A58:A59"/>
@@ -7077,165 +7179,75 @@
     <mergeCell ref="P26:R26"/>
     <mergeCell ref="P27:R27"/>
     <mergeCell ref="P24:R24"/>
-    <mergeCell ref="V1:Y1"/>
-    <mergeCell ref="P16:R16"/>
-    <mergeCell ref="S16:U16"/>
-    <mergeCell ref="P17:R17"/>
-    <mergeCell ref="P18:R18"/>
-    <mergeCell ref="S17:U17"/>
-    <mergeCell ref="S18:U18"/>
-    <mergeCell ref="P4:R4"/>
-    <mergeCell ref="S4:U4"/>
-    <mergeCell ref="P5:R5"/>
-    <mergeCell ref="S5:U5"/>
-    <mergeCell ref="P6:R6"/>
-    <mergeCell ref="S6:U6"/>
-    <mergeCell ref="P7:R7"/>
-    <mergeCell ref="N11:U11"/>
-    <mergeCell ref="S9:U9"/>
-    <mergeCell ref="L15:O15"/>
-    <mergeCell ref="P9:R9"/>
-    <mergeCell ref="K11:M11"/>
-    <mergeCell ref="P10:R10"/>
-    <mergeCell ref="K13:M13"/>
-    <mergeCell ref="N13:U13"/>
-    <mergeCell ref="K12:M12"/>
-    <mergeCell ref="N12:U12"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="K35:M35"/>
-    <mergeCell ref="N35:U35"/>
-    <mergeCell ref="K36:M36"/>
-    <mergeCell ref="N36:U36"/>
-    <mergeCell ref="P28:R28"/>
-    <mergeCell ref="P29:R29"/>
-    <mergeCell ref="P30:R30"/>
-    <mergeCell ref="P19:R19"/>
-    <mergeCell ref="P20:R20"/>
-    <mergeCell ref="P21:R21"/>
-    <mergeCell ref="P22:R22"/>
-    <mergeCell ref="P23:R23"/>
-    <mergeCell ref="S28:U28"/>
-    <mergeCell ref="S29:U29"/>
-    <mergeCell ref="S30:U30"/>
-    <mergeCell ref="S31:U31"/>
-    <mergeCell ref="P31:R31"/>
-    <mergeCell ref="S19:U19"/>
-    <mergeCell ref="S20:U20"/>
-    <mergeCell ref="S21:U21"/>
-    <mergeCell ref="S22:U22"/>
-    <mergeCell ref="S23:U23"/>
-    <mergeCell ref="S24:U24"/>
-    <mergeCell ref="S25:U25"/>
-    <mergeCell ref="S26:U26"/>
-    <mergeCell ref="V57:Y57"/>
-    <mergeCell ref="V58:Y58"/>
-    <mergeCell ref="N52:U52"/>
-    <mergeCell ref="N53:U53"/>
-    <mergeCell ref="N54:U54"/>
-    <mergeCell ref="N55:U55"/>
-    <mergeCell ref="N56:U56"/>
-    <mergeCell ref="V52:Y52"/>
-    <mergeCell ref="V53:Y53"/>
-    <mergeCell ref="V54:Y54"/>
-    <mergeCell ref="V55:Y55"/>
-    <mergeCell ref="V56:Y56"/>
-    <mergeCell ref="N57:U57"/>
-    <mergeCell ref="K58:U58"/>
-    <mergeCell ref="N44:U44"/>
-    <mergeCell ref="N46:U46"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="P33:R33"/>
-    <mergeCell ref="S33:U33"/>
-    <mergeCell ref="K14:M14"/>
-    <mergeCell ref="N14:U14"/>
-    <mergeCell ref="N49:U49"/>
-    <mergeCell ref="N50:U50"/>
-    <mergeCell ref="N51:U51"/>
-    <mergeCell ref="N42:U42"/>
-    <mergeCell ref="N43:U43"/>
-    <mergeCell ref="N45:U45"/>
-    <mergeCell ref="N47:U47"/>
-    <mergeCell ref="N48:U48"/>
-    <mergeCell ref="O39:U39"/>
-    <mergeCell ref="J40:M40"/>
-    <mergeCell ref="N40:U40"/>
-    <mergeCell ref="J41:M41"/>
-    <mergeCell ref="N41:U41"/>
-    <mergeCell ref="O38:U38"/>
-    <mergeCell ref="J37:P37"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="F4:U57 K58:K59 F58:I59">
-    <cfRule type="cellIs" dxfId="18" priority="10" operator="equal">
+  <conditionalFormatting sqref="F58:K59">
+    <cfRule type="cellIs" dxfId="18" priority="1" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="17" priority="2" operator="containsText" text="imm">
+      <formula>NOT(ISERROR(SEARCH("imm",F58)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="3" operator="equal">
+      <formula>"imm3"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="4" operator="equal">
+      <formula>"imm5"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F4:U57">
+    <cfRule type="cellIs" dxfId="14" priority="10" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F41:M41 V41:Y41 F42:Y57 V58:Y59 F1:Y40 K58:K59 F58:I59">
-    <cfRule type="containsText" dxfId="17" priority="11" operator="containsText" text="imm">
+  <conditionalFormatting sqref="F1:Y40 F41:M41 V41:Y41 F42:Y57 V58:Y59">
+    <cfRule type="containsText" dxfId="13" priority="11" operator="containsText" text="imm">
       <formula>NOT(ISERROR(SEARCH("imm",F1)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="12" operator="equal">
       <formula>"imm3"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="13" operator="equal">
       <formula>"imm5"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:U31">
-    <cfRule type="cellIs" dxfId="14" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="14" operator="equal">
       <formula>"Rd"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="15" operator="equal">
       <formula>"Rn"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="16" operator="equal">
       <formula>"Rd"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="17" operator="equal">
       <formula>"Rdn"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="18" operator="equal">
       <formula>"Rm"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H33:U33">
-    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>"Rd"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
       <formula>"Rn"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="7" operator="equal">
       <formula>"Rd"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="8" operator="equal">
       <formula>"Rdn"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="9" operator="equal">
       <formula>"Rm"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P16:R16">
-    <cfRule type="cellIs" dxfId="4" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="19" operator="equal">
       <formula>"Rm"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J58:J59">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J58:J59">
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="imm">
-      <formula>NOT(ISERROR(SEARCH("imm",J58)))</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
-      <formula>"imm3"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
-      <formula>"imm5"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7244,15 +7256,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010096649AD79A527B47A67D905693C83B0C" ma:contentTypeVersion="7" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="44d09355696640e2dc56270e449341cd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="98b34aae-4bd1-40d2-80e1-46205a35d283" xmlns:ns4="4c17d7eb-fa2b-4fbc-8175-1cef2629d4d8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="73bda8d09c620ff6c543bf34844bea48" ns3:_="" ns4:_="">
     <xsd:import namespace="98b34aae-4bd1-40d2-80e1-46205a35d283"/>
@@ -7437,6 +7440,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -7444,14 +7456,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AAD58D5F-4A46-4F63-A2BD-BBB590555A8D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90060F17-AE26-48CA-A0B9-2F516B758ECF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7466,6 +7470,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AAD58D5F-4A46-4F63-A2BD-BBB590555A8D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Support of SP-relative address
</commit_message>
<xml_diff>
--- a/docs/ARM instructions.xlsx
+++ b/docs/ARM instructions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Drive\Etudes\Supérieur\SI3\Architecture et réseaux\Architecture\PARM\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BC655D6-233E-4AA0-BD98-B825F9F7E0DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9DF84F9-F3D3-46F3-AB7A-F210C7AD614C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1E4904EC-9B68-40DD-B685-7BD66B9DE8BA}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="140">
   <si>
     <t>Description</t>
   </si>
@@ -1871,6 +1871,30 @@
       </rPr>
       <t>lear</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Add</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (SP plus immediate)</t>
+    </r>
+  </si>
+  <si>
+    <t>Generate SP-relative address</t>
   </si>
 </sst>
 </file>
@@ -1938,7 +1962,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="19">
+  <fills count="21">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2047,6 +2071,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="54">
     <border>
@@ -2735,7 +2771,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="157">
+  <cellXfs count="166">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3058,6 +3094,113 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3067,131 +3210,253 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="19">
+  <dxfs count="44">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFF9999"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC99FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9999"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -3274,33 +3539,6 @@
           <bgColor theme="5" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF9999"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCC99FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9999"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
     </dxf>
     <dxf>
       <fill>
@@ -3656,10 +3894,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Z70"/>
+  <dimension ref="A1:Z72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" zoomScaleSheetLayoutView="145" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" zoomScaleSheetLayoutView="145" zoomScalePageLayoutView="145" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3672,50 +3910,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="114" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="118" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="116"/>
-      <c r="D1" s="116"/>
-      <c r="E1" s="117"/>
-      <c r="F1" s="116" t="s">
+      <c r="A1" s="154" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="156" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="142"/>
+      <c r="D1" s="142"/>
+      <c r="E1" s="143"/>
+      <c r="F1" s="142" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="116"/>
-      <c r="H1" s="116"/>
-      <c r="I1" s="116"/>
-      <c r="J1" s="116"/>
-      <c r="K1" s="116"/>
-      <c r="L1" s="116"/>
-      <c r="M1" s="116"/>
-      <c r="N1" s="116"/>
-      <c r="O1" s="116"/>
-      <c r="P1" s="116"/>
-      <c r="Q1" s="116"/>
-      <c r="R1" s="116"/>
-      <c r="S1" s="116"/>
-      <c r="T1" s="116"/>
-      <c r="U1" s="117"/>
-      <c r="V1" s="123" t="s">
+      <c r="G1" s="142"/>
+      <c r="H1" s="142"/>
+      <c r="I1" s="142"/>
+      <c r="J1" s="142"/>
+      <c r="K1" s="142"/>
+      <c r="L1" s="142"/>
+      <c r="M1" s="142"/>
+      <c r="N1" s="142"/>
+      <c r="O1" s="142"/>
+      <c r="P1" s="142"/>
+      <c r="Q1" s="142"/>
+      <c r="R1" s="142"/>
+      <c r="S1" s="142"/>
+      <c r="T1" s="142"/>
+      <c r="U1" s="143"/>
+      <c r="V1" s="141" t="s">
         <v>3</v>
       </c>
-      <c r="W1" s="116"/>
-      <c r="X1" s="116"/>
-      <c r="Y1" s="117"/>
+      <c r="W1" s="142"/>
+      <c r="X1" s="142"/>
+      <c r="Y1" s="143"/>
     </row>
     <row r="2" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="115"/>
+      <c r="A2" s="155"/>
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="116" t="s">
+      <c r="C2" s="142" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="116"/>
-      <c r="E2" s="117"/>
+      <c r="D2" s="142"/>
+      <c r="E2" s="143"/>
       <c r="F2" s="2">
         <v>15</v>
       </c>
@@ -3791,13 +4029,13 @@
       <c r="G3" s="10">
         <v>0</v>
       </c>
-      <c r="H3" s="120" t="s">
+      <c r="H3" s="148" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="120"/>
-      <c r="J3" s="120"/>
-      <c r="K3" s="120"/>
-      <c r="L3" s="120"/>
+      <c r="I3" s="148"/>
+      <c r="J3" s="148"/>
+      <c r="K3" s="148"/>
+      <c r="L3" s="148"/>
       <c r="M3" s="11"/>
       <c r="N3" s="11"/>
       <c r="O3" s="11"/>
@@ -3843,23 +4081,23 @@
       <c r="J4" s="20">
         <v>0</v>
       </c>
-      <c r="K4" s="119" t="s">
+      <c r="K4" s="112" t="s">
         <v>15</v>
       </c>
-      <c r="L4" s="119"/>
-      <c r="M4" s="119"/>
-      <c r="N4" s="119"/>
-      <c r="O4" s="119"/>
-      <c r="P4" s="128" t="s">
+      <c r="L4" s="112"/>
+      <c r="M4" s="112"/>
+      <c r="N4" s="112"/>
+      <c r="O4" s="112"/>
+      <c r="P4" s="122" t="s">
         <v>16</v>
       </c>
-      <c r="Q4" s="128"/>
-      <c r="R4" s="128"/>
-      <c r="S4" s="119" t="s">
+      <c r="Q4" s="122"/>
+      <c r="R4" s="122"/>
+      <c r="S4" s="112" t="s">
         <v>17</v>
       </c>
-      <c r="T4" s="119"/>
-      <c r="U4" s="121"/>
+      <c r="T4" s="112"/>
+      <c r="U4" s="113"/>
       <c r="V4" s="22" t="s">
         <v>18</v>
       </c>
@@ -3902,23 +4140,23 @@
       <c r="J5" s="26">
         <v>1</v>
       </c>
-      <c r="K5" s="119" t="s">
+      <c r="K5" s="112" t="s">
         <v>15</v>
       </c>
-      <c r="L5" s="119"/>
-      <c r="M5" s="119"/>
-      <c r="N5" s="119"/>
-      <c r="O5" s="119"/>
-      <c r="P5" s="119" t="s">
+      <c r="L5" s="112"/>
+      <c r="M5" s="112"/>
+      <c r="N5" s="112"/>
+      <c r="O5" s="112"/>
+      <c r="P5" s="112" t="s">
         <v>16</v>
       </c>
-      <c r="Q5" s="119"/>
-      <c r="R5" s="119"/>
-      <c r="S5" s="119" t="s">
+      <c r="Q5" s="112"/>
+      <c r="R5" s="112"/>
+      <c r="S5" s="112" t="s">
         <v>17</v>
       </c>
-      <c r="T5" s="119"/>
-      <c r="U5" s="121"/>
+      <c r="T5" s="112"/>
+      <c r="U5" s="113"/>
       <c r="V5" s="22" t="s">
         <v>18</v>
       </c>
@@ -3961,23 +4199,23 @@
       <c r="J6" s="20">
         <v>0</v>
       </c>
-      <c r="K6" s="119" t="s">
+      <c r="K6" s="112" t="s">
         <v>15</v>
       </c>
-      <c r="L6" s="119"/>
-      <c r="M6" s="119"/>
-      <c r="N6" s="119"/>
-      <c r="O6" s="119"/>
-      <c r="P6" s="119" t="s">
+      <c r="L6" s="112"/>
+      <c r="M6" s="112"/>
+      <c r="N6" s="112"/>
+      <c r="O6" s="112"/>
+      <c r="P6" s="112" t="s">
         <v>16</v>
       </c>
-      <c r="Q6" s="119"/>
-      <c r="R6" s="119"/>
-      <c r="S6" s="119" t="s">
+      <c r="Q6" s="112"/>
+      <c r="R6" s="112"/>
+      <c r="S6" s="112" t="s">
         <v>17</v>
       </c>
-      <c r="T6" s="119"/>
-      <c r="U6" s="121"/>
+      <c r="T6" s="112"/>
+      <c r="U6" s="113"/>
       <c r="V6" s="22" t="s">
         <v>18</v>
       </c>
@@ -4026,21 +4264,21 @@
       <c r="L7" s="31">
         <v>0</v>
       </c>
-      <c r="M7" s="119" t="s">
+      <c r="M7" s="112" t="s">
         <v>16</v>
       </c>
-      <c r="N7" s="119"/>
-      <c r="O7" s="119"/>
-      <c r="P7" s="119" t="s">
+      <c r="N7" s="112"/>
+      <c r="O7" s="112"/>
+      <c r="P7" s="112" t="s">
         <v>20</v>
       </c>
-      <c r="Q7" s="119"/>
-      <c r="R7" s="119"/>
-      <c r="S7" s="119" t="s">
+      <c r="Q7" s="112"/>
+      <c r="R7" s="112"/>
+      <c r="S7" s="112" t="s">
         <v>17</v>
       </c>
-      <c r="T7" s="119"/>
-      <c r="U7" s="121"/>
+      <c r="T7" s="112"/>
+      <c r="U7" s="113"/>
       <c r="V7" s="22" t="s">
         <v>18</v>
       </c>
@@ -4091,21 +4329,21 @@
       <c r="L8" s="32">
         <v>1</v>
       </c>
-      <c r="M8" s="119" t="s">
+      <c r="M8" s="112" t="s">
         <v>16</v>
       </c>
-      <c r="N8" s="119"/>
-      <c r="O8" s="119"/>
-      <c r="P8" s="119" t="s">
+      <c r="N8" s="112"/>
+      <c r="O8" s="112"/>
+      <c r="P8" s="112" t="s">
         <v>20</v>
       </c>
-      <c r="Q8" s="119"/>
-      <c r="R8" s="119"/>
-      <c r="S8" s="119" t="s">
+      <c r="Q8" s="112"/>
+      <c r="R8" s="112"/>
+      <c r="S8" s="112" t="s">
         <v>17</v>
       </c>
-      <c r="T8" s="119"/>
-      <c r="U8" s="121"/>
+      <c r="T8" s="112"/>
+      <c r="U8" s="113"/>
       <c r="V8" s="22" t="s">
         <v>18</v>
       </c>
@@ -4156,21 +4394,21 @@
       <c r="L9" s="31">
         <v>0</v>
       </c>
-      <c r="M9" s="119" t="s">
+      <c r="M9" s="112" t="s">
         <v>22</v>
       </c>
-      <c r="N9" s="119"/>
-      <c r="O9" s="119"/>
-      <c r="P9" s="119" t="s">
+      <c r="N9" s="112"/>
+      <c r="O9" s="112"/>
+      <c r="P9" s="112" t="s">
         <v>20</v>
       </c>
-      <c r="Q9" s="119"/>
-      <c r="R9" s="119"/>
-      <c r="S9" s="119" t="s">
+      <c r="Q9" s="112"/>
+      <c r="R9" s="112"/>
+      <c r="S9" s="112" t="s">
         <v>17</v>
       </c>
-      <c r="T9" s="119"/>
-      <c r="U9" s="121"/>
+      <c r="T9" s="112"/>
+      <c r="U9" s="113"/>
       <c r="V9" s="22" t="s">
         <v>18</v>
       </c>
@@ -4221,21 +4459,21 @@
       <c r="L10" s="32">
         <v>1</v>
       </c>
-      <c r="M10" s="119" t="s">
+      <c r="M10" s="112" t="s">
         <v>22</v>
       </c>
-      <c r="N10" s="119"/>
-      <c r="O10" s="119"/>
-      <c r="P10" s="119" t="s">
+      <c r="N10" s="112"/>
+      <c r="O10" s="112"/>
+      <c r="P10" s="112" t="s">
         <v>20</v>
       </c>
-      <c r="Q10" s="119"/>
-      <c r="R10" s="119"/>
-      <c r="S10" s="119" t="s">
+      <c r="Q10" s="112"/>
+      <c r="R10" s="112"/>
+      <c r="S10" s="112" t="s">
         <v>17</v>
       </c>
-      <c r="T10" s="119"/>
-      <c r="U10" s="121"/>
+      <c r="T10" s="112"/>
+      <c r="U10" s="113"/>
       <c r="V10" s="22" t="s">
         <v>18</v>
       </c>
@@ -4278,21 +4516,21 @@
       <c r="J11" s="31">
         <v>0</v>
       </c>
-      <c r="K11" s="129" t="s">
+      <c r="K11" s="123" t="s">
         <v>17</v>
       </c>
-      <c r="L11" s="129"/>
-      <c r="M11" s="129"/>
-      <c r="N11" s="119" t="s">
+      <c r="L11" s="123"/>
+      <c r="M11" s="123"/>
+      <c r="N11" s="112" t="s">
         <v>24</v>
       </c>
-      <c r="O11" s="119"/>
-      <c r="P11" s="119"/>
-      <c r="Q11" s="119"/>
-      <c r="R11" s="119"/>
-      <c r="S11" s="119"/>
-      <c r="T11" s="119"/>
-      <c r="U11" s="121"/>
+      <c r="O11" s="112"/>
+      <c r="P11" s="112"/>
+      <c r="Q11" s="112"/>
+      <c r="R11" s="112"/>
+      <c r="S11" s="112"/>
+      <c r="T11" s="112"/>
+      <c r="U11" s="113"/>
       <c r="V11" s="22"/>
       <c r="W11" s="19"/>
       <c r="X11" s="19" t="s">
@@ -4331,21 +4569,21 @@
       <c r="J12" s="32">
         <v>1</v>
       </c>
-      <c r="K12" s="129" t="s">
+      <c r="K12" s="123" t="s">
         <v>17</v>
       </c>
-      <c r="L12" s="129"/>
-      <c r="M12" s="129"/>
-      <c r="N12" s="119" t="s">
+      <c r="L12" s="123"/>
+      <c r="M12" s="123"/>
+      <c r="N12" s="112" t="s">
         <v>24</v>
       </c>
-      <c r="O12" s="119"/>
-      <c r="P12" s="119"/>
-      <c r="Q12" s="119"/>
-      <c r="R12" s="119"/>
-      <c r="S12" s="119"/>
-      <c r="T12" s="119"/>
-      <c r="U12" s="121"/>
+      <c r="O12" s="112"/>
+      <c r="P12" s="112"/>
+      <c r="Q12" s="112"/>
+      <c r="R12" s="112"/>
+      <c r="S12" s="112"/>
+      <c r="T12" s="112"/>
+      <c r="U12" s="113"/>
       <c r="V12" s="19" t="s">
         <v>18</v>
       </c>
@@ -4388,21 +4626,21 @@
       <c r="J13" s="31">
         <v>0</v>
       </c>
-      <c r="K13" s="129" t="s">
+      <c r="K13" s="123" t="s">
         <v>17</v>
       </c>
-      <c r="L13" s="129"/>
-      <c r="M13" s="129"/>
-      <c r="N13" s="119" t="s">
+      <c r="L13" s="123"/>
+      <c r="M13" s="123"/>
+      <c r="N13" s="112" t="s">
         <v>24</v>
       </c>
-      <c r="O13" s="119"/>
-      <c r="P13" s="119"/>
-      <c r="Q13" s="119"/>
-      <c r="R13" s="119"/>
-      <c r="S13" s="119"/>
-      <c r="T13" s="119"/>
-      <c r="U13" s="121"/>
+      <c r="O13" s="112"/>
+      <c r="P13" s="112"/>
+      <c r="Q13" s="112"/>
+      <c r="R13" s="112"/>
+      <c r="S13" s="112"/>
+      <c r="T13" s="112"/>
+      <c r="U13" s="113"/>
       <c r="V13" s="19" t="s">
         <v>18</v>
       </c>
@@ -4445,21 +4683,21 @@
       <c r="J14" s="31">
         <v>1</v>
       </c>
-      <c r="K14" s="129" t="s">
+      <c r="K14" s="123" t="s">
         <v>17</v>
       </c>
-      <c r="L14" s="129"/>
-      <c r="M14" s="129"/>
-      <c r="N14" s="119" t="s">
+      <c r="L14" s="123"/>
+      <c r="M14" s="123"/>
+      <c r="N14" s="112" t="s">
         <v>24</v>
       </c>
-      <c r="O14" s="119"/>
-      <c r="P14" s="119"/>
-      <c r="Q14" s="119"/>
-      <c r="R14" s="119"/>
-      <c r="S14" s="119"/>
-      <c r="T14" s="119"/>
-      <c r="U14" s="121"/>
+      <c r="O14" s="112"/>
+      <c r="P14" s="112"/>
+      <c r="Q14" s="112"/>
+      <c r="R14" s="112"/>
+      <c r="S14" s="112"/>
+      <c r="T14" s="112"/>
+      <c r="U14" s="113"/>
       <c r="V14" s="19" t="s">
         <v>18</v>
       </c>
@@ -4499,12 +4737,12 @@
       <c r="K15" s="39">
         <v>0</v>
       </c>
-      <c r="L15" s="120" t="s">
+      <c r="L15" s="148" t="s">
         <v>11</v>
       </c>
-      <c r="M15" s="120"/>
-      <c r="N15" s="120"/>
-      <c r="O15" s="120"/>
+      <c r="M15" s="148"/>
+      <c r="N15" s="148"/>
+      <c r="O15" s="148"/>
       <c r="P15" s="36"/>
       <c r="Q15" s="36"/>
       <c r="R15" s="40"/>
@@ -4568,16 +4806,16 @@
       <c r="O16" s="20">
         <v>0</v>
       </c>
-      <c r="P16" s="124" t="s">
+      <c r="P16" s="144" t="s">
         <v>16</v>
       </c>
-      <c r="Q16" s="125"/>
-      <c r="R16" s="125"/>
-      <c r="S16" s="126" t="s">
+      <c r="Q16" s="145"/>
+      <c r="R16" s="145"/>
+      <c r="S16" s="146" t="s">
         <v>27</v>
       </c>
-      <c r="T16" s="126"/>
-      <c r="U16" s="127"/>
+      <c r="T16" s="146"/>
+      <c r="U16" s="147"/>
       <c r="V16" s="22" t="s">
         <v>18</v>
       </c>
@@ -4633,16 +4871,16 @@
       <c r="O17" s="26">
         <v>1</v>
       </c>
-      <c r="P17" s="122" t="s">
+      <c r="P17" s="133" t="s">
         <v>16</v>
       </c>
-      <c r="Q17" s="119"/>
-      <c r="R17" s="119"/>
-      <c r="S17" s="119" t="s">
+      <c r="Q17" s="112"/>
+      <c r="R17" s="112"/>
+      <c r="S17" s="112" t="s">
         <v>27</v>
       </c>
-      <c r="T17" s="119"/>
-      <c r="U17" s="121"/>
+      <c r="T17" s="112"/>
+      <c r="U17" s="113"/>
       <c r="V17" s="22" t="s">
         <v>18</v>
       </c>
@@ -4698,16 +4936,16 @@
       <c r="O18" s="20">
         <v>0</v>
       </c>
-      <c r="P18" s="122" t="s">
+      <c r="P18" s="133" t="s">
         <v>16</v>
       </c>
-      <c r="Q18" s="119"/>
-      <c r="R18" s="119"/>
-      <c r="S18" s="119" t="s">
+      <c r="Q18" s="112"/>
+      <c r="R18" s="112"/>
+      <c r="S18" s="112" t="s">
         <v>27</v>
       </c>
-      <c r="T18" s="119"/>
-      <c r="U18" s="121"/>
+      <c r="T18" s="112"/>
+      <c r="U18" s="113"/>
       <c r="V18" s="22" t="s">
         <v>18</v>
       </c>
@@ -4763,16 +5001,16 @@
       <c r="O19" s="26">
         <v>1</v>
       </c>
-      <c r="P19" s="122" t="s">
+      <c r="P19" s="133" t="s">
         <v>16</v>
       </c>
-      <c r="Q19" s="119"/>
-      <c r="R19" s="119"/>
-      <c r="S19" s="119" t="s">
+      <c r="Q19" s="112"/>
+      <c r="R19" s="112"/>
+      <c r="S19" s="112" t="s">
         <v>27</v>
       </c>
-      <c r="T19" s="119"/>
-      <c r="U19" s="121"/>
+      <c r="T19" s="112"/>
+      <c r="U19" s="113"/>
       <c r="V19" s="22" t="s">
         <v>18</v>
       </c>
@@ -4828,16 +5066,16 @@
       <c r="O20" s="20">
         <v>0</v>
       </c>
-      <c r="P20" s="122" t="s">
+      <c r="P20" s="133" t="s">
         <v>16</v>
       </c>
-      <c r="Q20" s="119"/>
-      <c r="R20" s="119"/>
-      <c r="S20" s="119" t="s">
+      <c r="Q20" s="112"/>
+      <c r="R20" s="112"/>
+      <c r="S20" s="112" t="s">
         <v>27</v>
       </c>
-      <c r="T20" s="119"/>
-      <c r="U20" s="121"/>
+      <c r="T20" s="112"/>
+      <c r="U20" s="113"/>
       <c r="V20" s="22" t="s">
         <v>18</v>
       </c>
@@ -4893,16 +5131,16 @@
       <c r="O21" s="26">
         <v>1</v>
       </c>
-      <c r="P21" s="122" t="s">
+      <c r="P21" s="133" t="s">
         <v>16</v>
       </c>
-      <c r="Q21" s="119"/>
-      <c r="R21" s="119"/>
-      <c r="S21" s="119" t="s">
+      <c r="Q21" s="112"/>
+      <c r="R21" s="112"/>
+      <c r="S21" s="112" t="s">
         <v>27</v>
       </c>
-      <c r="T21" s="119"/>
-      <c r="U21" s="121"/>
+      <c r="T21" s="112"/>
+      <c r="U21" s="113"/>
       <c r="V21" s="22" t="s">
         <v>18</v>
       </c>
@@ -4960,16 +5198,16 @@
       <c r="O22" s="20">
         <v>0</v>
       </c>
-      <c r="P22" s="122" t="s">
+      <c r="P22" s="133" t="s">
         <v>16</v>
       </c>
-      <c r="Q22" s="119"/>
-      <c r="R22" s="119"/>
-      <c r="S22" s="119" t="s">
+      <c r="Q22" s="112"/>
+      <c r="R22" s="112"/>
+      <c r="S22" s="112" t="s">
         <v>27</v>
       </c>
-      <c r="T22" s="119"/>
-      <c r="U22" s="121"/>
+      <c r="T22" s="112"/>
+      <c r="U22" s="113"/>
       <c r="V22" s="22" t="s">
         <v>18</v>
       </c>
@@ -5027,16 +5265,16 @@
       <c r="O23" s="26">
         <v>1</v>
       </c>
-      <c r="P23" s="122" t="s">
+      <c r="P23" s="133" t="s">
         <v>16</v>
       </c>
-      <c r="Q23" s="119"/>
-      <c r="R23" s="119"/>
-      <c r="S23" s="119" t="s">
+      <c r="Q23" s="112"/>
+      <c r="R23" s="112"/>
+      <c r="S23" s="112" t="s">
         <v>27</v>
       </c>
-      <c r="T23" s="119"/>
-      <c r="U23" s="121"/>
+      <c r="T23" s="112"/>
+      <c r="U23" s="113"/>
       <c r="V23" s="22" t="s">
         <v>18</v>
       </c>
@@ -5092,16 +5330,16 @@
       <c r="O24" s="20">
         <v>0</v>
       </c>
-      <c r="P24" s="122" t="s">
+      <c r="P24" s="133" t="s">
         <v>16</v>
       </c>
-      <c r="Q24" s="119"/>
-      <c r="R24" s="119"/>
-      <c r="S24" s="119" t="s">
+      <c r="Q24" s="112"/>
+      <c r="R24" s="112"/>
+      <c r="S24" s="112" t="s">
         <v>20</v>
       </c>
-      <c r="T24" s="119"/>
-      <c r="U24" s="121"/>
+      <c r="T24" s="112"/>
+      <c r="U24" s="113"/>
       <c r="V24" s="22" t="s">
         <v>18</v>
       </c>
@@ -5159,16 +5397,16 @@
       <c r="O25" s="26">
         <v>1</v>
       </c>
-      <c r="P25" s="122" t="s">
+      <c r="P25" s="133" t="s">
         <v>20</v>
       </c>
-      <c r="Q25" s="119"/>
-      <c r="R25" s="119"/>
-      <c r="S25" s="119" t="s">
+      <c r="Q25" s="112"/>
+      <c r="R25" s="112"/>
+      <c r="S25" s="112" t="s">
         <v>17</v>
       </c>
-      <c r="T25" s="119"/>
-      <c r="U25" s="121"/>
+      <c r="T25" s="112"/>
+      <c r="U25" s="113"/>
       <c r="V25" s="22" t="s">
         <v>18</v>
       </c>
@@ -5226,16 +5464,16 @@
       <c r="O26" s="20">
         <v>0</v>
       </c>
-      <c r="P26" s="122" t="s">
+      <c r="P26" s="133" t="s">
         <v>16</v>
       </c>
-      <c r="Q26" s="119"/>
-      <c r="R26" s="119"/>
-      <c r="S26" s="119" t="s">
+      <c r="Q26" s="112"/>
+      <c r="R26" s="112"/>
+      <c r="S26" s="112" t="s">
         <v>20</v>
       </c>
-      <c r="T26" s="119"/>
-      <c r="U26" s="121"/>
+      <c r="T26" s="112"/>
+      <c r="U26" s="113"/>
       <c r="V26" s="22" t="s">
         <v>18</v>
       </c>
@@ -5293,16 +5531,16 @@
       <c r="O27" s="26">
         <v>1</v>
       </c>
-      <c r="P27" s="122" t="s">
+      <c r="P27" s="133" t="s">
         <v>16</v>
       </c>
-      <c r="Q27" s="119"/>
-      <c r="R27" s="119"/>
-      <c r="S27" s="119" t="s">
+      <c r="Q27" s="112"/>
+      <c r="R27" s="112"/>
+      <c r="S27" s="112" t="s">
         <v>20</v>
       </c>
-      <c r="T27" s="119"/>
-      <c r="U27" s="121"/>
+      <c r="T27" s="112"/>
+      <c r="U27" s="113"/>
       <c r="V27" s="22" t="s">
         <v>18</v>
       </c>
@@ -5360,16 +5598,16 @@
       <c r="O28" s="20">
         <v>0</v>
       </c>
-      <c r="P28" s="122" t="s">
+      <c r="P28" s="133" t="s">
         <v>16</v>
       </c>
-      <c r="Q28" s="119"/>
-      <c r="R28" s="119"/>
-      <c r="S28" s="119" t="s">
+      <c r="Q28" s="112"/>
+      <c r="R28" s="112"/>
+      <c r="S28" s="112" t="s">
         <v>27</v>
       </c>
-      <c r="T28" s="119"/>
-      <c r="U28" s="121"/>
+      <c r="T28" s="112"/>
+      <c r="U28" s="113"/>
       <c r="V28" s="22" t="s">
         <v>18</v>
       </c>
@@ -5427,16 +5665,16 @@
       <c r="O29" s="26">
         <v>1</v>
       </c>
-      <c r="P29" s="122" t="s">
+      <c r="P29" s="133" t="s">
         <v>20</v>
       </c>
-      <c r="Q29" s="119"/>
-      <c r="R29" s="119"/>
-      <c r="S29" s="138" t="s">
+      <c r="Q29" s="112"/>
+      <c r="R29" s="112"/>
+      <c r="S29" s="134" t="s">
         <v>36</v>
       </c>
-      <c r="T29" s="138"/>
-      <c r="U29" s="139"/>
+      <c r="T29" s="134"/>
+      <c r="U29" s="135"/>
       <c r="V29" s="22"/>
       <c r="W29" s="19"/>
       <c r="X29" s="19" t="s">
@@ -5490,16 +5728,16 @@
       <c r="O30" s="20">
         <v>0</v>
       </c>
-      <c r="P30" s="122" t="s">
+      <c r="P30" s="133" t="s">
         <v>16</v>
       </c>
-      <c r="Q30" s="119"/>
-      <c r="R30" s="119"/>
-      <c r="S30" s="119" t="s">
+      <c r="Q30" s="112"/>
+      <c r="R30" s="112"/>
+      <c r="S30" s="112" t="s">
         <v>27</v>
       </c>
-      <c r="T30" s="119"/>
-      <c r="U30" s="121"/>
+      <c r="T30" s="112"/>
+      <c r="U30" s="113"/>
       <c r="V30" s="22" t="s">
         <v>18</v>
       </c>
@@ -5555,16 +5793,16 @@
       <c r="O31" s="58">
         <v>1</v>
       </c>
-      <c r="P31" s="141" t="s">
+      <c r="P31" s="136" t="s">
         <v>16</v>
       </c>
-      <c r="Q31" s="112"/>
-      <c r="R31" s="112"/>
-      <c r="S31" s="112" t="s">
+      <c r="Q31" s="127"/>
+      <c r="R31" s="127"/>
+      <c r="S31" s="127" t="s">
         <v>17</v>
       </c>
-      <c r="T31" s="112"/>
-      <c r="U31" s="140"/>
+      <c r="T31" s="127"/>
+      <c r="U31" s="128"/>
       <c r="V31" s="22" t="s">
         <v>18</v>
       </c>
@@ -5576,7 +5814,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A32" s="82" t="s">
         <v>132</v>
       </c>
@@ -5625,7 +5863,7 @@
       <c r="A33" s="84" t="s">
         <v>133</v>
       </c>
-      <c r="B33" s="43" t="s">
+      <c r="B33" s="162" t="s">
         <v>87</v>
       </c>
       <c r="C33" s="99" t="s">
@@ -5659,22 +5897,22 @@
       <c r="M33" s="97">
         <v>0</v>
       </c>
-      <c r="N33" s="97">
-        <v>0</v>
-      </c>
-      <c r="O33" s="97">
-        <v>0</v>
-      </c>
-      <c r="P33" s="128" t="s">
+      <c r="N33" s="157">
+        <v>0</v>
+      </c>
+      <c r="O33" s="157">
+        <v>0</v>
+      </c>
+      <c r="P33" s="158" t="s">
         <v>16</v>
       </c>
-      <c r="Q33" s="128"/>
-      <c r="R33" s="128"/>
-      <c r="S33" s="119" t="s">
+      <c r="Q33" s="158"/>
+      <c r="R33" s="158"/>
+      <c r="S33" s="159" t="s">
         <v>17</v>
       </c>
-      <c r="T33" s="119"/>
-      <c r="U33" s="121"/>
+      <c r="T33" s="159"/>
+      <c r="U33" s="160"/>
       <c r="V33" s="22" t="s">
         <v>18</v>
       </c>
@@ -5741,10 +5979,10 @@
       <c r="C35" s="60" t="s">
         <v>40</v>
       </c>
-      <c r="D35" s="130" t="s">
+      <c r="D35" s="137" t="s">
         <v>43</v>
       </c>
-      <c r="E35" s="131"/>
+      <c r="E35" s="138"/>
       <c r="F35" s="61">
         <v>1</v>
       </c>
@@ -5760,21 +5998,21 @@
       <c r="J35" s="64">
         <v>0</v>
       </c>
-      <c r="K35" s="132" t="s">
+      <c r="K35" s="139" t="s">
         <v>41</v>
       </c>
-      <c r="L35" s="132"/>
-      <c r="M35" s="132"/>
-      <c r="N35" s="133" t="s">
+      <c r="L35" s="139"/>
+      <c r="M35" s="139"/>
+      <c r="N35" s="124" t="s">
         <v>24</v>
       </c>
-      <c r="O35" s="133"/>
-      <c r="P35" s="133"/>
-      <c r="Q35" s="133"/>
-      <c r="R35" s="133"/>
-      <c r="S35" s="133"/>
-      <c r="T35" s="133"/>
-      <c r="U35" s="134"/>
+      <c r="O35" s="124"/>
+      <c r="P35" s="124"/>
+      <c r="Q35" s="124"/>
+      <c r="R35" s="124"/>
+      <c r="S35" s="124"/>
+      <c r="T35" s="124"/>
+      <c r="U35" s="125"/>
       <c r="V35" s="22"/>
       <c r="W35" s="19"/>
       <c r="X35" s="19"/>
@@ -5790,10 +6028,10 @@
       <c r="C36" s="65" t="s">
         <v>40</v>
       </c>
-      <c r="D36" s="130" t="s">
+      <c r="D36" s="137" t="s">
         <v>43</v>
       </c>
-      <c r="E36" s="131"/>
+      <c r="E36" s="138"/>
       <c r="F36" s="67">
         <v>1</v>
       </c>
@@ -5809,21 +6047,21 @@
       <c r="J36" s="70">
         <v>1</v>
       </c>
-      <c r="K36" s="135" t="s">
+      <c r="K36" s="140" t="s">
         <v>41</v>
       </c>
-      <c r="L36" s="135"/>
-      <c r="M36" s="135"/>
-      <c r="N36" s="136" t="s">
+      <c r="L36" s="140"/>
+      <c r="M36" s="140"/>
+      <c r="N36" s="114" t="s">
         <v>24</v>
       </c>
-      <c r="O36" s="136"/>
-      <c r="P36" s="136"/>
-      <c r="Q36" s="136"/>
-      <c r="R36" s="136"/>
-      <c r="S36" s="136"/>
-      <c r="T36" s="136"/>
-      <c r="U36" s="137"/>
+      <c r="O36" s="114"/>
+      <c r="P36" s="114"/>
+      <c r="Q36" s="114"/>
+      <c r="R36" s="114"/>
+      <c r="S36" s="114"/>
+      <c r="T36" s="114"/>
+      <c r="U36" s="115"/>
       <c r="V36" s="22"/>
       <c r="W36" s="19"/>
       <c r="X36" s="19"/>
@@ -5831,7 +6069,7 @@
     </row>
     <row r="37" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="82" t="s">
-        <v>44</v>
+        <v>139</v>
       </c>
       <c r="B37" s="36"/>
       <c r="C37" s="36"/>
@@ -5847,17 +6085,17 @@
         <v>1</v>
       </c>
       <c r="I37" s="36">
-        <v>1</v>
-      </c>
-      <c r="J37" s="146" t="s">
-        <v>11</v>
-      </c>
-      <c r="K37" s="146"/>
-      <c r="L37" s="146"/>
-      <c r="M37" s="146"/>
-      <c r="N37" s="146"/>
-      <c r="O37" s="146"/>
-      <c r="P37" s="146"/>
+        <v>0</v>
+      </c>
+      <c r="J37" s="36">
+        <v>1</v>
+      </c>
+      <c r="K37" s="163"/>
+      <c r="L37" s="163"/>
+      <c r="M37" s="163"/>
+      <c r="N37" s="163"/>
+      <c r="O37" s="163"/>
+      <c r="P37" s="163"/>
       <c r="Q37" s="36"/>
       <c r="R37" s="36"/>
       <c r="S37" s="36"/>
@@ -5877,321 +6115,313 @@
       </c>
     </row>
     <row r="38" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A38" s="90" t="s">
-        <v>109</v>
+      <c r="A38" s="165" t="s">
+        <v>138</v>
       </c>
       <c r="B38" s="43" t="s">
         <v>45</v>
       </c>
-      <c r="C38" s="71" t="s">
+      <c r="C38" s="99" t="s">
+        <v>12</v>
+      </c>
+      <c r="D38" s="71" t="s">
         <v>46</v>
       </c>
-      <c r="D38" s="62" t="s">
-        <v>129</v>
-      </c>
-      <c r="E38" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="F38" s="72">
-        <v>1</v>
-      </c>
-      <c r="G38" s="62">
-        <v>0</v>
-      </c>
-      <c r="H38" s="62">
-        <v>1</v>
-      </c>
-      <c r="I38" s="62">
-        <v>1</v>
-      </c>
-      <c r="J38" s="64">
-        <v>0</v>
-      </c>
-      <c r="K38" s="64">
-        <v>0</v>
-      </c>
-      <c r="L38" s="64">
-        <v>0</v>
-      </c>
-      <c r="M38" s="64">
-        <v>0</v>
-      </c>
-      <c r="N38" s="64">
-        <v>0</v>
-      </c>
-      <c r="O38" s="133" t="s">
-        <v>48</v>
-      </c>
-      <c r="P38" s="133"/>
-      <c r="Q38" s="133"/>
-      <c r="R38" s="133"/>
-      <c r="S38" s="133"/>
-      <c r="T38" s="133"/>
-      <c r="U38" s="134"/>
-      <c r="V38" s="22"/>
+      <c r="E38" s="97" t="s">
+        <v>23</v>
+      </c>
+      <c r="F38" s="54">
+        <v>1</v>
+      </c>
+      <c r="G38" s="56">
+        <v>0</v>
+      </c>
+      <c r="H38" s="56">
+        <v>1</v>
+      </c>
+      <c r="I38" s="56">
+        <v>0</v>
+      </c>
+      <c r="J38" s="164">
+        <v>1</v>
+      </c>
+      <c r="K38" s="127" t="s">
+        <v>17</v>
+      </c>
+      <c r="L38" s="127"/>
+      <c r="M38" s="127"/>
+      <c r="N38" s="161" t="s">
+        <v>24</v>
+      </c>
+      <c r="O38" s="124"/>
+      <c r="P38" s="124"/>
+      <c r="Q38" s="124"/>
+      <c r="R38" s="124"/>
+      <c r="S38" s="124"/>
+      <c r="T38" s="124"/>
+      <c r="U38" s="125"/>
+      <c r="V38" s="18"/>
       <c r="W38" s="19"/>
       <c r="X38" s="19"/>
       <c r="Y38" s="21"/>
     </row>
     <row r="39" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="90" t="s">
-        <v>110</v>
-      </c>
-      <c r="B39" s="33" t="s">
-        <v>49</v>
-      </c>
-      <c r="C39" s="73" t="s">
-        <v>46</v>
-      </c>
-      <c r="D39" s="68" t="s">
-        <v>129</v>
-      </c>
-      <c r="E39" s="66" t="s">
-        <v>47</v>
-      </c>
-      <c r="F39" s="74">
-        <v>1</v>
-      </c>
-      <c r="G39" s="68">
-        <v>0</v>
-      </c>
-      <c r="H39" s="68">
-        <v>1</v>
-      </c>
-      <c r="I39" s="68">
-        <v>1</v>
-      </c>
-      <c r="J39" s="75">
-        <v>0</v>
-      </c>
-      <c r="K39" s="75">
-        <v>0</v>
-      </c>
-      <c r="L39" s="75">
-        <v>0</v>
-      </c>
-      <c r="M39" s="75">
-        <v>0</v>
-      </c>
-      <c r="N39" s="75">
-        <v>1</v>
-      </c>
-      <c r="O39" s="136" t="s">
-        <v>48</v>
-      </c>
-      <c r="P39" s="136"/>
-      <c r="Q39" s="136"/>
-      <c r="R39" s="136"/>
-      <c r="S39" s="136"/>
-      <c r="T39" s="136"/>
-      <c r="U39" s="137"/>
-      <c r="V39" s="22"/>
-      <c r="W39" s="19"/>
-      <c r="X39" s="19"/>
-      <c r="Y39" s="21"/>
+      <c r="A39" s="82" t="s">
+        <v>44</v>
+      </c>
+      <c r="B39" s="36"/>
+      <c r="C39" s="36"/>
+      <c r="D39" s="36"/>
+      <c r="E39" s="36"/>
+      <c r="F39" s="36">
+        <v>1</v>
+      </c>
+      <c r="G39" s="36">
+        <v>0</v>
+      </c>
+      <c r="H39" s="36">
+        <v>1</v>
+      </c>
+      <c r="I39" s="36">
+        <v>1</v>
+      </c>
+      <c r="J39" s="116" t="s">
+        <v>11</v>
+      </c>
+      <c r="K39" s="116"/>
+      <c r="L39" s="116"/>
+      <c r="M39" s="116"/>
+      <c r="N39" s="116"/>
+      <c r="O39" s="116"/>
+      <c r="P39" s="116"/>
+      <c r="Q39" s="36"/>
+      <c r="R39" s="36"/>
+      <c r="S39" s="36"/>
+      <c r="T39" s="36"/>
+      <c r="U39" s="37"/>
+      <c r="V39" s="42" t="s">
+        <v>6</v>
+      </c>
+      <c r="W39" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="X39" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y39" s="37" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="40" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A40" s="82" t="s">
-        <v>50</v>
-      </c>
-      <c r="B40" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="C40" s="36" t="s">
-        <v>52</v>
-      </c>
-      <c r="D40" s="36"/>
-      <c r="E40" s="36"/>
-      <c r="F40" s="36">
-        <v>1</v>
-      </c>
-      <c r="G40" s="36">
-        <v>1</v>
-      </c>
-      <c r="H40" s="36">
-        <v>0</v>
-      </c>
-      <c r="I40" s="36">
-        <v>1</v>
-      </c>
-      <c r="J40" s="146" t="s">
-        <v>11</v>
-      </c>
-      <c r="K40" s="146"/>
-      <c r="L40" s="146"/>
-      <c r="M40" s="146"/>
-      <c r="N40" s="146"/>
-      <c r="O40" s="146"/>
-      <c r="P40" s="146"/>
-      <c r="Q40" s="146"/>
-      <c r="R40" s="146"/>
-      <c r="S40" s="146"/>
-      <c r="T40" s="146"/>
-      <c r="U40" s="147"/>
-      <c r="V40" s="42"/>
-      <c r="W40" s="36"/>
-      <c r="X40" s="36"/>
-      <c r="Y40" s="37"/>
+      <c r="A40" s="90" t="s">
+        <v>109</v>
+      </c>
+      <c r="B40" s="43" t="s">
+        <v>45</v>
+      </c>
+      <c r="C40" s="71" t="s">
+        <v>46</v>
+      </c>
+      <c r="D40" s="62" t="s">
+        <v>129</v>
+      </c>
+      <c r="E40" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="F40" s="72">
+        <v>1</v>
+      </c>
+      <c r="G40" s="62">
+        <v>0</v>
+      </c>
+      <c r="H40" s="62">
+        <v>1</v>
+      </c>
+      <c r="I40" s="62">
+        <v>1</v>
+      </c>
+      <c r="J40" s="64">
+        <v>0</v>
+      </c>
+      <c r="K40" s="64">
+        <v>0</v>
+      </c>
+      <c r="L40" s="64">
+        <v>0</v>
+      </c>
+      <c r="M40" s="64">
+        <v>0</v>
+      </c>
+      <c r="N40" s="64">
+        <v>0</v>
+      </c>
+      <c r="O40" s="124" t="s">
+        <v>48</v>
+      </c>
+      <c r="P40" s="124"/>
+      <c r="Q40" s="124"/>
+      <c r="R40" s="124"/>
+      <c r="S40" s="124"/>
+      <c r="T40" s="124"/>
+      <c r="U40" s="125"/>
+      <c r="V40" s="22"/>
+      <c r="W40" s="19"/>
+      <c r="X40" s="19"/>
+      <c r="Y40" s="21"/>
     </row>
     <row r="41" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="82"/>
-      <c r="B41" s="36" t="s">
-        <v>53</v>
-      </c>
-      <c r="C41" s="36"/>
-      <c r="D41" s="36"/>
-      <c r="E41" s="36"/>
-      <c r="F41" s="36"/>
-      <c r="G41" s="36"/>
-      <c r="H41" s="36"/>
-      <c r="I41" s="36"/>
-      <c r="J41" s="146" t="s">
-        <v>54</v>
-      </c>
-      <c r="K41" s="146"/>
-      <c r="L41" s="146"/>
-      <c r="M41" s="146"/>
-      <c r="N41" s="146" t="s">
-        <v>24</v>
-      </c>
-      <c r="O41" s="146"/>
-      <c r="P41" s="146"/>
-      <c r="Q41" s="146"/>
-      <c r="R41" s="146"/>
-      <c r="S41" s="146"/>
-      <c r="T41" s="146"/>
-      <c r="U41" s="147"/>
-      <c r="V41" s="42" t="s">
-        <v>6</v>
-      </c>
-      <c r="W41" s="36" t="s">
-        <v>7</v>
-      </c>
-      <c r="X41" s="36" t="s">
-        <v>8</v>
-      </c>
-      <c r="Y41" s="37" t="s">
-        <v>9</v>
-      </c>
+      <c r="A41" s="90" t="s">
+        <v>110</v>
+      </c>
+      <c r="B41" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="C41" s="73" t="s">
+        <v>46</v>
+      </c>
+      <c r="D41" s="68" t="s">
+        <v>129</v>
+      </c>
+      <c r="E41" s="66" t="s">
+        <v>47</v>
+      </c>
+      <c r="F41" s="74">
+        <v>1</v>
+      </c>
+      <c r="G41" s="68">
+        <v>0</v>
+      </c>
+      <c r="H41" s="68">
+        <v>1</v>
+      </c>
+      <c r="I41" s="68">
+        <v>1</v>
+      </c>
+      <c r="J41" s="75">
+        <v>0</v>
+      </c>
+      <c r="K41" s="75">
+        <v>0</v>
+      </c>
+      <c r="L41" s="75">
+        <v>0</v>
+      </c>
+      <c r="M41" s="75">
+        <v>0</v>
+      </c>
+      <c r="N41" s="75">
+        <v>1</v>
+      </c>
+      <c r="O41" s="114" t="s">
+        <v>48</v>
+      </c>
+      <c r="P41" s="114"/>
+      <c r="Q41" s="114"/>
+      <c r="R41" s="114"/>
+      <c r="S41" s="114"/>
+      <c r="T41" s="114"/>
+      <c r="U41" s="115"/>
+      <c r="V41" s="22"/>
+      <c r="W41" s="19"/>
+      <c r="X41" s="19"/>
+      <c r="Y41" s="21"/>
     </row>
     <row r="42" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A42" s="148" t="s">
-        <v>111</v>
-      </c>
-      <c r="B42" s="76" t="s">
-        <v>55</v>
-      </c>
-      <c r="C42" s="71" t="s">
+      <c r="A42" s="82" t="s">
+        <v>50</v>
+      </c>
+      <c r="B42" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="C42" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="D42" s="62"/>
-      <c r="E42" s="45"/>
-      <c r="F42" s="18">
-        <v>1</v>
-      </c>
-      <c r="G42" s="19">
-        <v>1</v>
-      </c>
-      <c r="H42" s="19">
-        <v>0</v>
-      </c>
-      <c r="I42" s="19">
-        <v>1</v>
-      </c>
-      <c r="J42" s="20">
-        <v>0</v>
-      </c>
-      <c r="K42" s="20">
-        <v>0</v>
-      </c>
-      <c r="L42" s="20">
-        <v>0</v>
-      </c>
-      <c r="M42" s="20">
-        <v>0</v>
-      </c>
-      <c r="N42" s="119" t="s">
+      <c r="D42" s="36"/>
+      <c r="E42" s="36"/>
+      <c r="F42" s="36">
+        <v>1</v>
+      </c>
+      <c r="G42" s="36">
+        <v>1</v>
+      </c>
+      <c r="H42" s="36">
+        <v>0</v>
+      </c>
+      <c r="I42" s="36">
+        <v>1</v>
+      </c>
+      <c r="J42" s="116" t="s">
+        <v>11</v>
+      </c>
+      <c r="K42" s="116"/>
+      <c r="L42" s="116"/>
+      <c r="M42" s="116"/>
+      <c r="N42" s="116"/>
+      <c r="O42" s="116"/>
+      <c r="P42" s="116"/>
+      <c r="Q42" s="116"/>
+      <c r="R42" s="116"/>
+      <c r="S42" s="116"/>
+      <c r="T42" s="116"/>
+      <c r="U42" s="117"/>
+      <c r="V42" s="42"/>
+      <c r="W42" s="36"/>
+      <c r="X42" s="36"/>
+      <c r="Y42" s="37"/>
+    </row>
+    <row r="43" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="82"/>
+      <c r="B43" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="C43" s="36"/>
+      <c r="D43" s="36"/>
+      <c r="E43" s="36"/>
+      <c r="F43" s="36"/>
+      <c r="G43" s="36"/>
+      <c r="H43" s="36"/>
+      <c r="I43" s="36"/>
+      <c r="J43" s="116" t="s">
+        <v>54</v>
+      </c>
+      <c r="K43" s="116"/>
+      <c r="L43" s="116"/>
+      <c r="M43" s="116"/>
+      <c r="N43" s="116" t="s">
         <v>24</v>
       </c>
-      <c r="O42" s="119"/>
-      <c r="P42" s="119"/>
-      <c r="Q42" s="119"/>
-      <c r="R42" s="119"/>
-      <c r="S42" s="119"/>
-      <c r="T42" s="119"/>
-      <c r="U42" s="121"/>
-      <c r="V42" s="22"/>
-      <c r="W42" s="19"/>
-      <c r="X42" s="19"/>
-      <c r="Y42" s="21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A43" s="148" t="s">
-        <v>112</v>
-      </c>
-      <c r="B43" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="C43" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="D43" s="19"/>
-      <c r="E43" s="21"/>
-      <c r="F43" s="18">
-        <v>1</v>
-      </c>
-      <c r="G43" s="19">
-        <v>1</v>
-      </c>
-      <c r="H43" s="19">
-        <v>0</v>
-      </c>
-      <c r="I43" s="19">
-        <v>1</v>
-      </c>
-      <c r="J43" s="20">
-        <v>0</v>
-      </c>
-      <c r="K43" s="20">
-        <v>0</v>
-      </c>
-      <c r="L43" s="20">
-        <v>0</v>
-      </c>
-      <c r="M43" s="20">
-        <v>1</v>
-      </c>
-      <c r="N43" s="119" t="s">
-        <v>24</v>
-      </c>
-      <c r="O43" s="119"/>
-      <c r="P43" s="119"/>
-      <c r="Q43" s="119"/>
-      <c r="R43" s="119"/>
-      <c r="S43" s="119"/>
-      <c r="T43" s="119"/>
-      <c r="U43" s="121"/>
-      <c r="V43" s="22"/>
-      <c r="W43" s="19"/>
-      <c r="X43" s="19"/>
-      <c r="Y43" s="21">
-        <v>0</v>
+      <c r="O43" s="116"/>
+      <c r="P43" s="116"/>
+      <c r="Q43" s="116"/>
+      <c r="R43" s="116"/>
+      <c r="S43" s="116"/>
+      <c r="T43" s="116"/>
+      <c r="U43" s="117"/>
+      <c r="V43" s="42" t="s">
+        <v>6</v>
+      </c>
+      <c r="W43" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="X43" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y43" s="37" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="44" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A44" s="149" t="s">
-        <v>113</v>
-      </c>
-      <c r="B44" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="C44" s="18" t="s">
+      <c r="A44" s="108" t="s">
+        <v>111</v>
+      </c>
+      <c r="B44" s="76" t="s">
+        <v>55</v>
+      </c>
+      <c r="C44" s="71" t="s">
         <v>52</v>
       </c>
-      <c r="D44" s="19"/>
-      <c r="E44" s="21"/>
+      <c r="D44" s="62"/>
+      <c r="E44" s="45"/>
       <c r="F44" s="18">
         <v>1</v>
       </c>
@@ -6211,32 +6441,34 @@
         <v>0</v>
       </c>
       <c r="L44" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M44" s="20">
         <v>0</v>
       </c>
-      <c r="N44" s="119" t="s">
+      <c r="N44" s="112" t="s">
         <v>24</v>
       </c>
-      <c r="O44" s="119"/>
-      <c r="P44" s="119"/>
-      <c r="Q44" s="119"/>
-      <c r="R44" s="119"/>
-      <c r="S44" s="119"/>
-      <c r="T44" s="119"/>
-      <c r="U44" s="121"/>
-      <c r="V44" s="22">
-        <v>1</v>
-      </c>
+      <c r="O44" s="112"/>
+      <c r="P44" s="112"/>
+      <c r="Q44" s="112"/>
+      <c r="R44" s="112"/>
+      <c r="S44" s="112"/>
+      <c r="T44" s="112"/>
+      <c r="U44" s="113"/>
+      <c r="V44" s="22"/>
       <c r="W44" s="19"/>
       <c r="X44" s="19"/>
-      <c r="Y44" s="21"/>
+      <c r="Y44" s="21">
+        <v>1</v>
+      </c>
     </row>
     <row r="45" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A45" s="150"/>
+      <c r="A45" s="108" t="s">
+        <v>112</v>
+      </c>
       <c r="B45" s="14" t="s">
-        <v>130</v>
+        <v>56</v>
       </c>
       <c r="C45" s="18" t="s">
         <v>52</v>
@@ -6262,34 +6494,34 @@
         <v>0</v>
       </c>
       <c r="L45" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M45" s="20">
-        <v>0</v>
-      </c>
-      <c r="N45" s="119" t="s">
+        <v>1</v>
+      </c>
+      <c r="N45" s="112" t="s">
         <v>24</v>
       </c>
-      <c r="O45" s="119"/>
-      <c r="P45" s="119"/>
-      <c r="Q45" s="119"/>
-      <c r="R45" s="119"/>
-      <c r="S45" s="119"/>
-      <c r="T45" s="119"/>
-      <c r="U45" s="121"/>
-      <c r="V45" s="22">
-        <v>1</v>
-      </c>
+      <c r="O45" s="112"/>
+      <c r="P45" s="112"/>
+      <c r="Q45" s="112"/>
+      <c r="R45" s="112"/>
+      <c r="S45" s="112"/>
+      <c r="T45" s="112"/>
+      <c r="U45" s="113"/>
+      <c r="V45" s="22"/>
       <c r="W45" s="19"/>
       <c r="X45" s="19"/>
-      <c r="Y45" s="21"/>
+      <c r="Y45" s="21">
+        <v>0</v>
+      </c>
     </row>
     <row r="46" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A46" s="151" t="s">
-        <v>114</v>
+      <c r="A46" s="118" t="s">
+        <v>113</v>
       </c>
       <c r="B46" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C46" s="18" t="s">
         <v>52</v>
@@ -6318,29 +6550,29 @@
         <v>1</v>
       </c>
       <c r="M46" s="20">
-        <v>1</v>
-      </c>
-      <c r="N46" s="119" t="s">
+        <v>0</v>
+      </c>
+      <c r="N46" s="112" t="s">
         <v>24</v>
       </c>
-      <c r="O46" s="119"/>
-      <c r="P46" s="119"/>
-      <c r="Q46" s="119"/>
-      <c r="R46" s="119"/>
-      <c r="S46" s="119"/>
-      <c r="T46" s="119"/>
-      <c r="U46" s="121"/>
+      <c r="O46" s="112"/>
+      <c r="P46" s="112"/>
+      <c r="Q46" s="112"/>
+      <c r="R46" s="112"/>
+      <c r="S46" s="112"/>
+      <c r="T46" s="112"/>
+      <c r="U46" s="113"/>
       <c r="V46" s="22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W46" s="19"/>
       <c r="X46" s="19"/>
       <c r="Y46" s="21"/>
     </row>
     <row r="47" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A47" s="152"/>
+      <c r="A47" s="119"/>
       <c r="B47" s="14" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C47" s="18" t="s">
         <v>52</v>
@@ -6369,31 +6601,31 @@
         <v>1</v>
       </c>
       <c r="M47" s="20">
-        <v>1</v>
-      </c>
-      <c r="N47" s="119" t="s">
+        <v>0</v>
+      </c>
+      <c r="N47" s="112" t="s">
         <v>24</v>
       </c>
-      <c r="O47" s="119"/>
-      <c r="P47" s="119"/>
-      <c r="Q47" s="119"/>
-      <c r="R47" s="119"/>
-      <c r="S47" s="119"/>
-      <c r="T47" s="119"/>
-      <c r="U47" s="121"/>
+      <c r="O47" s="112"/>
+      <c r="P47" s="112"/>
+      <c r="Q47" s="112"/>
+      <c r="R47" s="112"/>
+      <c r="S47" s="112"/>
+      <c r="T47" s="112"/>
+      <c r="U47" s="113"/>
       <c r="V47" s="22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W47" s="19"/>
       <c r="X47" s="19"/>
       <c r="Y47" s="21"/>
     </row>
     <row r="48" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A48" s="153" t="s">
-        <v>115</v>
+      <c r="A48" s="120" t="s">
+        <v>114</v>
       </c>
       <c r="B48" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C48" s="18" t="s">
         <v>52</v>
@@ -6416,37 +6648,35 @@
         <v>0</v>
       </c>
       <c r="K48" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L48" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M48" s="20">
-        <v>0</v>
-      </c>
-      <c r="N48" s="119" t="s">
+        <v>1</v>
+      </c>
+      <c r="N48" s="112" t="s">
         <v>24</v>
       </c>
-      <c r="O48" s="119"/>
-      <c r="P48" s="119"/>
-      <c r="Q48" s="119"/>
-      <c r="R48" s="119"/>
-      <c r="S48" s="119"/>
-      <c r="T48" s="119"/>
-      <c r="U48" s="121"/>
-      <c r="V48" s="22"/>
+      <c r="O48" s="112"/>
+      <c r="P48" s="112"/>
+      <c r="Q48" s="112"/>
+      <c r="R48" s="112"/>
+      <c r="S48" s="112"/>
+      <c r="T48" s="112"/>
+      <c r="U48" s="113"/>
+      <c r="V48" s="22">
+        <v>0</v>
+      </c>
       <c r="W48" s="19"/>
-      <c r="X48" s="19">
-        <v>1</v>
-      </c>
+      <c r="X48" s="19"/>
       <c r="Y48" s="21"/>
     </row>
     <row r="49" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A49" s="153" t="s">
-        <v>116</v>
-      </c>
+      <c r="A49" s="121"/>
       <c r="B49" s="14" t="s">
-        <v>60</v>
+        <v>131</v>
       </c>
       <c r="C49" s="18" t="s">
         <v>52</v>
@@ -6469,37 +6699,37 @@
         <v>0</v>
       </c>
       <c r="K49" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L49" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M49" s="20">
         <v>1</v>
       </c>
-      <c r="N49" s="119" t="s">
+      <c r="N49" s="112" t="s">
         <v>24</v>
       </c>
-      <c r="O49" s="119"/>
-      <c r="P49" s="119"/>
-      <c r="Q49" s="119"/>
-      <c r="R49" s="119"/>
-      <c r="S49" s="119"/>
-      <c r="T49" s="119"/>
-      <c r="U49" s="121"/>
-      <c r="V49" s="22"/>
+      <c r="O49" s="112"/>
+      <c r="P49" s="112"/>
+      <c r="Q49" s="112"/>
+      <c r="R49" s="112"/>
+      <c r="S49" s="112"/>
+      <c r="T49" s="112"/>
+      <c r="U49" s="113"/>
+      <c r="V49" s="22">
+        <v>0</v>
+      </c>
       <c r="W49" s="19"/>
-      <c r="X49" s="19">
-        <v>0</v>
-      </c>
+      <c r="X49" s="19"/>
       <c r="Y49" s="21"/>
     </row>
     <row r="50" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A50" s="148" t="s">
-        <v>136</v>
+      <c r="A50" s="110" t="s">
+        <v>115</v>
       </c>
       <c r="B50" s="14" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C50" s="18" t="s">
         <v>52</v>
@@ -6525,34 +6755,34 @@
         <v>1</v>
       </c>
       <c r="L50" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M50" s="20">
         <v>0</v>
       </c>
-      <c r="N50" s="119" t="s">
+      <c r="N50" s="112" t="s">
         <v>24</v>
       </c>
-      <c r="O50" s="119"/>
-      <c r="P50" s="119"/>
-      <c r="Q50" s="119"/>
-      <c r="R50" s="119"/>
-      <c r="S50" s="119"/>
-      <c r="T50" s="119"/>
-      <c r="U50" s="121"/>
+      <c r="O50" s="112"/>
+      <c r="P50" s="112"/>
+      <c r="Q50" s="112"/>
+      <c r="R50" s="112"/>
+      <c r="S50" s="112"/>
+      <c r="T50" s="112"/>
+      <c r="U50" s="113"/>
       <c r="V50" s="22"/>
-      <c r="W50" s="19">
-        <v>1</v>
-      </c>
-      <c r="X50" s="19"/>
+      <c r="W50" s="19"/>
+      <c r="X50" s="19">
+        <v>1</v>
+      </c>
       <c r="Y50" s="21"/>
     </row>
     <row r="51" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A51" s="148" t="s">
-        <v>137</v>
+      <c r="A51" s="110" t="s">
+        <v>116</v>
       </c>
       <c r="B51" s="14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C51" s="18" t="s">
         <v>52</v>
@@ -6578,34 +6808,34 @@
         <v>1</v>
       </c>
       <c r="L51" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M51" s="20">
         <v>1</v>
       </c>
-      <c r="N51" s="119" t="s">
+      <c r="N51" s="112" t="s">
         <v>24</v>
       </c>
-      <c r="O51" s="119"/>
-      <c r="P51" s="119"/>
-      <c r="Q51" s="119"/>
-      <c r="R51" s="119"/>
-      <c r="S51" s="119"/>
-      <c r="T51" s="119"/>
-      <c r="U51" s="121"/>
+      <c r="O51" s="112"/>
+      <c r="P51" s="112"/>
+      <c r="Q51" s="112"/>
+      <c r="R51" s="112"/>
+      <c r="S51" s="112"/>
+      <c r="T51" s="112"/>
+      <c r="U51" s="113"/>
       <c r="V51" s="22"/>
-      <c r="W51" s="19">
-        <v>0</v>
-      </c>
-      <c r="X51" s="19"/>
+      <c r="W51" s="19"/>
+      <c r="X51" s="19">
+        <v>0</v>
+      </c>
       <c r="Y51" s="21"/>
     </row>
     <row r="52" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A52" s="154" t="s">
-        <v>117</v>
+      <c r="A52" s="108" t="s">
+        <v>136</v>
       </c>
       <c r="B52" s="14" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C52" s="18" t="s">
         <v>52</v>
@@ -6625,40 +6855,40 @@
         <v>1</v>
       </c>
       <c r="J52" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K52" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L52" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M52" s="20">
         <v>0</v>
       </c>
-      <c r="N52" s="119" t="s">
+      <c r="N52" s="112" t="s">
         <v>24</v>
       </c>
-      <c r="O52" s="119"/>
-      <c r="P52" s="119"/>
-      <c r="Q52" s="119"/>
-      <c r="R52" s="119"/>
-      <c r="S52" s="119"/>
-      <c r="T52" s="119"/>
-      <c r="U52" s="121"/>
-      <c r="V52" s="142" t="s">
-        <v>64</v>
-      </c>
-      <c r="W52" s="119"/>
-      <c r="X52" s="119"/>
-      <c r="Y52" s="121"/>
+      <c r="O52" s="112"/>
+      <c r="P52" s="112"/>
+      <c r="Q52" s="112"/>
+      <c r="R52" s="112"/>
+      <c r="S52" s="112"/>
+      <c r="T52" s="112"/>
+      <c r="U52" s="113"/>
+      <c r="V52" s="22"/>
+      <c r="W52" s="19">
+        <v>1</v>
+      </c>
+      <c r="X52" s="19"/>
+      <c r="Y52" s="21"/>
     </row>
     <row r="53" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A53" s="154" t="s">
-        <v>118</v>
+      <c r="A53" s="108" t="s">
+        <v>137</v>
       </c>
       <c r="B53" s="14" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C53" s="18" t="s">
         <v>52</v>
@@ -6678,40 +6908,40 @@
         <v>1</v>
       </c>
       <c r="J53" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K53" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L53" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M53" s="20">
         <v>1</v>
       </c>
-      <c r="N53" s="119" t="s">
+      <c r="N53" s="112" t="s">
         <v>24</v>
       </c>
-      <c r="O53" s="119"/>
-      <c r="P53" s="119"/>
-      <c r="Q53" s="119"/>
-      <c r="R53" s="119"/>
-      <c r="S53" s="119"/>
-      <c r="T53" s="119"/>
-      <c r="U53" s="121"/>
-      <c r="V53" s="142" t="s">
-        <v>66</v>
-      </c>
-      <c r="W53" s="119"/>
-      <c r="X53" s="119"/>
-      <c r="Y53" s="121"/>
+      <c r="O53" s="112"/>
+      <c r="P53" s="112"/>
+      <c r="Q53" s="112"/>
+      <c r="R53" s="112"/>
+      <c r="S53" s="112"/>
+      <c r="T53" s="112"/>
+      <c r="U53" s="113"/>
+      <c r="V53" s="22"/>
+      <c r="W53" s="19">
+        <v>0</v>
+      </c>
+      <c r="X53" s="19"/>
+      <c r="Y53" s="21"/>
     </row>
     <row r="54" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A54" s="154" t="s">
-        <v>119</v>
+      <c r="A54" s="111" t="s">
+        <v>117</v>
       </c>
       <c r="B54" s="14" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C54" s="18" t="s">
         <v>52</v>
@@ -6737,34 +6967,34 @@
         <v>0</v>
       </c>
       <c r="L54" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M54" s="20">
         <v>0</v>
       </c>
-      <c r="N54" s="119" t="s">
+      <c r="N54" s="112" t="s">
         <v>24</v>
       </c>
-      <c r="O54" s="119"/>
-      <c r="P54" s="119"/>
-      <c r="Q54" s="119"/>
-      <c r="R54" s="119"/>
-      <c r="S54" s="119"/>
-      <c r="T54" s="119"/>
-      <c r="U54" s="121"/>
-      <c r="V54" s="142" t="s">
-        <v>68</v>
-      </c>
-      <c r="W54" s="119"/>
-      <c r="X54" s="119"/>
-      <c r="Y54" s="121"/>
+      <c r="O54" s="112"/>
+      <c r="P54" s="112"/>
+      <c r="Q54" s="112"/>
+      <c r="R54" s="112"/>
+      <c r="S54" s="112"/>
+      <c r="T54" s="112"/>
+      <c r="U54" s="113"/>
+      <c r="V54" s="129" t="s">
+        <v>64</v>
+      </c>
+      <c r="W54" s="112"/>
+      <c r="X54" s="112"/>
+      <c r="Y54" s="113"/>
     </row>
     <row r="55" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A55" s="154" t="s">
-        <v>120</v>
+      <c r="A55" s="111" t="s">
+        <v>118</v>
       </c>
       <c r="B55" s="14" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C55" s="18" t="s">
         <v>52</v>
@@ -6790,34 +7020,34 @@
         <v>0</v>
       </c>
       <c r="L55" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M55" s="20">
         <v>1</v>
       </c>
-      <c r="N55" s="119" t="s">
+      <c r="N55" s="112" t="s">
         <v>24</v>
       </c>
-      <c r="O55" s="119"/>
-      <c r="P55" s="119"/>
-      <c r="Q55" s="119"/>
-      <c r="R55" s="119"/>
-      <c r="S55" s="119"/>
-      <c r="T55" s="119"/>
-      <c r="U55" s="121"/>
-      <c r="V55" s="142" t="s">
-        <v>70</v>
-      </c>
-      <c r="W55" s="119"/>
-      <c r="X55" s="119"/>
-      <c r="Y55" s="121"/>
+      <c r="O55" s="112"/>
+      <c r="P55" s="112"/>
+      <c r="Q55" s="112"/>
+      <c r="R55" s="112"/>
+      <c r="S55" s="112"/>
+      <c r="T55" s="112"/>
+      <c r="U55" s="113"/>
+      <c r="V55" s="129" t="s">
+        <v>66</v>
+      </c>
+      <c r="W55" s="112"/>
+      <c r="X55" s="112"/>
+      <c r="Y55" s="113"/>
     </row>
     <row r="56" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A56" s="154" t="s">
-        <v>121</v>
+      <c r="A56" s="111" t="s">
+        <v>119</v>
       </c>
       <c r="B56" s="14" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C56" s="18" t="s">
         <v>52</v>
@@ -6840,65 +7070,65 @@
         <v>1</v>
       </c>
       <c r="K56" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L56" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M56" s="20">
         <v>0</v>
       </c>
-      <c r="N56" s="119" t="s">
+      <c r="N56" s="112" t="s">
         <v>24</v>
       </c>
-      <c r="O56" s="119"/>
-      <c r="P56" s="119"/>
-      <c r="Q56" s="119"/>
-      <c r="R56" s="119"/>
-      <c r="S56" s="119"/>
-      <c r="T56" s="119"/>
-      <c r="U56" s="121"/>
-      <c r="V56" s="142" t="s">
-        <v>72</v>
-      </c>
-      <c r="W56" s="119"/>
-      <c r="X56" s="119"/>
-      <c r="Y56" s="121"/>
+      <c r="O56" s="112"/>
+      <c r="P56" s="112"/>
+      <c r="Q56" s="112"/>
+      <c r="R56" s="112"/>
+      <c r="S56" s="112"/>
+      <c r="T56" s="112"/>
+      <c r="U56" s="113"/>
+      <c r="V56" s="129" t="s">
+        <v>68</v>
+      </c>
+      <c r="W56" s="112"/>
+      <c r="X56" s="112"/>
+      <c r="Y56" s="113"/>
     </row>
     <row r="57" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A57" s="155" t="s">
-        <v>122</v>
-      </c>
-      <c r="B57" s="93" t="s">
-        <v>73</v>
-      </c>
-      <c r="C57" s="92" t="s">
+      <c r="A57" s="111" t="s">
+        <v>120</v>
+      </c>
+      <c r="B57" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C57" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="D57" s="56"/>
-      <c r="E57" s="59"/>
-      <c r="F57" s="92">
-        <v>1</v>
-      </c>
-      <c r="G57" s="56">
-        <v>1</v>
-      </c>
-      <c r="H57" s="56">
-        <v>0</v>
-      </c>
-      <c r="I57" s="56">
-        <v>1</v>
-      </c>
-      <c r="J57" s="101">
-        <v>1</v>
-      </c>
-      <c r="K57" s="101">
-        <v>1</v>
-      </c>
-      <c r="L57" s="101">
-        <v>0</v>
-      </c>
-      <c r="M57" s="101">
+      <c r="D57" s="19"/>
+      <c r="E57" s="21"/>
+      <c r="F57" s="18">
+        <v>1</v>
+      </c>
+      <c r="G57" s="19">
+        <v>1</v>
+      </c>
+      <c r="H57" s="19">
+        <v>0</v>
+      </c>
+      <c r="I57" s="19">
+        <v>1</v>
+      </c>
+      <c r="J57" s="20">
+        <v>1</v>
+      </c>
+      <c r="K57" s="20">
+        <v>0</v>
+      </c>
+      <c r="L57" s="20">
+        <v>1</v>
+      </c>
+      <c r="M57" s="20">
         <v>1</v>
       </c>
       <c r="N57" s="112" t="s">
@@ -6910,136 +7140,236 @@
       <c r="R57" s="112"/>
       <c r="S57" s="112"/>
       <c r="T57" s="112"/>
-      <c r="U57" s="140"/>
-      <c r="V57" s="111" t="s">
-        <v>74</v>
+      <c r="U57" s="113"/>
+      <c r="V57" s="129" t="s">
+        <v>70</v>
       </c>
       <c r="W57" s="112"/>
       <c r="X57" s="112"/>
-      <c r="Y57" s="140"/>
+      <c r="Y57" s="113"/>
     </row>
     <row r="58" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A58" s="149" t="s">
-        <v>128</v>
+      <c r="A58" s="111" t="s">
+        <v>121</v>
       </c>
       <c r="B58" s="14" t="s">
-        <v>125</v>
+        <v>71</v>
       </c>
       <c r="C58" s="18" t="s">
         <v>52</v>
       </c>
       <c r="D58" s="19"/>
-      <c r="E58" s="47"/>
-      <c r="F58" s="22">
+      <c r="E58" s="21"/>
+      <c r="F58" s="18">
         <v>1</v>
       </c>
       <c r="G58" s="19">
         <v>1</v>
       </c>
       <c r="H58" s="19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I58" s="19">
-        <v>0</v>
-      </c>
-      <c r="J58" s="19">
-        <v>0</v>
-      </c>
-      <c r="K58" s="143" t="s">
-        <v>127</v>
-      </c>
-      <c r="L58" s="144"/>
-      <c r="M58" s="144"/>
-      <c r="N58" s="144"/>
-      <c r="O58" s="144"/>
-      <c r="P58" s="144"/>
-      <c r="Q58" s="144"/>
-      <c r="R58" s="144"/>
-      <c r="S58" s="144"/>
-      <c r="T58" s="144"/>
-      <c r="U58" s="145"/>
-      <c r="V58" s="142"/>
-      <c r="W58" s="119"/>
-      <c r="X58" s="119"/>
-      <c r="Y58" s="143"/>
-      <c r="Z58" s="102"/>
+        <v>1</v>
+      </c>
+      <c r="J58" s="20">
+        <v>1</v>
+      </c>
+      <c r="K58" s="20">
+        <v>1</v>
+      </c>
+      <c r="L58" s="20">
+        <v>0</v>
+      </c>
+      <c r="M58" s="20">
+        <v>0</v>
+      </c>
+      <c r="N58" s="112" t="s">
+        <v>24</v>
+      </c>
+      <c r="O58" s="112"/>
+      <c r="P58" s="112"/>
+      <c r="Q58" s="112"/>
+      <c r="R58" s="112"/>
+      <c r="S58" s="112"/>
+      <c r="T58" s="112"/>
+      <c r="U58" s="113"/>
+      <c r="V58" s="129" t="s">
+        <v>72</v>
+      </c>
+      <c r="W58" s="112"/>
+      <c r="X58" s="112"/>
+      <c r="Y58" s="113"/>
     </row>
-    <row r="59" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="156"/>
-      <c r="B59" s="104" t="s">
-        <v>126</v>
-      </c>
-      <c r="C59" s="54" t="s">
+    <row r="59" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A59" s="109" t="s">
+        <v>122</v>
+      </c>
+      <c r="B59" s="93" t="s">
+        <v>73</v>
+      </c>
+      <c r="C59" s="92" t="s">
         <v>52</v>
       </c>
       <c r="D59" s="56"/>
-      <c r="E59" s="57"/>
-      <c r="F59" s="54">
+      <c r="E59" s="59"/>
+      <c r="F59" s="92">
         <v>1</v>
       </c>
       <c r="G59" s="56">
         <v>1</v>
       </c>
       <c r="H59" s="56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I59" s="56">
-        <v>0</v>
-      </c>
-      <c r="J59" s="56">
-        <v>0</v>
-      </c>
-      <c r="K59" s="108" t="s">
-        <v>127</v>
-      </c>
-      <c r="L59" s="109"/>
-      <c r="M59" s="109"/>
-      <c r="N59" s="109"/>
-      <c r="O59" s="109"/>
-      <c r="P59" s="109"/>
-      <c r="Q59" s="109"/>
-      <c r="R59" s="109"/>
-      <c r="S59" s="109"/>
-      <c r="T59" s="109"/>
-      <c r="U59" s="110"/>
-      <c r="V59" s="111"/>
-      <c r="W59" s="112"/>
-      <c r="X59" s="112"/>
-      <c r="Y59" s="113"/>
-      <c r="Z59" s="102"/>
+        <v>1</v>
+      </c>
+      <c r="J59" s="101">
+        <v>1</v>
+      </c>
+      <c r="K59" s="101">
+        <v>1</v>
+      </c>
+      <c r="L59" s="101">
+        <v>0</v>
+      </c>
+      <c r="M59" s="101">
+        <v>1</v>
+      </c>
+      <c r="N59" s="127" t="s">
+        <v>24</v>
+      </c>
+      <c r="O59" s="127"/>
+      <c r="P59" s="127"/>
+      <c r="Q59" s="127"/>
+      <c r="R59" s="127"/>
+      <c r="S59" s="127"/>
+      <c r="T59" s="127"/>
+      <c r="U59" s="128"/>
+      <c r="V59" s="126" t="s">
+        <v>74</v>
+      </c>
+      <c r="W59" s="127"/>
+      <c r="X59" s="127"/>
+      <c r="Y59" s="128"/>
     </row>
     <row r="60" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A60" s="105"/>
-      <c r="B60" s="106"/>
-      <c r="C60" s="103"/>
-      <c r="D60" s="103"/>
-      <c r="E60" s="103"/>
-      <c r="F60" s="103"/>
-      <c r="G60" s="103"/>
-      <c r="H60" s="103"/>
-      <c r="I60" s="103"/>
-      <c r="J60" s="103"/>
-      <c r="K60" s="103"/>
-      <c r="L60" s="103"/>
-      <c r="M60" s="103"/>
-      <c r="N60" s="103"/>
-      <c r="O60" s="103"/>
-      <c r="P60" s="103"/>
-      <c r="Q60" s="103"/>
-      <c r="R60" s="103"/>
-      <c r="S60" s="103"/>
-      <c r="T60" s="103"/>
-      <c r="U60" s="103"/>
-      <c r="V60" s="103"/>
-      <c r="W60" s="103"/>
-      <c r="X60" s="103"/>
-      <c r="Y60" s="103"/>
+      <c r="A60" s="118" t="s">
+        <v>128</v>
+      </c>
+      <c r="B60" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="C60" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="D60" s="19"/>
+      <c r="E60" s="47"/>
+      <c r="F60" s="22">
+        <v>1</v>
+      </c>
+      <c r="G60" s="19">
+        <v>1</v>
+      </c>
+      <c r="H60" s="19">
+        <v>1</v>
+      </c>
+      <c r="I60" s="19">
+        <v>0</v>
+      </c>
+      <c r="J60" s="19">
+        <v>0</v>
+      </c>
+      <c r="K60" s="130" t="s">
+        <v>127</v>
+      </c>
+      <c r="L60" s="131"/>
+      <c r="M60" s="131"/>
+      <c r="N60" s="131"/>
+      <c r="O60" s="131"/>
+      <c r="P60" s="131"/>
+      <c r="Q60" s="131"/>
+      <c r="R60" s="131"/>
+      <c r="S60" s="131"/>
+      <c r="T60" s="131"/>
+      <c r="U60" s="132"/>
+      <c r="V60" s="129"/>
+      <c r="W60" s="112"/>
+      <c r="X60" s="112"/>
+      <c r="Y60" s="130"/>
+      <c r="Z60" s="102"/>
     </row>
-    <row r="61" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B61" s="81"/>
+    <row r="61" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="153"/>
+      <c r="B61" s="104" t="s">
+        <v>126</v>
+      </c>
+      <c r="C61" s="54" t="s">
+        <v>52</v>
+      </c>
+      <c r="D61" s="56"/>
+      <c r="E61" s="57"/>
+      <c r="F61" s="54">
+        <v>1</v>
+      </c>
+      <c r="G61" s="56">
+        <v>1</v>
+      </c>
+      <c r="H61" s="56">
+        <v>1</v>
+      </c>
+      <c r="I61" s="56">
+        <v>0</v>
+      </c>
+      <c r="J61" s="56">
+        <v>0</v>
+      </c>
+      <c r="K61" s="149" t="s">
+        <v>127</v>
+      </c>
+      <c r="L61" s="150"/>
+      <c r="M61" s="150"/>
+      <c r="N61" s="150"/>
+      <c r="O61" s="150"/>
+      <c r="P61" s="150"/>
+      <c r="Q61" s="150"/>
+      <c r="R61" s="150"/>
+      <c r="S61" s="150"/>
+      <c r="T61" s="150"/>
+      <c r="U61" s="151"/>
+      <c r="V61" s="126"/>
+      <c r="W61" s="127"/>
+      <c r="X61" s="127"/>
+      <c r="Y61" s="152"/>
+      <c r="Z61" s="102"/>
     </row>
     <row r="62" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B62" s="81"/>
+      <c r="A62" s="105"/>
+      <c r="B62" s="106"/>
+      <c r="C62" s="103"/>
+      <c r="D62" s="103"/>
+      <c r="E62" s="103"/>
+      <c r="F62" s="103"/>
+      <c r="G62" s="103"/>
+      <c r="H62" s="103"/>
+      <c r="I62" s="103"/>
+      <c r="J62" s="103"/>
+      <c r="K62" s="103"/>
+      <c r="L62" s="103"/>
+      <c r="M62" s="103"/>
+      <c r="N62" s="103"/>
+      <c r="O62" s="103"/>
+      <c r="P62" s="103"/>
+      <c r="Q62" s="103"/>
+      <c r="R62" s="103"/>
+      <c r="S62" s="103"/>
+      <c r="T62" s="103"/>
+      <c r="U62" s="103"/>
+      <c r="V62" s="103"/>
+      <c r="W62" s="103"/>
+      <c r="X62" s="103"/>
+      <c r="Y62" s="103"/>
     </row>
     <row r="63" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B63" s="81"/>
@@ -7065,72 +7395,38 @@
     <row r="70" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B70" s="81"/>
     </row>
+    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B71" s="81"/>
+    </row>
+    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B72" s="81"/>
+    </row>
   </sheetData>
-  <mergeCells count="112">
-    <mergeCell ref="N50:U50"/>
-    <mergeCell ref="N51:U51"/>
-    <mergeCell ref="N42:U42"/>
-    <mergeCell ref="N43:U43"/>
-    <mergeCell ref="N45:U45"/>
-    <mergeCell ref="N47:U47"/>
-    <mergeCell ref="N48:U48"/>
-    <mergeCell ref="O39:U39"/>
-    <mergeCell ref="J40:M40"/>
-    <mergeCell ref="N40:U40"/>
-    <mergeCell ref="J41:M41"/>
-    <mergeCell ref="N41:U41"/>
-    <mergeCell ref="N44:U44"/>
-    <mergeCell ref="N46:U46"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="P33:R33"/>
-    <mergeCell ref="S33:U33"/>
-    <mergeCell ref="K14:M14"/>
-    <mergeCell ref="N14:U14"/>
-    <mergeCell ref="N49:U49"/>
-    <mergeCell ref="O38:U38"/>
-    <mergeCell ref="J37:P37"/>
-    <mergeCell ref="V57:Y57"/>
-    <mergeCell ref="V58:Y58"/>
-    <mergeCell ref="N52:U52"/>
-    <mergeCell ref="N53:U53"/>
-    <mergeCell ref="N54:U54"/>
-    <mergeCell ref="N55:U55"/>
-    <mergeCell ref="N56:U56"/>
-    <mergeCell ref="V52:Y52"/>
-    <mergeCell ref="V53:Y53"/>
-    <mergeCell ref="V54:Y54"/>
-    <mergeCell ref="V55:Y55"/>
-    <mergeCell ref="V56:Y56"/>
-    <mergeCell ref="N57:U57"/>
-    <mergeCell ref="K58:U58"/>
-    <mergeCell ref="P19:R19"/>
-    <mergeCell ref="P20:R20"/>
-    <mergeCell ref="P21:R21"/>
-    <mergeCell ref="P22:R22"/>
-    <mergeCell ref="P23:R23"/>
-    <mergeCell ref="S28:U28"/>
-    <mergeCell ref="S29:U29"/>
-    <mergeCell ref="S30:U30"/>
-    <mergeCell ref="S31:U31"/>
-    <mergeCell ref="P31:R31"/>
-    <mergeCell ref="S19:U19"/>
-    <mergeCell ref="S20:U20"/>
-    <mergeCell ref="S21:U21"/>
-    <mergeCell ref="S22:U22"/>
-    <mergeCell ref="S23:U23"/>
-    <mergeCell ref="S24:U24"/>
-    <mergeCell ref="S25:U25"/>
-    <mergeCell ref="S26:U26"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="K35:M35"/>
-    <mergeCell ref="N35:U35"/>
-    <mergeCell ref="K36:M36"/>
-    <mergeCell ref="N36:U36"/>
-    <mergeCell ref="P28:R28"/>
-    <mergeCell ref="P29:R29"/>
-    <mergeCell ref="P30:R30"/>
+  <mergeCells count="114">
+    <mergeCell ref="K61:U61"/>
+    <mergeCell ref="V61:Y61"/>
+    <mergeCell ref="A60:A61"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:U1"/>
+    <mergeCell ref="K4:O4"/>
+    <mergeCell ref="H3:L3"/>
+    <mergeCell ref="S10:U10"/>
+    <mergeCell ref="K5:O5"/>
+    <mergeCell ref="K6:O6"/>
+    <mergeCell ref="S7:U7"/>
+    <mergeCell ref="P8:R8"/>
+    <mergeCell ref="S8:U8"/>
+    <mergeCell ref="M7:O7"/>
+    <mergeCell ref="M8:O8"/>
+    <mergeCell ref="M9:O9"/>
+    <mergeCell ref="M10:O10"/>
+    <mergeCell ref="S27:U27"/>
+    <mergeCell ref="P25:R25"/>
+    <mergeCell ref="P26:R26"/>
+    <mergeCell ref="P27:R27"/>
+    <mergeCell ref="P24:R24"/>
     <mergeCell ref="V1:Y1"/>
     <mergeCell ref="P16:R16"/>
     <mergeCell ref="S16:U16"/>
@@ -7155,98 +7451,191 @@
     <mergeCell ref="N13:U13"/>
     <mergeCell ref="K12:M12"/>
     <mergeCell ref="N12:U12"/>
-    <mergeCell ref="K59:U59"/>
+    <mergeCell ref="S24:U24"/>
+    <mergeCell ref="S25:U25"/>
+    <mergeCell ref="S26:U26"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="K35:M35"/>
+    <mergeCell ref="N35:U35"/>
+    <mergeCell ref="K36:M36"/>
+    <mergeCell ref="N36:U36"/>
+    <mergeCell ref="P28:R28"/>
+    <mergeCell ref="P29:R29"/>
+    <mergeCell ref="P30:R30"/>
+    <mergeCell ref="K38:M38"/>
+    <mergeCell ref="N38:U38"/>
     <mergeCell ref="V59:Y59"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:U1"/>
-    <mergeCell ref="K4:O4"/>
-    <mergeCell ref="H3:L3"/>
-    <mergeCell ref="S10:U10"/>
-    <mergeCell ref="K5:O5"/>
-    <mergeCell ref="K6:O6"/>
-    <mergeCell ref="S7:U7"/>
-    <mergeCell ref="P8:R8"/>
-    <mergeCell ref="S8:U8"/>
-    <mergeCell ref="M7:O7"/>
-    <mergeCell ref="M8:O8"/>
-    <mergeCell ref="M9:O9"/>
-    <mergeCell ref="M10:O10"/>
-    <mergeCell ref="S27:U27"/>
-    <mergeCell ref="P25:R25"/>
-    <mergeCell ref="P26:R26"/>
-    <mergeCell ref="P27:R27"/>
-    <mergeCell ref="P24:R24"/>
+    <mergeCell ref="V60:Y60"/>
+    <mergeCell ref="N54:U54"/>
+    <mergeCell ref="N55:U55"/>
+    <mergeCell ref="N56:U56"/>
+    <mergeCell ref="N57:U57"/>
+    <mergeCell ref="N58:U58"/>
+    <mergeCell ref="V54:Y54"/>
+    <mergeCell ref="V55:Y55"/>
+    <mergeCell ref="V56:Y56"/>
+    <mergeCell ref="V57:Y57"/>
+    <mergeCell ref="V58:Y58"/>
+    <mergeCell ref="N59:U59"/>
+    <mergeCell ref="K60:U60"/>
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="P33:R33"/>
+    <mergeCell ref="S33:U33"/>
+    <mergeCell ref="K14:M14"/>
+    <mergeCell ref="N14:U14"/>
+    <mergeCell ref="N51:U51"/>
+    <mergeCell ref="O40:U40"/>
+    <mergeCell ref="J39:P39"/>
+    <mergeCell ref="P19:R19"/>
+    <mergeCell ref="P20:R20"/>
+    <mergeCell ref="P21:R21"/>
+    <mergeCell ref="P22:R22"/>
+    <mergeCell ref="P23:R23"/>
+    <mergeCell ref="S28:U28"/>
+    <mergeCell ref="S29:U29"/>
+    <mergeCell ref="S30:U30"/>
+    <mergeCell ref="S31:U31"/>
+    <mergeCell ref="P31:R31"/>
+    <mergeCell ref="S19:U19"/>
+    <mergeCell ref="S20:U20"/>
+    <mergeCell ref="S21:U21"/>
+    <mergeCell ref="S22:U22"/>
+    <mergeCell ref="S23:U23"/>
+    <mergeCell ref="N52:U52"/>
+    <mergeCell ref="N53:U53"/>
+    <mergeCell ref="N44:U44"/>
+    <mergeCell ref="N45:U45"/>
+    <mergeCell ref="N47:U47"/>
+    <mergeCell ref="N49:U49"/>
+    <mergeCell ref="N50:U50"/>
+    <mergeCell ref="O41:U41"/>
+    <mergeCell ref="J42:M42"/>
+    <mergeCell ref="N42:U42"/>
+    <mergeCell ref="J43:M43"/>
+    <mergeCell ref="N43:U43"/>
+    <mergeCell ref="N46:U46"/>
+    <mergeCell ref="N48:U48"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="F58:K59">
-    <cfRule type="cellIs" dxfId="18" priority="1" operator="equal">
+  <conditionalFormatting sqref="F60:K61">
+    <cfRule type="cellIs" dxfId="43" priority="26" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="2" operator="containsText" text="imm">
-      <formula>NOT(ISERROR(SEARCH("imm",F58)))</formula>
+    <cfRule type="containsText" dxfId="42" priority="27" operator="containsText" text="imm">
+      <formula>NOT(ISERROR(SEARCH("imm",F60)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="28" operator="equal">
       <formula>"imm3"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="29" operator="equal">
       <formula>"imm5"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F4:U57">
-    <cfRule type="cellIs" dxfId="14" priority="10" operator="equal">
+  <conditionalFormatting sqref="F4:U59">
+    <cfRule type="cellIs" dxfId="8" priority="35" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:Y40 F41:M41 V41:Y41 F42:Y57 V58:Y59">
-    <cfRule type="containsText" dxfId="13" priority="11" operator="containsText" text="imm">
+  <conditionalFormatting sqref="F43:M43 V43:Y43 F44:Y59 V60:Y61 F1:Y42">
+    <cfRule type="containsText" dxfId="7" priority="36" operator="containsText" text="imm">
       <formula>NOT(ISERROR(SEARCH("imm",F1)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="37" operator="equal">
       <formula>"imm3"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="38" operator="equal">
       <formula>"imm5"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:U31">
-    <cfRule type="cellIs" dxfId="10" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="39" operator="equal">
       <formula>"Rd"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="40" operator="equal">
       <formula>"Rn"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="41" operator="equal">
       <formula>"Rd"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="42" operator="equal">
       <formula>"Rdn"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="43" operator="equal">
       <formula>"Rm"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H33:U33">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="30" operator="equal">
       <formula>"Rd"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="31" operator="equal">
       <formula>"Rn"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="32" operator="equal">
       <formula>"Rd"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="33" operator="equal">
       <formula>"Rdn"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="34" operator="equal">
       <formula>"Rm"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P16:R16">
-    <cfRule type="cellIs" dxfId="0" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="44" operator="equal">
+      <formula>"Rm"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H38:J38">
+    <cfRule type="cellIs" dxfId="28" priority="16" operator="equal">
+      <formula>"Rd"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="27" priority="17" operator="equal">
+      <formula>"Rn"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="18" operator="equal">
+      <formula>"Rd"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="25" priority="19" operator="equal">
+      <formula>"Rdn"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="20" operator="equal">
+      <formula>"Rm"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K38:M38">
+    <cfRule type="cellIs" dxfId="23" priority="6" operator="equal">
+      <formula>"Rd"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="7" operator="equal">
+      <formula>"Rn"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="21" priority="8" operator="equal">
+      <formula>"Rd"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="9" operator="equal">
+      <formula>"Rdn"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="10" operator="equal">
+      <formula>"Rm"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K38:M38">
+    <cfRule type="cellIs" dxfId="18" priority="1" operator="equal">
+      <formula>"Rd"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="17" priority="2" operator="equal">
+      <formula>"Rn"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="3" operator="equal">
+      <formula>"Rd"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="4" operator="equal">
+      <formula>"Rdn"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="5" operator="equal">
       <formula>"Rm"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7256,6 +7645,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010096649AD79A527B47A67D905693C83B0C" ma:contentTypeVersion="7" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="44d09355696640e2dc56270e449341cd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="98b34aae-4bd1-40d2-80e1-46205a35d283" xmlns:ns4="4c17d7eb-fa2b-4fbc-8175-1cef2629d4d8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="73bda8d09c620ff6c543bf34844bea48" ns3:_="" ns4:_="">
     <xsd:import namespace="98b34aae-4bd1-40d2-80e1-46205a35d283"/>
@@ -7440,15 +7838,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -7456,6 +7845,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AAD58D5F-4A46-4F63-A2BD-BBB590555A8D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90060F17-AE26-48CA-A0B9-2F516B758ECF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7470,14 +7867,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AAD58D5F-4A46-4F63-A2BD-BBB590555A8D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Ajout de LDR (register)
</commit_message>
<xml_diff>
--- a/docs/ARM instructions.xlsx
+++ b/docs/ARM instructions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Drive\Etudes\Supérieur\SI3\Architecture et réseaux\Architecture\PARM\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9DF84F9-F3D3-46F3-AB7A-F210C7AD614C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1A3501F-C3B5-43A8-B4AC-65BE24DB06F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1E4904EC-9B68-40DD-B685-7BD66B9DE8BA}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="141">
   <si>
     <t>Description</t>
   </si>
@@ -150,9 +150,6 @@
     <t>Bitwise NOT</t>
   </si>
   <si>
-    <t>Load / Store</t>
-  </si>
-  <si>
     <t>STR</t>
   </si>
   <si>
@@ -1895,6 +1892,12 @@
   </si>
   <si>
     <t>Generate SP-relative address</t>
+  </si>
+  <si>
+    <t>Load / Store Register</t>
+  </si>
+  <si>
+    <t>Load / Store Immediate</t>
   </si>
 </sst>
 </file>
@@ -3098,62 +3101,144 @@
     <xf numFmtId="0" fontId="4" fillId="10" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3165,96 +3250,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="44">
+  <dxfs count="46">
     <dxf>
       <fill>
         <patternFill>
@@ -3316,41 +3319,6 @@
         <b/>
         <i val="0"/>
       </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -3473,6 +3441,20 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
@@ -3537,6 +3519,41 @@
       <fill>
         <patternFill>
           <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3894,10 +3911,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Z72"/>
+  <dimension ref="A1:Z74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" zoomScaleSheetLayoutView="145" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" zoomScaleSheetLayoutView="145" zoomScalePageLayoutView="145" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3910,50 +3927,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="154" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="156" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="142"/>
-      <c r="D1" s="142"/>
-      <c r="E1" s="143"/>
-      <c r="F1" s="142" t="s">
+      <c r="A1" s="125" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="129" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="127"/>
+      <c r="D1" s="127"/>
+      <c r="E1" s="128"/>
+      <c r="F1" s="127" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="142"/>
-      <c r="H1" s="142"/>
-      <c r="I1" s="142"/>
-      <c r="J1" s="142"/>
-      <c r="K1" s="142"/>
-      <c r="L1" s="142"/>
-      <c r="M1" s="142"/>
-      <c r="N1" s="142"/>
-      <c r="O1" s="142"/>
-      <c r="P1" s="142"/>
-      <c r="Q1" s="142"/>
-      <c r="R1" s="142"/>
-      <c r="S1" s="142"/>
-      <c r="T1" s="142"/>
-      <c r="U1" s="143"/>
-      <c r="V1" s="141" t="s">
+      <c r="G1" s="127"/>
+      <c r="H1" s="127"/>
+      <c r="I1" s="127"/>
+      <c r="J1" s="127"/>
+      <c r="K1" s="127"/>
+      <c r="L1" s="127"/>
+      <c r="M1" s="127"/>
+      <c r="N1" s="127"/>
+      <c r="O1" s="127"/>
+      <c r="P1" s="127"/>
+      <c r="Q1" s="127"/>
+      <c r="R1" s="127"/>
+      <c r="S1" s="127"/>
+      <c r="T1" s="127"/>
+      <c r="U1" s="128"/>
+      <c r="V1" s="134" t="s">
         <v>3</v>
       </c>
-      <c r="W1" s="142"/>
-      <c r="X1" s="142"/>
-      <c r="Y1" s="143"/>
+      <c r="W1" s="127"/>
+      <c r="X1" s="127"/>
+      <c r="Y1" s="128"/>
     </row>
     <row r="2" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="155"/>
+      <c r="A2" s="126"/>
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="142" t="s">
+      <c r="C2" s="127" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="142"/>
-      <c r="E2" s="143"/>
+      <c r="D2" s="127"/>
+      <c r="E2" s="128"/>
       <c r="F2" s="2">
         <v>15</v>
       </c>
@@ -4029,13 +4046,13 @@
       <c r="G3" s="10">
         <v>0</v>
       </c>
-      <c r="H3" s="148" t="s">
+      <c r="H3" s="131" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="148"/>
-      <c r="J3" s="148"/>
-      <c r="K3" s="148"/>
-      <c r="L3" s="148"/>
+      <c r="I3" s="131"/>
+      <c r="J3" s="131"/>
+      <c r="K3" s="131"/>
+      <c r="L3" s="131"/>
       <c r="M3" s="11"/>
       <c r="N3" s="11"/>
       <c r="O3" s="11"/>
@@ -4052,10 +4069,10 @@
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="83" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" s="14" t="s">
         <v>75</v>
-      </c>
-      <c r="B4" s="14" t="s">
-        <v>76</v>
       </c>
       <c r="C4" s="15" t="s">
         <v>12</v>
@@ -4081,23 +4098,23 @@
       <c r="J4" s="20">
         <v>0</v>
       </c>
-      <c r="K4" s="112" t="s">
+      <c r="K4" s="130" t="s">
         <v>15</v>
       </c>
-      <c r="L4" s="112"/>
-      <c r="M4" s="112"/>
-      <c r="N4" s="112"/>
-      <c r="O4" s="112"/>
-      <c r="P4" s="122" t="s">
+      <c r="L4" s="130"/>
+      <c r="M4" s="130"/>
+      <c r="N4" s="130"/>
+      <c r="O4" s="130"/>
+      <c r="P4" s="139" t="s">
         <v>16</v>
       </c>
-      <c r="Q4" s="122"/>
-      <c r="R4" s="122"/>
-      <c r="S4" s="112" t="s">
+      <c r="Q4" s="139"/>
+      <c r="R4" s="139"/>
+      <c r="S4" s="130" t="s">
         <v>17</v>
       </c>
-      <c r="T4" s="112"/>
-      <c r="U4" s="113"/>
+      <c r="T4" s="130"/>
+      <c r="U4" s="132"/>
       <c r="V4" s="22" t="s">
         <v>18</v>
       </c>
@@ -4111,10 +4128,10 @@
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="84" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" s="14" t="s">
         <v>77</v>
-      </c>
-      <c r="B5" s="14" t="s">
-        <v>78</v>
       </c>
       <c r="C5" s="23" t="s">
         <v>12</v>
@@ -4140,23 +4157,23 @@
       <c r="J5" s="26">
         <v>1</v>
       </c>
-      <c r="K5" s="112" t="s">
+      <c r="K5" s="130" t="s">
         <v>15</v>
       </c>
-      <c r="L5" s="112"/>
-      <c r="M5" s="112"/>
-      <c r="N5" s="112"/>
-      <c r="O5" s="112"/>
-      <c r="P5" s="112" t="s">
+      <c r="L5" s="130"/>
+      <c r="M5" s="130"/>
+      <c r="N5" s="130"/>
+      <c r="O5" s="130"/>
+      <c r="P5" s="130" t="s">
         <v>16</v>
       </c>
-      <c r="Q5" s="112"/>
-      <c r="R5" s="112"/>
-      <c r="S5" s="112" t="s">
+      <c r="Q5" s="130"/>
+      <c r="R5" s="130"/>
+      <c r="S5" s="130" t="s">
         <v>17</v>
       </c>
-      <c r="T5" s="112"/>
-      <c r="U5" s="113"/>
+      <c r="T5" s="130"/>
+      <c r="U5" s="132"/>
       <c r="V5" s="22" t="s">
         <v>18</v>
       </c>
@@ -4170,10 +4187,10 @@
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="85" t="s">
+        <v>78</v>
+      </c>
+      <c r="B6" s="14" t="s">
         <v>79</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>80</v>
       </c>
       <c r="C6" s="23" t="s">
         <v>12</v>
@@ -4199,23 +4216,23 @@
       <c r="J6" s="20">
         <v>0</v>
       </c>
-      <c r="K6" s="112" t="s">
+      <c r="K6" s="130" t="s">
         <v>15</v>
       </c>
-      <c r="L6" s="112"/>
-      <c r="M6" s="112"/>
-      <c r="N6" s="112"/>
-      <c r="O6" s="112"/>
-      <c r="P6" s="112" t="s">
+      <c r="L6" s="130"/>
+      <c r="M6" s="130"/>
+      <c r="N6" s="130"/>
+      <c r="O6" s="130"/>
+      <c r="P6" s="130" t="s">
         <v>16</v>
       </c>
-      <c r="Q6" s="112"/>
-      <c r="R6" s="112"/>
-      <c r="S6" s="112" t="s">
+      <c r="Q6" s="130"/>
+      <c r="R6" s="130"/>
+      <c r="S6" s="130" t="s">
         <v>17</v>
       </c>
-      <c r="T6" s="112"/>
-      <c r="U6" s="113"/>
+      <c r="T6" s="130"/>
+      <c r="U6" s="132"/>
       <c r="V6" s="22" t="s">
         <v>18</v>
       </c>
@@ -4229,10 +4246,10 @@
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="86" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" s="14" t="s">
         <v>81</v>
-      </c>
-      <c r="B7" s="14" t="s">
-        <v>82</v>
       </c>
       <c r="C7" s="23" t="s">
         <v>12</v>
@@ -4264,21 +4281,21 @@
       <c r="L7" s="31">
         <v>0</v>
       </c>
-      <c r="M7" s="112" t="s">
+      <c r="M7" s="130" t="s">
         <v>16</v>
       </c>
-      <c r="N7" s="112"/>
-      <c r="O7" s="112"/>
-      <c r="P7" s="112" t="s">
+      <c r="N7" s="130"/>
+      <c r="O7" s="130"/>
+      <c r="P7" s="130" t="s">
         <v>20</v>
       </c>
-      <c r="Q7" s="112"/>
-      <c r="R7" s="112"/>
-      <c r="S7" s="112" t="s">
+      <c r="Q7" s="130"/>
+      <c r="R7" s="130"/>
+      <c r="S7" s="130" t="s">
         <v>17</v>
       </c>
-      <c r="T7" s="112"/>
-      <c r="U7" s="113"/>
+      <c r="T7" s="130"/>
+      <c r="U7" s="132"/>
       <c r="V7" s="22" t="s">
         <v>18</v>
       </c>
@@ -4294,10 +4311,10 @@
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" s="84" t="s">
+        <v>82</v>
+      </c>
+      <c r="B8" s="14" t="s">
         <v>83</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>84</v>
       </c>
       <c r="C8" s="23" t="s">
         <v>12</v>
@@ -4329,21 +4346,21 @@
       <c r="L8" s="32">
         <v>1</v>
       </c>
-      <c r="M8" s="112" t="s">
+      <c r="M8" s="130" t="s">
         <v>16</v>
       </c>
-      <c r="N8" s="112"/>
-      <c r="O8" s="112"/>
-      <c r="P8" s="112" t="s">
+      <c r="N8" s="130"/>
+      <c r="O8" s="130"/>
+      <c r="P8" s="130" t="s">
         <v>20</v>
       </c>
-      <c r="Q8" s="112"/>
-      <c r="R8" s="112"/>
-      <c r="S8" s="112" t="s">
+      <c r="Q8" s="130"/>
+      <c r="R8" s="130"/>
+      <c r="S8" s="130" t="s">
         <v>17</v>
       </c>
-      <c r="T8" s="112"/>
-      <c r="U8" s="113"/>
+      <c r="T8" s="130"/>
+      <c r="U8" s="132"/>
       <c r="V8" s="22" t="s">
         <v>18</v>
       </c>
@@ -4359,10 +4376,10 @@
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" s="84" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C9" s="23" t="s">
         <v>12</v>
@@ -4394,21 +4411,21 @@
       <c r="L9" s="31">
         <v>0</v>
       </c>
-      <c r="M9" s="112" t="s">
+      <c r="M9" s="130" t="s">
         <v>22</v>
       </c>
-      <c r="N9" s="112"/>
-      <c r="O9" s="112"/>
-      <c r="P9" s="112" t="s">
+      <c r="N9" s="130"/>
+      <c r="O9" s="130"/>
+      <c r="P9" s="130" t="s">
         <v>20</v>
       </c>
-      <c r="Q9" s="112"/>
-      <c r="R9" s="112"/>
-      <c r="S9" s="112" t="s">
+      <c r="Q9" s="130"/>
+      <c r="R9" s="130"/>
+      <c r="S9" s="130" t="s">
         <v>17</v>
       </c>
-      <c r="T9" s="112"/>
-      <c r="U9" s="113"/>
+      <c r="T9" s="130"/>
+      <c r="U9" s="132"/>
       <c r="V9" s="22" t="s">
         <v>18</v>
       </c>
@@ -4424,10 +4441,10 @@
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" s="85" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B10" s="93" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C10" s="94" t="s">
         <v>12</v>
@@ -4459,21 +4476,21 @@
       <c r="L10" s="32">
         <v>1</v>
       </c>
-      <c r="M10" s="112" t="s">
+      <c r="M10" s="130" t="s">
         <v>22</v>
       </c>
-      <c r="N10" s="112"/>
-      <c r="O10" s="112"/>
-      <c r="P10" s="112" t="s">
+      <c r="N10" s="130"/>
+      <c r="O10" s="130"/>
+      <c r="P10" s="130" t="s">
         <v>20</v>
       </c>
-      <c r="Q10" s="112"/>
-      <c r="R10" s="112"/>
-      <c r="S10" s="112" t="s">
+      <c r="Q10" s="130"/>
+      <c r="R10" s="130"/>
+      <c r="S10" s="130" t="s">
         <v>17</v>
       </c>
-      <c r="T10" s="112"/>
-      <c r="U10" s="113"/>
+      <c r="T10" s="130"/>
+      <c r="U10" s="132"/>
       <c r="V10" s="22" t="s">
         <v>18</v>
       </c>
@@ -4489,10 +4506,10 @@
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" s="84" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B11" s="98" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C11" s="99" t="s">
         <v>12</v>
@@ -4516,21 +4533,21 @@
       <c r="J11" s="31">
         <v>0</v>
       </c>
-      <c r="K11" s="123" t="s">
+      <c r="K11" s="140" t="s">
         <v>17</v>
       </c>
-      <c r="L11" s="123"/>
-      <c r="M11" s="123"/>
-      <c r="N11" s="112" t="s">
+      <c r="L11" s="140"/>
+      <c r="M11" s="140"/>
+      <c r="N11" s="130" t="s">
         <v>24</v>
       </c>
-      <c r="O11" s="112"/>
-      <c r="P11" s="112"/>
-      <c r="Q11" s="112"/>
-      <c r="R11" s="112"/>
-      <c r="S11" s="112"/>
-      <c r="T11" s="112"/>
-      <c r="U11" s="113"/>
+      <c r="O11" s="130"/>
+      <c r="P11" s="130"/>
+      <c r="Q11" s="130"/>
+      <c r="R11" s="130"/>
+      <c r="S11" s="130"/>
+      <c r="T11" s="130"/>
+      <c r="U11" s="132"/>
       <c r="V11" s="22"/>
       <c r="W11" s="19"/>
       <c r="X11" s="19" t="s">
@@ -4542,7 +4559,7 @@
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="84" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B12" s="14" t="s">
         <v>32</v>
@@ -4569,21 +4586,21 @@
       <c r="J12" s="32">
         <v>1</v>
       </c>
-      <c r="K12" s="123" t="s">
+      <c r="K12" s="140" t="s">
         <v>17</v>
       </c>
-      <c r="L12" s="123"/>
-      <c r="M12" s="123"/>
-      <c r="N12" s="112" t="s">
+      <c r="L12" s="140"/>
+      <c r="M12" s="140"/>
+      <c r="N12" s="130" t="s">
         <v>24</v>
       </c>
-      <c r="O12" s="112"/>
-      <c r="P12" s="112"/>
-      <c r="Q12" s="112"/>
-      <c r="R12" s="112"/>
-      <c r="S12" s="112"/>
-      <c r="T12" s="112"/>
-      <c r="U12" s="113"/>
+      <c r="O12" s="130"/>
+      <c r="P12" s="130"/>
+      <c r="Q12" s="130"/>
+      <c r="R12" s="130"/>
+      <c r="S12" s="130"/>
+      <c r="T12" s="130"/>
+      <c r="U12" s="132"/>
       <c r="V12" s="19" t="s">
         <v>18</v>
       </c>
@@ -4599,10 +4616,10 @@
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="84" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C13" s="48" t="s">
         <v>26</v>
@@ -4626,21 +4643,21 @@
       <c r="J13" s="31">
         <v>0</v>
       </c>
-      <c r="K13" s="123" t="s">
+      <c r="K13" s="140" t="s">
         <v>17</v>
       </c>
-      <c r="L13" s="123"/>
-      <c r="M13" s="123"/>
-      <c r="N13" s="112" t="s">
+      <c r="L13" s="140"/>
+      <c r="M13" s="140"/>
+      <c r="N13" s="130" t="s">
         <v>24</v>
       </c>
-      <c r="O13" s="112"/>
-      <c r="P13" s="112"/>
-      <c r="Q13" s="112"/>
-      <c r="R13" s="112"/>
-      <c r="S13" s="112"/>
-      <c r="T13" s="112"/>
-      <c r="U13" s="113"/>
+      <c r="O13" s="130"/>
+      <c r="P13" s="130"/>
+      <c r="Q13" s="130"/>
+      <c r="R13" s="130"/>
+      <c r="S13" s="130"/>
+      <c r="T13" s="130"/>
+      <c r="U13" s="132"/>
       <c r="V13" s="19" t="s">
         <v>18</v>
       </c>
@@ -4656,10 +4673,10 @@
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" s="85" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C14" s="48" t="s">
         <v>26</v>
@@ -4683,21 +4700,21 @@
       <c r="J14" s="31">
         <v>1</v>
       </c>
-      <c r="K14" s="123" t="s">
+      <c r="K14" s="140" t="s">
         <v>17</v>
       </c>
-      <c r="L14" s="123"/>
-      <c r="M14" s="123"/>
-      <c r="N14" s="112" t="s">
+      <c r="L14" s="140"/>
+      <c r="M14" s="140"/>
+      <c r="N14" s="130" t="s">
         <v>24</v>
       </c>
-      <c r="O14" s="112"/>
-      <c r="P14" s="112"/>
-      <c r="Q14" s="112"/>
-      <c r="R14" s="112"/>
-      <c r="S14" s="112"/>
-      <c r="T14" s="112"/>
-      <c r="U14" s="113"/>
+      <c r="O14" s="130"/>
+      <c r="P14" s="130"/>
+      <c r="Q14" s="130"/>
+      <c r="R14" s="130"/>
+      <c r="S14" s="130"/>
+      <c r="T14" s="130"/>
+      <c r="U14" s="132"/>
       <c r="V14" s="19" t="s">
         <v>18</v>
       </c>
@@ -4737,12 +4754,12 @@
       <c r="K15" s="39">
         <v>0</v>
       </c>
-      <c r="L15" s="148" t="s">
+      <c r="L15" s="131" t="s">
         <v>11</v>
       </c>
-      <c r="M15" s="148"/>
-      <c r="N15" s="148"/>
-      <c r="O15" s="148"/>
+      <c r="M15" s="131"/>
+      <c r="N15" s="131"/>
+      <c r="O15" s="131"/>
       <c r="P15" s="36"/>
       <c r="Q15" s="36"/>
       <c r="R15" s="40"/>
@@ -4764,10 +4781,10 @@
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" s="87" t="s">
+        <v>87</v>
+      </c>
+      <c r="B16" s="43" t="s">
         <v>88</v>
-      </c>
-      <c r="B16" s="43" t="s">
-        <v>89</v>
       </c>
       <c r="C16" s="44" t="s">
         <v>26</v>
@@ -4806,16 +4823,16 @@
       <c r="O16" s="20">
         <v>0</v>
       </c>
-      <c r="P16" s="144" t="s">
+      <c r="P16" s="135" t="s">
         <v>16</v>
       </c>
-      <c r="Q16" s="145"/>
-      <c r="R16" s="145"/>
-      <c r="S16" s="146" t="s">
+      <c r="Q16" s="136"/>
+      <c r="R16" s="136"/>
+      <c r="S16" s="137" t="s">
         <v>27</v>
       </c>
-      <c r="T16" s="146"/>
-      <c r="U16" s="147"/>
+      <c r="T16" s="137"/>
+      <c r="U16" s="138"/>
       <c r="V16" s="22" t="s">
         <v>18</v>
       </c>
@@ -4829,10 +4846,10 @@
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17" s="87" t="s">
+        <v>89</v>
+      </c>
+      <c r="B17" s="14" t="s">
         <v>90</v>
-      </c>
-      <c r="B17" s="14" t="s">
-        <v>91</v>
       </c>
       <c r="C17" s="48" t="s">
         <v>26</v>
@@ -4874,13 +4891,13 @@
       <c r="P17" s="133" t="s">
         <v>16</v>
       </c>
-      <c r="Q17" s="112"/>
-      <c r="R17" s="112"/>
-      <c r="S17" s="112" t="s">
+      <c r="Q17" s="130"/>
+      <c r="R17" s="130"/>
+      <c r="S17" s="130" t="s">
         <v>27</v>
       </c>
-      <c r="T17" s="112"/>
-      <c r="U17" s="113"/>
+      <c r="T17" s="130"/>
+      <c r="U17" s="132"/>
       <c r="V17" s="22" t="s">
         <v>18</v>
       </c>
@@ -4894,10 +4911,10 @@
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18" s="87" t="s">
+        <v>74</v>
+      </c>
+      <c r="B18" s="14" t="s">
         <v>75</v>
-      </c>
-      <c r="B18" s="14" t="s">
-        <v>76</v>
       </c>
       <c r="C18" s="48" t="s">
         <v>26</v>
@@ -4939,13 +4956,13 @@
       <c r="P18" s="133" t="s">
         <v>16</v>
       </c>
-      <c r="Q18" s="112"/>
-      <c r="R18" s="112"/>
-      <c r="S18" s="112" t="s">
+      <c r="Q18" s="130"/>
+      <c r="R18" s="130"/>
+      <c r="S18" s="130" t="s">
         <v>27</v>
       </c>
-      <c r="T18" s="112"/>
-      <c r="U18" s="113"/>
+      <c r="T18" s="130"/>
+      <c r="U18" s="132"/>
       <c r="V18" s="22" t="s">
         <v>18</v>
       </c>
@@ -4959,10 +4976,10 @@
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A19" s="87" t="s">
+        <v>76</v>
+      </c>
+      <c r="B19" s="14" t="s">
         <v>77</v>
-      </c>
-      <c r="B19" s="14" t="s">
-        <v>78</v>
       </c>
       <c r="C19" s="48" t="s">
         <v>26</v>
@@ -5004,13 +5021,13 @@
       <c r="P19" s="133" t="s">
         <v>16</v>
       </c>
-      <c r="Q19" s="112"/>
-      <c r="R19" s="112"/>
-      <c r="S19" s="112" t="s">
+      <c r="Q19" s="130"/>
+      <c r="R19" s="130"/>
+      <c r="S19" s="130" t="s">
         <v>27</v>
       </c>
-      <c r="T19" s="112"/>
-      <c r="U19" s="113"/>
+      <c r="T19" s="130"/>
+      <c r="U19" s="132"/>
       <c r="V19" s="22" t="s">
         <v>18</v>
       </c>
@@ -5024,10 +5041,10 @@
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A20" s="87" t="s">
+        <v>78</v>
+      </c>
+      <c r="B20" s="14" t="s">
         <v>79</v>
-      </c>
-      <c r="B20" s="14" t="s">
-        <v>80</v>
       </c>
       <c r="C20" s="48" t="s">
         <v>26</v>
@@ -5069,13 +5086,13 @@
       <c r="P20" s="133" t="s">
         <v>16</v>
       </c>
-      <c r="Q20" s="112"/>
-      <c r="R20" s="112"/>
-      <c r="S20" s="112" t="s">
+      <c r="Q20" s="130"/>
+      <c r="R20" s="130"/>
+      <c r="S20" s="130" t="s">
         <v>27</v>
       </c>
-      <c r="T20" s="112"/>
-      <c r="U20" s="113"/>
+      <c r="T20" s="130"/>
+      <c r="U20" s="132"/>
       <c r="V20" s="22" t="s">
         <v>18</v>
       </c>
@@ -5089,10 +5106,10 @@
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21" s="87" t="s">
+        <v>91</v>
+      </c>
+      <c r="B21" s="14" t="s">
         <v>92</v>
-      </c>
-      <c r="B21" s="14" t="s">
-        <v>93</v>
       </c>
       <c r="C21" s="48" t="s">
         <v>26</v>
@@ -5134,13 +5151,13 @@
       <c r="P21" s="133" t="s">
         <v>16</v>
       </c>
-      <c r="Q21" s="112"/>
-      <c r="R21" s="112"/>
-      <c r="S21" s="112" t="s">
+      <c r="Q21" s="130"/>
+      <c r="R21" s="130"/>
+      <c r="S21" s="130" t="s">
         <v>27</v>
       </c>
-      <c r="T21" s="112"/>
-      <c r="U21" s="113"/>
+      <c r="T21" s="130"/>
+      <c r="U21" s="132"/>
       <c r="V21" s="22" t="s">
         <v>18</v>
       </c>
@@ -5156,10 +5173,10 @@
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A22" s="87" t="s">
+        <v>93</v>
+      </c>
+      <c r="B22" s="14" t="s">
         <v>94</v>
-      </c>
-      <c r="B22" s="14" t="s">
-        <v>95</v>
       </c>
       <c r="C22" s="48" t="s">
         <v>26</v>
@@ -5201,13 +5218,13 @@
       <c r="P22" s="133" t="s">
         <v>16</v>
       </c>
-      <c r="Q22" s="112"/>
-      <c r="R22" s="112"/>
-      <c r="S22" s="112" t="s">
+      <c r="Q22" s="130"/>
+      <c r="R22" s="130"/>
+      <c r="S22" s="130" t="s">
         <v>27</v>
       </c>
-      <c r="T22" s="112"/>
-      <c r="U22" s="113"/>
+      <c r="T22" s="130"/>
+      <c r="U22" s="132"/>
       <c r="V22" s="22" t="s">
         <v>18</v>
       </c>
@@ -5223,10 +5240,10 @@
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" s="87" t="s">
+        <v>95</v>
+      </c>
+      <c r="B23" s="14" t="s">
         <v>96</v>
-      </c>
-      <c r="B23" s="14" t="s">
-        <v>97</v>
       </c>
       <c r="C23" s="48" t="s">
         <v>26</v>
@@ -5268,13 +5285,13 @@
       <c r="P23" s="133" t="s">
         <v>16</v>
       </c>
-      <c r="Q23" s="112"/>
-      <c r="R23" s="112"/>
-      <c r="S23" s="112" t="s">
+      <c r="Q23" s="130"/>
+      <c r="R23" s="130"/>
+      <c r="S23" s="130" t="s">
         <v>27</v>
       </c>
-      <c r="T23" s="112"/>
-      <c r="U23" s="113"/>
+      <c r="T23" s="130"/>
+      <c r="U23" s="132"/>
       <c r="V23" s="22" t="s">
         <v>18</v>
       </c>
@@ -5333,13 +5350,13 @@
       <c r="P24" s="133" t="s">
         <v>16</v>
       </c>
-      <c r="Q24" s="112"/>
-      <c r="R24" s="112"/>
-      <c r="S24" s="112" t="s">
+      <c r="Q24" s="130"/>
+      <c r="R24" s="130"/>
+      <c r="S24" s="130" t="s">
         <v>20</v>
       </c>
-      <c r="T24" s="112"/>
-      <c r="U24" s="113"/>
+      <c r="T24" s="130"/>
+      <c r="U24" s="132"/>
       <c r="V24" s="22" t="s">
         <v>18</v>
       </c>
@@ -5353,10 +5370,10 @@
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25" s="87" t="s">
+        <v>97</v>
+      </c>
+      <c r="B25" s="14" t="s">
         <v>98</v>
-      </c>
-      <c r="B25" s="14" t="s">
-        <v>99</v>
       </c>
       <c r="C25" s="23" t="s">
         <v>12</v>
@@ -5400,13 +5417,13 @@
       <c r="P25" s="133" t="s">
         <v>20</v>
       </c>
-      <c r="Q25" s="112"/>
-      <c r="R25" s="112"/>
-      <c r="S25" s="112" t="s">
+      <c r="Q25" s="130"/>
+      <c r="R25" s="130"/>
+      <c r="S25" s="130" t="s">
         <v>17</v>
       </c>
-      <c r="T25" s="112"/>
-      <c r="U25" s="113"/>
+      <c r="T25" s="130"/>
+      <c r="U25" s="132"/>
       <c r="V25" s="22" t="s">
         <v>18</v>
       </c>
@@ -5467,13 +5484,13 @@
       <c r="P26" s="133" t="s">
         <v>16</v>
       </c>
-      <c r="Q26" s="112"/>
-      <c r="R26" s="112"/>
-      <c r="S26" s="112" t="s">
+      <c r="Q26" s="130"/>
+      <c r="R26" s="130"/>
+      <c r="S26" s="130" t="s">
         <v>20</v>
       </c>
-      <c r="T26" s="112"/>
-      <c r="U26" s="113"/>
+      <c r="T26" s="130"/>
+      <c r="U26" s="132"/>
       <c r="V26" s="22" t="s">
         <v>18</v>
       </c>
@@ -5534,13 +5551,13 @@
       <c r="P27" s="133" t="s">
         <v>16</v>
       </c>
-      <c r="Q27" s="112"/>
-      <c r="R27" s="112"/>
-      <c r="S27" s="112" t="s">
+      <c r="Q27" s="130"/>
+      <c r="R27" s="130"/>
+      <c r="S27" s="130" t="s">
         <v>20</v>
       </c>
-      <c r="T27" s="112"/>
-      <c r="U27" s="113"/>
+      <c r="T27" s="130"/>
+      <c r="U27" s="132"/>
       <c r="V27" s="22" t="s">
         <v>18</v>
       </c>
@@ -5556,10 +5573,10 @@
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A28" s="87" t="s">
+        <v>99</v>
+      </c>
+      <c r="B28" s="14" t="s">
         <v>100</v>
-      </c>
-      <c r="B28" s="14" t="s">
-        <v>101</v>
       </c>
       <c r="C28" s="48" t="s">
         <v>26</v>
@@ -5601,13 +5618,13 @@
       <c r="P28" s="133" t="s">
         <v>16</v>
       </c>
-      <c r="Q28" s="112"/>
-      <c r="R28" s="112"/>
-      <c r="S28" s="112" t="s">
+      <c r="Q28" s="130"/>
+      <c r="R28" s="130"/>
+      <c r="S28" s="130" t="s">
         <v>27</v>
       </c>
-      <c r="T28" s="112"/>
-      <c r="U28" s="113"/>
+      <c r="T28" s="130"/>
+      <c r="U28" s="132"/>
       <c r="V28" s="22" t="s">
         <v>18</v>
       </c>
@@ -5621,10 +5638,10 @@
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A29" s="87" t="s">
+        <v>101</v>
+      </c>
+      <c r="B29" s="14" t="s">
         <v>102</v>
-      </c>
-      <c r="B29" s="14" t="s">
-        <v>103</v>
       </c>
       <c r="C29" s="51" t="s">
         <v>35</v>
@@ -5668,13 +5685,13 @@
       <c r="P29" s="133" t="s">
         <v>20</v>
       </c>
-      <c r="Q29" s="112"/>
-      <c r="R29" s="112"/>
-      <c r="S29" s="134" t="s">
+      <c r="Q29" s="130"/>
+      <c r="R29" s="130"/>
+      <c r="S29" s="162" t="s">
         <v>36</v>
       </c>
-      <c r="T29" s="134"/>
-      <c r="U29" s="135"/>
+      <c r="T29" s="162"/>
+      <c r="U29" s="163"/>
       <c r="V29" s="22"/>
       <c r="W29" s="19"/>
       <c r="X29" s="19" t="s">
@@ -5686,10 +5703,10 @@
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A30" s="87" t="s">
+        <v>103</v>
+      </c>
+      <c r="B30" s="14" t="s">
         <v>104</v>
-      </c>
-      <c r="B30" s="14" t="s">
-        <v>105</v>
       </c>
       <c r="C30" s="48" t="s">
         <v>26</v>
@@ -5731,13 +5748,13 @@
       <c r="P30" s="133" t="s">
         <v>16</v>
       </c>
-      <c r="Q30" s="112"/>
-      <c r="R30" s="112"/>
-      <c r="S30" s="112" t="s">
+      <c r="Q30" s="130"/>
+      <c r="R30" s="130"/>
+      <c r="S30" s="130" t="s">
         <v>27</v>
       </c>
-      <c r="T30" s="112"/>
-      <c r="U30" s="113"/>
+      <c r="T30" s="130"/>
+      <c r="U30" s="132"/>
       <c r="V30" s="22" t="s">
         <v>18</v>
       </c>
@@ -5754,7 +5771,7 @@
         <v>37</v>
       </c>
       <c r="B31" s="33" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C31" s="34" t="s">
         <v>12</v>
@@ -5793,16 +5810,16 @@
       <c r="O31" s="58">
         <v>1</v>
       </c>
-      <c r="P31" s="136" t="s">
+      <c r="P31" s="164" t="s">
         <v>16</v>
       </c>
-      <c r="Q31" s="127"/>
-      <c r="R31" s="127"/>
-      <c r="S31" s="127" t="s">
+      <c r="Q31" s="121"/>
+      <c r="R31" s="121"/>
+      <c r="S31" s="121" t="s">
         <v>17</v>
       </c>
-      <c r="T31" s="127"/>
-      <c r="U31" s="128"/>
+      <c r="T31" s="121"/>
+      <c r="U31" s="150"/>
       <c r="V31" s="22" t="s">
         <v>18</v>
       </c>
@@ -5816,26 +5833,30 @@
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A32" s="82" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B32" s="36"/>
       <c r="C32" s="36"/>
       <c r="D32" s="36"/>
       <c r="E32" s="36"/>
       <c r="F32" s="36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G32" s="36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H32" s="36">
         <v>0</v>
       </c>
       <c r="I32" s="36">
-        <v>1</v>
-      </c>
-      <c r="J32" s="36"/>
-      <c r="K32" s="36"/>
+        <v>0</v>
+      </c>
+      <c r="J32" s="36">
+        <v>0</v>
+      </c>
+      <c r="K32" s="36">
+        <v>1</v>
+      </c>
       <c r="L32" s="36"/>
       <c r="M32" s="36"/>
       <c r="N32" s="36"/>
@@ -5861,10 +5882,10 @@
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A33" s="84" t="s">
-        <v>133</v>
-      </c>
-      <c r="B33" s="162" t="s">
-        <v>87</v>
+        <v>132</v>
+      </c>
+      <c r="B33" s="113" t="s">
+        <v>86</v>
       </c>
       <c r="C33" s="99" t="s">
         <v>12</v>
@@ -5897,10 +5918,10 @@
       <c r="M33" s="97">
         <v>0</v>
       </c>
-      <c r="N33" s="157">
-        <v>0</v>
-      </c>
-      <c r="O33" s="157">
+      <c r="N33" s="112">
+        <v>0</v>
+      </c>
+      <c r="O33" s="112">
         <v>0</v>
       </c>
       <c r="P33" s="158" t="s">
@@ -5926,17 +5947,17 @@
     </row>
     <row r="34" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="82" t="s">
-        <v>38</v>
+        <v>139</v>
       </c>
       <c r="B34" s="36"/>
       <c r="C34" s="36"/>
       <c r="D34" s="36"/>
       <c r="E34" s="36"/>
       <c r="F34" s="36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G34" s="36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H34" s="36">
         <v>0</v>
@@ -5973,201 +5994,205 @@
       <c r="A35" s="89" t="s">
         <v>107</v>
       </c>
-      <c r="B35" s="43" t="s">
+      <c r="B35" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="C35" s="65" t="s">
         <v>39</v>
       </c>
-      <c r="C35" s="60" t="s">
+      <c r="D35" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="E35" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="F35" s="68">
+        <v>0</v>
+      </c>
+      <c r="G35" s="68">
+        <v>1</v>
+      </c>
+      <c r="H35" s="68">
+        <v>0</v>
+      </c>
+      <c r="I35" s="69">
+        <v>1</v>
+      </c>
+      <c r="J35" s="70">
+        <v>1</v>
+      </c>
+      <c r="K35" s="75">
+        <v>0</v>
+      </c>
+      <c r="L35" s="75">
+        <v>0</v>
+      </c>
+      <c r="M35" s="158" t="s">
+        <v>16</v>
+      </c>
+      <c r="N35" s="158"/>
+      <c r="O35" s="158"/>
+      <c r="P35" s="130" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q35" s="130"/>
+      <c r="R35" s="132"/>
+      <c r="S35" s="143" t="s">
         <v>40</v>
       </c>
-      <c r="D35" s="137" t="s">
-        <v>43</v>
-      </c>
-      <c r="E35" s="138"/>
-      <c r="F35" s="61">
-        <v>1</v>
-      </c>
-      <c r="G35" s="62">
-        <v>0</v>
-      </c>
-      <c r="H35" s="62">
-        <v>0</v>
-      </c>
-      <c r="I35" s="63">
-        <v>1</v>
-      </c>
-      <c r="J35" s="64">
-        <v>0</v>
-      </c>
-      <c r="K35" s="139" t="s">
-        <v>41</v>
-      </c>
-      <c r="L35" s="139"/>
-      <c r="M35" s="139"/>
-      <c r="N35" s="124" t="s">
-        <v>24</v>
-      </c>
-      <c r="O35" s="124"/>
-      <c r="P35" s="124"/>
-      <c r="Q35" s="124"/>
-      <c r="R35" s="124"/>
-      <c r="S35" s="124"/>
-      <c r="T35" s="124"/>
-      <c r="U35" s="125"/>
+      <c r="T35" s="143"/>
+      <c r="U35" s="143"/>
       <c r="V35" s="22"/>
       <c r="W35" s="19"/>
       <c r="X35" s="19"/>
       <c r="Y35" s="21"/>
     </row>
     <row r="36" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="89" t="s">
-        <v>108</v>
-      </c>
-      <c r="B36" s="33" t="s">
-        <v>42</v>
-      </c>
-      <c r="C36" s="65" t="s">
-        <v>40</v>
-      </c>
-      <c r="D36" s="137" t="s">
-        <v>43</v>
-      </c>
-      <c r="E36" s="138"/>
-      <c r="F36" s="67">
-        <v>1</v>
-      </c>
-      <c r="G36" s="68">
-        <v>0</v>
-      </c>
-      <c r="H36" s="68">
-        <v>0</v>
-      </c>
-      <c r="I36" s="69">
-        <v>1</v>
-      </c>
-      <c r="J36" s="70">
-        <v>1</v>
-      </c>
-      <c r="K36" s="140" t="s">
-        <v>41</v>
-      </c>
-      <c r="L36" s="140"/>
-      <c r="M36" s="140"/>
-      <c r="N36" s="114" t="s">
-        <v>24</v>
-      </c>
-      <c r="O36" s="114"/>
-      <c r="P36" s="114"/>
-      <c r="Q36" s="114"/>
-      <c r="R36" s="114"/>
-      <c r="S36" s="114"/>
-      <c r="T36" s="114"/>
-      <c r="U36" s="115"/>
-      <c r="V36" s="22"/>
-      <c r="W36" s="19"/>
-      <c r="X36" s="19"/>
-      <c r="Y36" s="21"/>
+      <c r="A36" s="82" t="s">
+        <v>140</v>
+      </c>
+      <c r="B36" s="36"/>
+      <c r="C36" s="36"/>
+      <c r="D36" s="36"/>
+      <c r="E36" s="36"/>
+      <c r="F36" s="36">
+        <v>1</v>
+      </c>
+      <c r="G36" s="36">
+        <v>0</v>
+      </c>
+      <c r="H36" s="36">
+        <v>0</v>
+      </c>
+      <c r="I36" s="36">
+        <v>1</v>
+      </c>
+      <c r="J36" s="36"/>
+      <c r="K36" s="36"/>
+      <c r="L36" s="36"/>
+      <c r="M36" s="36"/>
+      <c r="N36" s="36"/>
+      <c r="O36" s="36"/>
+      <c r="P36" s="36"/>
+      <c r="Q36" s="36"/>
+      <c r="R36" s="36"/>
+      <c r="S36" s="36"/>
+      <c r="T36" s="36"/>
+      <c r="U36" s="37"/>
+      <c r="V36" s="42" t="s">
+        <v>6</v>
+      </c>
+      <c r="W36" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="X36" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y36" s="37" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="37" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="82" t="s">
-        <v>139</v>
-      </c>
-      <c r="B37" s="36"/>
-      <c r="C37" s="36"/>
-      <c r="D37" s="36"/>
-      <c r="E37" s="36"/>
-      <c r="F37" s="36">
-        <v>1</v>
-      </c>
-      <c r="G37" s="36">
-        <v>0</v>
-      </c>
-      <c r="H37" s="36">
-        <v>1</v>
-      </c>
-      <c r="I37" s="36">
-        <v>0</v>
-      </c>
-      <c r="J37" s="36">
-        <v>1</v>
-      </c>
-      <c r="K37" s="163"/>
-      <c r="L37" s="163"/>
-      <c r="M37" s="163"/>
-      <c r="N37" s="163"/>
-      <c r="O37" s="163"/>
-      <c r="P37" s="163"/>
-      <c r="Q37" s="36"/>
-      <c r="R37" s="36"/>
-      <c r="S37" s="36"/>
-      <c r="T37" s="36"/>
-      <c r="U37" s="37"/>
-      <c r="V37" s="42" t="s">
-        <v>6</v>
-      </c>
-      <c r="W37" s="36" t="s">
-        <v>7</v>
-      </c>
-      <c r="X37" s="36" t="s">
-        <v>8</v>
-      </c>
-      <c r="Y37" s="37" t="s">
-        <v>9</v>
-      </c>
+      <c r="A37" s="89" t="s">
+        <v>106</v>
+      </c>
+      <c r="B37" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="C37" s="60" t="s">
+        <v>39</v>
+      </c>
+      <c r="D37" s="141" t="s">
+        <v>42</v>
+      </c>
+      <c r="E37" s="142"/>
+      <c r="F37" s="61">
+        <v>1</v>
+      </c>
+      <c r="G37" s="62">
+        <v>0</v>
+      </c>
+      <c r="H37" s="62">
+        <v>0</v>
+      </c>
+      <c r="I37" s="63">
+        <v>1</v>
+      </c>
+      <c r="J37" s="64">
+        <v>0</v>
+      </c>
+      <c r="K37" s="143" t="s">
+        <v>40</v>
+      </c>
+      <c r="L37" s="143"/>
+      <c r="M37" s="143"/>
+      <c r="N37" s="144" t="s">
+        <v>24</v>
+      </c>
+      <c r="O37" s="144"/>
+      <c r="P37" s="144"/>
+      <c r="Q37" s="144"/>
+      <c r="R37" s="144"/>
+      <c r="S37" s="144"/>
+      <c r="T37" s="144"/>
+      <c r="U37" s="145"/>
+      <c r="V37" s="22"/>
+      <c r="W37" s="19"/>
+      <c r="X37" s="19"/>
+      <c r="Y37" s="21"/>
     </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A38" s="165" t="s">
-        <v>138</v>
-      </c>
-      <c r="B38" s="43" t="s">
-        <v>45</v>
-      </c>
-      <c r="C38" s="99" t="s">
-        <v>12</v>
-      </c>
-      <c r="D38" s="71" t="s">
-        <v>46</v>
-      </c>
-      <c r="E38" s="97" t="s">
-        <v>23</v>
-      </c>
-      <c r="F38" s="54">
-        <v>1</v>
-      </c>
-      <c r="G38" s="56">
-        <v>0</v>
-      </c>
-      <c r="H38" s="56">
-        <v>1</v>
-      </c>
-      <c r="I38" s="56">
-        <v>0</v>
-      </c>
-      <c r="J38" s="164">
-        <v>1</v>
-      </c>
-      <c r="K38" s="127" t="s">
-        <v>17</v>
-      </c>
-      <c r="L38" s="127"/>
-      <c r="M38" s="127"/>
-      <c r="N38" s="161" t="s">
+    <row r="38" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="89" t="s">
+        <v>107</v>
+      </c>
+      <c r="B38" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="C38" s="65" t="s">
+        <v>39</v>
+      </c>
+      <c r="D38" s="141" t="s">
+        <v>42</v>
+      </c>
+      <c r="E38" s="142"/>
+      <c r="F38" s="67">
+        <v>1</v>
+      </c>
+      <c r="G38" s="68">
+        <v>0</v>
+      </c>
+      <c r="H38" s="68">
+        <v>0</v>
+      </c>
+      <c r="I38" s="69">
+        <v>1</v>
+      </c>
+      <c r="J38" s="70">
+        <v>1</v>
+      </c>
+      <c r="K38" s="146" t="s">
+        <v>40</v>
+      </c>
+      <c r="L38" s="146"/>
+      <c r="M38" s="146"/>
+      <c r="N38" s="147" t="s">
         <v>24</v>
       </c>
-      <c r="O38" s="124"/>
-      <c r="P38" s="124"/>
-      <c r="Q38" s="124"/>
-      <c r="R38" s="124"/>
-      <c r="S38" s="124"/>
-      <c r="T38" s="124"/>
-      <c r="U38" s="125"/>
-      <c r="V38" s="18"/>
+      <c r="O38" s="147"/>
+      <c r="P38" s="147"/>
+      <c r="Q38" s="147"/>
+      <c r="R38" s="147"/>
+      <c r="S38" s="147"/>
+      <c r="T38" s="147"/>
+      <c r="U38" s="148"/>
+      <c r="V38" s="22"/>
       <c r="W38" s="19"/>
       <c r="X38" s="19"/>
       <c r="Y38" s="21"/>
     </row>
     <row r="39" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="82" t="s">
-        <v>44</v>
+        <v>138</v>
       </c>
       <c r="B39" s="36"/>
       <c r="C39" s="36"/>
@@ -6183,17 +6208,17 @@
         <v>1</v>
       </c>
       <c r="I39" s="36">
-        <v>1</v>
-      </c>
-      <c r="J39" s="116" t="s">
-        <v>11</v>
-      </c>
-      <c r="K39" s="116"/>
-      <c r="L39" s="116"/>
-      <c r="M39" s="116"/>
-      <c r="N39" s="116"/>
-      <c r="O39" s="116"/>
-      <c r="P39" s="116"/>
+        <v>0</v>
+      </c>
+      <c r="J39" s="36">
+        <v>1</v>
+      </c>
+      <c r="K39" s="114"/>
+      <c r="L39" s="114"/>
+      <c r="M39" s="114"/>
+      <c r="N39" s="114"/>
+      <c r="O39" s="114"/>
+      <c r="P39" s="114"/>
       <c r="Q39" s="36"/>
       <c r="R39" s="36"/>
       <c r="S39" s="36"/>
@@ -6213,321 +6238,313 @@
       </c>
     </row>
     <row r="40" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A40" s="90" t="s">
-        <v>109</v>
+      <c r="A40" s="116" t="s">
+        <v>137</v>
       </c>
       <c r="B40" s="43" t="s">
+        <v>44</v>
+      </c>
+      <c r="C40" s="99" t="s">
+        <v>12</v>
+      </c>
+      <c r="D40" s="71" t="s">
         <v>45</v>
       </c>
-      <c r="C40" s="71" t="s">
-        <v>46</v>
-      </c>
-      <c r="D40" s="62" t="s">
-        <v>129</v>
-      </c>
-      <c r="E40" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="F40" s="72">
-        <v>1</v>
-      </c>
-      <c r="G40" s="62">
-        <v>0</v>
-      </c>
-      <c r="H40" s="62">
-        <v>1</v>
-      </c>
-      <c r="I40" s="62">
-        <v>1</v>
-      </c>
-      <c r="J40" s="64">
-        <v>0</v>
-      </c>
-      <c r="K40" s="64">
-        <v>0</v>
-      </c>
-      <c r="L40" s="64">
-        <v>0</v>
-      </c>
-      <c r="M40" s="64">
-        <v>0</v>
-      </c>
-      <c r="N40" s="64">
-        <v>0</v>
-      </c>
-      <c r="O40" s="124" t="s">
-        <v>48</v>
-      </c>
-      <c r="P40" s="124"/>
-      <c r="Q40" s="124"/>
-      <c r="R40" s="124"/>
-      <c r="S40" s="124"/>
-      <c r="T40" s="124"/>
-      <c r="U40" s="125"/>
-      <c r="V40" s="22"/>
+      <c r="E40" s="97" t="s">
+        <v>23</v>
+      </c>
+      <c r="F40" s="54">
+        <v>1</v>
+      </c>
+      <c r="G40" s="56">
+        <v>0</v>
+      </c>
+      <c r="H40" s="56">
+        <v>1</v>
+      </c>
+      <c r="I40" s="56">
+        <v>0</v>
+      </c>
+      <c r="J40" s="115">
+        <v>1</v>
+      </c>
+      <c r="K40" s="121" t="s">
+        <v>17</v>
+      </c>
+      <c r="L40" s="121"/>
+      <c r="M40" s="121"/>
+      <c r="N40" s="149" t="s">
+        <v>24</v>
+      </c>
+      <c r="O40" s="144"/>
+      <c r="P40" s="144"/>
+      <c r="Q40" s="144"/>
+      <c r="R40" s="144"/>
+      <c r="S40" s="144"/>
+      <c r="T40" s="144"/>
+      <c r="U40" s="145"/>
+      <c r="V40" s="18"/>
       <c r="W40" s="19"/>
       <c r="X40" s="19"/>
       <c r="Y40" s="21"/>
     </row>
     <row r="41" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="90" t="s">
-        <v>110</v>
-      </c>
-      <c r="B41" s="33" t="s">
-        <v>49</v>
-      </c>
-      <c r="C41" s="73" t="s">
-        <v>46</v>
-      </c>
-      <c r="D41" s="68" t="s">
-        <v>129</v>
-      </c>
-      <c r="E41" s="66" t="s">
-        <v>47</v>
-      </c>
-      <c r="F41" s="74">
-        <v>1</v>
-      </c>
-      <c r="G41" s="68">
-        <v>0</v>
-      </c>
-      <c r="H41" s="68">
-        <v>1</v>
-      </c>
-      <c r="I41" s="68">
-        <v>1</v>
-      </c>
-      <c r="J41" s="75">
-        <v>0</v>
-      </c>
-      <c r="K41" s="75">
-        <v>0</v>
-      </c>
-      <c r="L41" s="75">
-        <v>0</v>
-      </c>
-      <c r="M41" s="75">
-        <v>0</v>
-      </c>
-      <c r="N41" s="75">
-        <v>1</v>
-      </c>
-      <c r="O41" s="114" t="s">
-        <v>48</v>
-      </c>
-      <c r="P41" s="114"/>
-      <c r="Q41" s="114"/>
-      <c r="R41" s="114"/>
-      <c r="S41" s="114"/>
-      <c r="T41" s="114"/>
-      <c r="U41" s="115"/>
-      <c r="V41" s="22"/>
-      <c r="W41" s="19"/>
-      <c r="X41" s="19"/>
-      <c r="Y41" s="21"/>
+      <c r="A41" s="82" t="s">
+        <v>43</v>
+      </c>
+      <c r="B41" s="36"/>
+      <c r="C41" s="36"/>
+      <c r="D41" s="36"/>
+      <c r="E41" s="36"/>
+      <c r="F41" s="36">
+        <v>1</v>
+      </c>
+      <c r="G41" s="36">
+        <v>0</v>
+      </c>
+      <c r="H41" s="36">
+        <v>1</v>
+      </c>
+      <c r="I41" s="36">
+        <v>1</v>
+      </c>
+      <c r="J41" s="161" t="s">
+        <v>11</v>
+      </c>
+      <c r="K41" s="161"/>
+      <c r="L41" s="161"/>
+      <c r="M41" s="161"/>
+      <c r="N41" s="161"/>
+      <c r="O41" s="161"/>
+      <c r="P41" s="161"/>
+      <c r="Q41" s="36"/>
+      <c r="R41" s="36"/>
+      <c r="S41" s="36"/>
+      <c r="T41" s="36"/>
+      <c r="U41" s="37"/>
+      <c r="V41" s="42" t="s">
+        <v>6</v>
+      </c>
+      <c r="W41" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="X41" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y41" s="37" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="42" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A42" s="82" t="s">
-        <v>50</v>
-      </c>
-      <c r="B42" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="C42" s="36" t="s">
-        <v>52</v>
-      </c>
-      <c r="D42" s="36"/>
-      <c r="E42" s="36"/>
-      <c r="F42" s="36">
-        <v>1</v>
-      </c>
-      <c r="G42" s="36">
-        <v>1</v>
-      </c>
-      <c r="H42" s="36">
-        <v>0</v>
-      </c>
-      <c r="I42" s="36">
-        <v>1</v>
-      </c>
-      <c r="J42" s="116" t="s">
-        <v>11</v>
-      </c>
-      <c r="K42" s="116"/>
-      <c r="L42" s="116"/>
-      <c r="M42" s="116"/>
-      <c r="N42" s="116"/>
-      <c r="O42" s="116"/>
-      <c r="P42" s="116"/>
-      <c r="Q42" s="116"/>
-      <c r="R42" s="116"/>
-      <c r="S42" s="116"/>
-      <c r="T42" s="116"/>
-      <c r="U42" s="117"/>
-      <c r="V42" s="42"/>
-      <c r="W42" s="36"/>
-      <c r="X42" s="36"/>
-      <c r="Y42" s="37"/>
+      <c r="A42" s="90" t="s">
+        <v>108</v>
+      </c>
+      <c r="B42" s="43" t="s">
+        <v>44</v>
+      </c>
+      <c r="C42" s="71" t="s">
+        <v>45</v>
+      </c>
+      <c r="D42" s="62" t="s">
+        <v>128</v>
+      </c>
+      <c r="E42" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="F42" s="72">
+        <v>1</v>
+      </c>
+      <c r="G42" s="62">
+        <v>0</v>
+      </c>
+      <c r="H42" s="62">
+        <v>1</v>
+      </c>
+      <c r="I42" s="62">
+        <v>1</v>
+      </c>
+      <c r="J42" s="64">
+        <v>0</v>
+      </c>
+      <c r="K42" s="64">
+        <v>0</v>
+      </c>
+      <c r="L42" s="64">
+        <v>0</v>
+      </c>
+      <c r="M42" s="64">
+        <v>0</v>
+      </c>
+      <c r="N42" s="64">
+        <v>0</v>
+      </c>
+      <c r="O42" s="144" t="s">
+        <v>47</v>
+      </c>
+      <c r="P42" s="144"/>
+      <c r="Q42" s="144"/>
+      <c r="R42" s="144"/>
+      <c r="S42" s="144"/>
+      <c r="T42" s="144"/>
+      <c r="U42" s="145"/>
+      <c r="V42" s="22"/>
+      <c r="W42" s="19"/>
+      <c r="X42" s="19"/>
+      <c r="Y42" s="21"/>
     </row>
     <row r="43" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="82"/>
-      <c r="B43" s="36" t="s">
-        <v>53</v>
-      </c>
-      <c r="C43" s="36"/>
-      <c r="D43" s="36"/>
-      <c r="E43" s="36"/>
-      <c r="F43" s="36"/>
-      <c r="G43" s="36"/>
-      <c r="H43" s="36"/>
-      <c r="I43" s="36"/>
-      <c r="J43" s="116" t="s">
-        <v>54</v>
-      </c>
-      <c r="K43" s="116"/>
-      <c r="L43" s="116"/>
-      <c r="M43" s="116"/>
-      <c r="N43" s="116" t="s">
-        <v>24</v>
-      </c>
-      <c r="O43" s="116"/>
-      <c r="P43" s="116"/>
-      <c r="Q43" s="116"/>
-      <c r="R43" s="116"/>
-      <c r="S43" s="116"/>
-      <c r="T43" s="116"/>
-      <c r="U43" s="117"/>
-      <c r="V43" s="42" t="s">
-        <v>6</v>
-      </c>
-      <c r="W43" s="36" t="s">
-        <v>7</v>
-      </c>
-      <c r="X43" s="36" t="s">
-        <v>8</v>
-      </c>
-      <c r="Y43" s="37" t="s">
-        <v>9</v>
-      </c>
+      <c r="A43" s="90" t="s">
+        <v>109</v>
+      </c>
+      <c r="B43" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="C43" s="73" t="s">
+        <v>45</v>
+      </c>
+      <c r="D43" s="68" t="s">
+        <v>128</v>
+      </c>
+      <c r="E43" s="66" t="s">
+        <v>46</v>
+      </c>
+      <c r="F43" s="74">
+        <v>1</v>
+      </c>
+      <c r="G43" s="68">
+        <v>0</v>
+      </c>
+      <c r="H43" s="68">
+        <v>1</v>
+      </c>
+      <c r="I43" s="68">
+        <v>1</v>
+      </c>
+      <c r="J43" s="75">
+        <v>0</v>
+      </c>
+      <c r="K43" s="75">
+        <v>0</v>
+      </c>
+      <c r="L43" s="75">
+        <v>0</v>
+      </c>
+      <c r="M43" s="75">
+        <v>0</v>
+      </c>
+      <c r="N43" s="75">
+        <v>1</v>
+      </c>
+      <c r="O43" s="147" t="s">
+        <v>47</v>
+      </c>
+      <c r="P43" s="147"/>
+      <c r="Q43" s="147"/>
+      <c r="R43" s="147"/>
+      <c r="S43" s="147"/>
+      <c r="T43" s="147"/>
+      <c r="U43" s="148"/>
+      <c r="V43" s="22"/>
+      <c r="W43" s="19"/>
+      <c r="X43" s="19"/>
+      <c r="Y43" s="21"/>
     </row>
     <row r="44" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A44" s="108" t="s">
-        <v>111</v>
-      </c>
-      <c r="B44" s="76" t="s">
-        <v>55</v>
-      </c>
-      <c r="C44" s="71" t="s">
+      <c r="A44" s="82" t="s">
+        <v>49</v>
+      </c>
+      <c r="B44" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="C44" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="D44" s="36"/>
+      <c r="E44" s="36"/>
+      <c r="F44" s="36">
+        <v>1</v>
+      </c>
+      <c r="G44" s="36">
+        <v>1</v>
+      </c>
+      <c r="H44" s="36">
+        <v>0</v>
+      </c>
+      <c r="I44" s="36">
+        <v>1</v>
+      </c>
+      <c r="J44" s="161" t="s">
+        <v>11</v>
+      </c>
+      <c r="K44" s="161"/>
+      <c r="L44" s="161"/>
+      <c r="M44" s="161"/>
+      <c r="N44" s="161"/>
+      <c r="O44" s="161"/>
+      <c r="P44" s="161"/>
+      <c r="Q44" s="161"/>
+      <c r="R44" s="161"/>
+      <c r="S44" s="161"/>
+      <c r="T44" s="161"/>
+      <c r="U44" s="165"/>
+      <c r="V44" s="42"/>
+      <c r="W44" s="36"/>
+      <c r="X44" s="36"/>
+      <c r="Y44" s="37"/>
+    </row>
+    <row r="45" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="82"/>
+      <c r="B45" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="D44" s="62"/>
-      <c r="E44" s="45"/>
-      <c r="F44" s="18">
-        <v>1</v>
-      </c>
-      <c r="G44" s="19">
-        <v>1</v>
-      </c>
-      <c r="H44" s="19">
-        <v>0</v>
-      </c>
-      <c r="I44" s="19">
-        <v>1</v>
-      </c>
-      <c r="J44" s="20">
-        <v>0</v>
-      </c>
-      <c r="K44" s="20">
-        <v>0</v>
-      </c>
-      <c r="L44" s="20">
-        <v>0</v>
-      </c>
-      <c r="M44" s="20">
-        <v>0</v>
-      </c>
-      <c r="N44" s="112" t="s">
+      <c r="C45" s="36"/>
+      <c r="D45" s="36"/>
+      <c r="E45" s="36"/>
+      <c r="F45" s="36"/>
+      <c r="G45" s="36"/>
+      <c r="H45" s="36"/>
+      <c r="I45" s="36"/>
+      <c r="J45" s="161" t="s">
+        <v>53</v>
+      </c>
+      <c r="K45" s="161"/>
+      <c r="L45" s="161"/>
+      <c r="M45" s="161"/>
+      <c r="N45" s="161" t="s">
         <v>24</v>
       </c>
-      <c r="O44" s="112"/>
-      <c r="P44" s="112"/>
-      <c r="Q44" s="112"/>
-      <c r="R44" s="112"/>
-      <c r="S44" s="112"/>
-      <c r="T44" s="112"/>
-      <c r="U44" s="113"/>
-      <c r="V44" s="22"/>
-      <c r="W44" s="19"/>
-      <c r="X44" s="19"/>
-      <c r="Y44" s="21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A45" s="108" t="s">
-        <v>112</v>
-      </c>
-      <c r="B45" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="C45" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="D45" s="19"/>
-      <c r="E45" s="21"/>
-      <c r="F45" s="18">
-        <v>1</v>
-      </c>
-      <c r="G45" s="19">
-        <v>1</v>
-      </c>
-      <c r="H45" s="19">
-        <v>0</v>
-      </c>
-      <c r="I45" s="19">
-        <v>1</v>
-      </c>
-      <c r="J45" s="20">
-        <v>0</v>
-      </c>
-      <c r="K45" s="20">
-        <v>0</v>
-      </c>
-      <c r="L45" s="20">
-        <v>0</v>
-      </c>
-      <c r="M45" s="20">
-        <v>1</v>
-      </c>
-      <c r="N45" s="112" t="s">
-        <v>24</v>
-      </c>
-      <c r="O45" s="112"/>
-      <c r="P45" s="112"/>
-      <c r="Q45" s="112"/>
-      <c r="R45" s="112"/>
-      <c r="S45" s="112"/>
-      <c r="T45" s="112"/>
-      <c r="U45" s="113"/>
-      <c r="V45" s="22"/>
-      <c r="W45" s="19"/>
-      <c r="X45" s="19"/>
-      <c r="Y45" s="21">
-        <v>0</v>
+      <c r="O45" s="161"/>
+      <c r="P45" s="161"/>
+      <c r="Q45" s="161"/>
+      <c r="R45" s="161"/>
+      <c r="S45" s="161"/>
+      <c r="T45" s="161"/>
+      <c r="U45" s="165"/>
+      <c r="V45" s="42" t="s">
+        <v>6</v>
+      </c>
+      <c r="W45" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="X45" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y45" s="37" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="46" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A46" s="118" t="s">
-        <v>113</v>
-      </c>
-      <c r="B46" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="C46" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="D46" s="19"/>
-      <c r="E46" s="21"/>
+      <c r="A46" s="108" t="s">
+        <v>110</v>
+      </c>
+      <c r="B46" s="76" t="s">
+        <v>54</v>
+      </c>
+      <c r="C46" s="71" t="s">
+        <v>51</v>
+      </c>
+      <c r="D46" s="62"/>
+      <c r="E46" s="45"/>
       <c r="F46" s="18">
         <v>1</v>
       </c>
@@ -6547,35 +6564,37 @@
         <v>0</v>
       </c>
       <c r="L46" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M46" s="20">
         <v>0</v>
       </c>
-      <c r="N46" s="112" t="s">
+      <c r="N46" s="130" t="s">
         <v>24</v>
       </c>
-      <c r="O46" s="112"/>
-      <c r="P46" s="112"/>
-      <c r="Q46" s="112"/>
-      <c r="R46" s="112"/>
-      <c r="S46" s="112"/>
-      <c r="T46" s="112"/>
-      <c r="U46" s="113"/>
-      <c r="V46" s="22">
-        <v>1</v>
-      </c>
+      <c r="O46" s="130"/>
+      <c r="P46" s="130"/>
+      <c r="Q46" s="130"/>
+      <c r="R46" s="130"/>
+      <c r="S46" s="130"/>
+      <c r="T46" s="130"/>
+      <c r="U46" s="132"/>
+      <c r="V46" s="22"/>
       <c r="W46" s="19"/>
       <c r="X46" s="19"/>
-      <c r="Y46" s="21"/>
+      <c r="Y46" s="21">
+        <v>1</v>
+      </c>
     </row>
     <row r="47" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A47" s="119"/>
+      <c r="A47" s="108" t="s">
+        <v>111</v>
+      </c>
       <c r="B47" s="14" t="s">
-        <v>130</v>
+        <v>55</v>
       </c>
       <c r="C47" s="18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D47" s="19"/>
       <c r="E47" s="21"/>
@@ -6598,37 +6617,37 @@
         <v>0</v>
       </c>
       <c r="L47" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M47" s="20">
-        <v>0</v>
-      </c>
-      <c r="N47" s="112" t="s">
+        <v>1</v>
+      </c>
+      <c r="N47" s="130" t="s">
         <v>24</v>
       </c>
-      <c r="O47" s="112"/>
-      <c r="P47" s="112"/>
-      <c r="Q47" s="112"/>
-      <c r="R47" s="112"/>
-      <c r="S47" s="112"/>
-      <c r="T47" s="112"/>
-      <c r="U47" s="113"/>
-      <c r="V47" s="22">
-        <v>1</v>
-      </c>
+      <c r="O47" s="130"/>
+      <c r="P47" s="130"/>
+      <c r="Q47" s="130"/>
+      <c r="R47" s="130"/>
+      <c r="S47" s="130"/>
+      <c r="T47" s="130"/>
+      <c r="U47" s="132"/>
+      <c r="V47" s="22"/>
       <c r="W47" s="19"/>
       <c r="X47" s="19"/>
-      <c r="Y47" s="21"/>
+      <c r="Y47" s="21">
+        <v>0</v>
+      </c>
     </row>
     <row r="48" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A48" s="120" t="s">
-        <v>114</v>
+      <c r="A48" s="123" t="s">
+        <v>112</v>
       </c>
       <c r="B48" s="14" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C48" s="18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D48" s="19"/>
       <c r="E48" s="21"/>
@@ -6654,32 +6673,32 @@
         <v>1</v>
       </c>
       <c r="M48" s="20">
-        <v>1</v>
-      </c>
-      <c r="N48" s="112" t="s">
+        <v>0</v>
+      </c>
+      <c r="N48" s="130" t="s">
         <v>24</v>
       </c>
-      <c r="O48" s="112"/>
-      <c r="P48" s="112"/>
-      <c r="Q48" s="112"/>
-      <c r="R48" s="112"/>
-      <c r="S48" s="112"/>
-      <c r="T48" s="112"/>
-      <c r="U48" s="113"/>
+      <c r="O48" s="130"/>
+      <c r="P48" s="130"/>
+      <c r="Q48" s="130"/>
+      <c r="R48" s="130"/>
+      <c r="S48" s="130"/>
+      <c r="T48" s="130"/>
+      <c r="U48" s="132"/>
       <c r="V48" s="22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W48" s="19"/>
       <c r="X48" s="19"/>
       <c r="Y48" s="21"/>
     </row>
     <row r="49" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A49" s="121"/>
+      <c r="A49" s="155"/>
       <c r="B49" s="14" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C49" s="18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D49" s="19"/>
       <c r="E49" s="21"/>
@@ -6705,34 +6724,34 @@
         <v>1</v>
       </c>
       <c r="M49" s="20">
-        <v>1</v>
-      </c>
-      <c r="N49" s="112" t="s">
+        <v>0</v>
+      </c>
+      <c r="N49" s="130" t="s">
         <v>24</v>
       </c>
-      <c r="O49" s="112"/>
-      <c r="P49" s="112"/>
-      <c r="Q49" s="112"/>
-      <c r="R49" s="112"/>
-      <c r="S49" s="112"/>
-      <c r="T49" s="112"/>
-      <c r="U49" s="113"/>
+      <c r="O49" s="130"/>
+      <c r="P49" s="130"/>
+      <c r="Q49" s="130"/>
+      <c r="R49" s="130"/>
+      <c r="S49" s="130"/>
+      <c r="T49" s="130"/>
+      <c r="U49" s="132"/>
       <c r="V49" s="22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W49" s="19"/>
       <c r="X49" s="19"/>
       <c r="Y49" s="21"/>
     </row>
     <row r="50" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A50" s="110" t="s">
-        <v>115</v>
+      <c r="A50" s="156" t="s">
+        <v>113</v>
       </c>
       <c r="B50" s="14" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C50" s="18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D50" s="19"/>
       <c r="E50" s="21"/>
@@ -6752,40 +6771,38 @@
         <v>0</v>
       </c>
       <c r="K50" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L50" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M50" s="20">
-        <v>0</v>
-      </c>
-      <c r="N50" s="112" t="s">
+        <v>1</v>
+      </c>
+      <c r="N50" s="130" t="s">
         <v>24</v>
       </c>
-      <c r="O50" s="112"/>
-      <c r="P50" s="112"/>
-      <c r="Q50" s="112"/>
-      <c r="R50" s="112"/>
-      <c r="S50" s="112"/>
-      <c r="T50" s="112"/>
-      <c r="U50" s="113"/>
-      <c r="V50" s="22"/>
+      <c r="O50" s="130"/>
+      <c r="P50" s="130"/>
+      <c r="Q50" s="130"/>
+      <c r="R50" s="130"/>
+      <c r="S50" s="130"/>
+      <c r="T50" s="130"/>
+      <c r="U50" s="132"/>
+      <c r="V50" s="22">
+        <v>0</v>
+      </c>
       <c r="W50" s="19"/>
-      <c r="X50" s="19">
-        <v>1</v>
-      </c>
+      <c r="X50" s="19"/>
       <c r="Y50" s="21"/>
     </row>
     <row r="51" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A51" s="110" t="s">
-        <v>116</v>
-      </c>
+      <c r="A51" s="157"/>
       <c r="B51" s="14" t="s">
-        <v>60</v>
+        <v>130</v>
       </c>
       <c r="C51" s="18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D51" s="19"/>
       <c r="E51" s="21"/>
@@ -6805,40 +6822,40 @@
         <v>0</v>
       </c>
       <c r="K51" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L51" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M51" s="20">
         <v>1</v>
       </c>
-      <c r="N51" s="112" t="s">
+      <c r="N51" s="130" t="s">
         <v>24</v>
       </c>
-      <c r="O51" s="112"/>
-      <c r="P51" s="112"/>
-      <c r="Q51" s="112"/>
-      <c r="R51" s="112"/>
-      <c r="S51" s="112"/>
-      <c r="T51" s="112"/>
-      <c r="U51" s="113"/>
-      <c r="V51" s="22"/>
+      <c r="O51" s="130"/>
+      <c r="P51" s="130"/>
+      <c r="Q51" s="130"/>
+      <c r="R51" s="130"/>
+      <c r="S51" s="130"/>
+      <c r="T51" s="130"/>
+      <c r="U51" s="132"/>
+      <c r="V51" s="22">
+        <v>0</v>
+      </c>
       <c r="W51" s="19"/>
-      <c r="X51" s="19">
-        <v>0</v>
-      </c>
+      <c r="X51" s="19"/>
       <c r="Y51" s="21"/>
     </row>
     <row r="52" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A52" s="108" t="s">
-        <v>136</v>
+      <c r="A52" s="110" t="s">
+        <v>114</v>
       </c>
       <c r="B52" s="14" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C52" s="18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D52" s="19"/>
       <c r="E52" s="21"/>
@@ -6861,37 +6878,37 @@
         <v>1</v>
       </c>
       <c r="L52" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M52" s="20">
         <v>0</v>
       </c>
-      <c r="N52" s="112" t="s">
+      <c r="N52" s="130" t="s">
         <v>24</v>
       </c>
-      <c r="O52" s="112"/>
-      <c r="P52" s="112"/>
-      <c r="Q52" s="112"/>
-      <c r="R52" s="112"/>
-      <c r="S52" s="112"/>
-      <c r="T52" s="112"/>
-      <c r="U52" s="113"/>
+      <c r="O52" s="130"/>
+      <c r="P52" s="130"/>
+      <c r="Q52" s="130"/>
+      <c r="R52" s="130"/>
+      <c r="S52" s="130"/>
+      <c r="T52" s="130"/>
+      <c r="U52" s="132"/>
       <c r="V52" s="22"/>
-      <c r="W52" s="19">
-        <v>1</v>
-      </c>
-      <c r="X52" s="19"/>
+      <c r="W52" s="19"/>
+      <c r="X52" s="19">
+        <v>1</v>
+      </c>
       <c r="Y52" s="21"/>
     </row>
     <row r="53" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A53" s="108" t="s">
-        <v>137</v>
+      <c r="A53" s="110" t="s">
+        <v>115</v>
       </c>
       <c r="B53" s="14" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C53" s="18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D53" s="19"/>
       <c r="E53" s="21"/>
@@ -6914,37 +6931,37 @@
         <v>1</v>
       </c>
       <c r="L53" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M53" s="20">
         <v>1</v>
       </c>
-      <c r="N53" s="112" t="s">
+      <c r="N53" s="130" t="s">
         <v>24</v>
       </c>
-      <c r="O53" s="112"/>
-      <c r="P53" s="112"/>
-      <c r="Q53" s="112"/>
-      <c r="R53" s="112"/>
-      <c r="S53" s="112"/>
-      <c r="T53" s="112"/>
-      <c r="U53" s="113"/>
+      <c r="O53" s="130"/>
+      <c r="P53" s="130"/>
+      <c r="Q53" s="130"/>
+      <c r="R53" s="130"/>
+      <c r="S53" s="130"/>
+      <c r="T53" s="130"/>
+      <c r="U53" s="132"/>
       <c r="V53" s="22"/>
-      <c r="W53" s="19">
-        <v>0</v>
-      </c>
-      <c r="X53" s="19"/>
+      <c r="W53" s="19"/>
+      <c r="X53" s="19">
+        <v>0</v>
+      </c>
       <c r="Y53" s="21"/>
     </row>
     <row r="54" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A54" s="111" t="s">
-        <v>117</v>
+      <c r="A54" s="108" t="s">
+        <v>135</v>
       </c>
       <c r="B54" s="14" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C54" s="18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D54" s="19"/>
       <c r="E54" s="21"/>
@@ -6961,43 +6978,43 @@
         <v>1</v>
       </c>
       <c r="J54" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K54" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L54" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M54" s="20">
         <v>0</v>
       </c>
-      <c r="N54" s="112" t="s">
+      <c r="N54" s="130" t="s">
         <v>24</v>
       </c>
-      <c r="O54" s="112"/>
-      <c r="P54" s="112"/>
-      <c r="Q54" s="112"/>
-      <c r="R54" s="112"/>
-      <c r="S54" s="112"/>
-      <c r="T54" s="112"/>
-      <c r="U54" s="113"/>
-      <c r="V54" s="129" t="s">
-        <v>64</v>
-      </c>
-      <c r="W54" s="112"/>
-      <c r="X54" s="112"/>
-      <c r="Y54" s="113"/>
+      <c r="O54" s="130"/>
+      <c r="P54" s="130"/>
+      <c r="Q54" s="130"/>
+      <c r="R54" s="130"/>
+      <c r="S54" s="130"/>
+      <c r="T54" s="130"/>
+      <c r="U54" s="132"/>
+      <c r="V54" s="22"/>
+      <c r="W54" s="19">
+        <v>1</v>
+      </c>
+      <c r="X54" s="19"/>
+      <c r="Y54" s="21"/>
     </row>
     <row r="55" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A55" s="111" t="s">
-        <v>118</v>
+      <c r="A55" s="108" t="s">
+        <v>136</v>
       </c>
       <c r="B55" s="14" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C55" s="18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D55" s="19"/>
       <c r="E55" s="21"/>
@@ -7014,43 +7031,43 @@
         <v>1</v>
       </c>
       <c r="J55" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K55" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L55" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M55" s="20">
         <v>1</v>
       </c>
-      <c r="N55" s="112" t="s">
+      <c r="N55" s="130" t="s">
         <v>24</v>
       </c>
-      <c r="O55" s="112"/>
-      <c r="P55" s="112"/>
-      <c r="Q55" s="112"/>
-      <c r="R55" s="112"/>
-      <c r="S55" s="112"/>
-      <c r="T55" s="112"/>
-      <c r="U55" s="113"/>
-      <c r="V55" s="129" t="s">
-        <v>66</v>
-      </c>
-      <c r="W55" s="112"/>
-      <c r="X55" s="112"/>
-      <c r="Y55" s="113"/>
+      <c r="O55" s="130"/>
+      <c r="P55" s="130"/>
+      <c r="Q55" s="130"/>
+      <c r="R55" s="130"/>
+      <c r="S55" s="130"/>
+      <c r="T55" s="130"/>
+      <c r="U55" s="132"/>
+      <c r="V55" s="22"/>
+      <c r="W55" s="19">
+        <v>0</v>
+      </c>
+      <c r="X55" s="19"/>
+      <c r="Y55" s="21"/>
     </row>
     <row r="56" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A56" s="111" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B56" s="14" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C56" s="18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D56" s="19"/>
       <c r="E56" s="21"/>
@@ -7073,37 +7090,37 @@
         <v>0</v>
       </c>
       <c r="L56" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M56" s="20">
         <v>0</v>
       </c>
-      <c r="N56" s="112" t="s">
+      <c r="N56" s="130" t="s">
         <v>24</v>
       </c>
-      <c r="O56" s="112"/>
-      <c r="P56" s="112"/>
-      <c r="Q56" s="112"/>
-      <c r="R56" s="112"/>
-      <c r="S56" s="112"/>
-      <c r="T56" s="112"/>
-      <c r="U56" s="113"/>
-      <c r="V56" s="129" t="s">
-        <v>68</v>
-      </c>
-      <c r="W56" s="112"/>
-      <c r="X56" s="112"/>
-      <c r="Y56" s="113"/>
+      <c r="O56" s="130"/>
+      <c r="P56" s="130"/>
+      <c r="Q56" s="130"/>
+      <c r="R56" s="130"/>
+      <c r="S56" s="130"/>
+      <c r="T56" s="130"/>
+      <c r="U56" s="132"/>
+      <c r="V56" s="151" t="s">
+        <v>63</v>
+      </c>
+      <c r="W56" s="130"/>
+      <c r="X56" s="130"/>
+      <c r="Y56" s="132"/>
     </row>
     <row r="57" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A57" s="111" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B57" s="14" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C57" s="18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D57" s="19"/>
       <c r="E57" s="21"/>
@@ -7126,37 +7143,37 @@
         <v>0</v>
       </c>
       <c r="L57" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M57" s="20">
         <v>1</v>
       </c>
-      <c r="N57" s="112" t="s">
+      <c r="N57" s="130" t="s">
         <v>24</v>
       </c>
-      <c r="O57" s="112"/>
-      <c r="P57" s="112"/>
-      <c r="Q57" s="112"/>
-      <c r="R57" s="112"/>
-      <c r="S57" s="112"/>
-      <c r="T57" s="112"/>
-      <c r="U57" s="113"/>
-      <c r="V57" s="129" t="s">
-        <v>70</v>
-      </c>
-      <c r="W57" s="112"/>
-      <c r="X57" s="112"/>
-      <c r="Y57" s="113"/>
+      <c r="O57" s="130"/>
+      <c r="P57" s="130"/>
+      <c r="Q57" s="130"/>
+      <c r="R57" s="130"/>
+      <c r="S57" s="130"/>
+      <c r="T57" s="130"/>
+      <c r="U57" s="132"/>
+      <c r="V57" s="151" t="s">
+        <v>65</v>
+      </c>
+      <c r="W57" s="130"/>
+      <c r="X57" s="130"/>
+      <c r="Y57" s="132"/>
     </row>
     <row r="58" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A58" s="111" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B58" s="14" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C58" s="18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D58" s="19"/>
       <c r="E58" s="21"/>
@@ -7176,206 +7193,306 @@
         <v>1</v>
       </c>
       <c r="K58" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L58" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M58" s="20">
         <v>0</v>
       </c>
-      <c r="N58" s="112" t="s">
+      <c r="N58" s="130" t="s">
         <v>24</v>
       </c>
-      <c r="O58" s="112"/>
-      <c r="P58" s="112"/>
-      <c r="Q58" s="112"/>
-      <c r="R58" s="112"/>
-      <c r="S58" s="112"/>
-      <c r="T58" s="112"/>
-      <c r="U58" s="113"/>
-      <c r="V58" s="129" t="s">
-        <v>72</v>
-      </c>
-      <c r="W58" s="112"/>
-      <c r="X58" s="112"/>
-      <c r="Y58" s="113"/>
+      <c r="O58" s="130"/>
+      <c r="P58" s="130"/>
+      <c r="Q58" s="130"/>
+      <c r="R58" s="130"/>
+      <c r="S58" s="130"/>
+      <c r="T58" s="130"/>
+      <c r="U58" s="132"/>
+      <c r="V58" s="151" t="s">
+        <v>67</v>
+      </c>
+      <c r="W58" s="130"/>
+      <c r="X58" s="130"/>
+      <c r="Y58" s="132"/>
     </row>
     <row r="59" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A59" s="109" t="s">
-        <v>122</v>
-      </c>
-      <c r="B59" s="93" t="s">
-        <v>73</v>
-      </c>
-      <c r="C59" s="92" t="s">
-        <v>52</v>
-      </c>
-      <c r="D59" s="56"/>
-      <c r="E59" s="59"/>
-      <c r="F59" s="92">
-        <v>1</v>
-      </c>
-      <c r="G59" s="56">
-        <v>1</v>
-      </c>
-      <c r="H59" s="56">
-        <v>0</v>
-      </c>
-      <c r="I59" s="56">
-        <v>1</v>
-      </c>
-      <c r="J59" s="101">
-        <v>1</v>
-      </c>
-      <c r="K59" s="101">
-        <v>1</v>
-      </c>
-      <c r="L59" s="101">
-        <v>0</v>
-      </c>
-      <c r="M59" s="101">
-        <v>1</v>
-      </c>
-      <c r="N59" s="127" t="s">
+      <c r="A59" s="111" t="s">
+        <v>119</v>
+      </c>
+      <c r="B59" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="C59" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="D59" s="19"/>
+      <c r="E59" s="21"/>
+      <c r="F59" s="18">
+        <v>1</v>
+      </c>
+      <c r="G59" s="19">
+        <v>1</v>
+      </c>
+      <c r="H59" s="19">
+        <v>0</v>
+      </c>
+      <c r="I59" s="19">
+        <v>1</v>
+      </c>
+      <c r="J59" s="20">
+        <v>1</v>
+      </c>
+      <c r="K59" s="20">
+        <v>0</v>
+      </c>
+      <c r="L59" s="20">
+        <v>1</v>
+      </c>
+      <c r="M59" s="20">
+        <v>1</v>
+      </c>
+      <c r="N59" s="130" t="s">
         <v>24</v>
       </c>
-      <c r="O59" s="127"/>
-      <c r="P59" s="127"/>
-      <c r="Q59" s="127"/>
-      <c r="R59" s="127"/>
-      <c r="S59" s="127"/>
-      <c r="T59" s="127"/>
-      <c r="U59" s="128"/>
-      <c r="V59" s="126" t="s">
-        <v>74</v>
-      </c>
-      <c r="W59" s="127"/>
-      <c r="X59" s="127"/>
-      <c r="Y59" s="128"/>
+      <c r="O59" s="130"/>
+      <c r="P59" s="130"/>
+      <c r="Q59" s="130"/>
+      <c r="R59" s="130"/>
+      <c r="S59" s="130"/>
+      <c r="T59" s="130"/>
+      <c r="U59" s="132"/>
+      <c r="V59" s="151" t="s">
+        <v>69</v>
+      </c>
+      <c r="W59" s="130"/>
+      <c r="X59" s="130"/>
+      <c r="Y59" s="132"/>
+      <c r="Z59" s="102"/>
     </row>
     <row r="60" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A60" s="118" t="s">
-        <v>128</v>
+      <c r="A60" s="111" t="s">
+        <v>120</v>
       </c>
       <c r="B60" s="14" t="s">
-        <v>125</v>
+        <v>70</v>
       </c>
       <c r="C60" s="18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D60" s="19"/>
-      <c r="E60" s="47"/>
-      <c r="F60" s="22">
+      <c r="E60" s="21"/>
+      <c r="F60" s="18">
         <v>1</v>
       </c>
       <c r="G60" s="19">
         <v>1</v>
       </c>
       <c r="H60" s="19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I60" s="19">
-        <v>0</v>
-      </c>
-      <c r="J60" s="19">
-        <v>0</v>
-      </c>
-      <c r="K60" s="130" t="s">
-        <v>127</v>
-      </c>
-      <c r="L60" s="131"/>
-      <c r="M60" s="131"/>
-      <c r="N60" s="131"/>
-      <c r="O60" s="131"/>
-      <c r="P60" s="131"/>
-      <c r="Q60" s="131"/>
-      <c r="R60" s="131"/>
-      <c r="S60" s="131"/>
-      <c r="T60" s="131"/>
+        <v>1</v>
+      </c>
+      <c r="J60" s="20">
+        <v>1</v>
+      </c>
+      <c r="K60" s="20">
+        <v>1</v>
+      </c>
+      <c r="L60" s="20">
+        <v>0</v>
+      </c>
+      <c r="M60" s="20">
+        <v>0</v>
+      </c>
+      <c r="N60" s="130" t="s">
+        <v>24</v>
+      </c>
+      <c r="O60" s="130"/>
+      <c r="P60" s="130"/>
+      <c r="Q60" s="130"/>
+      <c r="R60" s="130"/>
+      <c r="S60" s="130"/>
+      <c r="T60" s="130"/>
       <c r="U60" s="132"/>
-      <c r="V60" s="129"/>
-      <c r="W60" s="112"/>
-      <c r="X60" s="112"/>
-      <c r="Y60" s="130"/>
+      <c r="V60" s="151" t="s">
+        <v>71</v>
+      </c>
+      <c r="W60" s="130"/>
+      <c r="X60" s="130"/>
+      <c r="Y60" s="132"/>
       <c r="Z60" s="102"/>
     </row>
-    <row r="61" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="153"/>
-      <c r="B61" s="104" t="s">
-        <v>126</v>
-      </c>
-      <c r="C61" s="54" t="s">
-        <v>52</v>
+    <row r="61" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A61" s="109" t="s">
+        <v>121</v>
+      </c>
+      <c r="B61" s="93" t="s">
+        <v>72</v>
+      </c>
+      <c r="C61" s="92" t="s">
+        <v>51</v>
       </c>
       <c r="D61" s="56"/>
-      <c r="E61" s="57"/>
-      <c r="F61" s="54">
+      <c r="E61" s="59"/>
+      <c r="F61" s="92">
         <v>1</v>
       </c>
       <c r="G61" s="56">
         <v>1</v>
       </c>
       <c r="H61" s="56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I61" s="56">
-        <v>0</v>
-      </c>
-      <c r="J61" s="56">
-        <v>0</v>
-      </c>
-      <c r="K61" s="149" t="s">
-        <v>127</v>
-      </c>
-      <c r="L61" s="150"/>
-      <c r="M61" s="150"/>
-      <c r="N61" s="150"/>
-      <c r="O61" s="150"/>
-      <c r="P61" s="150"/>
-      <c r="Q61" s="150"/>
-      <c r="R61" s="150"/>
-      <c r="S61" s="150"/>
-      <c r="T61" s="150"/>
-      <c r="U61" s="151"/>
-      <c r="V61" s="126"/>
-      <c r="W61" s="127"/>
-      <c r="X61" s="127"/>
-      <c r="Y61" s="152"/>
-      <c r="Z61" s="102"/>
+        <v>1</v>
+      </c>
+      <c r="J61" s="101">
+        <v>1</v>
+      </c>
+      <c r="K61" s="101">
+        <v>1</v>
+      </c>
+      <c r="L61" s="101">
+        <v>0</v>
+      </c>
+      <c r="M61" s="101">
+        <v>1</v>
+      </c>
+      <c r="N61" s="121" t="s">
+        <v>24</v>
+      </c>
+      <c r="O61" s="121"/>
+      <c r="P61" s="121"/>
+      <c r="Q61" s="121"/>
+      <c r="R61" s="121"/>
+      <c r="S61" s="121"/>
+      <c r="T61" s="121"/>
+      <c r="U61" s="150"/>
+      <c r="V61" s="120" t="s">
+        <v>73</v>
+      </c>
+      <c r="W61" s="121"/>
+      <c r="X61" s="121"/>
+      <c r="Y61" s="150"/>
     </row>
     <row r="62" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A62" s="105"/>
-      <c r="B62" s="106"/>
-      <c r="C62" s="103"/>
-      <c r="D62" s="103"/>
-      <c r="E62" s="103"/>
-      <c r="F62" s="103"/>
-      <c r="G62" s="103"/>
-      <c r="H62" s="103"/>
-      <c r="I62" s="103"/>
-      <c r="J62" s="103"/>
-      <c r="K62" s="103"/>
-      <c r="L62" s="103"/>
-      <c r="M62" s="103"/>
-      <c r="N62" s="103"/>
-      <c r="O62" s="103"/>
-      <c r="P62" s="103"/>
-      <c r="Q62" s="103"/>
-      <c r="R62" s="103"/>
-      <c r="S62" s="103"/>
-      <c r="T62" s="103"/>
-      <c r="U62" s="103"/>
-      <c r="V62" s="103"/>
-      <c r="W62" s="103"/>
-      <c r="X62" s="103"/>
-      <c r="Y62" s="103"/>
+      <c r="A62" s="123" t="s">
+        <v>127</v>
+      </c>
+      <c r="B62" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="C62" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="D62" s="19"/>
+      <c r="E62" s="47"/>
+      <c r="F62" s="22">
+        <v>1</v>
+      </c>
+      <c r="G62" s="19">
+        <v>1</v>
+      </c>
+      <c r="H62" s="19">
+        <v>1</v>
+      </c>
+      <c r="I62" s="19">
+        <v>0</v>
+      </c>
+      <c r="J62" s="19">
+        <v>0</v>
+      </c>
+      <c r="K62" s="152" t="s">
+        <v>126</v>
+      </c>
+      <c r="L62" s="153"/>
+      <c r="M62" s="153"/>
+      <c r="N62" s="153"/>
+      <c r="O62" s="153"/>
+      <c r="P62" s="153"/>
+      <c r="Q62" s="153"/>
+      <c r="R62" s="153"/>
+      <c r="S62" s="153"/>
+      <c r="T62" s="153"/>
+      <c r="U62" s="154"/>
+      <c r="V62" s="151"/>
+      <c r="W62" s="130"/>
+      <c r="X62" s="130"/>
+      <c r="Y62" s="152"/>
     </row>
-    <row r="63" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B63" s="81"/>
+    <row r="63" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="124"/>
+      <c r="B63" s="104" t="s">
+        <v>125</v>
+      </c>
+      <c r="C63" s="54" t="s">
+        <v>51</v>
+      </c>
+      <c r="D63" s="56"/>
+      <c r="E63" s="57"/>
+      <c r="F63" s="54">
+        <v>1</v>
+      </c>
+      <c r="G63" s="56">
+        <v>1</v>
+      </c>
+      <c r="H63" s="56">
+        <v>1</v>
+      </c>
+      <c r="I63" s="56">
+        <v>0</v>
+      </c>
+      <c r="J63" s="56">
+        <v>0</v>
+      </c>
+      <c r="K63" s="117" t="s">
+        <v>126</v>
+      </c>
+      <c r="L63" s="118"/>
+      <c r="M63" s="118"/>
+      <c r="N63" s="118"/>
+      <c r="O63" s="118"/>
+      <c r="P63" s="118"/>
+      <c r="Q63" s="118"/>
+      <c r="R63" s="118"/>
+      <c r="S63" s="118"/>
+      <c r="T63" s="118"/>
+      <c r="U63" s="119"/>
+      <c r="V63" s="120"/>
+      <c r="W63" s="121"/>
+      <c r="X63" s="121"/>
+      <c r="Y63" s="122"/>
     </row>
     <row r="64" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B64" s="81"/>
+      <c r="A64" s="105"/>
+      <c r="B64" s="106"/>
+      <c r="C64" s="103"/>
+      <c r="D64" s="103"/>
+      <c r="E64" s="103"/>
+      <c r="F64" s="103"/>
+      <c r="G64" s="103"/>
+      <c r="H64" s="103"/>
+      <c r="I64" s="103"/>
+      <c r="J64" s="103"/>
+      <c r="K64" s="103"/>
+      <c r="L64" s="103"/>
+      <c r="M64" s="103"/>
+      <c r="N64" s="103"/>
+      <c r="O64" s="103"/>
+      <c r="P64" s="103"/>
+      <c r="Q64" s="103"/>
+      <c r="R64" s="103"/>
+      <c r="S64" s="103"/>
+      <c r="T64" s="103"/>
+      <c r="U64" s="103"/>
+      <c r="V64" s="103"/>
+      <c r="W64" s="103"/>
+      <c r="X64" s="103"/>
+      <c r="Y64" s="103"/>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B65" s="81"/>
@@ -7401,32 +7518,83 @@
     <row r="72" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B72" s="81"/>
     </row>
+    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B73" s="81"/>
+    </row>
+    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B74" s="81"/>
+    </row>
   </sheetData>
-  <mergeCells count="114">
-    <mergeCell ref="K61:U61"/>
+  <mergeCells count="117">
+    <mergeCell ref="J44:M44"/>
+    <mergeCell ref="N44:U44"/>
+    <mergeCell ref="J45:M45"/>
+    <mergeCell ref="N45:U45"/>
+    <mergeCell ref="N48:U48"/>
+    <mergeCell ref="N50:U50"/>
+    <mergeCell ref="M35:O35"/>
+    <mergeCell ref="S35:U35"/>
+    <mergeCell ref="P35:R35"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="P33:R33"/>
+    <mergeCell ref="S33:U33"/>
+    <mergeCell ref="K14:M14"/>
+    <mergeCell ref="N14:U14"/>
+    <mergeCell ref="N53:U53"/>
+    <mergeCell ref="O42:U42"/>
+    <mergeCell ref="J41:P41"/>
+    <mergeCell ref="P19:R19"/>
+    <mergeCell ref="P20:R20"/>
+    <mergeCell ref="P21:R21"/>
+    <mergeCell ref="P22:R22"/>
+    <mergeCell ref="P23:R23"/>
+    <mergeCell ref="S28:U28"/>
+    <mergeCell ref="S29:U29"/>
+    <mergeCell ref="S30:U30"/>
+    <mergeCell ref="S31:U31"/>
+    <mergeCell ref="P31:R31"/>
+    <mergeCell ref="S19:U19"/>
+    <mergeCell ref="S20:U20"/>
+    <mergeCell ref="S21:U21"/>
+    <mergeCell ref="S22:U22"/>
+    <mergeCell ref="S23:U23"/>
+    <mergeCell ref="K40:M40"/>
+    <mergeCell ref="N40:U40"/>
     <mergeCell ref="V61:Y61"/>
-    <mergeCell ref="A60:A61"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:U1"/>
-    <mergeCell ref="K4:O4"/>
-    <mergeCell ref="H3:L3"/>
-    <mergeCell ref="S10:U10"/>
-    <mergeCell ref="K5:O5"/>
-    <mergeCell ref="K6:O6"/>
-    <mergeCell ref="S7:U7"/>
-    <mergeCell ref="P8:R8"/>
-    <mergeCell ref="S8:U8"/>
-    <mergeCell ref="M7:O7"/>
-    <mergeCell ref="M8:O8"/>
-    <mergeCell ref="M9:O9"/>
-    <mergeCell ref="M10:O10"/>
-    <mergeCell ref="S27:U27"/>
-    <mergeCell ref="P25:R25"/>
-    <mergeCell ref="P26:R26"/>
-    <mergeCell ref="P27:R27"/>
-    <mergeCell ref="P24:R24"/>
+    <mergeCell ref="V62:Y62"/>
+    <mergeCell ref="N56:U56"/>
+    <mergeCell ref="N57:U57"/>
+    <mergeCell ref="N58:U58"/>
+    <mergeCell ref="N59:U59"/>
+    <mergeCell ref="N60:U60"/>
+    <mergeCell ref="V56:Y56"/>
+    <mergeCell ref="V57:Y57"/>
+    <mergeCell ref="V58:Y58"/>
+    <mergeCell ref="V59:Y59"/>
+    <mergeCell ref="V60:Y60"/>
+    <mergeCell ref="N61:U61"/>
+    <mergeCell ref="K62:U62"/>
+    <mergeCell ref="N54:U54"/>
+    <mergeCell ref="N55:U55"/>
+    <mergeCell ref="N46:U46"/>
+    <mergeCell ref="N47:U47"/>
+    <mergeCell ref="N49:U49"/>
+    <mergeCell ref="N51:U51"/>
+    <mergeCell ref="N52:U52"/>
+    <mergeCell ref="O43:U43"/>
+    <mergeCell ref="S24:U24"/>
+    <mergeCell ref="S25:U25"/>
+    <mergeCell ref="S26:U26"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="K37:M37"/>
+    <mergeCell ref="N37:U37"/>
+    <mergeCell ref="K38:M38"/>
+    <mergeCell ref="N38:U38"/>
+    <mergeCell ref="P28:R28"/>
+    <mergeCell ref="P29:R29"/>
+    <mergeCell ref="P30:R30"/>
     <mergeCell ref="V1:Y1"/>
     <mergeCell ref="P16:R16"/>
     <mergeCell ref="S16:U16"/>
@@ -7451,161 +7619,127 @@
     <mergeCell ref="N13:U13"/>
     <mergeCell ref="K12:M12"/>
     <mergeCell ref="N12:U12"/>
-    <mergeCell ref="S24:U24"/>
-    <mergeCell ref="S25:U25"/>
-    <mergeCell ref="S26:U26"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="K35:M35"/>
-    <mergeCell ref="N35:U35"/>
-    <mergeCell ref="K36:M36"/>
-    <mergeCell ref="N36:U36"/>
-    <mergeCell ref="P28:R28"/>
-    <mergeCell ref="P29:R29"/>
-    <mergeCell ref="P30:R30"/>
-    <mergeCell ref="K38:M38"/>
-    <mergeCell ref="N38:U38"/>
-    <mergeCell ref="V59:Y59"/>
-    <mergeCell ref="V60:Y60"/>
-    <mergeCell ref="N54:U54"/>
-    <mergeCell ref="N55:U55"/>
-    <mergeCell ref="N56:U56"/>
-    <mergeCell ref="N57:U57"/>
-    <mergeCell ref="N58:U58"/>
-    <mergeCell ref="V54:Y54"/>
-    <mergeCell ref="V55:Y55"/>
-    <mergeCell ref="V56:Y56"/>
-    <mergeCell ref="V57:Y57"/>
-    <mergeCell ref="V58:Y58"/>
-    <mergeCell ref="N59:U59"/>
-    <mergeCell ref="K60:U60"/>
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="P33:R33"/>
-    <mergeCell ref="S33:U33"/>
-    <mergeCell ref="K14:M14"/>
-    <mergeCell ref="N14:U14"/>
-    <mergeCell ref="N51:U51"/>
-    <mergeCell ref="O40:U40"/>
-    <mergeCell ref="J39:P39"/>
-    <mergeCell ref="P19:R19"/>
-    <mergeCell ref="P20:R20"/>
-    <mergeCell ref="P21:R21"/>
-    <mergeCell ref="P22:R22"/>
-    <mergeCell ref="P23:R23"/>
-    <mergeCell ref="S28:U28"/>
-    <mergeCell ref="S29:U29"/>
-    <mergeCell ref="S30:U30"/>
-    <mergeCell ref="S31:U31"/>
-    <mergeCell ref="P31:R31"/>
-    <mergeCell ref="S19:U19"/>
-    <mergeCell ref="S20:U20"/>
-    <mergeCell ref="S21:U21"/>
-    <mergeCell ref="S22:U22"/>
-    <mergeCell ref="S23:U23"/>
-    <mergeCell ref="N52:U52"/>
-    <mergeCell ref="N53:U53"/>
-    <mergeCell ref="N44:U44"/>
-    <mergeCell ref="N45:U45"/>
-    <mergeCell ref="N47:U47"/>
-    <mergeCell ref="N49:U49"/>
-    <mergeCell ref="N50:U50"/>
-    <mergeCell ref="O41:U41"/>
-    <mergeCell ref="J42:M42"/>
-    <mergeCell ref="N42:U42"/>
-    <mergeCell ref="J43:M43"/>
-    <mergeCell ref="N43:U43"/>
-    <mergeCell ref="N46:U46"/>
-    <mergeCell ref="N48:U48"/>
+    <mergeCell ref="K63:U63"/>
+    <mergeCell ref="V63:Y63"/>
+    <mergeCell ref="A62:A63"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:U1"/>
+    <mergeCell ref="K4:O4"/>
+    <mergeCell ref="H3:L3"/>
+    <mergeCell ref="S10:U10"/>
+    <mergeCell ref="K5:O5"/>
+    <mergeCell ref="K6:O6"/>
+    <mergeCell ref="S7:U7"/>
+    <mergeCell ref="P8:R8"/>
+    <mergeCell ref="S8:U8"/>
+    <mergeCell ref="M7:O7"/>
+    <mergeCell ref="M8:O8"/>
+    <mergeCell ref="M9:O9"/>
+    <mergeCell ref="M10:O10"/>
+    <mergeCell ref="S27:U27"/>
+    <mergeCell ref="P25:R25"/>
+    <mergeCell ref="P26:R26"/>
+    <mergeCell ref="P27:R27"/>
+    <mergeCell ref="P24:R24"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="F60:K61">
-    <cfRule type="cellIs" dxfId="43" priority="26" operator="equal">
+  <conditionalFormatting sqref="F62:K63">
+    <cfRule type="cellIs" dxfId="45" priority="36" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="27" operator="containsText" text="imm">
-      <formula>NOT(ISERROR(SEARCH("imm",F60)))</formula>
+    <cfRule type="containsText" dxfId="44" priority="37" operator="containsText" text="imm">
+      <formula>NOT(ISERROR(SEARCH("imm",F62)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="38" operator="equal">
       <formula>"imm3"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="39" operator="equal">
       <formula>"imm5"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F4:U59">
-    <cfRule type="cellIs" dxfId="8" priority="35" operator="equal">
+  <conditionalFormatting sqref="F4:U61">
+    <cfRule type="cellIs" dxfId="8" priority="45" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F43:M43 V43:Y43 F44:Y59 V60:Y61 F1:Y42">
-    <cfRule type="containsText" dxfId="7" priority="36" operator="containsText" text="imm">
+  <conditionalFormatting sqref="F45:M45 V45:Y45 F46:Y61 V62:Y63 F1:Y44">
+    <cfRule type="containsText" dxfId="7" priority="46" operator="containsText" text="imm">
       <formula>NOT(ISERROR(SEARCH("imm",F1)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="47" operator="equal">
       <formula>"imm3"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="48" operator="equal">
       <formula>"imm5"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:U31">
-    <cfRule type="cellIs" dxfId="39" priority="39" operator="equal">
+  <conditionalFormatting sqref="H40:M40">
+    <cfRule type="cellIs" dxfId="41" priority="12" operator="equal">
+      <formula>"Rn"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="40" priority="14" operator="equal">
+      <formula>"Rdn"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="39" priority="15" operator="equal">
+      <formula>"Rm"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="38" priority="16" operator="equal">
       <formula>"Rd"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="18" operator="equal">
+      <formula>"Rd"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2:U31">
+    <cfRule type="cellIs" dxfId="36" priority="49" operator="equal">
+      <formula>"Rd"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="35" priority="50" operator="equal">
       <formula>"Rn"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="51" operator="equal">
       <formula>"Rd"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="52" operator="equal">
       <formula>"Rdn"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="53" operator="equal">
       <formula>"Rm"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H33:U33">
-    <cfRule type="cellIs" dxfId="34" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="40" operator="equal">
       <formula>"Rd"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="41" operator="equal">
       <formula>"Rn"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="42" operator="equal">
       <formula>"Rd"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="43" operator="equal">
       <formula>"Rdn"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="44" operator="equal">
       <formula>"Rm"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="K40:M40">
+    <cfRule type="cellIs" dxfId="26" priority="11" operator="equal">
+      <formula>"Rd"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="25" priority="13" operator="equal">
+      <formula>"Rd"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="P16:R16">
-    <cfRule type="cellIs" dxfId="29" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="54" operator="equal">
       <formula>"Rm"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H38:J38">
-    <cfRule type="cellIs" dxfId="28" priority="16" operator="equal">
-      <formula>"Rd"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="17" operator="equal">
-      <formula>"Rn"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="18" operator="equal">
-      <formula>"Rd"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="19" operator="equal">
-      <formula>"Rdn"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="20" operator="equal">
-      <formula>"Rm"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K38:M38">
+  <conditionalFormatting sqref="M35:O35">
     <cfRule type="cellIs" dxfId="23" priority="6" operator="equal">
       <formula>"Rd"</formula>
     </cfRule>
@@ -7622,7 +7756,7 @@
       <formula>"Rm"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K38:M38">
+  <conditionalFormatting sqref="P35:R35">
     <cfRule type="cellIs" dxfId="18" priority="1" operator="equal">
       <formula>"Rd"</formula>
     </cfRule>
@@ -7645,15 +7779,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010096649AD79A527B47A67D905693C83B0C" ma:contentTypeVersion="7" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="44d09355696640e2dc56270e449341cd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="98b34aae-4bd1-40d2-80e1-46205a35d283" xmlns:ns4="4c17d7eb-fa2b-4fbc-8175-1cef2629d4d8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="73bda8d09c620ff6c543bf34844bea48" ns3:_="" ns4:_="">
     <xsd:import namespace="98b34aae-4bd1-40d2-80e1-46205a35d283"/>
@@ -7838,6 +7963,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -7845,14 +7979,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AAD58D5F-4A46-4F63-A2BD-BBB590555A8D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90060F17-AE26-48CA-A0B9-2F516B758ECF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7867,6 +7993,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AAD58D5F-4A46-4F63-A2BD-BBB590555A8D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Ajout de STR avec des registres
</commit_message>
<xml_diff>
--- a/docs/ARM instructions.xlsx
+++ b/docs/ARM instructions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Drive\Etudes\Supérieur\SI3\Architecture et réseaux\Architecture\PARM\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1A3501F-C3B5-43A8-B4AC-65BE24DB06F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24D6614E-06E8-4DE8-A292-0FDD1D225768}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1E4904EC-9B68-40DD-B685-7BD66B9DE8BA}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="141">
   <si>
     <t>Description</t>
   </si>
@@ -3257,7 +3257,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="46">
+  <dxfs count="56">
     <dxf>
       <fill>
         <patternFill>
@@ -3295,30 +3295,73 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF9999"/>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFCC99FF"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF9999"/>
+          <bgColor theme="4" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -3556,6 +3599,33 @@
           <bgColor theme="8" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFF9999"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC99FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9999"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
     </dxf>
     <dxf>
       <fill>
@@ -3911,10 +3981,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Z74"/>
+  <dimension ref="A1:Z75"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" zoomScaleSheetLayoutView="145" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+      <selection activeCell="N38" sqref="N38:U38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5992,10 +6062,10 @@
     </row>
     <row r="35" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="89" t="s">
-        <v>107</v>
-      </c>
-      <c r="B35" s="33" t="s">
-        <v>41</v>
+        <v>106</v>
+      </c>
+      <c r="B35" s="43" t="s">
+        <v>38</v>
       </c>
       <c r="C35" s="65" t="s">
         <v>39</v>
@@ -6018,8 +6088,8 @@
       <c r="I35" s="69">
         <v>1</v>
       </c>
-      <c r="J35" s="70">
-        <v>1</v>
+      <c r="J35" s="75">
+        <v>0</v>
       </c>
       <c r="K35" s="75">
         <v>0</v>
@@ -6048,471 +6118,495 @@
       <c r="Y35" s="21"/>
     </row>
     <row r="36" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="82" t="s">
-        <v>140</v>
-      </c>
-      <c r="B36" s="36"/>
-      <c r="C36" s="36"/>
-      <c r="D36" s="36"/>
-      <c r="E36" s="36"/>
-      <c r="F36" s="36">
-        <v>1</v>
-      </c>
-      <c r="G36" s="36">
-        <v>0</v>
-      </c>
-      <c r="H36" s="36">
-        <v>0</v>
-      </c>
-      <c r="I36" s="36">
-        <v>1</v>
-      </c>
-      <c r="J36" s="36"/>
-      <c r="K36" s="36"/>
-      <c r="L36" s="36"/>
-      <c r="M36" s="36"/>
-      <c r="N36" s="36"/>
-      <c r="O36" s="36"/>
-      <c r="P36" s="36"/>
-      <c r="Q36" s="36"/>
-      <c r="R36" s="36"/>
-      <c r="S36" s="36"/>
-      <c r="T36" s="36"/>
-      <c r="U36" s="37"/>
-      <c r="V36" s="42" t="s">
-        <v>6</v>
-      </c>
-      <c r="W36" s="36" t="s">
-        <v>7</v>
-      </c>
-      <c r="X36" s="36" t="s">
-        <v>8</v>
-      </c>
-      <c r="Y36" s="37" t="s">
-        <v>9</v>
-      </c>
+      <c r="A36" s="89" t="s">
+        <v>107</v>
+      </c>
+      <c r="B36" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="C36" s="65" t="s">
+        <v>39</v>
+      </c>
+      <c r="D36" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="E36" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="F36" s="68">
+        <v>0</v>
+      </c>
+      <c r="G36" s="68">
+        <v>1</v>
+      </c>
+      <c r="H36" s="68">
+        <v>0</v>
+      </c>
+      <c r="I36" s="69">
+        <v>1</v>
+      </c>
+      <c r="J36" s="70">
+        <v>1</v>
+      </c>
+      <c r="K36" s="75">
+        <v>0</v>
+      </c>
+      <c r="L36" s="75">
+        <v>0</v>
+      </c>
+      <c r="M36" s="158" t="s">
+        <v>16</v>
+      </c>
+      <c r="N36" s="158"/>
+      <c r="O36" s="158"/>
+      <c r="P36" s="130" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q36" s="130"/>
+      <c r="R36" s="132"/>
+      <c r="S36" s="143" t="s">
+        <v>40</v>
+      </c>
+      <c r="T36" s="143"/>
+      <c r="U36" s="143"/>
+      <c r="V36" s="22"/>
+      <c r="W36" s="19"/>
+      <c r="X36" s="19"/>
+      <c r="Y36" s="21"/>
     </row>
     <row r="37" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="89" t="s">
-        <v>106</v>
-      </c>
-      <c r="B37" s="43" t="s">
-        <v>38</v>
-      </c>
-      <c r="C37" s="60" t="s">
-        <v>39</v>
-      </c>
-      <c r="D37" s="141" t="s">
-        <v>42</v>
-      </c>
-      <c r="E37" s="142"/>
-      <c r="F37" s="61">
-        <v>1</v>
-      </c>
-      <c r="G37" s="62">
-        <v>0</v>
-      </c>
-      <c r="H37" s="62">
-        <v>0</v>
-      </c>
-      <c r="I37" s="63">
-        <v>1</v>
-      </c>
-      <c r="J37" s="64">
-        <v>0</v>
-      </c>
-      <c r="K37" s="143" t="s">
-        <v>40</v>
-      </c>
-      <c r="L37" s="143"/>
-      <c r="M37" s="143"/>
-      <c r="N37" s="144" t="s">
-        <v>24</v>
-      </c>
-      <c r="O37" s="144"/>
-      <c r="P37" s="144"/>
-      <c r="Q37" s="144"/>
-      <c r="R37" s="144"/>
-      <c r="S37" s="144"/>
-      <c r="T37" s="144"/>
-      <c r="U37" s="145"/>
-      <c r="V37" s="22"/>
-      <c r="W37" s="19"/>
-      <c r="X37" s="19"/>
-      <c r="Y37" s="21"/>
+      <c r="A37" s="82" t="s">
+        <v>140</v>
+      </c>
+      <c r="B37" s="36"/>
+      <c r="C37" s="36"/>
+      <c r="D37" s="36"/>
+      <c r="E37" s="36"/>
+      <c r="F37" s="36">
+        <v>1</v>
+      </c>
+      <c r="G37" s="36">
+        <v>0</v>
+      </c>
+      <c r="H37" s="36">
+        <v>0</v>
+      </c>
+      <c r="I37" s="36">
+        <v>1</v>
+      </c>
+      <c r="J37" s="36"/>
+      <c r="K37" s="36"/>
+      <c r="L37" s="36"/>
+      <c r="M37" s="36"/>
+      <c r="N37" s="36"/>
+      <c r="O37" s="36"/>
+      <c r="P37" s="36"/>
+      <c r="Q37" s="36"/>
+      <c r="R37" s="36"/>
+      <c r="S37" s="36"/>
+      <c r="T37" s="36"/>
+      <c r="U37" s="37"/>
+      <c r="V37" s="42" t="s">
+        <v>6</v>
+      </c>
+      <c r="W37" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="X37" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y37" s="37" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="38" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="89" t="s">
-        <v>107</v>
-      </c>
-      <c r="B38" s="33" t="s">
-        <v>41</v>
-      </c>
-      <c r="C38" s="65" t="s">
+        <v>106</v>
+      </c>
+      <c r="B38" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="C38" s="60" t="s">
         <v>39</v>
       </c>
       <c r="D38" s="141" t="s">
         <v>42</v>
       </c>
       <c r="E38" s="142"/>
-      <c r="F38" s="67">
-        <v>1</v>
-      </c>
-      <c r="G38" s="68">
-        <v>0</v>
-      </c>
-      <c r="H38" s="68">
-        <v>0</v>
-      </c>
-      <c r="I38" s="69">
-        <v>1</v>
-      </c>
-      <c r="J38" s="70">
-        <v>1</v>
-      </c>
-      <c r="K38" s="146" t="s">
+      <c r="F38" s="61">
+        <v>1</v>
+      </c>
+      <c r="G38" s="62">
+        <v>0</v>
+      </c>
+      <c r="H38" s="62">
+        <v>0</v>
+      </c>
+      <c r="I38" s="63">
+        <v>1</v>
+      </c>
+      <c r="J38" s="64">
+        <v>0</v>
+      </c>
+      <c r="K38" s="143" t="s">
         <v>40</v>
       </c>
-      <c r="L38" s="146"/>
-      <c r="M38" s="146"/>
-      <c r="N38" s="147" t="s">
+      <c r="L38" s="143"/>
+      <c r="M38" s="143"/>
+      <c r="N38" s="144" t="s">
         <v>24</v>
       </c>
-      <c r="O38" s="147"/>
-      <c r="P38" s="147"/>
-      <c r="Q38" s="147"/>
-      <c r="R38" s="147"/>
-      <c r="S38" s="147"/>
-      <c r="T38" s="147"/>
-      <c r="U38" s="148"/>
+      <c r="O38" s="144"/>
+      <c r="P38" s="144"/>
+      <c r="Q38" s="144"/>
+      <c r="R38" s="144"/>
+      <c r="S38" s="144"/>
+      <c r="T38" s="144"/>
+      <c r="U38" s="145"/>
       <c r="V38" s="22"/>
       <c r="W38" s="19"/>
       <c r="X38" s="19"/>
       <c r="Y38" s="21"/>
     </row>
     <row r="39" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="82" t="s">
+      <c r="A39" s="89" t="s">
+        <v>107</v>
+      </c>
+      <c r="B39" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="C39" s="65" t="s">
+        <v>39</v>
+      </c>
+      <c r="D39" s="141" t="s">
+        <v>42</v>
+      </c>
+      <c r="E39" s="142"/>
+      <c r="F39" s="67">
+        <v>1</v>
+      </c>
+      <c r="G39" s="68">
+        <v>0</v>
+      </c>
+      <c r="H39" s="68">
+        <v>0</v>
+      </c>
+      <c r="I39" s="69">
+        <v>1</v>
+      </c>
+      <c r="J39" s="70">
+        <v>1</v>
+      </c>
+      <c r="K39" s="146" t="s">
+        <v>40</v>
+      </c>
+      <c r="L39" s="146"/>
+      <c r="M39" s="146"/>
+      <c r="N39" s="147" t="s">
+        <v>24</v>
+      </c>
+      <c r="O39" s="147"/>
+      <c r="P39" s="147"/>
+      <c r="Q39" s="147"/>
+      <c r="R39" s="147"/>
+      <c r="S39" s="147"/>
+      <c r="T39" s="147"/>
+      <c r="U39" s="148"/>
+      <c r="V39" s="22"/>
+      <c r="W39" s="19"/>
+      <c r="X39" s="19"/>
+      <c r="Y39" s="21"/>
+    </row>
+    <row r="40" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="82" t="s">
         <v>138</v>
       </c>
-      <c r="B39" s="36"/>
-      <c r="C39" s="36"/>
-      <c r="D39" s="36"/>
-      <c r="E39" s="36"/>
-      <c r="F39" s="36">
-        <v>1</v>
-      </c>
-      <c r="G39" s="36">
-        <v>0</v>
-      </c>
-      <c r="H39" s="36">
-        <v>1</v>
-      </c>
-      <c r="I39" s="36">
-        <v>0</v>
-      </c>
-      <c r="J39" s="36">
-        <v>1</v>
-      </c>
-      <c r="K39" s="114"/>
-      <c r="L39" s="114"/>
-      <c r="M39" s="114"/>
-      <c r="N39" s="114"/>
-      <c r="O39" s="114"/>
-      <c r="P39" s="114"/>
-      <c r="Q39" s="36"/>
-      <c r="R39" s="36"/>
-      <c r="S39" s="36"/>
-      <c r="T39" s="36"/>
-      <c r="U39" s="37"/>
-      <c r="V39" s="42" t="s">
+      <c r="B40" s="36"/>
+      <c r="C40" s="36"/>
+      <c r="D40" s="36"/>
+      <c r="E40" s="36"/>
+      <c r="F40" s="36">
+        <v>1</v>
+      </c>
+      <c r="G40" s="36">
+        <v>0</v>
+      </c>
+      <c r="H40" s="36">
+        <v>1</v>
+      </c>
+      <c r="I40" s="36">
+        <v>0</v>
+      </c>
+      <c r="J40" s="36">
+        <v>1</v>
+      </c>
+      <c r="K40" s="114"/>
+      <c r="L40" s="114"/>
+      <c r="M40" s="114"/>
+      <c r="N40" s="114"/>
+      <c r="O40" s="114"/>
+      <c r="P40" s="114"/>
+      <c r="Q40" s="36"/>
+      <c r="R40" s="36"/>
+      <c r="S40" s="36"/>
+      <c r="T40" s="36"/>
+      <c r="U40" s="37"/>
+      <c r="V40" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="W39" s="36" t="s">
+      <c r="W40" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="X39" s="36" t="s">
+      <c r="X40" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="Y39" s="37" t="s">
+      <c r="Y40" s="37" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A40" s="116" t="s">
+    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A41" s="116" t="s">
         <v>137</v>
       </c>
-      <c r="B40" s="43" t="s">
+      <c r="B41" s="43" t="s">
         <v>44</v>
       </c>
-      <c r="C40" s="99" t="s">
+      <c r="C41" s="99" t="s">
         <v>12</v>
       </c>
-      <c r="D40" s="71" t="s">
+      <c r="D41" s="71" t="s">
         <v>45</v>
       </c>
-      <c r="E40" s="97" t="s">
+      <c r="E41" s="97" t="s">
         <v>23</v>
       </c>
-      <c r="F40" s="54">
-        <v>1</v>
-      </c>
-      <c r="G40" s="56">
-        <v>0</v>
-      </c>
-      <c r="H40" s="56">
-        <v>1</v>
-      </c>
-      <c r="I40" s="56">
-        <v>0</v>
-      </c>
-      <c r="J40" s="115">
-        <v>1</v>
-      </c>
-      <c r="K40" s="121" t="s">
+      <c r="F41" s="54">
+        <v>1</v>
+      </c>
+      <c r="G41" s="56">
+        <v>0</v>
+      </c>
+      <c r="H41" s="56">
+        <v>1</v>
+      </c>
+      <c r="I41" s="56">
+        <v>0</v>
+      </c>
+      <c r="J41" s="115">
+        <v>1</v>
+      </c>
+      <c r="K41" s="121" t="s">
         <v>17</v>
       </c>
-      <c r="L40" s="121"/>
-      <c r="M40" s="121"/>
-      <c r="N40" s="149" t="s">
+      <c r="L41" s="121"/>
+      <c r="M41" s="121"/>
+      <c r="N41" s="149" t="s">
         <v>24</v>
       </c>
-      <c r="O40" s="144"/>
-      <c r="P40" s="144"/>
-      <c r="Q40" s="144"/>
-      <c r="R40" s="144"/>
-      <c r="S40" s="144"/>
-      <c r="T40" s="144"/>
-      <c r="U40" s="145"/>
-      <c r="V40" s="18"/>
-      <c r="W40" s="19"/>
-      <c r="X40" s="19"/>
-      <c r="Y40" s="21"/>
+      <c r="O41" s="144"/>
+      <c r="P41" s="144"/>
+      <c r="Q41" s="144"/>
+      <c r="R41" s="144"/>
+      <c r="S41" s="144"/>
+      <c r="T41" s="144"/>
+      <c r="U41" s="145"/>
+      <c r="V41" s="18"/>
+      <c r="W41" s="19"/>
+      <c r="X41" s="19"/>
+      <c r="Y41" s="21"/>
     </row>
-    <row r="41" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="82" t="s">
+    <row r="42" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="82" t="s">
         <v>43</v>
       </c>
-      <c r="B41" s="36"/>
-      <c r="C41" s="36"/>
-      <c r="D41" s="36"/>
-      <c r="E41" s="36"/>
-      <c r="F41" s="36">
-        <v>1</v>
-      </c>
-      <c r="G41" s="36">
-        <v>0</v>
-      </c>
-      <c r="H41" s="36">
-        <v>1</v>
-      </c>
-      <c r="I41" s="36">
-        <v>1</v>
-      </c>
-      <c r="J41" s="161" t="s">
+      <c r="B42" s="36"/>
+      <c r="C42" s="36"/>
+      <c r="D42" s="36"/>
+      <c r="E42" s="36"/>
+      <c r="F42" s="36">
+        <v>1</v>
+      </c>
+      <c r="G42" s="36">
+        <v>0</v>
+      </c>
+      <c r="H42" s="36">
+        <v>1</v>
+      </c>
+      <c r="I42" s="36">
+        <v>1</v>
+      </c>
+      <c r="J42" s="161" t="s">
         <v>11</v>
       </c>
-      <c r="K41" s="161"/>
-      <c r="L41" s="161"/>
-      <c r="M41" s="161"/>
-      <c r="N41" s="161"/>
-      <c r="O41" s="161"/>
-      <c r="P41" s="161"/>
-      <c r="Q41" s="36"/>
-      <c r="R41" s="36"/>
-      <c r="S41" s="36"/>
-      <c r="T41" s="36"/>
-      <c r="U41" s="37"/>
-      <c r="V41" s="42" t="s">
+      <c r="K42" s="161"/>
+      <c r="L42" s="161"/>
+      <c r="M42" s="161"/>
+      <c r="N42" s="161"/>
+      <c r="O42" s="161"/>
+      <c r="P42" s="161"/>
+      <c r="Q42" s="36"/>
+      <c r="R42" s="36"/>
+      <c r="S42" s="36"/>
+      <c r="T42" s="36"/>
+      <c r="U42" s="37"/>
+      <c r="V42" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="W41" s="36" t="s">
+      <c r="W42" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="X41" s="36" t="s">
+      <c r="X42" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="Y41" s="37" t="s">
+      <c r="Y42" s="37" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A42" s="90" t="s">
+    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A43" s="90" t="s">
         <v>108</v>
       </c>
-      <c r="B42" s="43" t="s">
+      <c r="B43" s="43" t="s">
         <v>44</v>
       </c>
-      <c r="C42" s="71" t="s">
+      <c r="C43" s="71" t="s">
         <v>45</v>
       </c>
-      <c r="D42" s="62" t="s">
+      <c r="D43" s="62" t="s">
         <v>128</v>
       </c>
-      <c r="E42" s="17" t="s">
+      <c r="E43" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="F42" s="72">
-        <v>1</v>
-      </c>
-      <c r="G42" s="62">
-        <v>0</v>
-      </c>
-      <c r="H42" s="62">
-        <v>1</v>
-      </c>
-      <c r="I42" s="62">
-        <v>1</v>
-      </c>
-      <c r="J42" s="64">
-        <v>0</v>
-      </c>
-      <c r="K42" s="64">
-        <v>0</v>
-      </c>
-      <c r="L42" s="64">
-        <v>0</v>
-      </c>
-      <c r="M42" s="64">
-        <v>0</v>
-      </c>
-      <c r="N42" s="64">
-        <v>0</v>
-      </c>
-      <c r="O42" s="144" t="s">
+      <c r="F43" s="72">
+        <v>1</v>
+      </c>
+      <c r="G43" s="62">
+        <v>0</v>
+      </c>
+      <c r="H43" s="62">
+        <v>1</v>
+      </c>
+      <c r="I43" s="62">
+        <v>1</v>
+      </c>
+      <c r="J43" s="64">
+        <v>0</v>
+      </c>
+      <c r="K43" s="64">
+        <v>0</v>
+      </c>
+      <c r="L43" s="64">
+        <v>0</v>
+      </c>
+      <c r="M43" s="64">
+        <v>0</v>
+      </c>
+      <c r="N43" s="64">
+        <v>0</v>
+      </c>
+      <c r="O43" s="144" t="s">
         <v>47</v>
       </c>
-      <c r="P42" s="144"/>
-      <c r="Q42" s="144"/>
-      <c r="R42" s="144"/>
-      <c r="S42" s="144"/>
-      <c r="T42" s="144"/>
-      <c r="U42" s="145"/>
-      <c r="V42" s="22"/>
-      <c r="W42" s="19"/>
-      <c r="X42" s="19"/>
-      <c r="Y42" s="21"/>
-    </row>
-    <row r="43" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="90" t="s">
-        <v>109</v>
-      </c>
-      <c r="B43" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="C43" s="73" t="s">
-        <v>45</v>
-      </c>
-      <c r="D43" s="68" t="s">
-        <v>128</v>
-      </c>
-      <c r="E43" s="66" t="s">
-        <v>46</v>
-      </c>
-      <c r="F43" s="74">
-        <v>1</v>
-      </c>
-      <c r="G43" s="68">
-        <v>0</v>
-      </c>
-      <c r="H43" s="68">
-        <v>1</v>
-      </c>
-      <c r="I43" s="68">
-        <v>1</v>
-      </c>
-      <c r="J43" s="75">
-        <v>0</v>
-      </c>
-      <c r="K43" s="75">
-        <v>0</v>
-      </c>
-      <c r="L43" s="75">
-        <v>0</v>
-      </c>
-      <c r="M43" s="75">
-        <v>0</v>
-      </c>
-      <c r="N43" s="75">
-        <v>1</v>
-      </c>
-      <c r="O43" s="147" t="s">
-        <v>47</v>
-      </c>
-      <c r="P43" s="147"/>
-      <c r="Q43" s="147"/>
-      <c r="R43" s="147"/>
-      <c r="S43" s="147"/>
-      <c r="T43" s="147"/>
-      <c r="U43" s="148"/>
+      <c r="P43" s="144"/>
+      <c r="Q43" s="144"/>
+      <c r="R43" s="144"/>
+      <c r="S43" s="144"/>
+      <c r="T43" s="144"/>
+      <c r="U43" s="145"/>
       <c r="V43" s="22"/>
       <c r="W43" s="19"/>
       <c r="X43" s="19"/>
       <c r="Y43" s="21"/>
     </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A44" s="82" t="s">
+    <row r="44" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="90" t="s">
+        <v>109</v>
+      </c>
+      <c r="B44" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="C44" s="73" t="s">
+        <v>45</v>
+      </c>
+      <c r="D44" s="68" t="s">
+        <v>128</v>
+      </c>
+      <c r="E44" s="66" t="s">
+        <v>46</v>
+      </c>
+      <c r="F44" s="74">
+        <v>1</v>
+      </c>
+      <c r="G44" s="68">
+        <v>0</v>
+      </c>
+      <c r="H44" s="68">
+        <v>1</v>
+      </c>
+      <c r="I44" s="68">
+        <v>1</v>
+      </c>
+      <c r="J44" s="75">
+        <v>0</v>
+      </c>
+      <c r="K44" s="75">
+        <v>0</v>
+      </c>
+      <c r="L44" s="75">
+        <v>0</v>
+      </c>
+      <c r="M44" s="75">
+        <v>0</v>
+      </c>
+      <c r="N44" s="75">
+        <v>1</v>
+      </c>
+      <c r="O44" s="147" t="s">
+        <v>47</v>
+      </c>
+      <c r="P44" s="147"/>
+      <c r="Q44" s="147"/>
+      <c r="R44" s="147"/>
+      <c r="S44" s="147"/>
+      <c r="T44" s="147"/>
+      <c r="U44" s="148"/>
+      <c r="V44" s="22"/>
+      <c r="W44" s="19"/>
+      <c r="X44" s="19"/>
+      <c r="Y44" s="21"/>
+    </row>
+    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A45" s="82" t="s">
         <v>49</v>
       </c>
-      <c r="B44" s="36" t="s">
+      <c r="B45" s="36" t="s">
         <v>50</v>
       </c>
-      <c r="C44" s="36" t="s">
+      <c r="C45" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="D44" s="36"/>
-      <c r="E44" s="36"/>
-      <c r="F44" s="36">
-        <v>1</v>
-      </c>
-      <c r="G44" s="36">
-        <v>1</v>
-      </c>
-      <c r="H44" s="36">
-        <v>0</v>
-      </c>
-      <c r="I44" s="36">
-        <v>1</v>
-      </c>
-      <c r="J44" s="161" t="s">
-        <v>11</v>
-      </c>
-      <c r="K44" s="161"/>
-      <c r="L44" s="161"/>
-      <c r="M44" s="161"/>
-      <c r="N44" s="161"/>
-      <c r="O44" s="161"/>
-      <c r="P44" s="161"/>
-      <c r="Q44" s="161"/>
-      <c r="R44" s="161"/>
-      <c r="S44" s="161"/>
-      <c r="T44" s="161"/>
-      <c r="U44" s="165"/>
-      <c r="V44" s="42"/>
-      <c r="W44" s="36"/>
-      <c r="X44" s="36"/>
-      <c r="Y44" s="37"/>
-    </row>
-    <row r="45" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="82"/>
-      <c r="B45" s="36" t="s">
-        <v>52</v>
-      </c>
-      <c r="C45" s="36"/>
       <c r="D45" s="36"/>
       <c r="E45" s="36"/>
-      <c r="F45" s="36"/>
-      <c r="G45" s="36"/>
-      <c r="H45" s="36"/>
-      <c r="I45" s="36"/>
+      <c r="F45" s="36">
+        <v>1</v>
+      </c>
+      <c r="G45" s="36">
+        <v>1</v>
+      </c>
+      <c r="H45" s="36">
+        <v>0</v>
+      </c>
+      <c r="I45" s="36">
+        <v>1</v>
+      </c>
       <c r="J45" s="161" t="s">
-        <v>53</v>
+        <v>11</v>
       </c>
       <c r="K45" s="161"/>
       <c r="L45" s="161"/>
       <c r="M45" s="161"/>
-      <c r="N45" s="161" t="s">
-        <v>24</v>
-      </c>
+      <c r="N45" s="161"/>
       <c r="O45" s="161"/>
       <c r="P45" s="161"/>
       <c r="Q45" s="161"/>
@@ -6520,84 +6614,64 @@
       <c r="S45" s="161"/>
       <c r="T45" s="161"/>
       <c r="U45" s="165"/>
-      <c r="V45" s="42" t="s">
+      <c r="V45" s="42"/>
+      <c r="W45" s="36"/>
+      <c r="X45" s="36"/>
+      <c r="Y45" s="37"/>
+    </row>
+    <row r="46" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="82"/>
+      <c r="B46" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="C46" s="36"/>
+      <c r="D46" s="36"/>
+      <c r="E46" s="36"/>
+      <c r="F46" s="36"/>
+      <c r="G46" s="36"/>
+      <c r="H46" s="36"/>
+      <c r="I46" s="36"/>
+      <c r="J46" s="161" t="s">
+        <v>53</v>
+      </c>
+      <c r="K46" s="161"/>
+      <c r="L46" s="161"/>
+      <c r="M46" s="161"/>
+      <c r="N46" s="161" t="s">
+        <v>24</v>
+      </c>
+      <c r="O46" s="161"/>
+      <c r="P46" s="161"/>
+      <c r="Q46" s="161"/>
+      <c r="R46" s="161"/>
+      <c r="S46" s="161"/>
+      <c r="T46" s="161"/>
+      <c r="U46" s="165"/>
+      <c r="V46" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="W45" s="36" t="s">
+      <c r="W46" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="X45" s="36" t="s">
+      <c r="X46" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="Y45" s="37" t="s">
+      <c r="Y46" s="37" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A46" s="108" t="s">
-        <v>110</v>
-      </c>
-      <c r="B46" s="76" t="s">
-        <v>54</v>
-      </c>
-      <c r="C46" s="71" t="s">
-        <v>51</v>
-      </c>
-      <c r="D46" s="62"/>
-      <c r="E46" s="45"/>
-      <c r="F46" s="18">
-        <v>1</v>
-      </c>
-      <c r="G46" s="19">
-        <v>1</v>
-      </c>
-      <c r="H46" s="19">
-        <v>0</v>
-      </c>
-      <c r="I46" s="19">
-        <v>1</v>
-      </c>
-      <c r="J46" s="20">
-        <v>0</v>
-      </c>
-      <c r="K46" s="20">
-        <v>0</v>
-      </c>
-      <c r="L46" s="20">
-        <v>0</v>
-      </c>
-      <c r="M46" s="20">
-        <v>0</v>
-      </c>
-      <c r="N46" s="130" t="s">
-        <v>24</v>
-      </c>
-      <c r="O46" s="130"/>
-      <c r="P46" s="130"/>
-      <c r="Q46" s="130"/>
-      <c r="R46" s="130"/>
-      <c r="S46" s="130"/>
-      <c r="T46" s="130"/>
-      <c r="U46" s="132"/>
-      <c r="V46" s="22"/>
-      <c r="W46" s="19"/>
-      <c r="X46" s="19"/>
-      <c r="Y46" s="21">
-        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A47" s="108" t="s">
-        <v>111</v>
-      </c>
-      <c r="B47" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="C47" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="B47" s="76" t="s">
+        <v>54</v>
+      </c>
+      <c r="C47" s="71" t="s">
         <v>51</v>
       </c>
-      <c r="D47" s="19"/>
-      <c r="E47" s="21"/>
+      <c r="D47" s="62"/>
+      <c r="E47" s="45"/>
       <c r="F47" s="18">
         <v>1</v>
       </c>
@@ -6620,7 +6694,7 @@
         <v>0</v>
       </c>
       <c r="M47" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N47" s="130" t="s">
         <v>24</v>
@@ -6636,15 +6710,15 @@
       <c r="W47" s="19"/>
       <c r="X47" s="19"/>
       <c r="Y47" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A48" s="123" t="s">
-        <v>112</v>
+      <c r="A48" s="108" t="s">
+        <v>111</v>
       </c>
       <c r="B48" s="14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C48" s="18" t="s">
         <v>51</v>
@@ -6670,10 +6744,10 @@
         <v>0</v>
       </c>
       <c r="L48" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M48" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N48" s="130" t="s">
         <v>24</v>
@@ -6685,17 +6759,19 @@
       <c r="S48" s="130"/>
       <c r="T48" s="130"/>
       <c r="U48" s="132"/>
-      <c r="V48" s="22">
-        <v>1</v>
-      </c>
+      <c r="V48" s="22"/>
       <c r="W48" s="19"/>
       <c r="X48" s="19"/>
-      <c r="Y48" s="21"/>
+      <c r="Y48" s="21">
+        <v>0</v>
+      </c>
     </row>
     <row r="49" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A49" s="155"/>
+      <c r="A49" s="123" t="s">
+        <v>112</v>
+      </c>
       <c r="B49" s="14" t="s">
-        <v>129</v>
+        <v>56</v>
       </c>
       <c r="C49" s="18" t="s">
         <v>51</v>
@@ -6744,11 +6820,9 @@
       <c r="Y49" s="21"/>
     </row>
     <row r="50" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A50" s="156" t="s">
-        <v>113</v>
-      </c>
+      <c r="A50" s="155"/>
       <c r="B50" s="14" t="s">
-        <v>57</v>
+        <v>129</v>
       </c>
       <c r="C50" s="18" t="s">
         <v>51</v>
@@ -6777,7 +6851,7 @@
         <v>1</v>
       </c>
       <c r="M50" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N50" s="130" t="s">
         <v>24</v>
@@ -6790,16 +6864,18 @@
       <c r="T50" s="130"/>
       <c r="U50" s="132"/>
       <c r="V50" s="22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W50" s="19"/>
       <c r="X50" s="19"/>
       <c r="Y50" s="21"/>
     </row>
     <row r="51" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A51" s="157"/>
+      <c r="A51" s="156" t="s">
+        <v>113</v>
+      </c>
       <c r="B51" s="14" t="s">
-        <v>130</v>
+        <v>57</v>
       </c>
       <c r="C51" s="18" t="s">
         <v>51</v>
@@ -6848,11 +6924,9 @@
       <c r="Y51" s="21"/>
     </row>
     <row r="52" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A52" s="110" t="s">
-        <v>114</v>
-      </c>
+      <c r="A52" s="157"/>
       <c r="B52" s="14" t="s">
-        <v>58</v>
+        <v>130</v>
       </c>
       <c r="C52" s="18" t="s">
         <v>51</v>
@@ -6875,13 +6949,13 @@
         <v>0</v>
       </c>
       <c r="K52" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L52" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M52" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N52" s="130" t="s">
         <v>24</v>
@@ -6893,19 +6967,19 @@
       <c r="S52" s="130"/>
       <c r="T52" s="130"/>
       <c r="U52" s="132"/>
-      <c r="V52" s="22"/>
+      <c r="V52" s="22">
+        <v>0</v>
+      </c>
       <c r="W52" s="19"/>
-      <c r="X52" s="19">
-        <v>1</v>
-      </c>
+      <c r="X52" s="19"/>
       <c r="Y52" s="21"/>
     </row>
     <row r="53" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A53" s="110" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B53" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C53" s="18" t="s">
         <v>51</v>
@@ -6934,7 +7008,7 @@
         <v>0</v>
       </c>
       <c r="M53" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N53" s="130" t="s">
         <v>24</v>
@@ -6949,16 +7023,16 @@
       <c r="V53" s="22"/>
       <c r="W53" s="19"/>
       <c r="X53" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y53" s="21"/>
     </row>
     <row r="54" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A54" s="108" t="s">
-        <v>135</v>
+      <c r="A54" s="110" t="s">
+        <v>115</v>
       </c>
       <c r="B54" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C54" s="18" t="s">
         <v>51</v>
@@ -6984,10 +7058,10 @@
         <v>1</v>
       </c>
       <c r="L54" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M54" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N54" s="130" t="s">
         <v>24</v>
@@ -7000,18 +7074,18 @@
       <c r="T54" s="130"/>
       <c r="U54" s="132"/>
       <c r="V54" s="22"/>
-      <c r="W54" s="19">
-        <v>1</v>
-      </c>
-      <c r="X54" s="19"/>
+      <c r="W54" s="19"/>
+      <c r="X54" s="19">
+        <v>0</v>
+      </c>
       <c r="Y54" s="21"/>
     </row>
     <row r="55" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A55" s="108" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B55" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C55" s="18" t="s">
         <v>51</v>
@@ -7040,7 +7114,7 @@
         <v>1</v>
       </c>
       <c r="M55" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N55" s="130" t="s">
         <v>24</v>
@@ -7054,17 +7128,17 @@
       <c r="U55" s="132"/>
       <c r="V55" s="22"/>
       <c r="W55" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X55" s="19"/>
       <c r="Y55" s="21"/>
     </row>
     <row r="56" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A56" s="111" t="s">
-        <v>116</v>
+      <c r="A56" s="108" t="s">
+        <v>136</v>
       </c>
       <c r="B56" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C56" s="18" t="s">
         <v>51</v>
@@ -7084,16 +7158,16 @@
         <v>1</v>
       </c>
       <c r="J56" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K56" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L56" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M56" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N56" s="130" t="s">
         <v>24</v>
@@ -7105,19 +7179,19 @@
       <c r="S56" s="130"/>
       <c r="T56" s="130"/>
       <c r="U56" s="132"/>
-      <c r="V56" s="151" t="s">
-        <v>63</v>
-      </c>
-      <c r="W56" s="130"/>
-      <c r="X56" s="130"/>
-      <c r="Y56" s="132"/>
+      <c r="V56" s="22"/>
+      <c r="W56" s="19">
+        <v>0</v>
+      </c>
+      <c r="X56" s="19"/>
+      <c r="Y56" s="21"/>
     </row>
     <row r="57" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A57" s="111" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B57" s="14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C57" s="18" t="s">
         <v>51</v>
@@ -7146,7 +7220,7 @@
         <v>0</v>
       </c>
       <c r="M57" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N57" s="130" t="s">
         <v>24</v>
@@ -7159,7 +7233,7 @@
       <c r="T57" s="130"/>
       <c r="U57" s="132"/>
       <c r="V57" s="151" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="W57" s="130"/>
       <c r="X57" s="130"/>
@@ -7167,10 +7241,10 @@
     </row>
     <row r="58" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A58" s="111" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B58" s="14" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C58" s="18" t="s">
         <v>51</v>
@@ -7196,10 +7270,10 @@
         <v>0</v>
       </c>
       <c r="L58" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M58" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N58" s="130" t="s">
         <v>24</v>
@@ -7212,7 +7286,7 @@
       <c r="T58" s="130"/>
       <c r="U58" s="132"/>
       <c r="V58" s="151" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="W58" s="130"/>
       <c r="X58" s="130"/>
@@ -7220,10 +7294,10 @@
     </row>
     <row r="59" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A59" s="111" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B59" s="14" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C59" s="18" t="s">
         <v>51</v>
@@ -7252,7 +7326,7 @@
         <v>1</v>
       </c>
       <c r="M59" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N59" s="130" t="s">
         <v>24</v>
@@ -7265,19 +7339,18 @@
       <c r="T59" s="130"/>
       <c r="U59" s="132"/>
       <c r="V59" s="151" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="W59" s="130"/>
       <c r="X59" s="130"/>
       <c r="Y59" s="132"/>
-      <c r="Z59" s="102"/>
     </row>
     <row r="60" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A60" s="111" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B60" s="14" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C60" s="18" t="s">
         <v>51</v>
@@ -7300,13 +7373,13 @@
         <v>1</v>
       </c>
       <c r="K60" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L60" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M60" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N60" s="130" t="s">
         <v>24</v>
@@ -7319,7 +7392,7 @@
       <c r="T60" s="130"/>
       <c r="U60" s="132"/>
       <c r="V60" s="151" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="W60" s="130"/>
       <c r="X60" s="130"/>
@@ -7327,223 +7400,277 @@
       <c r="Z60" s="102"/>
     </row>
     <row r="61" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A61" s="109" t="s">
-        <v>121</v>
-      </c>
-      <c r="B61" s="93" t="s">
-        <v>72</v>
-      </c>
-      <c r="C61" s="92" t="s">
+      <c r="A61" s="111" t="s">
+        <v>120</v>
+      </c>
+      <c r="B61" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="C61" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="D61" s="56"/>
-      <c r="E61" s="59"/>
-      <c r="F61" s="92">
-        <v>1</v>
-      </c>
-      <c r="G61" s="56">
-        <v>1</v>
-      </c>
-      <c r="H61" s="56">
-        <v>0</v>
-      </c>
-      <c r="I61" s="56">
-        <v>1</v>
-      </c>
-      <c r="J61" s="101">
-        <v>1</v>
-      </c>
-      <c r="K61" s="101">
-        <v>1</v>
-      </c>
-      <c r="L61" s="101">
-        <v>0</v>
-      </c>
-      <c r="M61" s="101">
-        <v>1</v>
-      </c>
-      <c r="N61" s="121" t="s">
+      <c r="D61" s="19"/>
+      <c r="E61" s="21"/>
+      <c r="F61" s="18">
+        <v>1</v>
+      </c>
+      <c r="G61" s="19">
+        <v>1</v>
+      </c>
+      <c r="H61" s="19">
+        <v>0</v>
+      </c>
+      <c r="I61" s="19">
+        <v>1</v>
+      </c>
+      <c r="J61" s="20">
+        <v>1</v>
+      </c>
+      <c r="K61" s="20">
+        <v>1</v>
+      </c>
+      <c r="L61" s="20">
+        <v>0</v>
+      </c>
+      <c r="M61" s="20">
+        <v>0</v>
+      </c>
+      <c r="N61" s="130" t="s">
         <v>24</v>
       </c>
-      <c r="O61" s="121"/>
-      <c r="P61" s="121"/>
-      <c r="Q61" s="121"/>
-      <c r="R61" s="121"/>
-      <c r="S61" s="121"/>
-      <c r="T61" s="121"/>
-      <c r="U61" s="150"/>
-      <c r="V61" s="120" t="s">
-        <v>73</v>
-      </c>
-      <c r="W61" s="121"/>
-      <c r="X61" s="121"/>
-      <c r="Y61" s="150"/>
+      <c r="O61" s="130"/>
+      <c r="P61" s="130"/>
+      <c r="Q61" s="130"/>
+      <c r="R61" s="130"/>
+      <c r="S61" s="130"/>
+      <c r="T61" s="130"/>
+      <c r="U61" s="132"/>
+      <c r="V61" s="151" t="s">
+        <v>71</v>
+      </c>
+      <c r="W61" s="130"/>
+      <c r="X61" s="130"/>
+      <c r="Y61" s="132"/>
+      <c r="Z61" s="102"/>
     </row>
     <row r="62" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A62" s="123" t="s">
+      <c r="A62" s="109" t="s">
+        <v>121</v>
+      </c>
+      <c r="B62" s="93" t="s">
+        <v>72</v>
+      </c>
+      <c r="C62" s="92" t="s">
+        <v>51</v>
+      </c>
+      <c r="D62" s="56"/>
+      <c r="E62" s="59"/>
+      <c r="F62" s="92">
+        <v>1</v>
+      </c>
+      <c r="G62" s="56">
+        <v>1</v>
+      </c>
+      <c r="H62" s="56">
+        <v>0</v>
+      </c>
+      <c r="I62" s="56">
+        <v>1</v>
+      </c>
+      <c r="J62" s="101">
+        <v>1</v>
+      </c>
+      <c r="K62" s="101">
+        <v>1</v>
+      </c>
+      <c r="L62" s="101">
+        <v>0</v>
+      </c>
+      <c r="M62" s="101">
+        <v>1</v>
+      </c>
+      <c r="N62" s="121" t="s">
+        <v>24</v>
+      </c>
+      <c r="O62" s="121"/>
+      <c r="P62" s="121"/>
+      <c r="Q62" s="121"/>
+      <c r="R62" s="121"/>
+      <c r="S62" s="121"/>
+      <c r="T62" s="121"/>
+      <c r="U62" s="150"/>
+      <c r="V62" s="120" t="s">
+        <v>73</v>
+      </c>
+      <c r="W62" s="121"/>
+      <c r="X62" s="121"/>
+      <c r="Y62" s="150"/>
+    </row>
+    <row r="63" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A63" s="123" t="s">
         <v>127</v>
       </c>
-      <c r="B62" s="14" t="s">
+      <c r="B63" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="C62" s="18" t="s">
+      <c r="C63" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="D62" s="19"/>
-      <c r="E62" s="47"/>
-      <c r="F62" s="22">
-        <v>1</v>
-      </c>
-      <c r="G62" s="19">
-        <v>1</v>
-      </c>
-      <c r="H62" s="19">
-        <v>1</v>
-      </c>
-      <c r="I62" s="19">
-        <v>0</v>
-      </c>
-      <c r="J62" s="19">
-        <v>0</v>
-      </c>
-      <c r="K62" s="152" t="s">
+      <c r="D63" s="19"/>
+      <c r="E63" s="47"/>
+      <c r="F63" s="22">
+        <v>1</v>
+      </c>
+      <c r="G63" s="19">
+        <v>1</v>
+      </c>
+      <c r="H63" s="19">
+        <v>1</v>
+      </c>
+      <c r="I63" s="19">
+        <v>0</v>
+      </c>
+      <c r="J63" s="19">
+        <v>0</v>
+      </c>
+      <c r="K63" s="152" t="s">
         <v>126</v>
       </c>
-      <c r="L62" s="153"/>
-      <c r="M62" s="153"/>
-      <c r="N62" s="153"/>
-      <c r="O62" s="153"/>
-      <c r="P62" s="153"/>
-      <c r="Q62" s="153"/>
-      <c r="R62" s="153"/>
-      <c r="S62" s="153"/>
-      <c r="T62" s="153"/>
-      <c r="U62" s="154"/>
-      <c r="V62" s="151"/>
-      <c r="W62" s="130"/>
-      <c r="X62" s="130"/>
-      <c r="Y62" s="152"/>
+      <c r="L63" s="153"/>
+      <c r="M63" s="153"/>
+      <c r="N63" s="153"/>
+      <c r="O63" s="153"/>
+      <c r="P63" s="153"/>
+      <c r="Q63" s="153"/>
+      <c r="R63" s="153"/>
+      <c r="S63" s="153"/>
+      <c r="T63" s="153"/>
+      <c r="U63" s="154"/>
+      <c r="V63" s="151"/>
+      <c r="W63" s="130"/>
+      <c r="X63" s="130"/>
+      <c r="Y63" s="152"/>
     </row>
-    <row r="63" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="124"/>
-      <c r="B63" s="104" t="s">
+    <row r="64" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="124"/>
+      <c r="B64" s="104" t="s">
         <v>125</v>
       </c>
-      <c r="C63" s="54" t="s">
+      <c r="C64" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="D63" s="56"/>
-      <c r="E63" s="57"/>
-      <c r="F63" s="54">
-        <v>1</v>
-      </c>
-      <c r="G63" s="56">
-        <v>1</v>
-      </c>
-      <c r="H63" s="56">
-        <v>1</v>
-      </c>
-      <c r="I63" s="56">
-        <v>0</v>
-      </c>
-      <c r="J63" s="56">
-        <v>0</v>
-      </c>
-      <c r="K63" s="117" t="s">
+      <c r="D64" s="56"/>
+      <c r="E64" s="57"/>
+      <c r="F64" s="54">
+        <v>1</v>
+      </c>
+      <c r="G64" s="56">
+        <v>1</v>
+      </c>
+      <c r="H64" s="56">
+        <v>1</v>
+      </c>
+      <c r="I64" s="56">
+        <v>0</v>
+      </c>
+      <c r="J64" s="56">
+        <v>0</v>
+      </c>
+      <c r="K64" s="117" t="s">
         <v>126</v>
       </c>
-      <c r="L63" s="118"/>
-      <c r="M63" s="118"/>
-      <c r="N63" s="118"/>
-      <c r="O63" s="118"/>
-      <c r="P63" s="118"/>
-      <c r="Q63" s="118"/>
-      <c r="R63" s="118"/>
-      <c r="S63" s="118"/>
-      <c r="T63" s="118"/>
-      <c r="U63" s="119"/>
-      <c r="V63" s="120"/>
-      <c r="W63" s="121"/>
-      <c r="X63" s="121"/>
-      <c r="Y63" s="122"/>
+      <c r="L64" s="118"/>
+      <c r="M64" s="118"/>
+      <c r="N64" s="118"/>
+      <c r="O64" s="118"/>
+      <c r="P64" s="118"/>
+      <c r="Q64" s="118"/>
+      <c r="R64" s="118"/>
+      <c r="S64" s="118"/>
+      <c r="T64" s="118"/>
+      <c r="U64" s="119"/>
+      <c r="V64" s="120"/>
+      <c r="W64" s="121"/>
+      <c r="X64" s="121"/>
+      <c r="Y64" s="122"/>
     </row>
-    <row r="64" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A64" s="105"/>
-      <c r="B64" s="106"/>
-      <c r="C64" s="103"/>
-      <c r="D64" s="103"/>
-      <c r="E64" s="103"/>
-      <c r="F64" s="103"/>
-      <c r="G64" s="103"/>
-      <c r="H64" s="103"/>
-      <c r="I64" s="103"/>
-      <c r="J64" s="103"/>
-      <c r="K64" s="103"/>
-      <c r="L64" s="103"/>
-      <c r="M64" s="103"/>
-      <c r="N64" s="103"/>
-      <c r="O64" s="103"/>
-      <c r="P64" s="103"/>
-      <c r="Q64" s="103"/>
-      <c r="R64" s="103"/>
-      <c r="S64" s="103"/>
-      <c r="T64" s="103"/>
-      <c r="U64" s="103"/>
-      <c r="V64" s="103"/>
-      <c r="W64" s="103"/>
-      <c r="X64" s="103"/>
-      <c r="Y64" s="103"/>
+    <row r="65" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A65" s="105"/>
+      <c r="B65" s="106"/>
+      <c r="C65" s="103"/>
+      <c r="D65" s="103"/>
+      <c r="E65" s="103"/>
+      <c r="F65" s="103"/>
+      <c r="G65" s="103"/>
+      <c r="H65" s="103"/>
+      <c r="I65" s="103"/>
+      <c r="J65" s="103"/>
+      <c r="K65" s="103"/>
+      <c r="L65" s="103"/>
+      <c r="M65" s="103"/>
+      <c r="N65" s="103"/>
+      <c r="O65" s="103"/>
+      <c r="P65" s="103"/>
+      <c r="Q65" s="103"/>
+      <c r="R65" s="103"/>
+      <c r="S65" s="103"/>
+      <c r="T65" s="103"/>
+      <c r="U65" s="103"/>
+      <c r="V65" s="103"/>
+      <c r="W65" s="103"/>
+      <c r="X65" s="103"/>
+      <c r="Y65" s="103"/>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B65" s="81"/>
-    </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B66" s="81"/>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B67" s="81"/>
     </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B68" s="81"/>
     </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B69" s="81"/>
     </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B70" s="81"/>
     </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B71" s="81"/>
     </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B72" s="81"/>
     </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B73" s="81"/>
     </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B74" s="81"/>
     </row>
+    <row r="75" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B75" s="81"/>
+    </row>
   </sheetData>
-  <mergeCells count="117">
-    <mergeCell ref="J44:M44"/>
-    <mergeCell ref="N44:U44"/>
+  <mergeCells count="120">
     <mergeCell ref="J45:M45"/>
     <mergeCell ref="N45:U45"/>
-    <mergeCell ref="N48:U48"/>
-    <mergeCell ref="N50:U50"/>
-    <mergeCell ref="M35:O35"/>
-    <mergeCell ref="S35:U35"/>
-    <mergeCell ref="P35:R35"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="J46:M46"/>
+    <mergeCell ref="N46:U46"/>
+    <mergeCell ref="N49:U49"/>
+    <mergeCell ref="N51:U51"/>
+    <mergeCell ref="M36:O36"/>
+    <mergeCell ref="S36:U36"/>
+    <mergeCell ref="P36:R36"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="A51:A52"/>
     <mergeCell ref="P33:R33"/>
     <mergeCell ref="S33:U33"/>
     <mergeCell ref="K14:M14"/>
     <mergeCell ref="N14:U14"/>
-    <mergeCell ref="N53:U53"/>
-    <mergeCell ref="O42:U42"/>
-    <mergeCell ref="J41:P41"/>
+    <mergeCell ref="N54:U54"/>
+    <mergeCell ref="O43:U43"/>
+    <mergeCell ref="J42:P42"/>
     <mergeCell ref="P19:R19"/>
     <mergeCell ref="P20:R20"/>
     <mergeCell ref="P21:R21"/>
@@ -7559,42 +7686,45 @@
     <mergeCell ref="S21:U21"/>
     <mergeCell ref="S22:U22"/>
     <mergeCell ref="S23:U23"/>
-    <mergeCell ref="K40:M40"/>
-    <mergeCell ref="N40:U40"/>
-    <mergeCell ref="V61:Y61"/>
+    <mergeCell ref="K41:M41"/>
+    <mergeCell ref="N41:U41"/>
     <mergeCell ref="V62:Y62"/>
-    <mergeCell ref="N56:U56"/>
+    <mergeCell ref="V63:Y63"/>
     <mergeCell ref="N57:U57"/>
     <mergeCell ref="N58:U58"/>
     <mergeCell ref="N59:U59"/>
     <mergeCell ref="N60:U60"/>
-    <mergeCell ref="V56:Y56"/>
+    <mergeCell ref="N61:U61"/>
     <mergeCell ref="V57:Y57"/>
     <mergeCell ref="V58:Y58"/>
     <mergeCell ref="V59:Y59"/>
     <mergeCell ref="V60:Y60"/>
-    <mergeCell ref="N61:U61"/>
-    <mergeCell ref="K62:U62"/>
-    <mergeCell ref="N54:U54"/>
+    <mergeCell ref="V61:Y61"/>
+    <mergeCell ref="N62:U62"/>
+    <mergeCell ref="K63:U63"/>
     <mergeCell ref="N55:U55"/>
-    <mergeCell ref="N46:U46"/>
+    <mergeCell ref="N56:U56"/>
     <mergeCell ref="N47:U47"/>
-    <mergeCell ref="N49:U49"/>
-    <mergeCell ref="N51:U51"/>
+    <mergeCell ref="N48:U48"/>
+    <mergeCell ref="N50:U50"/>
     <mergeCell ref="N52:U52"/>
-    <mergeCell ref="O43:U43"/>
+    <mergeCell ref="N53:U53"/>
+    <mergeCell ref="O44:U44"/>
     <mergeCell ref="S24:U24"/>
     <mergeCell ref="S25:U25"/>
     <mergeCell ref="S26:U26"/>
-    <mergeCell ref="D37:E37"/>
     <mergeCell ref="D38:E38"/>
-    <mergeCell ref="K37:M37"/>
-    <mergeCell ref="N37:U37"/>
+    <mergeCell ref="D39:E39"/>
     <mergeCell ref="K38:M38"/>
     <mergeCell ref="N38:U38"/>
+    <mergeCell ref="K39:M39"/>
+    <mergeCell ref="N39:U39"/>
     <mergeCell ref="P28:R28"/>
     <mergeCell ref="P29:R29"/>
     <mergeCell ref="P30:R30"/>
+    <mergeCell ref="M35:O35"/>
+    <mergeCell ref="P35:R35"/>
+    <mergeCell ref="S35:U35"/>
     <mergeCell ref="V1:Y1"/>
     <mergeCell ref="P16:R16"/>
     <mergeCell ref="S16:U16"/>
@@ -7619,9 +7749,9 @@
     <mergeCell ref="N13:U13"/>
     <mergeCell ref="K12:M12"/>
     <mergeCell ref="N12:U12"/>
-    <mergeCell ref="K63:U63"/>
-    <mergeCell ref="V63:Y63"/>
-    <mergeCell ref="A62:A63"/>
+    <mergeCell ref="K64:U64"/>
+    <mergeCell ref="V64:Y64"/>
+    <mergeCell ref="A63:A64"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="B1:E1"/>
@@ -7645,131 +7775,165 @@
     <mergeCell ref="P24:R24"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="F62:K63">
-    <cfRule type="cellIs" dxfId="45" priority="36" operator="equal">
+  <conditionalFormatting sqref="F63:K64">
+    <cfRule type="cellIs" dxfId="55" priority="46" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="44" priority="37" operator="containsText" text="imm">
-      <formula>NOT(ISERROR(SEARCH("imm",F62)))</formula>
+    <cfRule type="containsText" dxfId="54" priority="47" operator="containsText" text="imm">
+      <formula>NOT(ISERROR(SEARCH("imm",F63)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="48" operator="equal">
       <formula>"imm3"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="49" operator="equal">
       <formula>"imm5"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F4:U61">
-    <cfRule type="cellIs" dxfId="8" priority="45" operator="equal">
+  <conditionalFormatting sqref="F4:U62">
+    <cfRule type="cellIs" dxfId="51" priority="55" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F45:M45 V45:Y45 F46:Y61 V62:Y63 F1:Y44">
-    <cfRule type="containsText" dxfId="7" priority="46" operator="containsText" text="imm">
+  <conditionalFormatting sqref="F46:M46 V46:Y46 F47:Y62 V63:Y64 F1:Y45">
+    <cfRule type="containsText" dxfId="50" priority="56" operator="containsText" text="imm">
       <formula>NOT(ISERROR(SEARCH("imm",F1)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="57" operator="equal">
       <formula>"imm3"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="58" operator="equal">
       <formula>"imm5"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H40:M40">
-    <cfRule type="cellIs" dxfId="41" priority="12" operator="equal">
+  <conditionalFormatting sqref="H41:M41">
+    <cfRule type="cellIs" dxfId="47" priority="22" operator="equal">
       <formula>"Rn"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="24" operator="equal">
       <formula>"Rdn"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="25" operator="equal">
       <formula>"Rm"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="26" operator="equal">
       <formula>"Rd"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="28" operator="equal">
       <formula>"Rd"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:U31">
-    <cfRule type="cellIs" dxfId="36" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="59" operator="equal">
       <formula>"Rd"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="60" operator="equal">
       <formula>"Rn"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="61" operator="equal">
       <formula>"Rd"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="62" operator="equal">
       <formula>"Rdn"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="63" operator="equal">
       <formula>"Rm"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H33:U33">
-    <cfRule type="cellIs" dxfId="31" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="50" operator="equal">
       <formula>"Rd"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="51" operator="equal">
       <formula>"Rn"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="52" operator="equal">
       <formula>"Rd"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="53" operator="equal">
       <formula>"Rdn"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="54" operator="equal">
       <formula>"Rm"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K40:M40">
-    <cfRule type="cellIs" dxfId="26" priority="11" operator="equal">
+  <conditionalFormatting sqref="K41:M41">
+    <cfRule type="cellIs" dxfId="32" priority="21" operator="equal">
       <formula>"Rd"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="23" operator="equal">
       <formula>"Rd"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P16:R16">
-    <cfRule type="cellIs" dxfId="24" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="64" operator="equal">
+      <formula>"Rm"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M36:O36">
+    <cfRule type="cellIs" dxfId="29" priority="16" operator="equal">
+      <formula>"Rd"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="17" operator="equal">
+      <formula>"Rn"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="27" priority="18" operator="equal">
+      <formula>"Rd"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="19" operator="equal">
+      <formula>"Rdn"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="25" priority="20" operator="equal">
+      <formula>"Rm"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P36:R36">
+    <cfRule type="cellIs" dxfId="24" priority="11" operator="equal">
+      <formula>"Rd"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="23" priority="12" operator="equal">
+      <formula>"Rn"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="13" operator="equal">
+      <formula>"Rd"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="21" priority="14" operator="equal">
+      <formula>"Rdn"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="15" operator="equal">
       <formula>"Rm"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M35:O35">
-    <cfRule type="cellIs" dxfId="23" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="6" operator="equal">
       <formula>"Rd"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
       <formula>"Rn"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
       <formula>"Rd"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="9" operator="equal">
       <formula>"Rdn"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="10" operator="equal">
       <formula>"Rm"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P35:R35">
-    <cfRule type="cellIs" dxfId="18" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
       <formula>"Rd"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>"Rn"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"Rd"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
       <formula>"Rdn"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="5" operator="equal">
       <formula>"Rm"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>